<commit_message>
Added code for icons. Added them to Chapter 1 About panel
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wilkinson_audrey_epa_gov/Documents/Documents/Projects/Metro-CERI/FY22/ERB/Static_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{AE9160BF-963E-4238-BF53-C2D836C009B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16CAD98C-BE73-4154-894D-65AD9D937C84}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E27E00-9E7D-4C7A-B951-34351BBFACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -626,6 +626,90 @@
   </si>
   <si>
     <t>00000002</t>
+  </si>
+  <si>
+    <t>Word cloud</t>
+  </si>
+  <si>
+    <t>000000001</t>
+  </si>
+  <si>
+    <t>000000002</t>
+  </si>
+  <si>
+    <t>000000003</t>
+  </si>
+  <si>
+    <t>People and Lightbulb (Centering Equity)</t>
+  </si>
+  <si>
+    <t>Clock Image (Planning)</t>
+  </si>
+  <si>
+    <t>Clipboard (Planning)</t>
+  </si>
+  <si>
+    <t>000000004</t>
+  </si>
+  <si>
+    <t>Tiers of People (Centering Equity)</t>
+  </si>
+  <si>
+    <t>000000005</t>
+  </si>
+  <si>
+    <t>Microphone (Centering Equity)</t>
+  </si>
+  <si>
+    <t>000000006</t>
+  </si>
+  <si>
+    <t>000000007</t>
+  </si>
+  <si>
+    <t>000000008</t>
+  </si>
+  <si>
+    <t>000000009</t>
+  </si>
+  <si>
+    <t>Headphones (Centering Equity)</t>
+  </si>
+  <si>
+    <t>Teacher and Students with Board (Centering Equity)</t>
+  </si>
+  <si>
+    <t>People around Table (Planning)</t>
+  </si>
+  <si>
+    <t>Scroll with Swirls (Planning)</t>
+  </si>
+  <si>
+    <t>000000010</t>
+  </si>
+  <si>
+    <t>Cloud with Lightening (Centering Equity)</t>
+  </si>
+  <si>
+    <t>000000011</t>
+  </si>
+  <si>
+    <t>Person Balancing (Centering Equity)</t>
+  </si>
+  <si>
+    <t>Icons</t>
+  </si>
+  <si>
+    <t>000000012</t>
+  </si>
+  <si>
+    <t>Checkmark</t>
+  </si>
+  <si>
+    <t>000000013</t>
+  </si>
+  <si>
+    <t>Bullet Point</t>
   </si>
 </sst>
 </file>
@@ -925,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1073,15 +1157,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1474,10 +1561,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="76"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -1494,7 +1581,7 @@
       <c r="V2" s="23"/>
     </row>
     <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="75" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="45" t="s">
@@ -3260,10 +3347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3271,13 +3358,13 @@
     <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="76" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.77734375" customWidth="1"/>
     <col min="12" max="12" width="86.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.77734375" customWidth="1"/>
@@ -3285,7 +3372,7 @@
     <col min="16" max="16" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
         <v>93</v>
       </c>
@@ -3310,8 +3397,9 @@
       <c r="H1" s="66" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="79"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
         <v>93</v>
       </c>
@@ -3337,7 +3425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
         <v>94</v>
       </c>
@@ -3363,7 +3451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="63" t="s">
         <v>95</v>
       </c>
@@ -3389,7 +3477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="63" t="s">
         <v>96</v>
       </c>
@@ -3411,7 +3499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
         <v>97</v>
       </c>
@@ -3421,7 +3509,7 @@
       <c r="C6" s="59"/>
       <c r="D6" s="59"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
         <v>114</v>
       </c>
@@ -3431,7 +3519,7 @@
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="64" t="s">
         <v>115</v>
       </c>
@@ -3441,7 +3529,7 @@
       <c r="C8" s="59"/>
       <c r="D8" s="59"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="65" t="s">
         <v>97</v>
       </c>
@@ -3466,8 +3554,14 @@
       <c r="H11" s="66" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="80">
+        <v>9</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="63" t="s">
         <v>101</v>
       </c>
@@ -3492,8 +3586,14 @@
       <c r="H12" s="58" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="J12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
         <v>102</v>
       </c>
@@ -3512,8 +3612,20 @@
       <c r="F13" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I13" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="J13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="63" t="s">
         <v>103</v>
       </c>
@@ -3532,8 +3644,14 @@
       <c r="F14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="J14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="63" t="s">
         <v>104</v>
       </c>
@@ -3552,8 +3670,14 @@
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="J15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="64" t="s">
         <v>105</v>
       </c>
@@ -3572,8 +3696,14 @@
       <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I16" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="J16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="63" t="s">
         <v>122</v>
       </c>
@@ -3586,8 +3716,14 @@
       <c r="F17" s="58" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I17" s="76" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" s="63" t="s">
         <v>123</v>
       </c>
@@ -3595,8 +3731,14 @@
         <v>20</v>
       </c>
       <c r="E18" s="67"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I18" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="J18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C19" s="63" t="s">
         <v>124</v>
       </c>
@@ -3604,8 +3746,14 @@
         <v>21</v>
       </c>
       <c r="E19" s="67"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I19" s="76" t="s">
+        <v>209</v>
+      </c>
+      <c r="J19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" s="63" t="s">
         <v>125</v>
       </c>
@@ -3613,8 +3761,14 @@
         <v>9</v>
       </c>
       <c r="E20" s="67"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I20" s="76" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C21" s="63" t="s">
         <v>126</v>
       </c>
@@ -3622,8 +3776,14 @@
         <v>37</v>
       </c>
       <c r="E21" s="67"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I21" s="76" t="s">
+        <v>215</v>
+      </c>
+      <c r="J21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" s="63" t="s">
         <v>127</v>
       </c>
@@ -3631,8 +3791,14 @@
         <v>38</v>
       </c>
       <c r="E22" s="67"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I22" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="J22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" s="63" t="s">
         <v>128</v>
       </c>
@@ -3640,8 +3806,14 @@
         <v>39</v>
       </c>
       <c r="E23" s="67"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I23" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="J23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" s="63" t="s">
         <v>129</v>
       </c>
@@ -3649,8 +3821,14 @@
         <v>12</v>
       </c>
       <c r="E24" s="67"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I24" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" s="63" t="s">
         <v>130</v>
       </c>
@@ -3659,7 +3837,7 @@
       </c>
       <c r="E25" s="67"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" s="63" t="s">
         <v>131</v>
       </c>
@@ -3668,7 +3846,7 @@
       </c>
       <c r="E26" s="67"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C27" s="63" t="s">
         <v>132</v>
       </c>
@@ -3677,7 +3855,7 @@
       </c>
       <c r="E27" s="67"/>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="63" t="s">
         <v>133</v>
       </c>
@@ -3686,7 +3864,7 @@
       </c>
       <c r="E28" s="67"/>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C29" s="63" t="s">
         <v>134</v>
       </c>
@@ -3695,7 +3873,7 @@
       </c>
       <c r="E29" s="67"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C30" s="63" t="s">
         <v>135</v>
       </c>
@@ -3704,7 +3882,7 @@
       </c>
       <c r="E30" s="67"/>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C31" s="63" t="s">
         <v>136</v>
       </c>
@@ -3713,7 +3891,7 @@
       </c>
       <c r="E31" s="67"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C32" s="63" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
Added Chapter 2 content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E27E00-9E7D-4C7A-B951-34351BBFACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24391FB-D39C-4A1F-974F-61DE53B761F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="9576" yWindow="168" windowWidth="13464" windowHeight="12360" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="231">
   <si>
     <t>ID</t>
   </si>
@@ -710,6 +710,27 @@
   </si>
   <si>
     <t>Bullet Point</t>
+  </si>
+  <si>
+    <t>000031</t>
+  </si>
+  <si>
+    <t>Set goals for using ERB</t>
+  </si>
+  <si>
+    <t>Select activites to do in ERB</t>
+  </si>
+  <si>
+    <t>Centering Equity</t>
+  </si>
+  <si>
+    <t>000032</t>
+  </si>
+  <si>
+    <t>000033</t>
+  </si>
+  <si>
+    <t>Start Engaging!</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1161,14 +1182,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1561,10 +1584,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="77" t="s">
+      <c r="G2" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="78"/>
+      <c r="H2" s="80"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -3347,17 +3370,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="76" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="86.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
@@ -3397,7 +3420,7 @@
       <c r="H1" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="79"/>
+      <c r="I1" s="77"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
@@ -3484,7 +3507,7 @@
       <c r="B5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="59"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="59"/>
       <c r="E5" s="64" t="s">
         <v>92</v>
@@ -3506,7 +3529,7 @@
       <c r="B6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="59"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="59"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -3516,7 +3539,7 @@
       <c r="B7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="59"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="59"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3526,7 +3549,7 @@
       <c r="B8" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="59"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -3554,7 +3577,7 @@
       <c r="H11" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="80">
+      <c r="I11" s="78">
         <v>9</v>
       </c>
       <c r="J11" s="66" t="s">
@@ -3604,7 +3627,7 @@
         <v>118</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>6</v>
+        <v>226</v>
       </c>
       <c r="E13" s="63" t="s">
         <v>107</v>
@@ -3980,6 +4003,30 @@
         <v>9</v>
       </c>
       <c r="E41" s="67"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C42" s="76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="81" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="76" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="76" t="s">
+        <v>229</v>
+      </c>
+      <c r="D44" s="81" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed sizing of icons
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24391FB-D39C-4A1F-974F-61DE53B761F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE39781-54D9-445E-882C-FD6708BDD075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9576" yWindow="168" windowWidth="13464" windowHeight="12360" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="248">
   <si>
     <t>ID</t>
   </si>
@@ -731,6 +731,57 @@
   </si>
   <si>
     <t>Start Engaging!</t>
+  </si>
+  <si>
+    <t>Introduction to examples</t>
+  </si>
+  <si>
+    <t>0000008</t>
+  </si>
+  <si>
+    <t>Goal setting examples</t>
+  </si>
+  <si>
+    <t>Activity selection examples</t>
+  </si>
+  <si>
+    <t>Summary Output form</t>
+  </si>
+  <si>
+    <t>0000009</t>
+  </si>
+  <si>
+    <t>0000010</t>
+  </si>
+  <si>
+    <t>000000014</t>
+  </si>
+  <si>
+    <t>000000015</t>
+  </si>
+  <si>
+    <t>000000016</t>
+  </si>
+  <si>
+    <t>000000017</t>
+  </si>
+  <si>
+    <t>000000018</t>
+  </si>
+  <si>
+    <t>Community example 1</t>
+  </si>
+  <si>
+    <t>Community example 2</t>
+  </si>
+  <si>
+    <t>Community example 3</t>
+  </si>
+  <si>
+    <t>Goal setting table</t>
+  </si>
+  <si>
+    <t>Activity selection table</t>
   </si>
 </sst>
 </file>
@@ -3372,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3717,7 +3768,7 @@
         <v>110</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="I16" s="76" t="s">
         <v>205</v>
@@ -3733,11 +3784,11 @@
       <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="64" t="s">
+      <c r="E17" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="F17" s="58" t="s">
-        <v>26</v>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I17" s="76" t="s">
         <v>207</v>
@@ -3753,7 +3804,12 @@
       <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="67"/>
+      <c r="E18" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>26</v>
+      </c>
       <c r="I18" s="76" t="s">
         <v>208</v>
       </c>
@@ -3768,7 +3824,12 @@
       <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="67" t="s">
+        <v>232</v>
+      </c>
+      <c r="F19" s="81" t="s">
+        <v>231</v>
+      </c>
       <c r="I19" s="76" t="s">
         <v>209</v>
       </c>
@@ -3783,7 +3844,12 @@
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="67" t="s">
+        <v>236</v>
+      </c>
+      <c r="F20" s="81" t="s">
+        <v>233</v>
+      </c>
       <c r="I20" s="76" t="s">
         <v>210</v>
       </c>
@@ -3798,7 +3864,12 @@
       <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="67"/>
+      <c r="E21" s="67" t="s">
+        <v>237</v>
+      </c>
+      <c r="F21" s="81" t="s">
+        <v>234</v>
+      </c>
       <c r="I21" s="76" t="s">
         <v>215</v>
       </c>
@@ -3859,6 +3930,12 @@
         <v>13</v>
       </c>
       <c r="E25" s="67"/>
+      <c r="I25" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="J25" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" s="63" t="s">
@@ -3868,6 +3945,12 @@
         <v>40</v>
       </c>
       <c r="E26" s="67"/>
+      <c r="I26" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="J26" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C27" s="63" t="s">
@@ -3877,6 +3960,12 @@
         <v>41</v>
       </c>
       <c r="E27" s="67"/>
+      <c r="I27" s="76" t="s">
+        <v>240</v>
+      </c>
+      <c r="J27" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="63" t="s">
@@ -3886,6 +3975,12 @@
         <v>9</v>
       </c>
       <c r="E28" s="67"/>
+      <c r="I28" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="J28" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C29" s="63" t="s">
@@ -3895,6 +3990,12 @@
         <v>14</v>
       </c>
       <c r="E29" s="67"/>
+      <c r="I29" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="J29" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C30" s="63" t="s">
@@ -4011,6 +4112,7 @@
       <c r="D42" s="81" t="s">
         <v>225</v>
       </c>
+      <c r="E42" s="67"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="76" t="s">

</xml_diff>

<commit_message>
Updated Activity ID chart
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE39781-54D9-445E-882C-FD6708BDD075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60222997-DB43-4DC3-9333-97D113B54C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-13635" yWindow="1350" windowWidth="13470" windowHeight="16980" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="256">
   <si>
     <t>ID</t>
   </si>
@@ -769,6 +769,18 @@
     <t>000000018</t>
   </si>
   <si>
+    <t>000000019</t>
+  </si>
+  <si>
+    <t>000000020</t>
+  </si>
+  <si>
+    <t>000000021</t>
+  </si>
+  <si>
+    <t>000000022</t>
+  </si>
+  <si>
     <t>Community example 1</t>
   </si>
   <si>
@@ -782,6 +794,18 @@
   </si>
   <si>
     <t>Activity selection table</t>
+  </si>
+  <si>
+    <t>Heart in Circle</t>
+  </si>
+  <si>
+    <t>Person in Circle with Node Branches</t>
+  </si>
+  <si>
+    <t>Infinity Symbol</t>
+  </si>
+  <si>
+    <t>Shield with Checkmark</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1243,6 +1267,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3423,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3930,11 +3956,11 @@
         <v>13</v>
       </c>
       <c r="E25" s="67"/>
-      <c r="I25" s="76" t="s">
+      <c r="I25" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="J25" t="s">
-        <v>243</v>
+      <c r="J25" s="84" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
@@ -3945,11 +3971,11 @@
         <v>40</v>
       </c>
       <c r="E26" s="67"/>
-      <c r="I26" s="76" t="s">
+      <c r="I26" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="J26" t="s">
-        <v>244</v>
+      <c r="J26" s="84" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.3">
@@ -3960,11 +3986,11 @@
         <v>41</v>
       </c>
       <c r="E27" s="67"/>
-      <c r="I27" s="76" t="s">
+      <c r="I27" s="83" t="s">
         <v>240</v>
       </c>
-      <c r="J27" t="s">
-        <v>245</v>
+      <c r="J27" s="84" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.3">
@@ -3975,11 +4001,11 @@
         <v>9</v>
       </c>
       <c r="E28" s="67"/>
-      <c r="I28" s="76" t="s">
+      <c r="I28" s="83" t="s">
         <v>241</v>
       </c>
-      <c r="J28" t="s">
-        <v>246</v>
+      <c r="J28" s="84" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.3">
@@ -4005,6 +4031,12 @@
         <v>15</v>
       </c>
       <c r="E30" s="67"/>
+      <c r="I30" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="J30" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C31" s="63" t="s">
@@ -4014,6 +4046,12 @@
         <v>24</v>
       </c>
       <c r="E31" s="67"/>
+      <c r="I31" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="J31" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C32" s="63" t="s">
@@ -4023,8 +4061,14 @@
         <v>9</v>
       </c>
       <c r="E32" s="67"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I32" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="J32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="63" t="s">
         <v>138</v>
       </c>
@@ -4032,8 +4076,14 @@
         <v>27</v>
       </c>
       <c r="E33" s="67"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I33" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="J33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" s="63" t="s">
         <v>139</v>
       </c>
@@ -4042,7 +4092,7 @@
       </c>
       <c r="E34" s="67"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" s="63" t="s">
         <v>140</v>
       </c>
@@ -4051,7 +4101,7 @@
       </c>
       <c r="E35" s="67"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C36" s="63" t="s">
         <v>141</v>
       </c>
@@ -4060,7 +4110,7 @@
       </c>
       <c r="E36" s="67"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" s="63" t="s">
         <v>142</v>
       </c>
@@ -4069,7 +4119,7 @@
       </c>
       <c r="E37" s="67"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C38" s="63" t="s">
         <v>143</v>
       </c>
@@ -4078,7 +4128,7 @@
       </c>
       <c r="E38" s="67"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C39" s="63" t="s">
         <v>144</v>
       </c>
@@ -4087,7 +4137,7 @@
       </c>
       <c r="E39" s="67"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C40" s="63" t="s">
         <v>145</v>
       </c>
@@ -4096,7 +4146,7 @@
       </c>
       <c r="E40" s="67"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C41" s="64" t="s">
         <v>146</v>
       </c>
@@ -4105,7 +4155,7 @@
       </c>
       <c r="E41" s="67"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C42" s="76" t="s">
         <v>224</v>
       </c>
@@ -4114,7 +4164,7 @@
       </c>
       <c r="E42" s="67"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C43" s="76" t="s">
         <v>228</v>
       </c>
@@ -4122,7 +4172,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C44" s="76" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Replaced old static data
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60222997-DB43-4DC3-9333-97D113B54C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D965A7-BF6F-4A4E-BE9D-8A09ADE364AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13635" yWindow="1350" windowWidth="13470" windowHeight="16980" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="29595" yWindow="0" windowWidth="11460" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
     <sheet name="Panels" sheetId="2" r:id="rId2"/>
     <sheet name="Mapping" sheetId="3" r:id="rId3"/>
+    <sheet name="New_Mapping" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="379">
   <si>
     <t>ID</t>
   </si>
@@ -806,6 +807,375 @@
   </si>
   <si>
     <t>Shield with Checkmark</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>MainForm</t>
+  </si>
+  <si>
+    <t>The Importance of Storytelling</t>
+  </si>
+  <si>
+    <t>Storytelling Best Practices</t>
+  </si>
+  <si>
+    <t>Equity and Resilience</t>
+  </si>
+  <si>
+    <t>Who are ERB users?</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>What makes ERB different?</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>About ERB</t>
+  </si>
+  <si>
+    <t>What are indicators of Equitable Resilience?</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Chapter 1 About</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Chapter 2 About</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Chapter 3 About</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Chapter 4 About</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Chapter 5 About</t>
+  </si>
+  <si>
+    <t>Team Storytelling</t>
+  </si>
+  <si>
+    <t>Goal Setting Scenario</t>
+  </si>
+  <si>
+    <t>Activity To Goal Matching Example</t>
+  </si>
+  <si>
+    <t>OutputForm</t>
+  </si>
+  <si>
+    <t>Summary of Hazards, Disasters, Threats, and Equity Issues in your community</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Lay your cards on the table</t>
+  </si>
+  <si>
+    <t>Sorting indicator cards</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>How have communities used ERB?</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>AlternativeForm</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>How have other communities used the ERB tool? Goal setting examples</t>
+  </si>
+  <si>
+    <t>How have other communities used the ERB tool? Activity selection examples</t>
+  </si>
+  <si>
+    <t>Select activities to do in ERB</t>
+  </si>
+  <si>
+    <t>Reflection and next steps (Ch 1)</t>
+  </si>
+  <si>
+    <t>Identify and Diagram Community Connections</t>
+  </si>
+  <si>
+    <t>Diagram Community Connections</t>
+  </si>
+  <si>
+    <t>Develop a Community Engagement Plan: Determine scope of engagement</t>
+  </si>
+  <si>
+    <t>Develop a Community Engagement Plan: Write the plan</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Reflection and next steps (Ch 2)</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Gather information on hazards, disasters, and threats your community may face</t>
+  </si>
+  <si>
+    <t>Gather information on equity in your community</t>
+  </si>
+  <si>
+    <t>Learn about group dynamics and vulnerability</t>
+  </si>
+  <si>
+    <t>Mapping Activity: Locating hazards and assets in the community</t>
+  </si>
+  <si>
+    <t>Participatory Social Vulnerability Assessment Activity</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Reflection and next steps (Ch 3)</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>Kickoff meeting to review and selected indicators that are relevant to your community</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>Reflect on the workshop accomplishments and discuss next steps</t>
+  </si>
+  <si>
+    <t>How might we…so that statements</t>
+  </si>
+  <si>
+    <t>Evaluate Actions</t>
+  </si>
+  <si>
+    <t>Identify next steps and reflect (Ch 4)</t>
+  </si>
+  <si>
+    <t>Reflection and next steps (Ch 5)</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Centering Equity in Engagement</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>Checklist</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>3 People w/Lightbulb idea</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>Tiers of people</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>Microphone</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>3 People around table</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>Headphones</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>Teacher at board point w/ students</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Scroll w/topography</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>Cloud w/ lightening</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>Person balancing</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Bullet point</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Heart in circle</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>People networking nodes</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>Infinity symbol</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>People at white board</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Person with headphones</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>Person in hazard vest</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>InteractiveActivity</t>
+  </si>
+  <si>
+    <t>Wordcloud</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>Noteboard Activity</t>
+  </si>
+  <si>
+    <t>ERBInnerPanel</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Project Creation</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Not in content.xml</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1259,16 +1629,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,10 +2033,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="80"/>
+      <c r="H2" s="86"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -3449,8 +3821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3584,7 +3956,7 @@
       <c r="B5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="59"/>
       <c r="E5" s="64" t="s">
         <v>92</v>
@@ -3606,7 +3978,7 @@
       <c r="B6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="82"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="59"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -3616,7 +3988,7 @@
       <c r="B7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="82"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="59"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3626,7 +3998,7 @@
       <c r="B8" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="59"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -3853,7 +4225,7 @@
       <c r="E19" s="67" t="s">
         <v>232</v>
       </c>
-      <c r="F19" s="81" t="s">
+      <c r="F19" s="79" t="s">
         <v>231</v>
       </c>
       <c r="I19" s="76" t="s">
@@ -3873,7 +4245,7 @@
       <c r="E20" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="79" t="s">
         <v>233</v>
       </c>
       <c r="I20" s="76" t="s">
@@ -3893,7 +4265,7 @@
       <c r="E21" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="F21" s="81" t="s">
+      <c r="F21" s="79" t="s">
         <v>234</v>
       </c>
       <c r="I21" s="76" t="s">
@@ -3956,10 +4328,10 @@
         <v>13</v>
       </c>
       <c r="E25" s="67"/>
-      <c r="I25" s="83" t="s">
+      <c r="I25" s="81" t="s">
         <v>238</v>
       </c>
-      <c r="J25" s="84" t="s">
+      <c r="J25" s="82" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3971,10 +4343,10 @@
         <v>40</v>
       </c>
       <c r="E26" s="67"/>
-      <c r="I26" s="83" t="s">
+      <c r="I26" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="J26" s="84" t="s">
+      <c r="J26" s="82" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3986,10 +4358,10 @@
         <v>41</v>
       </c>
       <c r="E27" s="67"/>
-      <c r="I27" s="83" t="s">
+      <c r="I27" s="81" t="s">
         <v>240</v>
       </c>
-      <c r="J27" s="84" t="s">
+      <c r="J27" s="82" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4001,10 +4373,10 @@
         <v>9</v>
       </c>
       <c r="E28" s="67"/>
-      <c r="I28" s="83" t="s">
+      <c r="I28" s="81" t="s">
         <v>241</v>
       </c>
-      <c r="J28" s="84" t="s">
+      <c r="J28" s="82" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4159,7 +4531,7 @@
       <c r="C42" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="D42" s="81" t="s">
+      <c r="D42" s="79" t="s">
         <v>225</v>
       </c>
       <c r="E42" s="67"/>
@@ -4168,7 +4540,7 @@
       <c r="C43" s="76" t="s">
         <v>228</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="D43" s="79" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4176,7 +4548,7 @@
       <c r="C44" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="D44" s="81" t="s">
+      <c r="D44" s="79" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4190,8 +4562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C403D9B-4156-4D53-B432-05D214EB9E6F}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5024,4 +5396,1045 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
+  <dimension ref="A1:D91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="83" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="76" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="76" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="76" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="76" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="76" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="76" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="76" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="76" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="76" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" t="s">
+        <v>289</v>
+      </c>
+      <c r="C29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="B30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>258</v>
+      </c>
+      <c r="C34" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="76" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="76" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="76" t="s">
+        <v>301</v>
+      </c>
+      <c r="B40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C40" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C43" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" t="s">
+        <v>258</v>
+      </c>
+      <c r="C45" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="76" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="76" t="s">
+        <v>309</v>
+      </c>
+      <c r="B47" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="76" t="s">
+        <v>311</v>
+      </c>
+      <c r="B48" t="s">
+        <v>258</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="76" t="s">
+        <v>312</v>
+      </c>
+      <c r="B49" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="76" t="s">
+        <v>313</v>
+      </c>
+      <c r="B50" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" t="s">
+        <v>258</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" t="s">
+        <v>258</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56" t="s">
+        <v>258</v>
+      </c>
+      <c r="C56" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" t="s">
+        <v>258</v>
+      </c>
+      <c r="C57" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="B62" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="B64" t="s">
+        <v>323</v>
+      </c>
+      <c r="C64" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="76" t="s">
+        <v>327</v>
+      </c>
+      <c r="B65" t="s">
+        <v>323</v>
+      </c>
+      <c r="C65" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="B66" t="s">
+        <v>323</v>
+      </c>
+      <c r="C66" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="76" t="s">
+        <v>331</v>
+      </c>
+      <c r="B67" t="s">
+        <v>323</v>
+      </c>
+      <c r="C67" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="76" t="s">
+        <v>333</v>
+      </c>
+      <c r="B68" t="s">
+        <v>323</v>
+      </c>
+      <c r="C68" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="76" t="s">
+        <v>335</v>
+      </c>
+      <c r="B69" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="76" t="s">
+        <v>337</v>
+      </c>
+      <c r="B70" t="s">
+        <v>323</v>
+      </c>
+      <c r="C70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="76" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" t="s">
+        <v>323</v>
+      </c>
+      <c r="C71" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="76" t="s">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s">
+        <v>323</v>
+      </c>
+      <c r="C72" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="76" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s">
+        <v>323</v>
+      </c>
+      <c r="C73" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="76" t="s">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s">
+        <v>323</v>
+      </c>
+      <c r="C74" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="76" t="s">
+        <v>346</v>
+      </c>
+      <c r="B75" t="s">
+        <v>323</v>
+      </c>
+      <c r="C75" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="76" t="s">
+        <v>348</v>
+      </c>
+      <c r="B76" t="s">
+        <v>323</v>
+      </c>
+      <c r="C76" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="76" t="s">
+        <v>350</v>
+      </c>
+      <c r="B77" t="s">
+        <v>323</v>
+      </c>
+      <c r="C77" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="76" t="s">
+        <v>352</v>
+      </c>
+      <c r="B78" t="s">
+        <v>323</v>
+      </c>
+      <c r="C78" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="76" t="s">
+        <v>354</v>
+      </c>
+      <c r="B79" t="s">
+        <v>323</v>
+      </c>
+      <c r="C79" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="76" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" t="s">
+        <v>357</v>
+      </c>
+      <c r="C80" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="76" t="s">
+        <v>359</v>
+      </c>
+      <c r="B81" t="s">
+        <v>357</v>
+      </c>
+      <c r="C81" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="76" t="s">
+        <v>361</v>
+      </c>
+      <c r="B82" t="s">
+        <v>357</v>
+      </c>
+      <c r="C82" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="76" t="s">
+        <v>363</v>
+      </c>
+      <c r="B83" t="s">
+        <v>357</v>
+      </c>
+      <c r="C83" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="76" t="s">
+        <v>364</v>
+      </c>
+      <c r="B84" t="s">
+        <v>357</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="76" t="s">
+        <v>365</v>
+      </c>
+      <c r="B85" t="s">
+        <v>366</v>
+      </c>
+      <c r="C85" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="76" t="s">
+        <v>368</v>
+      </c>
+      <c r="B86" t="s">
+        <v>366</v>
+      </c>
+      <c r="C86" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="76" t="s">
+        <v>371</v>
+      </c>
+      <c r="B87" t="s">
+        <v>370</v>
+      </c>
+      <c r="C87" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="D87" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="76" t="s">
+        <v>372</v>
+      </c>
+      <c r="B88" t="s">
+        <v>370</v>
+      </c>
+      <c r="C88" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="76" t="s">
+        <v>373</v>
+      </c>
+      <c r="B89" t="s">
+        <v>370</v>
+      </c>
+      <c r="C89" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="76" t="s">
+        <v>374</v>
+      </c>
+      <c r="B90" t="s">
+        <v>370</v>
+      </c>
+      <c r="C90" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="76" t="s">
+        <v>375</v>
+      </c>
+      <c r="B91" t="s">
+        <v>370</v>
+      </c>
+      <c r="C91" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D91" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added content for Ch3 section 1
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35837A12-C206-42F2-9A23-03A2830E12C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F126703B-480D-492D-9185-1C9EE87904A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1185" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-30" yWindow="270" windowWidth="12090" windowHeight="15060" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="419">
   <si>
     <t>ID</t>
   </si>
@@ -1175,13 +1175,127 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Not in content.xml</t>
-  </si>
-  <si>
     <t>91</t>
   </si>
   <si>
     <t>ERB Dashboard</t>
+  </si>
+  <si>
+    <t>Not in contentXMLs directory</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>Listen and Connect</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>Plan Workshop While Centering Equity</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>Share Stories</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>Explore Future Scenarios</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>Build Relationships</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>Expand Your Knowledge</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Scope Information Needs</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>Hazards Data</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Equity Data</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>Resilient Systems Data</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>Gather the Data</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>Manage the Data</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>Collaborate on Assessment</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>Participatory Mapping</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Sort Resilience Indicators</t>
+  </si>
+  <si>
+    <t>Discuss Equity</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 3/4)</t>
+  </si>
+  <si>
+    <t>Not in content.xml AND Not in contentXMLs directory</t>
+  </si>
+  <si>
+    <t>Ch 3 About 4 column image</t>
+  </si>
+  <si>
+    <t>Ch 3 About 3 column image</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1266,8 +1380,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1477,11 +1603,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1639,14 +1804,40 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2039,10 +2230,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="86"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -3827,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5406,1051 +5597,1379 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:C84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="96" customWidth="1"/>
+    <col min="2" max="2" width="4" style="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="83" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:5" s="89" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="95"/>
+      <c r="B1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="C1" s="98" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="D1" s="98" t="s">
         <v>256</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="E1" s="98" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="90"/>
+      <c r="B2" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="94" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="E2" s="94"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="91"/>
+      <c r="B3" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="86" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="91"/>
+      <c r="B4" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="86" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="91"/>
+      <c r="B5" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C5" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="86" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="91"/>
+      <c r="B6" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="86" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="91"/>
+      <c r="B7" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C7" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="86" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="91"/>
+      <c r="B8" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C8" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="86" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="91"/>
+      <c r="B9" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="B9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C9" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="86" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="91"/>
+      <c r="B10" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="B10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C10" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="86" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="76" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="91"/>
+      <c r="B11" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="B11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="86" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="91"/>
+      <c r="B12" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="B12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C12" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="86" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="76" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="91"/>
+      <c r="B13" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="B13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C13" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="86" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="91"/>
+      <c r="B14" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="B14" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="C14" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" s="86" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="91"/>
+      <c r="B15" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="B15" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C15" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="86" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="92"/>
+      <c r="B16" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="B16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C16" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="86" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="92"/>
+      <c r="B17" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="B17" t="s">
-        <v>258</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C17" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="86" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="92"/>
+      <c r="B18" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="B18" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C18" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="86" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="76" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="92"/>
+      <c r="B19" s="85" t="s">
         <v>274</v>
       </c>
-      <c r="B19" t="s">
-        <v>258</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C19" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="86" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="92"/>
+      <c r="B20" s="85" t="s">
         <v>276</v>
       </c>
-      <c r="B20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C20" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="86" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="76" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="92"/>
+      <c r="B21" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="B21" t="s">
-        <v>258</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C21" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="86" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="76" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="93"/>
+      <c r="B22" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="B22" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C22" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="86" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="76" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="93"/>
+      <c r="B23" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="B23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="C23" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="86" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="93"/>
+      <c r="B24" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="B24" t="s">
-        <v>258</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C24" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="86" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="76" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="92"/>
+      <c r="B25" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="86" t="s">
         <v>281</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="86" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="76" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="93"/>
+      <c r="B26" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="B26" t="s">
-        <v>258</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="C26" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="86" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="76" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="93"/>
+      <c r="B27" s="85" t="s">
         <v>283</v>
       </c>
-      <c r="B27" t="s">
-        <v>258</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="C27" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="86" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="76" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="92"/>
+      <c r="B28" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="86" t="s">
         <v>289</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="86" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="76" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="92"/>
+      <c r="B29" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="86" t="s">
         <v>289</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="86" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="76" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="92"/>
+      <c r="B30" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="86" t="s">
         <v>289</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" s="86" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="76" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="92"/>
+      <c r="B31" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="B31" t="s">
-        <v>258</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C31" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="86" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="76" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="92"/>
+      <c r="B32" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="B32" t="s">
-        <v>258</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C32" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="86" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="76" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="92"/>
+      <c r="B33" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="B33" t="s">
-        <v>258</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="C33" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="86" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="76" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="92"/>
+      <c r="B34" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="B34" t="s">
-        <v>258</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C34" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="86" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="92"/>
+      <c r="B35" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="B35" t="s">
-        <v>258</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C35" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="86" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="76" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="92"/>
+      <c r="B36" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="B36" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="C36" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="86" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="76" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="92"/>
+      <c r="B37" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="B37" t="s">
-        <v>258</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C37" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="86" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="76" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="92"/>
+      <c r="B38" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="B38" t="s">
-        <v>258</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C38" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="86" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="92"/>
+      <c r="B39" s="85" t="s">
         <v>299</v>
       </c>
-      <c r="B39" t="s">
-        <v>258</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="C39" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="86" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="76" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="92"/>
+      <c r="B40" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="B40" t="s">
-        <v>258</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C40" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="86" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="76" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="92"/>
+      <c r="B41" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="B41" t="s">
-        <v>258</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C41" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="86" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="76" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="92"/>
+      <c r="B42" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="B42" t="s">
-        <v>258</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="C42" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="76" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="93"/>
+      <c r="B43" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="B43" t="s">
-        <v>258</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="C43" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="86" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="76" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="92"/>
+      <c r="B44" s="85" t="s">
         <v>176</v>
       </c>
-      <c r="B44" t="s">
-        <v>258</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="C44" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="86" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="76" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="92"/>
+      <c r="B45" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="B45" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C45" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="86" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="76" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="92"/>
+      <c r="B46" s="85" t="s">
         <v>307</v>
       </c>
-      <c r="B46" t="s">
-        <v>258</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="C46" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="86" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="76" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="92"/>
+      <c r="B47" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="B47" t="s">
-        <v>258</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="C47" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="86" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="76" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="92"/>
+      <c r="B48" s="85" t="s">
         <v>311</v>
       </c>
-      <c r="B48" t="s">
-        <v>258</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="C48" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="76" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="92"/>
+      <c r="B49" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="B49" t="s">
-        <v>258</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="C49" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="86" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="76" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="93"/>
+      <c r="B50" s="85" t="s">
         <v>313</v>
       </c>
-      <c r="B50" t="s">
-        <v>258</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C50" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="86" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="76" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="92"/>
+      <c r="B51" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="B51" t="s">
-        <v>258</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="C51" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="86" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="76" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="92"/>
+      <c r="B52" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="B52" t="s">
-        <v>258</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C52" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="86" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="76" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="92"/>
+      <c r="B53" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="B53" t="s">
-        <v>258</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="C53" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="86" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="76" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="92"/>
+      <c r="B54" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="B54" t="s">
-        <v>258</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="C54" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="86" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="76" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="92"/>
+      <c r="B55" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="B55" t="s">
-        <v>258</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="C55" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="86" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="76" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="92"/>
+      <c r="B56" s="85" t="s">
         <v>182</v>
       </c>
-      <c r="B56" t="s">
-        <v>258</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="C56" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="86" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="76" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="92"/>
+      <c r="B57" s="85" t="s">
         <v>183</v>
       </c>
-      <c r="B57" t="s">
-        <v>258</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="C57" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="86" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="76" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="92"/>
+      <c r="B58" s="85" t="s">
         <v>184</v>
       </c>
-      <c r="B58" t="s">
-        <v>258</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="C58" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="86" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="76" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="92"/>
+      <c r="B59" s="85" t="s">
         <v>185</v>
       </c>
-      <c r="B59" t="s">
-        <v>258</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="C59" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="86" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="76" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="92"/>
+      <c r="B60" s="85" t="s">
         <v>186</v>
       </c>
-      <c r="B60" t="s">
-        <v>258</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="C60" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="86" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="76" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="92"/>
+      <c r="B61" s="85" t="s">
         <v>319</v>
       </c>
-      <c r="B61" t="s">
-        <v>258</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="C61" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="86" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="76" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="92"/>
+      <c r="B62" s="85" t="s">
         <v>321</v>
       </c>
-      <c r="B62" t="s">
-        <v>258</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="C62" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="86" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="76" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="91"/>
+      <c r="B63" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" s="86" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="76" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="91"/>
+      <c r="B64" s="85" t="s">
         <v>325</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" s="86" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="76" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="91"/>
+      <c r="B65" s="85" t="s">
         <v>327</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" s="86" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="76" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="91"/>
+      <c r="B66" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" s="86" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="76" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="91"/>
+      <c r="B67" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" s="86" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="76" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="91"/>
+      <c r="B68" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" s="86" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="76" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="91"/>
+      <c r="B69" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" s="86" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="76" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="91"/>
+      <c r="B70" s="85" t="s">
         <v>337</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" s="86" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="76" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="91"/>
+      <c r="B71" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" s="86" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="76" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="91"/>
+      <c r="B72" s="85" t="s">
         <v>341</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" s="86" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="76" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="91"/>
+      <c r="B73" s="85" t="s">
         <v>343</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" s="86" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="76" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="91"/>
+      <c r="B74" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" s="86" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="76" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="91"/>
+      <c r="B75" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" s="86" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="76" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="91"/>
+      <c r="B76" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" s="86" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="76" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="91"/>
+      <c r="B77" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" s="86" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="76" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="91"/>
+      <c r="B78" s="85" t="s">
         <v>352</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" s="86" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="76" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="91"/>
+      <c r="B79" s="85" t="s">
         <v>354</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" s="86" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="76" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="91"/>
+      <c r="B80" s="85" t="s">
         <v>356</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" s="86" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="76" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="91"/>
+      <c r="B81" s="85" t="s">
         <v>359</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" s="86" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="76" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="91"/>
+      <c r="B82" s="85" t="s">
         <v>361</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" s="86" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="76" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="91"/>
+      <c r="B83" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" s="86" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="76" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="91"/>
+      <c r="B84" s="85" t="s">
         <v>364</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" s="86" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="76" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="92"/>
+      <c r="B85" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" s="86" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="76" t="s">
+      <c r="E85" s="86" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="92"/>
+      <c r="B86" s="85" t="s">
         <v>368</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" s="86" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="76" t="s">
+      <c r="E86" s="86" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="91"/>
+      <c r="B87" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="86" t="s">
         <v>370</v>
       </c>
-      <c r="C87" s="59" t="s">
+      <c r="D87" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="91"/>
+      <c r="B88" s="85" t="s">
+        <v>372</v>
+      </c>
+      <c r="C88" s="86" t="s">
+        <v>370</v>
+      </c>
+      <c r="D88" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="91"/>
+      <c r="B89" s="85" t="s">
+        <v>373</v>
+      </c>
+      <c r="C89" s="86" t="s">
+        <v>370</v>
+      </c>
+      <c r="D89" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="91"/>
+      <c r="B90" s="85" t="s">
+        <v>374</v>
+      </c>
+      <c r="C90" s="86" t="s">
+        <v>370</v>
+      </c>
+      <c r="D90" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="E90" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="91"/>
+      <c r="B91" s="85" t="s">
+        <v>375</v>
+      </c>
+      <c r="C91" s="86" t="s">
+        <v>370</v>
+      </c>
+      <c r="D91" s="87" t="s">
+        <v>376</v>
+      </c>
+      <c r="E91" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="91"/>
+      <c r="B92" s="85" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="76" t="s">
-        <v>372</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C92" s="86" t="s">
         <v>370</v>
       </c>
-      <c r="C88" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="D88" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="76" t="s">
-        <v>373</v>
-      </c>
-      <c r="B89" t="s">
-        <v>370</v>
-      </c>
-      <c r="C89" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="76" t="s">
-        <v>374</v>
-      </c>
-      <c r="B90" t="s">
-        <v>370</v>
-      </c>
-      <c r="C90" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="D90" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="76" t="s">
-        <v>375</v>
-      </c>
-      <c r="B91" t="s">
-        <v>370</v>
-      </c>
-      <c r="C91" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="D91" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="76" t="s">
+      <c r="D92" s="87" t="s">
         <v>379</v>
       </c>
-      <c r="B92" t="s">
-        <v>370</v>
-      </c>
-      <c r="C92" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="D92" t="s">
-        <v>378</v>
+      <c r="E92" s="88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="92"/>
+      <c r="B93" s="85" t="s">
+        <v>381</v>
+      </c>
+      <c r="C93" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="87" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="92"/>
+      <c r="B94" s="85" t="s">
+        <v>383</v>
+      </c>
+      <c r="C94" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="87" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="92"/>
+      <c r="B95" s="85" t="s">
+        <v>385</v>
+      </c>
+      <c r="C95" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="87" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="92"/>
+      <c r="B96" s="85" t="s">
+        <v>387</v>
+      </c>
+      <c r="C96" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="87" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="92"/>
+      <c r="B97" s="85" t="s">
+        <v>389</v>
+      </c>
+      <c r="C97" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="87" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="92"/>
+      <c r="B98" s="85" t="s">
+        <v>391</v>
+      </c>
+      <c r="C98" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="87" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="92"/>
+      <c r="B99" s="85" t="s">
+        <v>393</v>
+      </c>
+      <c r="C99" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="87" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="92"/>
+      <c r="B100" s="85" t="s">
+        <v>397</v>
+      </c>
+      <c r="C100" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="87" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="92"/>
+      <c r="B101" s="85" t="s">
+        <v>399</v>
+      </c>
+      <c r="C101" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="87" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="92"/>
+      <c r="B102" s="85" t="s">
+        <v>401</v>
+      </c>
+      <c r="C102" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="87" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="92"/>
+      <c r="B103" s="85" t="s">
+        <v>403</v>
+      </c>
+      <c r="C103" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="87" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="92"/>
+      <c r="B104" s="85" t="s">
+        <v>405</v>
+      </c>
+      <c r="C104" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="87" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="92"/>
+      <c r="B105" s="85" t="s">
+        <v>407</v>
+      </c>
+      <c r="C105" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="87" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="92"/>
+      <c r="B106" s="85" t="s">
+        <v>409</v>
+      </c>
+      <c r="C106" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="87" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="92"/>
+      <c r="B107" s="85" t="s">
+        <v>411</v>
+      </c>
+      <c r="C107" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="87" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="92"/>
+      <c r="B108" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="87" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="92"/>
+      <c r="B109" s="85" t="s">
+        <v>414</v>
+      </c>
+      <c r="C109" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="87" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="92"/>
+      <c r="B110" s="85" t="s">
+        <v>395</v>
+      </c>
+      <c r="C110" s="86" t="s">
+        <v>357</v>
+      </c>
+      <c r="D110" s="86" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="92"/>
+      <c r="B111" s="85" t="s">
+        <v>396</v>
+      </c>
+      <c r="C111" s="86" t="s">
+        <v>357</v>
+      </c>
+      <c r="D111" s="86" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added links to ch3 content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F126703B-480D-492D-9185-1C9EE87904A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB195E56-540E-4352-9C39-20643A03C131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="270" windowWidth="12090" windowHeight="15060" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="440">
   <si>
     <t>ID</t>
   </si>
@@ -1296,6 +1296,69 @@
   </si>
   <si>
     <t>Ch 3 About 3 column image</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Ch 2 Activity 1 figure</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Data Scoping Example</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>Data Scoping Example Image</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>Hazards Data Example</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Equity Data Example Image</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>Equity Data Example</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>Equitable Resilience Systems Image</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Map w/Stickies Image</t>
+  </si>
+  <si>
+    <t>Map w/Stickies</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Sorted Cards Example Image</t>
+  </si>
+  <si>
+    <t>Sorted Cards Example</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1383,12 +1446,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1646,7 +1703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1804,12 +1861,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1817,27 +1868,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2230,10 +2285,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="84"/>
+      <c r="H2" s="93"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5597,1379 +5652,1419 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="96" customWidth="1"/>
-    <col min="2" max="2" width="4" style="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="86" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" style="86" customWidth="1"/>
+    <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="89" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="95"/>
-      <c r="B1" s="97" t="s">
+    <row r="1" spans="1:5" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94"/>
+      <c r="B1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="91" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="91" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="85" t="s">
+      <c r="A2" s="95"/>
+      <c r="B2" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="94" t="s">
+      <c r="C2" s="89" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="94"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="91"/>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="85" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="91"/>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="86" t="s">
+      <c r="C4" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="85" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="86" t="s">
+      <c r="C5" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="85" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="86" t="s">
+      <c r="C6" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="85" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="86" t="s">
+      <c r="C7" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="85" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="86" t="s">
+      <c r="C8" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="85" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="83" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="86" t="s">
+      <c r="C9" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="85" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="83" t="s">
         <v>265</v>
       </c>
-      <c r="C10" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="86" t="s">
+      <c r="C10" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="85" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="86" t="s">
+      <c r="C11" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="85" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="86" t="s">
+      <c r="C12" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="85" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" s="86" t="s">
+      <c r="C13" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="85" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="91"/>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D14" s="86" t="s">
+      <c r="C14" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" s="85" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D15" s="86" t="s">
+      <c r="C15" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="85" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="83" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="86" t="s">
+      <c r="C16" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="85" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="83" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="86" t="s">
+      <c r="C17" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="85" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="83" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="86" t="s">
+      <c r="C18" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="85" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="92"/>
-      <c r="B19" s="85" t="s">
+      <c r="A19" s="88"/>
+      <c r="B19" s="98" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="86" t="s">
+      <c r="C19" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="97" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="85" t="s">
+      <c r="A20" s="88"/>
+      <c r="B20" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="C20" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="86" t="s">
+      <c r="C20" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="97" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="86" t="s">
+      <c r="C21" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="85" t="s">
+      <c r="A22" s="88"/>
+      <c r="B22" s="98" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="86" t="s">
+      <c r="C22" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="97" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="93"/>
-      <c r="B23" s="85" t="s">
+      <c r="A23" s="88"/>
+      <c r="B23" s="98" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="86" t="s">
+      <c r="C23" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="97" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="93"/>
-      <c r="B24" s="85" t="s">
+      <c r="A24" s="88"/>
+      <c r="B24" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="86" t="s">
+      <c r="C24" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="97" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="85" t="s">
+      <c r="A25" s="88"/>
+      <c r="B25" s="98" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="97" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="86" t="s">
+      <c r="D25" s="97" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="93"/>
-      <c r="B26" s="85" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="86" t="s">
+      <c r="C26" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="97" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="93"/>
-      <c r="B27" s="85" t="s">
+      <c r="A27" s="88"/>
+      <c r="B27" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="86" t="s">
+      <c r="C27" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="97" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
-      <c r="B28" s="85" t="s">
+      <c r="B28" s="83" t="s">
         <v>286</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="84" t="s">
         <v>289</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="D28" s="85" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="83" t="s">
         <v>288</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="84" t="s">
         <v>289</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="85" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="85" t="s">
+      <c r="B30" s="83" t="s">
         <v>290</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="84" t="s">
         <v>289</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="85" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
-      <c r="B31" s="85" t="s">
+      <c r="B31" s="83" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="86" t="s">
+      <c r="C31" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="85" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
-      <c r="B32" s="85" t="s">
+      <c r="B32" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="86" t="s">
+      <c r="C32" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="85" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="85" t="s">
+      <c r="B33" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="86" t="s">
+      <c r="C33" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="85" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
-      <c r="B34" s="85" t="s">
+      <c r="B34" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="86" t="s">
+      <c r="C34" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="85" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
-      <c r="B35" s="85" t="s">
+      <c r="B35" s="83" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="86" t="s">
+      <c r="C35" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="85" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="86" t="s">
+      <c r="C36" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="85" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="92"/>
-      <c r="B37" s="85" t="s">
+      <c r="B37" s="83" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="86" t="s">
+      <c r="C37" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="85" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="92"/>
-      <c r="B38" s="85" t="s">
+      <c r="B38" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="86" t="s">
+      <c r="C38" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="85" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="92"/>
-      <c r="B39" s="85" t="s">
+      <c r="B39" s="83" t="s">
         <v>299</v>
       </c>
-      <c r="C39" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="86" t="s">
+      <c r="C39" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="85" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="92"/>
-      <c r="B40" s="85" t="s">
+      <c r="A40" s="88"/>
+      <c r="B40" s="98" t="s">
         <v>301</v>
       </c>
-      <c r="C40" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="86" t="s">
+      <c r="C40" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="97" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="92"/>
-      <c r="B41" s="85" t="s">
+      <c r="A41" s="88"/>
+      <c r="B41" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="86" t="s">
+      <c r="C41" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="97" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="92"/>
-      <c r="B42" s="85" t="s">
+      <c r="A42" s="88"/>
+      <c r="B42" s="98" t="s">
         <v>174</v>
       </c>
-      <c r="C42" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="86" t="s">
+      <c r="C42" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="97" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="85" t="s">
+      <c r="A43" s="88"/>
+      <c r="B43" s="98" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="86" t="s">
+      <c r="C43" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="97" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="92"/>
-      <c r="B44" s="85" t="s">
+      <c r="A44" s="88"/>
+      <c r="B44" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="86" t="s">
+      <c r="C44" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="97" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="92"/>
-      <c r="B45" s="85" t="s">
+      <c r="A45" s="88"/>
+      <c r="B45" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="86" t="s">
+      <c r="C45" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="97" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="92"/>
-      <c r="B46" s="85" t="s">
+      <c r="A46" s="88"/>
+      <c r="B46" s="98" t="s">
         <v>307</v>
       </c>
-      <c r="C46" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="86" t="s">
+      <c r="C46" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="97" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="92"/>
-      <c r="B47" s="85" t="s">
+      <c r="A47" s="88"/>
+      <c r="B47" s="98" t="s">
         <v>309</v>
       </c>
-      <c r="C47" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="86" t="s">
+      <c r="C47" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="97" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
-      <c r="B48" s="85" t="s">
+      <c r="A48" s="88"/>
+      <c r="B48" s="98" t="s">
         <v>311</v>
       </c>
-      <c r="C48" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="86" t="s">
+      <c r="C48" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="97" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="92"/>
-      <c r="B49" s="85" t="s">
+      <c r="A49" s="88"/>
+      <c r="B49" s="98" t="s">
         <v>312</v>
       </c>
-      <c r="C49" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="86" t="s">
+      <c r="C49" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="97" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="93"/>
-      <c r="B50" s="85" t="s">
+      <c r="A50" s="88"/>
+      <c r="B50" s="98" t="s">
         <v>313</v>
       </c>
-      <c r="C50" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="86" t="s">
+      <c r="C50" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="97" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="92"/>
-      <c r="B51" s="85" t="s">
+      <c r="A51" s="88"/>
+      <c r="B51" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="86" t="s">
+      <c r="C51" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="97" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="92"/>
-      <c r="B52" s="85" t="s">
+      <c r="A52" s="88"/>
+      <c r="B52" s="98" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="86" t="s">
+      <c r="C52" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="97" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="92"/>
-      <c r="B53" s="85" t="s">
+      <c r="A53" s="88"/>
+      <c r="B53" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="86" t="s">
+      <c r="C53" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="97" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="92"/>
-      <c r="B54" s="85" t="s">
+      <c r="A54" s="88"/>
+      <c r="B54" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="86" t="s">
+      <c r="C54" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="97" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="92"/>
-      <c r="B55" s="85" t="s">
+      <c r="A55" s="88"/>
+      <c r="B55" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="C55" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="86" t="s">
+      <c r="C55" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="97" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="92"/>
-      <c r="B56" s="85" t="s">
+      <c r="A56" s="88"/>
+      <c r="B56" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="86" t="s">
+      <c r="C56" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="97" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="92"/>
-      <c r="B57" s="85" t="s">
+      <c r="A57" s="88"/>
+      <c r="B57" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="C57" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="86" t="s">
+      <c r="C57" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="97" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="92"/>
-      <c r="B58" s="85" t="s">
+      <c r="A58" s="88"/>
+      <c r="B58" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="86" t="s">
+      <c r="C58" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="97" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="92"/>
-      <c r="B59" s="85" t="s">
+      <c r="A59" s="88"/>
+      <c r="B59" s="98" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="86" t="s">
+      <c r="C59" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="97" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="92"/>
-      <c r="B60" s="85" t="s">
+      <c r="B60" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="86" t="s">
+      <c r="C60" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="85" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="92"/>
-      <c r="B61" s="85" t="s">
+      <c r="B61" s="83" t="s">
         <v>319</v>
       </c>
-      <c r="C61" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="86" t="s">
+      <c r="C61" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="85" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="92"/>
-      <c r="B62" s="85" t="s">
+      <c r="B62" s="83" t="s">
         <v>321</v>
       </c>
-      <c r="C62" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="86" t="s">
+      <c r="C62" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="85" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="91"/>
-      <c r="B63" s="85" t="s">
+      <c r="B63" s="83" t="s">
         <v>322</v>
       </c>
-      <c r="C63" s="86" t="s">
+      <c r="C63" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D63" s="86" t="s">
+      <c r="D63" s="84" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="91"/>
-      <c r="B64" s="85" t="s">
+      <c r="B64" s="83" t="s">
         <v>325</v>
       </c>
-      <c r="C64" s="86" t="s">
+      <c r="C64" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D64" s="86" t="s">
+      <c r="D64" s="84" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="91"/>
-      <c r="B65" s="85" t="s">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="83" t="s">
         <v>327</v>
       </c>
-      <c r="C65" s="86" t="s">
+      <c r="C65" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D65" s="86" t="s">
+      <c r="D65" s="84" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="91"/>
-      <c r="B66" s="85" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="83" t="s">
         <v>329</v>
       </c>
-      <c r="C66" s="86" t="s">
+      <c r="C66" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D66" s="86" t="s">
+      <c r="D66" s="84" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="91"/>
-      <c r="B67" s="85" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="83" t="s">
         <v>331</v>
       </c>
-      <c r="C67" s="86" t="s">
+      <c r="C67" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D67" s="86" t="s">
+      <c r="D67" s="84" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="91"/>
-      <c r="B68" s="85" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="83" t="s">
         <v>333</v>
       </c>
-      <c r="C68" s="86" t="s">
+      <c r="C68" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D68" s="86" t="s">
+      <c r="D68" s="84" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="91"/>
-      <c r="B69" s="85" t="s">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="83" t="s">
         <v>335</v>
       </c>
-      <c r="C69" s="86" t="s">
+      <c r="C69" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D69" s="86" t="s">
+      <c r="D69" s="84" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="91"/>
-      <c r="B70" s="85" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="C70" s="86" t="s">
+      <c r="C70" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D70" s="86" t="s">
+      <c r="D70" s="84" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="91"/>
-      <c r="B71" s="85" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="83" t="s">
         <v>339</v>
       </c>
-      <c r="C71" s="86" t="s">
+      <c r="C71" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D71" s="86" t="s">
+      <c r="D71" s="84" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="91"/>
-      <c r="B72" s="85" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="83" t="s">
         <v>341</v>
       </c>
-      <c r="C72" s="86" t="s">
+      <c r="C72" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D72" s="86" t="s">
+      <c r="D72" s="84" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="91"/>
-      <c r="B73" s="85" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="83" t="s">
         <v>343</v>
       </c>
-      <c r="C73" s="86" t="s">
+      <c r="C73" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D73" s="86" t="s">
+      <c r="D73" s="84" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="91"/>
-      <c r="B74" s="85" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="83" t="s">
         <v>345</v>
       </c>
-      <c r="C74" s="86" t="s">
+      <c r="C74" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D74" s="86" t="s">
+      <c r="D74" s="84" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="91"/>
-      <c r="B75" s="85" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="83" t="s">
         <v>346</v>
       </c>
-      <c r="C75" s="86" t="s">
+      <c r="C75" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D75" s="86" t="s">
+      <c r="D75" s="84" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="91"/>
-      <c r="B76" s="85" t="s">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="83" t="s">
         <v>348</v>
       </c>
-      <c r="C76" s="86" t="s">
+      <c r="C76" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D76" s="86" t="s">
+      <c r="D76" s="84" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="91"/>
-      <c r="B77" s="85" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="83" t="s">
         <v>350</v>
       </c>
-      <c r="C77" s="86" t="s">
+      <c r="C77" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D77" s="86" t="s">
+      <c r="D77" s="84" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="91"/>
-      <c r="B78" s="85" t="s">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="83" t="s">
         <v>352</v>
       </c>
-      <c r="C78" s="86" t="s">
+      <c r="C78" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D78" s="86" t="s">
+      <c r="D78" s="84" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="91"/>
-      <c r="B79" s="85" t="s">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="83" t="s">
         <v>354</v>
       </c>
-      <c r="C79" s="86" t="s">
+      <c r="C79" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="D79" s="86" t="s">
+      <c r="D79" s="84" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="91"/>
-      <c r="B80" s="85" t="s">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="83" t="s">
         <v>356</v>
       </c>
-      <c r="C80" s="86" t="s">
+      <c r="C80" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D80" s="86" t="s">
+      <c r="D80" s="84" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="91"/>
-      <c r="B81" s="85" t="s">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="C81" s="86" t="s">
+      <c r="C81" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D81" s="86" t="s">
+      <c r="D81" s="84" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="91"/>
-      <c r="B82" s="85" t="s">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="C82" s="86" t="s">
+      <c r="C82" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D82" s="86" t="s">
+      <c r="D82" s="84" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="91"/>
-      <c r="B83" s="85" t="s">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="83" t="s">
         <v>363</v>
       </c>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D83" s="86" t="s">
+      <c r="D83" s="84" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="91"/>
-      <c r="B84" s="85" t="s">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="83" t="s">
         <v>364</v>
       </c>
-      <c r="C84" s="86" t="s">
+      <c r="C84" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D84" s="86" t="s">
+      <c r="D84" s="85" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="92"/>
-      <c r="B85" s="85" t="s">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="83" t="s">
         <v>365</v>
       </c>
-      <c r="C85" s="86" t="s">
+      <c r="C85" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="D85" s="86" t="s">
+      <c r="D85" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="E85" s="86" t="s">
+      <c r="E85" s="84" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="92"/>
-      <c r="B86" s="85" t="s">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="83" t="s">
         <v>368</v>
       </c>
-      <c r="C86" s="86" t="s">
+      <c r="C86" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="D86" s="86" t="s">
+      <c r="D86" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="E86" s="86" t="s">
+      <c r="E86" s="84" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="91"/>
-      <c r="B87" s="85" t="s">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="83" t="s">
         <v>371</v>
       </c>
-      <c r="C87" s="86" t="s">
+      <c r="C87" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D87" s="86" t="s">
+      <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E87" s="88" t="s">
+      <c r="E87" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="91"/>
-      <c r="B88" s="85" t="s">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="83" t="s">
         <v>372</v>
       </c>
-      <c r="C88" s="86" t="s">
+      <c r="C88" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D88" s="86" t="s">
+      <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="88" t="s">
+      <c r="E88" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="91"/>
-      <c r="B89" s="85" t="s">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="83" t="s">
         <v>373</v>
       </c>
-      <c r="C89" s="86" t="s">
+      <c r="C89" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D89" s="86" t="s">
+      <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="E89" s="88" t="s">
+      <c r="E89" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="91"/>
-      <c r="B90" s="85" t="s">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="83" t="s">
         <v>374</v>
       </c>
-      <c r="C90" s="86" t="s">
+      <c r="C90" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D90" s="86" t="s">
+      <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="E90" s="88" t="s">
+      <c r="E90" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="91"/>
-      <c r="B91" s="85" t="s">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="83" t="s">
         <v>375</v>
       </c>
-      <c r="C91" s="86" t="s">
+      <c r="C91" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D91" s="87" t="s">
+      <c r="D91" s="85" t="s">
         <v>376</v>
       </c>
-      <c r="E91" s="88" t="s">
+      <c r="E91" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="91"/>
-      <c r="B92" s="85" t="s">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="83" t="s">
         <v>378</v>
       </c>
-      <c r="C92" s="86" t="s">
+      <c r="C92" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="87" t="s">
+      <c r="D92" s="85" t="s">
         <v>379</v>
       </c>
-      <c r="E92" s="88" t="s">
+      <c r="E92" s="86" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="92"/>
-      <c r="B93" s="85" t="s">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="C93" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="87" t="s">
+      <c r="C93" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="85" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="92"/>
-      <c r="B94" s="85" t="s">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="83" t="s">
         <v>383</v>
       </c>
-      <c r="C94" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="87" t="s">
+      <c r="C94" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="85" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="92"/>
-      <c r="B95" s="85" t="s">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="83" t="s">
         <v>385</v>
       </c>
-      <c r="C95" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="87" t="s">
+      <c r="C95" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="85" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="92"/>
-      <c r="B96" s="85" t="s">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="83" t="s">
         <v>387</v>
       </c>
-      <c r="C96" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="87" t="s">
+      <c r="C96" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="85" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="92"/>
-      <c r="B97" s="85" t="s">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="83" t="s">
         <v>389</v>
       </c>
-      <c r="C97" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="87" t="s">
+      <c r="C97" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="85" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="92"/>
-      <c r="B98" s="85" t="s">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="83" t="s">
         <v>391</v>
       </c>
-      <c r="C98" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="87" t="s">
+      <c r="C98" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="85" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="92"/>
-      <c r="B99" s="85" t="s">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="83" t="s">
         <v>393</v>
       </c>
-      <c r="C99" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="87" t="s">
+      <c r="C99" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="85" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="92"/>
-      <c r="B100" s="85" t="s">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="83" t="s">
         <v>397</v>
       </c>
-      <c r="C100" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="87" t="s">
+      <c r="C100" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="85" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="92"/>
-      <c r="B101" s="85" t="s">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="83" t="s">
         <v>399</v>
       </c>
-      <c r="C101" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="87" t="s">
+      <c r="C101" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="85" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="92"/>
-      <c r="B102" s="85" t="s">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="83" t="s">
         <v>401</v>
       </c>
-      <c r="C102" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="87" t="s">
+      <c r="C102" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="85" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="92"/>
-      <c r="B103" s="85" t="s">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="83" t="s">
         <v>403</v>
       </c>
-      <c r="C103" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="87" t="s">
+      <c r="C103" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="85" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="92"/>
-      <c r="B104" s="85" t="s">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="83" t="s">
         <v>405</v>
       </c>
-      <c r="C104" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="87" t="s">
+      <c r="C104" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="85" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="92"/>
-      <c r="B105" s="85" t="s">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="83" t="s">
         <v>407</v>
       </c>
-      <c r="C105" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="87" t="s">
+      <c r="C105" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="85" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="92"/>
-      <c r="B106" s="85" t="s">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="83" t="s">
         <v>409</v>
       </c>
-      <c r="C106" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="87" t="s">
+      <c r="C106" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="85" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="92"/>
-      <c r="B107" s="85" t="s">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="83" t="s">
         <v>411</v>
       </c>
-      <c r="C107" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="87" t="s">
+      <c r="C107" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="85" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="92"/>
-      <c r="B108" s="85" t="s">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="87" t="s">
+      <c r="C108" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="85" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="92"/>
-      <c r="B109" s="85" t="s">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="83" t="s">
         <v>414</v>
       </c>
-      <c r="C109" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="87" t="s">
+      <c r="C109" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="85" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="92"/>
-      <c r="B110" s="85" t="s">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="83" t="s">
         <v>395</v>
       </c>
-      <c r="C110" s="86" t="s">
+      <c r="C110" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D110" s="86" t="s">
+      <c r="D110" s="84" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="92"/>
-      <c r="B111" s="85" t="s">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="83" t="s">
         <v>396</v>
       </c>
-      <c r="C111" s="86" t="s">
+      <c r="C111" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="D111" s="86" t="s">
+      <c r="D111" s="84" t="s">
         <v>418</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="83" t="s">
+        <v>419</v>
+      </c>
+      <c r="C112" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D112" s="84" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="83" t="s">
+        <v>421</v>
+      </c>
+      <c r="C113" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="84" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="83" t="s">
+        <v>423</v>
+      </c>
+      <c r="C114" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D114" s="84" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="83" t="s">
+        <v>425</v>
+      </c>
+      <c r="C115" s="84" t="s">
+        <v>289</v>
+      </c>
+      <c r="D115" s="84" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="83" t="s">
+        <v>427</v>
+      </c>
+      <c r="C116" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D116" s="84" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="83" t="s">
+        <v>429</v>
+      </c>
+      <c r="C117" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D117" s="84" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="83" t="s">
+        <v>431</v>
+      </c>
+      <c r="C118" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D118" s="84" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="83" t="s">
+        <v>433</v>
+      </c>
+      <c r="C119" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D119" s="84" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="83" t="s">
+        <v>188</v>
+      </c>
+      <c r="C120" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="84" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="83" t="s">
+        <v>436</v>
+      </c>
+      <c r="C121" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D121" s="84" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="83" t="s">
+        <v>437</v>
+      </c>
+      <c r="C122" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="84" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Ch4&5 supporting documents
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB195E56-540E-4352-9C39-20643A03C131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4E4B7D-3513-404B-B6ED-DF051B3AF847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28800" yWindow="120" windowWidth="14655" windowHeight="15465" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="471">
   <si>
     <t>ID</t>
   </si>
@@ -1359,6 +1359,99 @@
   </si>
   <si>
     <t>Sorted Cards Example</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>Put Results into Action</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>Storytelling on Project Implementation</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Define the Problems to Solve</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Workshop 3- Results to Action</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>Warm Up Activity</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Create Vision Statements</t>
+  </si>
+  <si>
+    <t>Brainstorm Actions</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>Strategy Planning</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>Workshop Wrap-Up</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>Ch 4 Reflection</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Key Takeaways from Strategizing</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>Document Your Project</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Next Steps for Outreach and Engagement</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Next Steps for Implementation</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>Use Monitoring to Support Future Action</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>Ch 5 Reflection</t>
   </si>
 </sst>
 </file>
@@ -1874,12 +1967,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1893,6 +1980,12 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2285,10 +2378,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="93"/>
+      <c r="H2" s="100"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5652,15 +5745,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="96" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="94" customWidth="1"/>
     <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
     <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
@@ -5668,7 +5761,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94"/>
+      <c r="A1" s="92"/>
       <c r="B1" s="90" t="s">
         <v>0</v>
       </c>
@@ -5683,14 +5776,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
+      <c r="A2" s="93"/>
       <c r="B2" s="83" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="89" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="98" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="89"/>
@@ -5872,26 +5965,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="97" t="s">
+      <c r="C19" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="85" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="97" t="s">
         <v>276</v>
       </c>
-      <c r="C20" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="97" t="s">
+      <c r="C20" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="85" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5908,73 +5999,73 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="88"/>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="97" t="s">
+      <c r="C22" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="95" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="88"/>
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="97" t="s">
+      <c r="C23" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="95" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="88"/>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="96" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="97" t="s">
+      <c r="C24" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="95" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="88"/>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="97" t="s">
+      <c r="C25" s="95" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="97" t="s">
+      <c r="D25" s="95" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="88"/>
-      <c r="B26" s="98" t="s">
+      <c r="B26" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="97" t="s">
+      <c r="C26" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="95" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="88"/>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="96" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="97" t="s">
+      <c r="C27" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="95" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6023,7 +6114,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="99" t="s">
+      <c r="B32" s="97" t="s">
         <v>166</v>
       </c>
       <c r="C32" s="85" t="s">
@@ -6112,241 +6203,241 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="88"/>
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="96" t="s">
         <v>301</v>
       </c>
-      <c r="C40" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="97" t="s">
+      <c r="C40" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="95" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="88"/>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="97" t="s">
+      <c r="C41" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="95" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="88"/>
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="C42" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="97" t="s">
+      <c r="C42" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="95" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="88"/>
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="97" t="s">
+      <c r="C43" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="95" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="88"/>
-      <c r="B44" s="98" t="s">
+      <c r="B44" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="97" t="s">
+      <c r="C44" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="95" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="88"/>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="97" t="s">
+      <c r="C45" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="95" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="88"/>
-      <c r="B46" s="98" t="s">
+      <c r="B46" s="96" t="s">
         <v>307</v>
       </c>
-      <c r="C46" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="97" t="s">
+      <c r="C46" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="95" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="88"/>
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="C47" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="97" t="s">
+      <c r="C47" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="95" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="88"/>
-      <c r="B48" s="98" t="s">
+      <c r="B48" s="96" t="s">
         <v>311</v>
       </c>
-      <c r="C48" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="97" t="s">
+      <c r="C48" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="88"/>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="96" t="s">
         <v>312</v>
       </c>
-      <c r="C49" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="97" t="s">
+      <c r="C49" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="95" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="88"/>
-      <c r="B50" s="98" t="s">
+      <c r="B50" s="96" t="s">
         <v>313</v>
       </c>
-      <c r="C50" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="97" t="s">
+      <c r="C50" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="95" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="88"/>
-      <c r="B51" s="98" t="s">
+      <c r="B51" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="97" t="s">
+      <c r="C51" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="95" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="88"/>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="97" t="s">
+      <c r="C52" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="95" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="88"/>
-      <c r="B53" s="98" t="s">
+      <c r="B53" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="97" t="s">
+      <c r="C53" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="95" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="88"/>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="97" t="s">
+      <c r="C54" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="95" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="88"/>
-      <c r="B55" s="98" t="s">
+      <c r="B55" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="C55" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="97" t="s">
+      <c r="C55" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="95" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="88"/>
-      <c r="B56" s="98" t="s">
+      <c r="B56" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="97" t="s">
+      <c r="C56" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="95" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="88"/>
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="96" t="s">
         <v>183</v>
       </c>
-      <c r="C57" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="97" t="s">
+      <c r="C57" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="95" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="88"/>
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="96" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="97" t="s">
+      <c r="C58" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="95" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="88"/>
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="96" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="97" t="s">
+      <c r="C59" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="95" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7065,6 +7156,193 @@
       </c>
       <c r="D122" s="84" t="s">
         <v>439</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="83" t="s">
+        <v>440</v>
+      </c>
+      <c r="C123" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="84" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="83" t="s">
+        <v>442</v>
+      </c>
+      <c r="C124" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="84" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="83" t="s">
+        <v>444</v>
+      </c>
+      <c r="C125" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="84" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="83" t="s">
+        <v>446</v>
+      </c>
+      <c r="C126" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="84" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="83" t="s">
+        <v>448</v>
+      </c>
+      <c r="C127" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="84" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="83" t="s">
+        <v>450</v>
+      </c>
+      <c r="C128" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="84" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="83" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="84" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="84" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="83" t="s">
+        <v>453</v>
+      </c>
+      <c r="C131" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="84" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="83" t="s">
+        <v>455</v>
+      </c>
+      <c r="C132" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="84" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="83" t="s">
+        <v>457</v>
+      </c>
+      <c r="C133" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="84" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="83" t="s">
+        <v>459</v>
+      </c>
+      <c r="C134" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="D134" s="84" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="83" t="s">
+        <v>461</v>
+      </c>
+      <c r="C135" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="84" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="83" t="s">
+        <v>463</v>
+      </c>
+      <c r="C136" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="84" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="C137" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="84" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="83" t="s">
+        <v>467</v>
+      </c>
+      <c r="C138" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="84" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="83" t="s">
+        <v>469</v>
+      </c>
+      <c r="C139" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="84" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new content panels to tree
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4E4B7D-3513-404B-B6ED-DF051B3AF847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8846662-14A7-4374-8126-D3B1F8B63E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="120" windowWidth="14655" windowHeight="15465" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -5747,7 +5747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed duel naming of 'How have communities used ERB'
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8846662-14A7-4374-8126-D3B1F8B63E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E52F6-DFA5-4784-B7E4-488990BC654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="120" windowWidth="14655" windowHeight="15465" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-75" yWindow="60" windowWidth="17505" windowHeight="15480" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="469">
   <si>
     <t>ID</t>
   </si>
@@ -912,12 +912,6 @@
   </si>
   <si>
     <t>29</t>
-  </si>
-  <si>
-    <t>How have other communities used the ERB tool? Goal setting examples</t>
-  </si>
-  <si>
-    <t>How have other communities used the ERB tool? Activity selection examples</t>
   </si>
   <si>
     <t>Select activities to do in ERB</t>
@@ -5747,8 +5741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5772,7 +5766,7 @@
         <v>256</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6088,7 +6082,7 @@
         <v>289</v>
       </c>
       <c r="D29" s="85" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -6099,7 +6093,7 @@
         <v>289</v>
       </c>
       <c r="D30" s="85" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -6121,7 +6115,7 @@
         <v>258</v>
       </c>
       <c r="D32" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -6143,7 +6137,7 @@
         <v>258</v>
       </c>
       <c r="D34" s="85" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -6154,7 +6148,7 @@
         <v>258</v>
       </c>
       <c r="D35" s="85" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6165,7 +6159,7 @@
         <v>258</v>
       </c>
       <c r="D36" s="85" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6176,7 +6170,7 @@
         <v>258</v>
       </c>
       <c r="D37" s="85" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -6187,30 +6181,30 @@
         <v>258</v>
       </c>
       <c r="D38" s="85" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="83" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C39" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D39" s="85" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="88"/>
       <c r="B40" s="96" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C40" s="95" t="s">
         <v>258</v>
       </c>
       <c r="D40" s="95" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6222,7 +6216,7 @@
         <v>258</v>
       </c>
       <c r="D41" s="95" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6246,7 +6240,7 @@
         <v>258</v>
       </c>
       <c r="D43" s="95" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6258,7 +6252,7 @@
         <v>258</v>
       </c>
       <c r="D44" s="95" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6270,37 +6264,37 @@
         <v>258</v>
       </c>
       <c r="D45" s="95" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="88"/>
       <c r="B46" s="96" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C46" s="95" t="s">
         <v>258</v>
       </c>
       <c r="D46" s="95" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="88"/>
       <c r="B47" s="96" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C47" s="95" t="s">
         <v>258</v>
       </c>
       <c r="D47" s="95" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="88"/>
       <c r="B48" s="96" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C48" s="95" t="s">
         <v>258</v>
@@ -6312,7 +6306,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="88"/>
       <c r="B49" s="96" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C49" s="95" t="s">
         <v>258</v>
@@ -6324,13 +6318,13 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="88"/>
       <c r="B50" s="96" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C50" s="95" t="s">
         <v>258</v>
       </c>
       <c r="D50" s="95" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6366,7 +6360,7 @@
         <v>258</v>
       </c>
       <c r="D53" s="95" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6402,7 +6396,7 @@
         <v>258</v>
       </c>
       <c r="D56" s="95" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -6414,7 +6408,7 @@
         <v>258</v>
       </c>
       <c r="D57" s="95" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -6438,7 +6432,7 @@
         <v>258</v>
       </c>
       <c r="D59" s="95" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6454,18 +6448,18 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="83" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C61" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D61" s="85" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="83" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C62" s="84" t="s">
         <v>258</v>
@@ -6476,131 +6470,131 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="83" t="s">
+        <v>320</v>
+      </c>
+      <c r="C63" s="84" t="s">
+        <v>321</v>
+      </c>
+      <c r="D63" s="84" t="s">
         <v>322</v>
-      </c>
-      <c r="C63" s="84" t="s">
-        <v>323</v>
-      </c>
-      <c r="D63" s="84" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="83" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C64" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D64" s="84" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="83" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C65" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D65" s="84" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="83" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C66" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D66" s="84" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="83" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C67" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D67" s="84" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="83" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C68" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D68" s="84" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="83" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C69" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D69" s="84" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="83" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C70" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D70" s="84" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="83" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C71" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D71" s="84" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="83" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C72" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D72" s="84" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="83" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C73" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D73" s="84" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="83" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C74" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D74" s="84" t="s">
         <v>221</v>
@@ -6608,98 +6602,98 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="83" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C75" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D75" s="84" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="83" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C76" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D76" s="84" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="83" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D77" s="84" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="83" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C78" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D78" s="84" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="83" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C79" s="84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D79" s="84" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="83" t="s">
+        <v>354</v>
+      </c>
+      <c r="C80" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="D80" s="84" t="s">
         <v>356</v>
-      </c>
-      <c r="C80" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D80" s="84" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="83" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D81" s="84" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="83" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C82" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D82" s="84" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="83" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C83" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D83" s="84" t="s">
         <v>233</v>
@@ -6707,10 +6701,10 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="83" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C84" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D84" s="85" t="s">
         <v>234</v>
@@ -6718,279 +6712,279 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="83" t="s">
+        <v>363</v>
+      </c>
+      <c r="C85" s="84" t="s">
+        <v>364</v>
+      </c>
+      <c r="D85" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="C85" s="84" t="s">
-        <v>366</v>
-      </c>
-      <c r="D85" s="85" t="s">
-        <v>367</v>
-      </c>
       <c r="E85" s="84" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="83" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C86" s="84" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D86" s="85" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E86" s="84" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="83" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C87" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
       <c r="E87" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="83" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C88" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
       <c r="E88" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="83" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C89" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
       <c r="E89" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="83" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C90" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
       <c r="E90" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="83" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C91" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D91" s="85" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E91" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="83" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C92" s="84" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D92" s="85" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E92" s="86" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="83" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C93" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D93" s="85" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="83" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C94" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D94" s="85" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="83" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C95" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D95" s="85" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="83" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C96" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D96" s="85" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="83" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C97" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D97" s="85" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="83" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C98" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D98" s="85" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="83" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C99" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D99" s="85" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="83" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C100" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D100" s="85" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="83" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C101" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D101" s="85" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="83" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C102" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D102" s="85" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="83" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C103" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D103" s="85" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="83" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C104" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D104" s="85" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="83" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C105" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D105" s="85" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="83" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C106" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D106" s="85" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="83" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C107" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D107" s="85" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
@@ -7001,128 +6995,128 @@
         <v>258</v>
       </c>
       <c r="D108" s="85" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="83" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C109" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D109" s="85" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="83" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C110" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D110" s="84" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="83" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C111" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D111" s="84" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="83" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C112" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D112" s="84" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="83" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C113" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D113" s="84" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="83" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C114" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D114" s="84" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="83" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C115" s="84" t="s">
         <v>289</v>
       </c>
       <c r="D115" s="84" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="83" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C116" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D116" s="84" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="83" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C117" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D117" s="84" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="83" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C118" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D118" s="84" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="83" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C119" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D119" s="84" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
@@ -7133,95 +7127,95 @@
         <v>258</v>
       </c>
       <c r="D120" s="84" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="83" t="s">
+        <v>434</v>
+      </c>
+      <c r="C121" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="D121" s="84" t="s">
         <v>436</v>
-      </c>
-      <c r="C121" s="84" t="s">
-        <v>357</v>
-      </c>
-      <c r="D121" s="84" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="83" t="s">
+        <v>435</v>
+      </c>
+      <c r="C122" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="84" t="s">
         <v>437</v>
-      </c>
-      <c r="C122" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="84" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="83" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C123" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D123" s="84" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="83" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C124" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D124" s="84" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="83" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C125" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D125" s="84" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="83" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C126" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D126" s="84" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="83" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C127" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D127" s="84" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="83" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C128" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D128" s="84" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
@@ -7232,7 +7226,7 @@
         <v>258</v>
       </c>
       <c r="D129" s="84" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
@@ -7243,106 +7237,106 @@
         <v>258</v>
       </c>
       <c r="D130" s="84" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="83" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C131" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D131" s="84" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="83" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C132" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D132" s="84" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="83" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C133" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D133" s="84" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="83" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C134" s="84" t="s">
         <v>281</v>
       </c>
       <c r="D134" s="84" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="83" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C135" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D135" s="84" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="83" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C136" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D136" s="84" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="83" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C137" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D137" s="84" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="83" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C138" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D138" s="84" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="83" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C139" s="84" t="s">
         <v>258</v>
       </c>
       <c r="D139" s="84" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Key Takeaways Form
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E52F6-DFA5-4784-B7E4-488990BC654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B0A609-00AD-4B09-8005-04BA51C09BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="60" windowWidth="17505" windowHeight="15480" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-75" yWindow="60" windowWidth="9045" windowHeight="15480" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -5741,8 +5741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Actions Brainstorming Form
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B0A609-00AD-4B09-8005-04BA51C09BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F410398-47E8-4076-BEBF-C4EC951B8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="60" windowWidth="9045" windowHeight="15480" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="471">
   <si>
     <t>ID</t>
   </si>
@@ -1446,6 +1446,12 @@
   </si>
   <si>
     <t>Ch 5 Reflection</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>Actions Brainstorming Example</t>
   </si>
 </sst>
 </file>
@@ -5739,10 +5745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7339,6 +7345,17 @@
         <v>468</v>
       </c>
     </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="83" t="s">
+        <v>469</v>
+      </c>
+      <c r="C140" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="D140" s="84" t="s">
+        <v>470</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated content XML with April 15th content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F410398-47E8-4076-BEBF-C4EC951B8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C84F01-9EC7-4CB8-B274-FEE86B3915A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="2835" yWindow="750" windowWidth="10725" windowHeight="13755" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="475">
   <si>
     <t>ID</t>
   </si>
@@ -848,36 +848,18 @@
     <t>15</t>
   </si>
   <si>
-    <t>Chapter 1 About</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
-    <t>Chapter 2 About</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t>Chapter 3 About</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
-    <t>Chapter 4 About</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
-    <t>Chapter 5 About</t>
-  </si>
-  <si>
-    <t>Team Storytelling</t>
-  </si>
-  <si>
     <t>Goal Setting Scenario</t>
   </si>
   <si>
@@ -896,9 +878,6 @@
     <t>Lay your cards on the table</t>
   </si>
   <si>
-    <t>Sorting indicator cards</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -914,30 +893,12 @@
     <t>29</t>
   </si>
   <si>
-    <t>Select activities to do in ERB</t>
-  </si>
-  <si>
-    <t>Reflection and next steps (Ch 1)</t>
-  </si>
-  <si>
-    <t>Identify and Diagram Community Connections</t>
-  </si>
-  <si>
     <t>Diagram Community Connections</t>
   </si>
   <si>
-    <t>Develop a Community Engagement Plan: Determine scope of engagement</t>
-  </si>
-  <si>
-    <t>Develop a Community Engagement Plan: Write the plan</t>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
-    <t>Reflection and next steps (Ch 2)</t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
@@ -1187,9 +1148,6 @@
     <t>93</t>
   </si>
   <si>
-    <t>Plan Workshop While Centering Equity</t>
-  </si>
-  <si>
     <t>94</t>
   </si>
   <si>
@@ -1247,21 +1205,12 @@
     <t>106</t>
   </si>
   <si>
-    <t>Gather the Data</t>
-  </si>
-  <si>
     <t>107</t>
   </si>
   <si>
-    <t>Manage the Data</t>
-  </si>
-  <si>
     <t>108</t>
   </si>
   <si>
-    <t>Collaborate on Assessment</t>
-  </si>
-  <si>
     <t>109</t>
   </si>
   <si>
@@ -1280,9 +1229,6 @@
     <t>112</t>
   </si>
   <si>
-    <t>Reflection and Next Steps (Ch 3/4)</t>
-  </si>
-  <si>
     <t>Not in content.xml AND Not in contentXMLs directory</t>
   </si>
   <si>
@@ -1370,9 +1316,6 @@
     <t>127</t>
   </si>
   <si>
-    <t>Define the Problems to Solve</t>
-  </si>
-  <si>
     <t>128</t>
   </si>
   <si>
@@ -1409,9 +1352,6 @@
     <t>135</t>
   </si>
   <si>
-    <t>Ch 4 Reflection</t>
-  </si>
-  <si>
     <t>136</t>
   </si>
   <si>
@@ -1427,15 +1367,9 @@
     <t>139</t>
   </si>
   <si>
-    <t>Next Steps for Outreach and Engagement</t>
-  </si>
-  <si>
     <t>140</t>
   </si>
   <si>
-    <t>Next Steps for Implementation</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
@@ -1445,13 +1379,91 @@
     <t>142</t>
   </si>
   <si>
-    <t>Ch 5 Reflection</t>
-  </si>
-  <si>
     <t>143</t>
   </si>
   <si>
     <t>Actions Brainstorming Example</t>
+  </si>
+  <si>
+    <t>(Section 1) Plan Your Project</t>
+  </si>
+  <si>
+    <t>Get a Core Team Together</t>
+  </si>
+  <si>
+    <t>Team Storytelling Exercise</t>
+  </si>
+  <si>
+    <t>Set Goals for Using ERB</t>
+  </si>
+  <si>
+    <t>Select ERB Activities</t>
+  </si>
+  <si>
+    <t>(Section 2) Engage Your Community</t>
+  </si>
+  <si>
+    <t>Identify Community Connections</t>
+  </si>
+  <si>
+    <t>Develop a Community Engagement Plan</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 2)</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 1)</t>
+  </si>
+  <si>
+    <t>(Section 3) Assess Hazards, Equity, and Resilience</t>
+  </si>
+  <si>
+    <t>Plan Workshop 1: Listen and Connect</t>
+  </si>
+  <si>
+    <t>Gather Data</t>
+  </si>
+  <si>
+    <t>Manage Data</t>
+  </si>
+  <si>
+    <t>Assess Resilience</t>
+  </si>
+  <si>
+    <t>Plan Workshop 2: Collaborative Assessment</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 3)</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>Key Takeaways from Assessment</t>
+  </si>
+  <si>
+    <t>(Section 4) Strategize Actions</t>
+  </si>
+  <si>
+    <t>Define your Action Areas</t>
+  </si>
+  <si>
+    <t>Plan Workshop 3</t>
+  </si>
+  <si>
+    <t>Reflection and Next Steps (Ch 4)</t>
+  </si>
+  <si>
+    <t>(Section 5) Wrap Up and Move Forward</t>
+  </si>
+  <si>
+    <t>Implement Actions</t>
+  </si>
+  <si>
+    <t>Maintain Outreach and Engagement</t>
+  </si>
+  <si>
+    <t>Reflect and Celebrate (Ch 5)</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1550,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1796,7 +1808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1961,9 +1973,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1976,10 +1985,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2378,10 +2391,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="99" t="s">
+      <c r="G2" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="100"/>
+      <c r="H2" s="101"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5745,15 +5758,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:XFD135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="94" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="93" customWidth="1"/>
     <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
     <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
@@ -5761,32 +5774,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92"/>
-      <c r="B1" s="90" t="s">
+      <c r="A1" s="91"/>
+      <c r="B1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="90" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="91" t="s">
-        <v>375</v>
+      <c r="E1" s="90" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="93"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="89" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="98" t="s">
+      <c r="C2" s="88" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="89"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="83" t="s">
@@ -5931,676 +5944,744 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="83" t="s">
+    <row r="16" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="96"/>
+      <c r="B16" s="97" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="85" t="s">
+      <c r="C16" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="98" t="s">
+        <v>448</v>
+      </c>
+      <c r="E16" s="98"/>
+    </row>
+    <row r="17" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="96"/>
+      <c r="B17" s="97" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="83" t="s">
+      <c r="C17" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="98" t="s">
+        <v>453</v>
+      </c>
+      <c r="E17" s="98"/>
+    </row>
+    <row r="18" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="96"/>
+      <c r="B18" s="97" t="s">
         <v>270</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="85" t="s">
+      <c r="C18" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="98" t="s">
+        <v>458</v>
+      </c>
+      <c r="E18" s="98"/>
+    </row>
+    <row r="19" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="96"/>
+      <c r="B19" s="97" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="83" t="s">
+      <c r="C19" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="98" t="s">
+        <v>467</v>
+      </c>
+      <c r="E19" s="98"/>
+    </row>
+    <row r="20" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="96"/>
+      <c r="B20" s="97" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="85" t="s">
+      <c r="C20" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="98" t="s">
+        <v>471</v>
+      </c>
+      <c r="E20" s="98"/>
+    </row>
+    <row r="21" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="96"/>
+      <c r="B21" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="98" t="s">
+        <v>450</v>
+      </c>
+      <c r="E21" s="98"/>
+    </row>
+    <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="93"/>
+      <c r="B22" s="94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="85" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="97" t="s">
+      <c r="E22" s="85"/>
+    </row>
+    <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="93"/>
+      <c r="B23" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="85" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="85" t="s">
+      <c r="E23" s="85"/>
+    </row>
+    <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="93"/>
+      <c r="B24" s="94" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="85"/>
+    </row>
+    <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="93"/>
+      <c r="B25" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="85" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="97" t="s">
+      <c r="D25" s="85" t="s">
         <v>276</v>
       </c>
-      <c r="C20" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="85" t="s">
+      <c r="E25" s="85"/>
+    </row>
+    <row r="26" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="96"/>
+      <c r="B26" s="97" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="98" t="s">
+        <v>469</v>
+      </c>
+      <c r="E26" s="98"/>
+    </row>
+    <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="93"/>
+      <c r="B27" s="94" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="83" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="85" t="s">
+      <c r="C27" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="85" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="88"/>
-      <c r="B22" s="96" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="95" t="s">
+      <c r="E27" s="85"/>
+    </row>
+    <row r="28" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="96"/>
+      <c r="B28" s="97" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="96" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="95" t="s">
+      <c r="C28" s="98" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" s="98" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="88"/>
-      <c r="B24" s="96" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="95" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="96" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="95" t="s">
+      <c r="E28" s="98"/>
+    </row>
+    <row r="29" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="96"/>
+      <c r="B29" s="97" t="s">
         <v>281</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="C29" s="98" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="88"/>
-      <c r="B26" s="96" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="95" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="96" t="s">
+      <c r="D29" s="98" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="98"/>
+    </row>
+    <row r="30" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="96"/>
+      <c r="B30" s="97" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="95" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="83" t="s">
-        <v>286</v>
-      </c>
-      <c r="C28" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D28" s="85" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="83" t="s">
-        <v>288</v>
-      </c>
-      <c r="C29" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D29" s="85" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="83" t="s">
-        <v>290</v>
-      </c>
-      <c r="C30" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D30" s="85" t="s">
+      <c r="C30" s="98" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="98" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="83" t="s">
+      <c r="E30" s="98"/>
+    </row>
+    <row r="31" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="96"/>
+      <c r="B31" s="97" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="85" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="98" t="s">
+        <v>449</v>
+      </c>
+      <c r="E31" s="98"/>
+    </row>
+    <row r="32" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="96"/>
       <c r="B32" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="85" t="s">
+      <c r="C32" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="98" t="s">
+        <v>452</v>
+      </c>
+      <c r="E32" s="98"/>
+    </row>
+    <row r="33" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="96"/>
+      <c r="B33" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="98"/>
+    </row>
+    <row r="34" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="96"/>
+      <c r="B34" s="97" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="98" t="s">
+        <v>457</v>
+      </c>
+      <c r="E34" s="98"/>
+    </row>
+    <row r="35" spans="1:5" s="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="96"/>
+      <c r="B35" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="98" t="s">
+        <v>454</v>
+      </c>
+      <c r="E35" s="98"/>
+    </row>
+    <row r="36" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="96"/>
+      <c r="B36" s="97" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="98" t="s">
+        <v>284</v>
+      </c>
+      <c r="E36" s="98"/>
+    </row>
+    <row r="37" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="96"/>
+      <c r="B37" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="98" t="s">
+        <v>455</v>
+      </c>
+      <c r="E37" s="98"/>
+    </row>
+    <row r="38" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="96"/>
+      <c r="B38" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="98" t="s">
+        <v>463</v>
+      </c>
+      <c r="E38" s="98"/>
+    </row>
+    <row r="39" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="96"/>
+      <c r="B39" s="97" t="s">
+        <v>285</v>
+      </c>
+      <c r="C39" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="98" t="s">
+        <v>456</v>
+      </c>
+      <c r="E39" s="98"/>
+    </row>
+    <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="93"/>
+      <c r="B40" s="94" t="s">
+        <v>286</v>
+      </c>
+      <c r="C40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>287</v>
+      </c>
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="93"/>
+      <c r="B41" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="E41" s="85"/>
+    </row>
+    <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="93"/>
+      <c r="B42" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="85"/>
+    </row>
+    <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="93"/>
+      <c r="B43" s="94" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="85" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="85"/>
+    </row>
+    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="93"/>
+      <c r="B44" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="85" t="s">
+        <v>290</v>
+      </c>
+      <c r="E44" s="85"/>
+    </row>
+    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="93"/>
+      <c r="B45" s="94" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="85" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="85" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="85" t="s">
+      <c r="E45" s="85"/>
+    </row>
+    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="93"/>
+      <c r="B46" s="94" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="85" t="s">
+      <c r="C46" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="85" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="83" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="85" t="s">
+      <c r="E46" s="85"/>
+    </row>
+    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="93"/>
+      <c r="B47" s="94" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="85" t="s">
+      <c r="C47" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="85" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="85" t="s">
+      <c r="E47" s="85"/>
+    </row>
+    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="93"/>
+      <c r="B48" s="94" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="83" t="s">
+      <c r="C48" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="85"/>
+    </row>
+    <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="93"/>
+      <c r="B49" s="94" t="s">
         <v>297</v>
       </c>
-      <c r="C39" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="85" t="s">
+      <c r="C49" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="85"/>
+    </row>
+    <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="93"/>
+      <c r="B50" s="94" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="96" t="s">
+      <c r="C50" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="85" t="s">
         <v>299</v>
       </c>
-      <c r="C40" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="95" t="s">
+      <c r="E50" s="85"/>
+    </row>
+    <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="93"/>
+      <c r="B51" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="85" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="85"/>
+    </row>
+    <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="93"/>
+      <c r="B52" s="94" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="85"/>
+    </row>
+    <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="93"/>
+      <c r="B53" s="94" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="85" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="88"/>
-      <c r="B41" s="96" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="95" t="s">
+      <c r="E53" s="85"/>
+    </row>
+    <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="93"/>
+      <c r="B54" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="85"/>
+    </row>
+    <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="93"/>
+      <c r="B55" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="85"/>
+    </row>
+    <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="93"/>
+      <c r="B56" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="85" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="88"/>
-      <c r="B42" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="95" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="88"/>
-      <c r="B43" s="96" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="95" t="s">
+      <c r="E56" s="85"/>
+    </row>
+    <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="93"/>
+      <c r="B57" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="85" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="96" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="95" t="s">
+      <c r="E57" s="85"/>
+    </row>
+    <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="93"/>
+      <c r="B58" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="85"/>
+    </row>
+    <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="93"/>
+      <c r="B59" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="85" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="96" t="s">
-        <v>177</v>
-      </c>
-      <c r="C45" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="95" t="s">
+      <c r="E59" s="85"/>
+    </row>
+    <row r="60" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="96"/>
+      <c r="B60" s="97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="98" t="s">
+        <v>451</v>
+      </c>
+      <c r="E60" s="98"/>
+    </row>
+    <row r="61" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="96"/>
+      <c r="B61" s="97" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="88"/>
-      <c r="B46" s="96" t="s">
+      <c r="C61" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="98" t="s">
         <v>305</v>
       </c>
-      <c r="C46" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="95" t="s">
+      <c r="E61" s="98"/>
+    </row>
+    <row r="62" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="96"/>
+      <c r="B62" s="97" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="88"/>
-      <c r="B47" s="96" t="s">
+      <c r="C62" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="98" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" s="98"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="C47" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="95" t="s">
+      <c r="C63" s="84" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="88"/>
-      <c r="B48" s="96" t="s">
+      <c r="D63" s="84" t="s">
         <v>309</v>
       </c>
-      <c r="C48" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="95" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="88"/>
-      <c r="B49" s="96" t="s">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="83" t="s">
         <v>310</v>
       </c>
-      <c r="C49" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="95" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="88"/>
-      <c r="B50" s="96" t="s">
+      <c r="C64" s="84" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" s="84" t="s">
         <v>311</v>
-      </c>
-      <c r="C50" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="95" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="88"/>
-      <c r="B51" s="96" t="s">
-        <v>156</v>
-      </c>
-      <c r="C51" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="95" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="88"/>
-      <c r="B52" s="96" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="95" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="88"/>
-      <c r="B53" s="96" t="s">
-        <v>179</v>
-      </c>
-      <c r="C53" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="95" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="88"/>
-      <c r="B54" s="96" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="95" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="88"/>
-      <c r="B55" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="88"/>
-      <c r="B56" s="96" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="95" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="88"/>
-      <c r="B57" s="96" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="95" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="88"/>
-      <c r="B58" s="96" t="s">
-        <v>184</v>
-      </c>
-      <c r="C58" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="95" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="88"/>
-      <c r="B59" s="96" t="s">
-        <v>185</v>
-      </c>
-      <c r="C59" s="95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="95" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="C60" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="85" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="83" t="s">
-        <v>317</v>
-      </c>
-      <c r="C61" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="85" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="83" t="s">
-        <v>319</v>
-      </c>
-      <c r="C62" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="85" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="83" t="s">
-        <v>320</v>
-      </c>
-      <c r="C63" s="84" t="s">
-        <v>321</v>
-      </c>
-      <c r="D63" s="84" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="83" t="s">
-        <v>323</v>
-      </c>
-      <c r="C64" s="84" t="s">
-        <v>321</v>
-      </c>
-      <c r="D64" s="84" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="83" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="C65" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D65" s="84" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="83" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="C66" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D66" s="84" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="83" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C67" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D67" s="84" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="83" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C68" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D68" s="84" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="83" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="C69" s="84" t="s">
+        <v>308</v>
+      </c>
+      <c r="D69" s="84" t="s">
         <v>321</v>
-      </c>
-      <c r="D69" s="84" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="83" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="C70" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D70" s="84" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="83" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="C71" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D71" s="84" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="83" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="C72" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D72" s="84" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="83" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="C73" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D73" s="84" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="83" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="C74" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D74" s="84" t="s">
         <v>221</v>
@@ -6608,524 +6689,558 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="83" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C75" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D75" s="84" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="83" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C76" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D76" s="84" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="83" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D77" s="84" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="83" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="C78" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D78" s="84" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="83" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="C79" s="84" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D79" s="84" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="83" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C80" s="84" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D80" s="84" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" s="83" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D81" s="84" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="83" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="C82" s="84" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D82" s="84" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" s="83" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C83" s="84" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D83" s="84" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" s="83" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="C84" s="84" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D84" s="85" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B85" s="83" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="C85" s="84" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="D85" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="E85" s="84" t="s">
         <v>365</v>
       </c>
-      <c r="E85" s="84" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" s="83" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="C86" s="84" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="D86" s="85" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="E86" s="84" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" s="83" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="C87" s="84" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
       <c r="E87" s="86" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B88" s="83" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="C88" s="84" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
       <c r="E88" s="86" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" s="83" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="C89" s="84" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
       <c r="E89" s="86" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="83" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="C90" s="84" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
       <c r="E90" s="86" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="83" t="s">
+        <v>360</v>
+      </c>
+      <c r="C91" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="D91" s="85" t="s">
+        <v>361</v>
+      </c>
+      <c r="E91" s="86" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="83" t="s">
+        <v>363</v>
+      </c>
+      <c r="C92" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="D92" s="85" t="s">
+        <v>364</v>
+      </c>
+      <c r="E92" s="86" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="96"/>
+      <c r="B93" s="97" t="s">
+        <v>366</v>
+      </c>
+      <c r="C93" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="98" t="s">
+        <v>367</v>
+      </c>
+      <c r="E93" s="98"/>
+    </row>
+    <row r="94" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="96"/>
+      <c r="B94" s="97" t="s">
+        <v>368</v>
+      </c>
+      <c r="C94" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="98" t="s">
+        <v>459</v>
+      </c>
+      <c r="E94" s="98"/>
+    </row>
+    <row r="95" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="96"/>
+      <c r="B95" s="97" t="s">
+        <v>369</v>
+      </c>
+      <c r="C95" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="98" t="s">
+        <v>370</v>
+      </c>
+      <c r="E95" s="98"/>
+    </row>
+    <row r="96" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="96"/>
+      <c r="B96" s="97" t="s">
+        <v>371</v>
+      </c>
+      <c r="C96" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="98" t="s">
+        <v>372</v>
+      </c>
+      <c r="E96" s="98"/>
+    </row>
+    <row r="97" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="96"/>
+      <c r="B97" s="97" t="s">
+        <v>373</v>
+      </c>
+      <c r="C97" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="98" t="s">
+        <v>374</v>
+      </c>
+      <c r="E97" s="98"/>
+    </row>
+    <row r="98" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="96"/>
+      <c r="B98" s="97" t="s">
+        <v>375</v>
+      </c>
+      <c r="C98" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="98" t="s">
+        <v>376</v>
+      </c>
+      <c r="E98" s="98"/>
+    </row>
+    <row r="99" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="96"/>
+      <c r="B99" s="97" t="s">
+        <v>377</v>
+      </c>
+      <c r="C99" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="98" t="s">
+        <v>378</v>
+      </c>
+      <c r="E99" s="98"/>
+    </row>
+    <row r="100" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="96"/>
+      <c r="B100" s="97" t="s">
+        <v>381</v>
+      </c>
+      <c r="C100" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="98" t="s">
+        <v>382</v>
+      </c>
+      <c r="E100" s="98"/>
+    </row>
+    <row r="101" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="96"/>
+      <c r="B101" s="97" t="s">
+        <v>383</v>
+      </c>
+      <c r="C101" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="98" t="s">
+        <v>384</v>
+      </c>
+      <c r="E101" s="98"/>
+    </row>
+    <row r="102" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="96"/>
+      <c r="B102" s="97" t="s">
+        <v>385</v>
+      </c>
+      <c r="C102" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="98" t="s">
+        <v>386</v>
+      </c>
+      <c r="E102" s="98"/>
+    </row>
+    <row r="103" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="96"/>
+      <c r="B103" s="97" t="s">
+        <v>387</v>
+      </c>
+      <c r="C103" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="98" t="s">
+        <v>460</v>
+      </c>
+      <c r="E103" s="98"/>
+    </row>
+    <row r="104" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="96"/>
+      <c r="B104" s="97" t="s">
+        <v>388</v>
+      </c>
+      <c r="C104" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="98" t="s">
+        <v>461</v>
+      </c>
+      <c r="E104" s="98"/>
+    </row>
+    <row r="105" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="96"/>
+      <c r="B105" s="97" t="s">
+        <v>389</v>
+      </c>
+      <c r="C105" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="98" t="s">
+        <v>462</v>
+      </c>
+      <c r="E105" s="98"/>
+    </row>
+    <row r="106" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="96"/>
+      <c r="B106" s="97" t="s">
+        <v>390</v>
+      </c>
+      <c r="C106" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="98" t="s">
+        <v>391</v>
+      </c>
+      <c r="E106" s="98"/>
+    </row>
+    <row r="107" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="96"/>
+      <c r="B107" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="C107" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="98" t="s">
+        <v>393</v>
+      </c>
+      <c r="E107" s="98"/>
+    </row>
+    <row r="108" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="96"/>
+      <c r="B108" s="97" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="98" t="s">
+        <v>394</v>
+      </c>
+      <c r="E108" s="98"/>
+    </row>
+    <row r="109" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="96"/>
+      <c r="B109" s="97" t="s">
+        <v>395</v>
+      </c>
+      <c r="C109" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="98" t="s">
+        <v>464</v>
+      </c>
+      <c r="E109" s="98"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="83" t="s">
+        <v>379</v>
+      </c>
+      <c r="C110" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D110" s="84" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="83" t="s">
+        <v>380</v>
+      </c>
+      <c r="C111" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D111" s="84" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="83" t="s">
+        <v>399</v>
+      </c>
+      <c r="C112" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D112" s="84" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="83" t="s">
+        <v>401</v>
+      </c>
+      <c r="C113" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="84" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="83" t="s">
+        <v>403</v>
+      </c>
+      <c r="C114" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D114" s="84" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="83" t="s">
+        <v>405</v>
+      </c>
+      <c r="C115" s="84" t="s">
+        <v>282</v>
+      </c>
+      <c r="D115" s="84" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="83" t="s">
+        <v>407</v>
+      </c>
+      <c r="C116" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D116" s="84" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="83" t="s">
+        <v>409</v>
+      </c>
+      <c r="C117" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D117" s="84" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="83" t="s">
+        <v>411</v>
+      </c>
+      <c r="C118" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D118" s="84" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="83" t="s">
+        <v>413</v>
+      </c>
+      <c r="C119" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D119" s="84" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="83" t="s">
-        <v>373</v>
-      </c>
-      <c r="C91" s="84" t="s">
-        <v>368</v>
-      </c>
-      <c r="D91" s="85" t="s">
-        <v>374</v>
-      </c>
-      <c r="E91" s="86" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="83" t="s">
-        <v>376</v>
-      </c>
-      <c r="C92" s="84" t="s">
-        <v>368</v>
-      </c>
-      <c r="D92" s="85" t="s">
-        <v>377</v>
-      </c>
-      <c r="E92" s="86" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="83" t="s">
-        <v>379</v>
-      </c>
-      <c r="C93" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="85" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="83" t="s">
-        <v>381</v>
-      </c>
-      <c r="C94" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="85" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="83" t="s">
-        <v>383</v>
-      </c>
-      <c r="C95" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="85" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="83" t="s">
-        <v>385</v>
-      </c>
-      <c r="C96" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="85" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="83" t="s">
-        <v>387</v>
-      </c>
-      <c r="C97" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="85" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="83" t="s">
-        <v>389</v>
-      </c>
-      <c r="C98" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="85" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="83" t="s">
-        <v>391</v>
-      </c>
-      <c r="C99" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="85" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="83" t="s">
-        <v>395</v>
-      </c>
-      <c r="C100" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="85" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="83" t="s">
-        <v>397</v>
-      </c>
-      <c r="C101" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="85" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="83" t="s">
-        <v>399</v>
-      </c>
-      <c r="C102" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="85" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="83" t="s">
-        <v>401</v>
-      </c>
-      <c r="C103" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="85" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="83" t="s">
-        <v>403</v>
-      </c>
-      <c r="C104" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="85" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="83" t="s">
-        <v>405</v>
-      </c>
-      <c r="C105" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="85" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="83" t="s">
-        <v>407</v>
-      </c>
-      <c r="C106" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="85" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="83" t="s">
-        <v>409</v>
-      </c>
-      <c r="C107" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="85" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="83" t="s">
-        <v>187</v>
-      </c>
-      <c r="C108" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="85" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="83" t="s">
-        <v>412</v>
-      </c>
-      <c r="C109" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="85" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="83" t="s">
-        <v>393</v>
-      </c>
-      <c r="C110" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D110" s="84" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="83" t="s">
-        <v>394</v>
-      </c>
-      <c r="C111" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D111" s="84" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="83" t="s">
-        <v>417</v>
-      </c>
-      <c r="C112" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D112" s="84" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="83" t="s">
-        <v>419</v>
-      </c>
-      <c r="C113" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="84" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="83" t="s">
-        <v>421</v>
-      </c>
-      <c r="C114" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D114" s="84" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="83" t="s">
-        <v>423</v>
-      </c>
-      <c r="C115" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="D115" s="84" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="83" t="s">
-        <v>425</v>
-      </c>
-      <c r="C116" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D116" s="84" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="83" t="s">
-        <v>427</v>
-      </c>
-      <c r="C117" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D117" s="84" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="83" t="s">
-        <v>429</v>
-      </c>
-      <c r="C118" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D118" s="84" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="83" t="s">
-        <v>431</v>
-      </c>
-      <c r="C119" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D119" s="84" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B120" s="83" t="s">
         <v>188</v>
       </c>
@@ -7133,228 +7248,275 @@
         <v>258</v>
       </c>
       <c r="D120" s="84" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="83" t="s">
+        <v>416</v>
+      </c>
+      <c r="C121" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="D121" s="84" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="83" t="s">
+        <v>417</v>
+      </c>
+      <c r="C122" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="84" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="96"/>
+      <c r="B123" s="97" t="s">
+        <v>420</v>
+      </c>
+      <c r="C123" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="98" t="s">
+        <v>421</v>
+      </c>
+      <c r="E123" s="98"/>
+    </row>
+    <row r="124" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="96"/>
+      <c r="B124" s="97" t="s">
+        <v>422</v>
+      </c>
+      <c r="C124" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="98" t="s">
+        <v>423</v>
+      </c>
+      <c r="E124" s="98"/>
+    </row>
+    <row r="125" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="96"/>
+      <c r="B125" s="97" t="s">
+        <v>424</v>
+      </c>
+      <c r="C125" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="98" t="s">
+        <v>468</v>
+      </c>
+      <c r="E125" s="98"/>
+    </row>
+    <row r="126" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="96"/>
+      <c r="B126" s="97" t="s">
+        <v>425</v>
+      </c>
+      <c r="C126" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="98" t="s">
+        <v>426</v>
+      </c>
+      <c r="E126" s="98"/>
+    </row>
+    <row r="127" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="96"/>
+      <c r="B127" s="97" t="s">
+        <v>427</v>
+      </c>
+      <c r="C127" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="98" t="s">
+        <v>428</v>
+      </c>
+      <c r="E127" s="98"/>
+    </row>
+    <row r="128" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="96"/>
+      <c r="B128" s="97" t="s">
+        <v>429</v>
+      </c>
+      <c r="C128" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="98" t="s">
+        <v>430</v>
+      </c>
+      <c r="E128" s="98"/>
+    </row>
+    <row r="129" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="96"/>
+      <c r="B129" s="97" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="98" t="s">
+        <v>431</v>
+      </c>
+      <c r="E129" s="98"/>
+    </row>
+    <row r="130" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="96"/>
+      <c r="B130" s="97" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="98" t="s">
+        <v>301</v>
+      </c>
+      <c r="E130" s="98"/>
+    </row>
+    <row r="131" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="96"/>
+      <c r="B131" s="97" t="s">
+        <v>432</v>
+      </c>
+      <c r="C131" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="98" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="83" t="s">
+      <c r="E131" s="98"/>
+    </row>
+    <row r="132" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="96"/>
+      <c r="B132" s="97" t="s">
         <v>434</v>
       </c>
-      <c r="C121" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D121" s="84" t="s">
+      <c r="C132" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="98" t="s">
+        <v>435</v>
+      </c>
+      <c r="E132" s="98"/>
+    </row>
+    <row r="133" spans="1:5" s="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="96"/>
+      <c r="B133" s="97" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="83" t="s">
-        <v>435</v>
-      </c>
-      <c r="C122" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="84" t="s">
+      <c r="C133" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="98" t="s">
+        <v>470</v>
+      </c>
+      <c r="E133" s="98"/>
+    </row>
+    <row r="134" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="96"/>
+      <c r="B134" s="97" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="83" t="s">
+      <c r="C134" s="98" t="s">
+        <v>275</v>
+      </c>
+      <c r="D134" s="98" t="s">
         <v>438</v>
       </c>
-      <c r="C123" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="84" t="s">
+      <c r="E134" s="98"/>
+    </row>
+    <row r="135" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="96"/>
+      <c r="B135" s="97" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="83" t="s">
+      <c r="C135" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="98" t="s">
         <v>440</v>
       </c>
-      <c r="C124" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="84" t="s">
+      <c r="E135" s="98"/>
+    </row>
+    <row r="136" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="96"/>
+      <c r="B136" s="97" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="83" t="s">
+      <c r="C136" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="98" t="s">
+        <v>473</v>
+      </c>
+      <c r="E136" s="98"/>
+    </row>
+    <row r="137" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="96"/>
+      <c r="B137" s="97" t="s">
         <v>442</v>
       </c>
-      <c r="C125" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="84" t="s">
+      <c r="C137" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="98" t="s">
+        <v>472</v>
+      </c>
+      <c r="E137" s="98"/>
+    </row>
+    <row r="138" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="96"/>
+      <c r="B138" s="97" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="83" t="s">
+      <c r="C138" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="98" t="s">
         <v>444</v>
       </c>
-      <c r="C126" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="84" t="s">
+      <c r="E138" s="98"/>
+    </row>
+    <row r="139" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="96"/>
+      <c r="B139" s="97" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="83" t="s">
+      <c r="C139" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="98" t="s">
+        <v>474</v>
+      </c>
+      <c r="E139" s="98"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="83" t="s">
         <v>446</v>
       </c>
-      <c r="C127" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="84" t="s">
+      <c r="C140" s="84" t="s">
+        <v>275</v>
+      </c>
+      <c r="D140" s="84" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="83" t="s">
-        <v>448</v>
-      </c>
-      <c r="C128" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="84" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="83" t="s">
-        <v>189</v>
-      </c>
-      <c r="C129" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="84" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C130" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="84" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="83" t="s">
-        <v>451</v>
-      </c>
-      <c r="C131" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="84" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="83" t="s">
-        <v>453</v>
-      </c>
-      <c r="C132" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="84" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="83" t="s">
-        <v>455</v>
-      </c>
-      <c r="C133" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="84" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="83" t="s">
-        <v>457</v>
-      </c>
-      <c r="C134" s="84" t="s">
-        <v>281</v>
-      </c>
-      <c r="D134" s="84" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="83" t="s">
-        <v>459</v>
-      </c>
-      <c r="C135" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D135" s="84" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="83" t="s">
-        <v>461</v>
-      </c>
-      <c r="C136" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="84" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="83" t="s">
-        <v>463</v>
-      </c>
-      <c r="C137" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="84" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="83" t="s">
+    <row r="141" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="96"/>
+      <c r="B141" s="97" t="s">
         <v>465</v>
       </c>
-      <c r="C138" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="84" t="s">
+      <c r="C141" s="98" t="s">
+        <v>275</v>
+      </c>
+      <c r="D141" s="98" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="83" t="s">
-        <v>467</v>
-      </c>
-      <c r="C139" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="84" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="83" t="s">
-        <v>469</v>
-      </c>
-      <c r="C140" s="84" t="s">
-        <v>281</v>
-      </c>
-      <c r="D140" s="84" t="s">
-        <v>470</v>
-      </c>
+      <c r="E141" s="98"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated treeview with 2.0 content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C84F01-9EC7-4CB8-B274-FEE86B3915A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD3867F-D5E1-4513-A6E1-7C2474744C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="750" windowWidth="10725" windowHeight="13755" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="14655" yWindow="30" windowWidth="14250" windowHeight="14475" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="498">
   <si>
     <t>ID</t>
   </si>
@@ -818,15 +818,6 @@
     <t>MainForm</t>
   </si>
   <si>
-    <t>The Importance of Storytelling</t>
-  </si>
-  <si>
-    <t>Storytelling Best Practices</t>
-  </si>
-  <si>
-    <t>Equity and Resilience</t>
-  </si>
-  <si>
     <t>Who are ERB users?</t>
   </si>
   <si>
@@ -1235,15 +1226,9 @@
     <t>Ch 3 About 4 column image</t>
   </si>
   <si>
-    <t>Ch 3 About 3 column image</t>
-  </si>
-  <si>
     <t>113</t>
   </si>
   <si>
-    <t>Ch 2 Activity 1 figure</t>
-  </si>
-  <si>
     <t>114</t>
   </si>
   <si>
@@ -1464,6 +1449,90 @@
   </si>
   <si>
     <t>Reflect and Celebrate (Ch 5)</t>
+  </si>
+  <si>
+    <t>Storytelling</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Second Bullet</t>
+  </si>
+  <si>
+    <t>Equitable Resilience</t>
+  </si>
+  <si>
+    <t>The ERB Process</t>
+  </si>
+  <si>
+    <t>Trauma-informed Approach</t>
+  </si>
+  <si>
+    <t>Circle Picture. Trauma informed</t>
+  </si>
+  <si>
+    <t>Data Ethics</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>Types of data used in ERB</t>
+  </si>
+  <si>
+    <t>Resilience Indicators Background</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>Gather data on hazards, equity, and resilience</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 1.</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 2.</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Youth Engagement. Figure 3.</t>
+  </si>
+  <si>
+    <t>Youth Engagement Guide</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Results to Action Workshop Agenda Builder</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>Strategy Chart Example</t>
+  </si>
+  <si>
+    <t>Strategy Chart Image</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>ERB Activity Chart</t>
   </si>
 </sst>
 </file>
@@ -1550,7 +1619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1808,7 +1877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1969,36 +2038,53 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2008,9 +2094,9 @@
   <colors>
     <mruColors>
       <color rgb="FFB1E36F"/>
+      <color rgb="FF80DEF8"/>
+      <color rgb="FFBAF8E2"/>
       <color rgb="FFFB9B9B"/>
-      <color rgb="FFBAF8E2"/>
-      <color rgb="FF80DEF8"/>
       <color rgb="FFE0C1FF"/>
     </mruColors>
   </colors>
@@ -2391,10 +2477,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="101"/>
+      <c r="H2" s="97"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5758,299 +5844,325 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135:XFD135"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="93" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="90" customWidth="1"/>
     <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
     <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="66.7109375" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="87" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91"/>
-      <c r="B1" s="89" t="s">
+    <row r="1" spans="1:5" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89"/>
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="88" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="88" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="90" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="83" t="s">
+      <c r="E1" s="88" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="107"/>
+      <c r="B2" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="95" t="s">
+      <c r="C2" s="108" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="88"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="E2" s="108"/>
+    </row>
+    <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="92"/>
+      <c r="B3" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>470</v>
+      </c>
+      <c r="E3" s="94"/>
+    </row>
+    <row r="4" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="92"/>
+      <c r="B4" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>475</v>
+      </c>
+      <c r="E4" s="94"/>
+    </row>
+    <row r="5" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="92"/>
+      <c r="B5" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>473</v>
+      </c>
+      <c r="E5" s="94"/>
+    </row>
+    <row r="6" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="92"/>
+      <c r="B6" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>477</v>
+      </c>
+      <c r="E6" s="94"/>
+    </row>
+    <row r="7" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="92"/>
+      <c r="B7" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>480</v>
+      </c>
+      <c r="E7" s="94"/>
+    </row>
+    <row r="8" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="109"/>
+      <c r="B8" s="110" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="111" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="85" t="s">
+      <c r="E8" s="111"/>
+    </row>
+    <row r="9" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="109"/>
+      <c r="B9" s="110" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="85" t="s">
+      <c r="C9" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="111" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="85" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="85" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="85" t="s">
+      <c r="E9" s="111"/>
+    </row>
+    <row r="10" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="109"/>
+      <c r="B10" s="110" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="83" t="s">
+      <c r="C10" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="85" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="85" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="83" t="s">
+      <c r="E10" s="111"/>
+    </row>
+    <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="92"/>
+      <c r="B11" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="85" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="83" t="s">
+      <c r="C11" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>489</v>
+      </c>
+      <c r="E11" s="94"/>
+    </row>
+    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="90"/>
+      <c r="B12" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D12" s="85" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="83" t="s">
+      <c r="E12" s="85"/>
+    </row>
+    <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="90"/>
+      <c r="B13" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D13" s="85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="83" t="s">
+      <c r="E13" s="85"/>
+    </row>
+    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="90"/>
+      <c r="B14" s="91" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="83" t="s">
+        <v>264</v>
+      </c>
+      <c r="E14" s="85"/>
+    </row>
+    <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="90"/>
+      <c r="B15" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D15" s="85" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="96"/>
-      <c r="B16" s="97" t="s">
+      <c r="E15" s="85"/>
+    </row>
+    <row r="16" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="103"/>
+      <c r="B16" s="104" t="s">
+        <v>265</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="105" t="s">
+        <v>443</v>
+      </c>
+      <c r="E16" s="105"/>
+    </row>
+    <row r="17" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="103"/>
+      <c r="B17" s="104" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="105" t="s">
+        <v>448</v>
+      </c>
+      <c r="E17" s="105"/>
+    </row>
+    <row r="18" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="103"/>
+      <c r="B18" s="104" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="105" t="s">
+        <v>453</v>
+      </c>
+      <c r="E18" s="105"/>
+    </row>
+    <row r="19" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="103"/>
+      <c r="B19" s="104" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="98" t="s">
-        <v>448</v>
-      </c>
-      <c r="E16" s="98"/>
-    </row>
-    <row r="17" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="97" t="s">
+      <c r="C19" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="105" t="s">
+        <v>462</v>
+      </c>
+      <c r="E19" s="105"/>
+    </row>
+    <row r="20" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="103"/>
+      <c r="B20" s="104" t="s">
         <v>269</v>
       </c>
-      <c r="C17" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="98" t="s">
-        <v>453</v>
-      </c>
-      <c r="E17" s="98"/>
-    </row>
-    <row r="18" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="97" t="s">
+      <c r="C20" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="105" t="s">
+        <v>466</v>
+      </c>
+      <c r="E20" s="105"/>
+    </row>
+    <row r="21" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="103"/>
+      <c r="B21" s="104" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>445</v>
+      </c>
+      <c r="E21" s="105"/>
+    </row>
+    <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="90"/>
+      <c r="B22" s="91" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="C18" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="98" t="s">
-        <v>458</v>
-      </c>
-      <c r="E18" s="98"/>
-    </row>
-    <row r="19" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="97" t="s">
+      <c r="E22" s="85"/>
+    </row>
+    <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="90"/>
+      <c r="B23" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" s="85" t="s">
         <v>271</v>
       </c>
-      <c r="C19" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="98" t="s">
-        <v>467</v>
-      </c>
-      <c r="E19" s="98"/>
-    </row>
-    <row r="20" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="97" t="s">
-        <v>272</v>
-      </c>
-      <c r="C20" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="98" t="s">
-        <v>471</v>
-      </c>
-      <c r="E20" s="98"/>
-    </row>
-    <row r="21" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
-      <c r="B21" s="97" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="98" t="s">
-        <v>450</v>
-      </c>
-      <c r="E21" s="98"/>
-    </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="94" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="85" t="s">
-        <v>273</v>
-      </c>
-      <c r="E22" s="85"/>
-    </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="93"/>
-      <c r="B23" s="94" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="85" t="s">
-        <v>274</v>
-      </c>
       <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93"/>
-      <c r="B24" s="94" t="s">
+      <c r="A24" s="90"/>
+      <c r="B24" s="91" t="s">
         <v>163</v>
       </c>
       <c r="C24" s="85" t="s">
@@ -6062,229 +6174,229 @@
       <c r="E24" s="85"/>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="93"/>
-      <c r="B25" s="94" t="s">
+      <c r="A25" s="90"/>
+      <c r="B25" s="91" t="s">
         <v>164</v>
       </c>
       <c r="C25" s="85" t="s">
+        <v>272</v>
+      </c>
+      <c r="D25" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" s="85"/>
+    </row>
+    <row r="26" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="103"/>
+      <c r="B26" s="104" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>464</v>
+      </c>
+      <c r="E26" s="105"/>
+    </row>
+    <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="90"/>
+      <c r="B27" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D25" s="85" t="s">
+      <c r="E27" s="85"/>
+    </row>
+    <row r="28" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="103"/>
+      <c r="B28" s="104" t="s">
         <v>276</v>
       </c>
-      <c r="E25" s="85"/>
-    </row>
-    <row r="26" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
-      <c r="B26" s="97" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="98" t="s">
-        <v>469</v>
-      </c>
-      <c r="E26" s="98"/>
-    </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="93"/>
-      <c r="B27" s="94" t="s">
+      <c r="C28" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="D28" s="105" t="s">
         <v>277</v>
       </c>
-      <c r="C27" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="85" t="s">
+      <c r="E28" s="105"/>
+    </row>
+    <row r="29" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="103"/>
+      <c r="B29" s="104" t="s">
         <v>278</v>
       </c>
-      <c r="E27" s="85"/>
-    </row>
-    <row r="28" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96"/>
-      <c r="B28" s="97" t="s">
+      <c r="C29" s="105" t="s">
         <v>279</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="D29" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="105"/>
+    </row>
+    <row r="30" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="103"/>
+      <c r="B30" s="104" t="s">
+        <v>280</v>
+      </c>
+      <c r="C30" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="D30" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="105"/>
+    </row>
+    <row r="31" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="103"/>
+      <c r="B31" s="104" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="105" t="s">
+        <v>444</v>
+      </c>
+      <c r="E31" s="105"/>
+    </row>
+    <row r="32" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="103"/>
+      <c r="B32" s="104" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="105" t="s">
+        <v>447</v>
+      </c>
+      <c r="E32" s="105"/>
+    </row>
+    <row r="33" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="103"/>
+      <c r="B33" s="104" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="105"/>
+    </row>
+    <row r="34" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="103"/>
+      <c r="B34" s="104" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="105" t="s">
+        <v>452</v>
+      </c>
+      <c r="E34" s="105"/>
+    </row>
+    <row r="35" spans="1:5" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="103"/>
+      <c r="B35" s="104" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="105" t="s">
+        <v>449</v>
+      </c>
+      <c r="E35" s="105"/>
+    </row>
+    <row r="36" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="103"/>
+      <c r="B36" s="104" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="105" t="s">
+        <v>281</v>
+      </c>
+      <c r="E36" s="105"/>
+    </row>
+    <row r="37" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="103"/>
+      <c r="B37" s="104" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="105" t="s">
+        <v>450</v>
+      </c>
+      <c r="E37" s="105"/>
+    </row>
+    <row r="38" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="103"/>
+      <c r="B38" s="104" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="105" t="s">
+        <v>458</v>
+      </c>
+      <c r="E38" s="105"/>
+    </row>
+    <row r="39" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="103"/>
+      <c r="B39" s="104" t="s">
         <v>282</v>
       </c>
-      <c r="D28" s="98" t="s">
-        <v>280</v>
-      </c>
-      <c r="E28" s="98"/>
-    </row>
-    <row r="29" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="96"/>
-      <c r="B29" s="97" t="s">
-        <v>281</v>
-      </c>
-      <c r="C29" s="98" t="s">
-        <v>282</v>
-      </c>
-      <c r="D29" s="98" t="s">
-        <v>233</v>
-      </c>
-      <c r="E29" s="98"/>
-    </row>
-    <row r="30" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="96"/>
-      <c r="B30" s="97" t="s">
+      <c r="C39" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="105" t="s">
+        <v>451</v>
+      </c>
+      <c r="E39" s="105"/>
+    </row>
+    <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="90"/>
+      <c r="B40" s="91" t="s">
         <v>283</v>
       </c>
-      <c r="C30" s="98" t="s">
-        <v>282</v>
-      </c>
-      <c r="D30" s="98" t="s">
-        <v>234</v>
-      </c>
-      <c r="E30" s="98"/>
-    </row>
-    <row r="31" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="96"/>
-      <c r="B31" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="98" t="s">
-        <v>449</v>
-      </c>
-      <c r="E31" s="98"/>
-    </row>
-    <row r="32" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="96"/>
-      <c r="B32" s="97" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="98" t="s">
-        <v>452</v>
-      </c>
-      <c r="E32" s="98"/>
-    </row>
-    <row r="33" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="96"/>
-      <c r="B33" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="98" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="98"/>
-    </row>
-    <row r="34" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="96"/>
-      <c r="B34" s="97" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="98" t="s">
-        <v>457</v>
-      </c>
-      <c r="E34" s="98"/>
-    </row>
-    <row r="35" spans="1:5" s="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="96"/>
-      <c r="B35" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="98" t="s">
-        <v>454</v>
-      </c>
-      <c r="E35" s="98"/>
-    </row>
-    <row r="36" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="96"/>
-      <c r="B36" s="97" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="98" t="s">
+      <c r="C40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="85" t="s">
         <v>284</v>
       </c>
-      <c r="E36" s="98"/>
-    </row>
-    <row r="37" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="96"/>
-      <c r="B37" s="97" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="98" t="s">
-        <v>455</v>
-      </c>
-      <c r="E37" s="98"/>
-    </row>
-    <row r="38" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="96"/>
-      <c r="B38" s="97" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="98" t="s">
-        <v>463</v>
-      </c>
-      <c r="E38" s="98"/>
-    </row>
-    <row r="39" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="96"/>
-      <c r="B39" s="97" t="s">
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="90"/>
+      <c r="B41" s="91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="85" t="s">
         <v>285</v>
       </c>
-      <c r="C39" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="98" t="s">
-        <v>456</v>
-      </c>
-      <c r="E39" s="98"/>
-    </row>
-    <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="93"/>
-      <c r="B40" s="94" t="s">
-        <v>286</v>
-      </c>
-      <c r="C40" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="85" t="s">
-        <v>287</v>
-      </c>
-      <c r="E40" s="85"/>
-    </row>
-    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="93"/>
-      <c r="B41" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="85" t="s">
-        <v>288</v>
-      </c>
       <c r="E41" s="85"/>
     </row>
     <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93"/>
-      <c r="B42" s="94" t="s">
+      <c r="A42" s="90"/>
+      <c r="B42" s="91" t="s">
         <v>174</v>
       </c>
       <c r="C42" s="85" t="s">
@@ -6296,74 +6408,74 @@
       <c r="E42" s="85"/>
     </row>
     <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="94" t="s">
+      <c r="A43" s="90"/>
+      <c r="B43" s="91" t="s">
         <v>175</v>
       </c>
       <c r="C43" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D43" s="85" t="s">
+        <v>286</v>
+      </c>
+      <c r="E43" s="85"/>
+    </row>
+    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="90"/>
+      <c r="B44" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="85" t="s">
+        <v>287</v>
+      </c>
+      <c r="E44" s="85"/>
+    </row>
+    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="90"/>
+      <c r="B45" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="E45" s="85"/>
+    </row>
+    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="90"/>
+      <c r="B46" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="E43" s="85"/>
-    </row>
-    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93"/>
-      <c r="B44" s="94" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="85" t="s">
+      <c r="C46" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="E44" s="85"/>
-    </row>
-    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="93"/>
-      <c r="B45" s="94" t="s">
-        <v>177</v>
-      </c>
-      <c r="C45" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="85" t="s">
+      <c r="E46" s="85"/>
+    </row>
+    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="90"/>
+      <c r="B47" s="91" t="s">
         <v>291</v>
       </c>
-      <c r="E45" s="85"/>
-    </row>
-    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="93"/>
-      <c r="B46" s="94" t="s">
+      <c r="C47" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="85" t="s">
         <v>292</v>
       </c>
-      <c r="C46" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="85" t="s">
+      <c r="E47" s="85"/>
+    </row>
+    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="90"/>
+      <c r="B48" s="91" t="s">
         <v>293</v>
-      </c>
-      <c r="E46" s="85"/>
-    </row>
-    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="93"/>
-      <c r="B47" s="94" t="s">
-        <v>294</v>
-      </c>
-      <c r="C47" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="85" t="s">
-        <v>295</v>
-      </c>
-      <c r="E47" s="85"/>
-    </row>
-    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="93"/>
-      <c r="B48" s="94" t="s">
-        <v>296</v>
       </c>
       <c r="C48" s="85" t="s">
         <v>258</v>
@@ -6374,9 +6486,9 @@
       <c r="E48" s="85"/>
     </row>
     <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="93"/>
-      <c r="B49" s="94" t="s">
-        <v>297</v>
+      <c r="A49" s="90"/>
+      <c r="B49" s="91" t="s">
+        <v>294</v>
       </c>
       <c r="C49" s="85" t="s">
         <v>258</v>
@@ -6387,21 +6499,21 @@
       <c r="E49" s="85"/>
     </row>
     <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="93"/>
-      <c r="B50" s="94" t="s">
-        <v>298</v>
+      <c r="A50" s="90"/>
+      <c r="B50" s="91" t="s">
+        <v>295</v>
       </c>
       <c r="C50" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D50" s="85" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E50" s="85"/>
     </row>
     <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="93"/>
-      <c r="B51" s="94" t="s">
+      <c r="A51" s="90"/>
+      <c r="B51" s="91" t="s">
         <v>156</v>
       </c>
       <c r="C51" s="85" t="s">
@@ -6413,8 +6525,8 @@
       <c r="E51" s="85"/>
     </row>
     <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="93"/>
-      <c r="B52" s="94" t="s">
+      <c r="A52" s="90"/>
+      <c r="B52" s="91" t="s">
         <v>178</v>
       </c>
       <c r="C52" s="85" t="s">
@@ -6426,21 +6538,21 @@
       <c r="E52" s="85"/>
     </row>
     <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="93"/>
-      <c r="B53" s="94" t="s">
+      <c r="A53" s="90"/>
+      <c r="B53" s="91" t="s">
         <v>179</v>
       </c>
       <c r="C53" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D53" s="85" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E53" s="85"/>
     </row>
     <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="93"/>
-      <c r="B54" s="94" t="s">
+      <c r="A54" s="90"/>
+      <c r="B54" s="91" t="s">
         <v>180</v>
       </c>
       <c r="C54" s="85" t="s">
@@ -6452,8 +6564,8 @@
       <c r="E54" s="85"/>
     </row>
     <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="93"/>
-      <c r="B55" s="94" t="s">
+      <c r="A55" s="90"/>
+      <c r="B55" s="91" t="s">
         <v>181</v>
       </c>
       <c r="C55" s="85" t="s">
@@ -6465,34 +6577,34 @@
       <c r="E55" s="85"/>
     </row>
     <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="93"/>
-      <c r="B56" s="94" t="s">
+      <c r="A56" s="90"/>
+      <c r="B56" s="91" t="s">
         <v>182</v>
       </c>
       <c r="C56" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D56" s="85" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E56" s="85"/>
     </row>
     <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="93"/>
-      <c r="B57" s="94" t="s">
+      <c r="A57" s="90"/>
+      <c r="B57" s="91" t="s">
         <v>183</v>
       </c>
       <c r="C57" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D57" s="85" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E57" s="85"/>
     </row>
     <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="93"/>
-      <c r="B58" s="94" t="s">
+      <c r="A58" s="90"/>
+      <c r="B58" s="91" t="s">
         <v>184</v>
       </c>
       <c r="C58" s="85" t="s">
@@ -6504,1019 +6616,1236 @@
       <c r="E58" s="85"/>
     </row>
     <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="93"/>
-      <c r="B59" s="94" t="s">
+      <c r="A59" s="90"/>
+      <c r="B59" s="91" t="s">
         <v>185</v>
       </c>
       <c r="C59" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D59" s="85" t="s">
+        <v>300</v>
+      </c>
+      <c r="E59" s="85"/>
+    </row>
+    <row r="60" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="103"/>
+      <c r="B60" s="104" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="105" t="s">
+        <v>446</v>
+      </c>
+      <c r="E60" s="105"/>
+    </row>
+    <row r="61" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="103"/>
+      <c r="B61" s="104" t="s">
+        <v>301</v>
+      </c>
+      <c r="C61" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="E61" s="105"/>
+    </row>
+    <row r="62" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="103"/>
+      <c r="B62" s="104" t="s">
         <v>303</v>
       </c>
-      <c r="E59" s="85"/>
-    </row>
-    <row r="60" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="96"/>
-      <c r="B60" s="97" t="s">
-        <v>186</v>
-      </c>
-      <c r="C60" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="98" t="s">
-        <v>451</v>
-      </c>
-      <c r="E60" s="98"/>
-    </row>
-    <row r="61" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="96"/>
-      <c r="B61" s="97" t="s">
+      <c r="C62" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="105" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" s="105"/>
+    </row>
+    <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="90"/>
+      <c r="B63" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="C61" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="98" t="s">
+      <c r="C63" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="E61" s="98"/>
-    </row>
-    <row r="62" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="96"/>
-      <c r="B62" s="97" t="s">
+      <c r="D63" s="85" t="s">
         <v>306</v>
       </c>
-      <c r="C62" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="98" t="s">
-        <v>230</v>
-      </c>
-      <c r="E62" s="98"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="83" t="s">
+      <c r="E63" s="85"/>
+    </row>
+    <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="90"/>
+      <c r="B64" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="C63" s="84" t="s">
+      <c r="C64" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D64" s="85" t="s">
         <v>308</v>
       </c>
-      <c r="D63" s="84" t="s">
+      <c r="E64" s="85"/>
+    </row>
+    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="90"/>
+      <c r="B65" s="91" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="83" t="s">
+      <c r="C65" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D65" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="C64" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D64" s="84" t="s">
+      <c r="E65" s="85"/>
+    </row>
+    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="90"/>
+      <c r="B66" s="91" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="83" t="s">
+      <c r="C66" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D66" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="C65" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D65" s="84" t="s">
+      <c r="E66" s="85"/>
+    </row>
+    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="90"/>
+      <c r="B67" s="91" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="83" t="s">
+      <c r="C67" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D67" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="C66" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D66" s="84" t="s">
+      <c r="E67" s="85"/>
+    </row>
+    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="90"/>
+      <c r="B68" s="91" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="83" t="s">
+      <c r="C68" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D68" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="C67" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D67" s="84" t="s">
+      <c r="E68" s="85"/>
+    </row>
+    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="90"/>
+      <c r="B69" s="91" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="83" t="s">
+      <c r="C69" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D69" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="C68" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D68" s="84" t="s">
+      <c r="E69" s="85"/>
+    </row>
+    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="90"/>
+      <c r="B70" s="91" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="83" t="s">
+      <c r="C70" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D70" s="85" t="s">
         <v>320</v>
       </c>
-      <c r="C69" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D69" s="84" t="s">
+      <c r="E70" s="85"/>
+    </row>
+    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="90"/>
+      <c r="B71" s="91" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="83" t="s">
+      <c r="C71" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="C70" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D70" s="84" t="s">
+      <c r="E71" s="85"/>
+    </row>
+    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="90"/>
+      <c r="B72" s="91" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="83" t="s">
+      <c r="C72" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" s="85" t="s">
         <v>324</v>
       </c>
-      <c r="C71" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D71" s="84" t="s">
+      <c r="E72" s="85"/>
+    </row>
+    <row r="73" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="90"/>
+      <c r="B73" s="91" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="83" t="s">
+      <c r="C73" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C72" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D72" s="84" t="s">
+      <c r="E73" s="85"/>
+    </row>
+    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="90"/>
+      <c r="B74" s="91" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="83" t="s">
+      <c r="C74" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D74" s="85" t="s">
+        <v>221</v>
+      </c>
+      <c r="E74" s="85"/>
+    </row>
+    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="90"/>
+      <c r="B75" s="91" t="s">
         <v>328</v>
       </c>
-      <c r="C73" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D73" s="84" t="s">
+      <c r="C75" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" s="85" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="83" t="s">
+      <c r="E75" s="85"/>
+    </row>
+    <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="90"/>
+      <c r="B76" s="91" t="s">
         <v>330</v>
       </c>
-      <c r="C74" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D74" s="84" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="83" t="s">
+      <c r="C76" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D76" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="C75" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D75" s="84" t="s">
+      <c r="E76" s="85"/>
+    </row>
+    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="90"/>
+      <c r="B77" s="91" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="83" t="s">
+      <c r="C77" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D77" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="C76" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D76" s="84" t="s">
+      <c r="E77" s="85"/>
+    </row>
+    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="90"/>
+      <c r="B78" s="91" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="83" t="s">
+      <c r="C78" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="C77" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D77" s="84" t="s">
+      <c r="E78" s="85"/>
+    </row>
+    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="90"/>
+      <c r="B79" s="91" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="83" t="s">
+      <c r="C79" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D79" s="85" t="s">
         <v>337</v>
       </c>
-      <c r="C78" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D78" s="84" t="s">
+      <c r="E79" s="85"/>
+    </row>
+    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="90"/>
+      <c r="B80" s="91" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="83" t="s">
+      <c r="C80" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="C79" s="84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D79" s="84" t="s">
+      <c r="D80" s="85" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="83" t="s">
+      <c r="E80" s="85"/>
+    </row>
+    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="90"/>
+      <c r="B81" s="91" t="s">
         <v>341</v>
       </c>
-      <c r="C80" s="84" t="s">
+      <c r="C81" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D81" s="85" t="s">
         <v>342</v>
       </c>
-      <c r="D80" s="84" t="s">
+      <c r="E81" s="85"/>
+    </row>
+    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="90"/>
+      <c r="B82" s="91" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="83" t="s">
+      <c r="C82" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D82" s="85" t="s">
         <v>344</v>
       </c>
-      <c r="C81" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D81" s="84" t="s">
+      <c r="E82" s="85"/>
+    </row>
+    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="90"/>
+      <c r="B83" s="91" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="83" t="s">
+      <c r="C83" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D83" s="85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E83" s="85"/>
+    </row>
+    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="90"/>
+      <c r="B84" s="91" t="s">
         <v>346</v>
       </c>
-      <c r="C82" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D82" s="84" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="83" t="s">
-        <v>348</v>
-      </c>
-      <c r="C83" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D83" s="84" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="83" t="s">
-        <v>349</v>
-      </c>
-      <c r="C84" s="84" t="s">
-        <v>342</v>
+      <c r="C84" s="85" t="s">
+        <v>339</v>
       </c>
       <c r="D84" s="85" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="83" t="s">
+      <c r="E84" s="85"/>
+    </row>
+    <row r="85" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="103"/>
+      <c r="B85" s="104" t="s">
+        <v>347</v>
+      </c>
+      <c r="C85" s="105" t="s">
+        <v>348</v>
+      </c>
+      <c r="D85" s="105" t="s">
+        <v>349</v>
+      </c>
+      <c r="E85" s="105" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="103"/>
+      <c r="B86" s="104" t="s">
         <v>350</v>
       </c>
-      <c r="C85" s="84" t="s">
+      <c r="C86" s="105" t="s">
+        <v>348</v>
+      </c>
+      <c r="D86" s="105" t="s">
         <v>351</v>
       </c>
-      <c r="D85" s="85" t="s">
+      <c r="E86" s="105" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="90"/>
+      <c r="B87" s="91" t="s">
+        <v>353</v>
+      </c>
+      <c r="C87" s="85" t="s">
         <v>352</v>
-      </c>
-      <c r="E85" s="84" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="83" t="s">
-        <v>353</v>
-      </c>
-      <c r="C86" s="84" t="s">
-        <v>351</v>
-      </c>
-      <c r="D86" s="85" t="s">
-        <v>354</v>
-      </c>
-      <c r="E86" s="84" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="83" t="s">
-        <v>356</v>
-      </c>
-      <c r="C87" s="84" t="s">
-        <v>355</v>
       </c>
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E87" s="86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="83" t="s">
-        <v>357</v>
-      </c>
-      <c r="C88" s="84" t="s">
-        <v>355</v>
+      <c r="E87" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="90"/>
+      <c r="B88" s="91" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="83" t="s">
-        <v>358</v>
-      </c>
-      <c r="C89" s="84" t="s">
+      <c r="E88" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="90"/>
+      <c r="B89" s="91" t="s">
         <v>355</v>
+      </c>
+      <c r="C89" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="E89" s="86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="83" t="s">
-        <v>359</v>
-      </c>
-      <c r="C90" s="84" t="s">
-        <v>355</v>
+      <c r="E89" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="90"/>
+      <c r="B90" s="91" t="s">
+        <v>356</v>
+      </c>
+      <c r="C90" s="85" t="s">
+        <v>352</v>
       </c>
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="E90" s="86" t="s">
+      <c r="E90" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="90"/>
+      <c r="B91" s="91" t="s">
+        <v>357</v>
+      </c>
+      <c r="C91" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="D91" s="85" t="s">
+        <v>358</v>
+      </c>
+      <c r="E91" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="90"/>
+      <c r="B92" s="91" t="s">
+        <v>360</v>
+      </c>
+      <c r="C92" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="D92" s="85" t="s">
+        <v>361</v>
+      </c>
+      <c r="E92" s="99" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="103"/>
+      <c r="B93" s="104" t="s">
+        <v>363</v>
+      </c>
+      <c r="C93" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="105" t="s">
+        <v>364</v>
+      </c>
+      <c r="E93" s="105"/>
+    </row>
+    <row r="94" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="103"/>
+      <c r="B94" s="104" t="s">
+        <v>365</v>
+      </c>
+      <c r="C94" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="105" t="s">
+        <v>454</v>
+      </c>
+      <c r="E94" s="105"/>
+    </row>
+    <row r="95" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="103"/>
+      <c r="B95" s="104" t="s">
+        <v>366</v>
+      </c>
+      <c r="C95" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="105" t="s">
+        <v>367</v>
+      </c>
+      <c r="E95" s="105"/>
+    </row>
+    <row r="96" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="103"/>
+      <c r="B96" s="104" t="s">
+        <v>368</v>
+      </c>
+      <c r="C96" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="105" t="s">
+        <v>369</v>
+      </c>
+      <c r="E96" s="105"/>
+    </row>
+    <row r="97" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="103"/>
+      <c r="B97" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="C97" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="105" t="s">
+        <v>371</v>
+      </c>
+      <c r="E97" s="105"/>
+    </row>
+    <row r="98" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="103"/>
+      <c r="B98" s="104" t="s">
+        <v>372</v>
+      </c>
+      <c r="C98" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="105" t="s">
+        <v>373</v>
+      </c>
+      <c r="E98" s="105"/>
+    </row>
+    <row r="99" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="103"/>
+      <c r="B99" s="104" t="s">
+        <v>374</v>
+      </c>
+      <c r="C99" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="105" t="s">
+        <v>375</v>
+      </c>
+      <c r="E99" s="105"/>
+    </row>
+    <row r="100" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="103"/>
+      <c r="B100" s="104" t="s">
+        <v>378</v>
+      </c>
+      <c r="C100" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="105" t="s">
+        <v>379</v>
+      </c>
+      <c r="E100" s="105"/>
+    </row>
+    <row r="101" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="103"/>
+      <c r="B101" s="104" t="s">
+        <v>380</v>
+      </c>
+      <c r="C101" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="105" t="s">
+        <v>381</v>
+      </c>
+      <c r="E101" s="105"/>
+    </row>
+    <row r="102" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="103"/>
+      <c r="B102" s="104" t="s">
+        <v>382</v>
+      </c>
+      <c r="C102" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="105" t="s">
+        <v>383</v>
+      </c>
+      <c r="E102" s="105"/>
+    </row>
+    <row r="103" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="103"/>
+      <c r="B103" s="104" t="s">
+        <v>384</v>
+      </c>
+      <c r="C103" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="E103" s="105"/>
+    </row>
+    <row r="104" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="103"/>
+      <c r="B104" s="104" t="s">
+        <v>385</v>
+      </c>
+      <c r="C104" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="105" t="s">
+        <v>456</v>
+      </c>
+      <c r="E104" s="105"/>
+    </row>
+    <row r="105" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="103"/>
+      <c r="B105" s="104" t="s">
+        <v>386</v>
+      </c>
+      <c r="C105" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="105" t="s">
+        <v>457</v>
+      </c>
+      <c r="E105" s="105"/>
+    </row>
+    <row r="106" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="103"/>
+      <c r="B106" s="104" t="s">
+        <v>387</v>
+      </c>
+      <c r="C106" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="105" t="s">
+        <v>388</v>
+      </c>
+      <c r="E106" s="105"/>
+    </row>
+    <row r="107" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="103"/>
+      <c r="B107" s="104" t="s">
+        <v>389</v>
+      </c>
+      <c r="C107" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="105" t="s">
+        <v>390</v>
+      </c>
+      <c r="E107" s="105"/>
+    </row>
+    <row r="108" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="103"/>
+      <c r="B108" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="105" t="s">
+        <v>391</v>
+      </c>
+      <c r="E108" s="105"/>
+    </row>
+    <row r="109" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="103"/>
+      <c r="B109" s="104" t="s">
+        <v>392</v>
+      </c>
+      <c r="C109" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="105" t="s">
+        <v>459</v>
+      </c>
+      <c r="E109" s="105"/>
+    </row>
+    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="90"/>
+      <c r="B110" s="91" t="s">
+        <v>376</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D110" s="85" t="s">
+        <v>394</v>
+      </c>
+      <c r="E110" s="85"/>
+    </row>
+    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="90"/>
+      <c r="B111" s="91" t="s">
+        <v>377</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D111" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="E111" s="85"/>
+    </row>
+    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="90"/>
+      <c r="B112" s="91" t="s">
+        <v>395</v>
+      </c>
+      <c r="C112" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D112" s="85" t="s">
+        <v>476</v>
+      </c>
+      <c r="E112" s="85"/>
+    </row>
+    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="90"/>
+      <c r="B113" s="91" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="83" t="s">
-        <v>360</v>
-      </c>
-      <c r="C91" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D91" s="85" t="s">
-        <v>361</v>
-      </c>
-      <c r="E91" s="86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="83" t="s">
-        <v>363</v>
-      </c>
-      <c r="C92" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="D92" s="85" t="s">
-        <v>364</v>
-      </c>
-      <c r="E92" s="86" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="96"/>
-      <c r="B93" s="97" t="s">
-        <v>366</v>
-      </c>
-      <c r="C93" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="98" t="s">
-        <v>367</v>
-      </c>
-      <c r="E93" s="98"/>
-    </row>
-    <row r="94" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="96"/>
-      <c r="B94" s="97" t="s">
-        <v>368</v>
-      </c>
-      <c r="C94" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="98" t="s">
-        <v>459</v>
-      </c>
-      <c r="E94" s="98"/>
-    </row>
-    <row r="95" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="96"/>
-      <c r="B95" s="97" t="s">
-        <v>369</v>
-      </c>
-      <c r="C95" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="98" t="s">
-        <v>370</v>
-      </c>
-      <c r="E95" s="98"/>
-    </row>
-    <row r="96" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="96"/>
-      <c r="B96" s="97" t="s">
-        <v>371</v>
-      </c>
-      <c r="C96" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="98" t="s">
-        <v>372</v>
-      </c>
-      <c r="E96" s="98"/>
-    </row>
-    <row r="97" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="96"/>
-      <c r="B97" s="97" t="s">
-        <v>373</v>
-      </c>
-      <c r="C97" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="98" t="s">
-        <v>374</v>
-      </c>
-      <c r="E97" s="98"/>
-    </row>
-    <row r="98" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="96"/>
-      <c r="B98" s="97" t="s">
-        <v>375</v>
-      </c>
-      <c r="C98" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="98" t="s">
-        <v>376</v>
-      </c>
-      <c r="E98" s="98"/>
-    </row>
-    <row r="99" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="96"/>
-      <c r="B99" s="97" t="s">
-        <v>377</v>
-      </c>
-      <c r="C99" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="98" t="s">
-        <v>378</v>
-      </c>
-      <c r="E99" s="98"/>
-    </row>
-    <row r="100" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="96"/>
-      <c r="B100" s="97" t="s">
-        <v>381</v>
-      </c>
-      <c r="C100" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="98" t="s">
-        <v>382</v>
-      </c>
-      <c r="E100" s="98"/>
-    </row>
-    <row r="101" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="96"/>
-      <c r="B101" s="97" t="s">
-        <v>383</v>
-      </c>
-      <c r="C101" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="98" t="s">
-        <v>384</v>
-      </c>
-      <c r="E101" s="98"/>
-    </row>
-    <row r="102" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="96"/>
-      <c r="B102" s="97" t="s">
-        <v>385</v>
-      </c>
-      <c r="C102" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="98" t="s">
-        <v>386</v>
-      </c>
-      <c r="E102" s="98"/>
-    </row>
-    <row r="103" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="96"/>
-      <c r="B103" s="97" t="s">
-        <v>387</v>
-      </c>
-      <c r="C103" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="98" t="s">
+      <c r="C113" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="85" t="s">
+        <v>397</v>
+      </c>
+      <c r="E113" s="85"/>
+    </row>
+    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="90"/>
+      <c r="B114" s="91" t="s">
+        <v>398</v>
+      </c>
+      <c r="C114" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D114" s="85" t="s">
+        <v>399</v>
+      </c>
+      <c r="E114" s="85"/>
+    </row>
+    <row r="115" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="103"/>
+      <c r="B115" s="104" t="s">
+        <v>400</v>
+      </c>
+      <c r="C115" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="D115" s="105" t="s">
+        <v>401</v>
+      </c>
+      <c r="E115" s="105"/>
+    </row>
+    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="90"/>
+      <c r="B116" s="91" t="s">
+        <v>402</v>
+      </c>
+      <c r="C116" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D116" s="85" t="s">
+        <v>403</v>
+      </c>
+      <c r="E116" s="85"/>
+    </row>
+    <row r="117" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="103"/>
+      <c r="B117" s="104" t="s">
+        <v>404</v>
+      </c>
+      <c r="C117" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="D117" s="105" t="s">
+        <v>405</v>
+      </c>
+      <c r="E117" s="105"/>
+    </row>
+    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="90"/>
+      <c r="B118" s="91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C118" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D118" s="85" t="s">
+        <v>407</v>
+      </c>
+      <c r="E118" s="85"/>
+    </row>
+    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="90"/>
+      <c r="B119" s="91" t="s">
+        <v>408</v>
+      </c>
+      <c r="C119" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D119" s="85" t="s">
+        <v>409</v>
+      </c>
+      <c r="E119" s="85"/>
+    </row>
+    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="90"/>
+      <c r="B120" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C120" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="85" t="s">
+        <v>410</v>
+      </c>
+      <c r="E120" s="85"/>
+    </row>
+    <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="90"/>
+      <c r="B121" s="91" t="s">
+        <v>411</v>
+      </c>
+      <c r="C121" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D121" s="85" t="s">
+        <v>413</v>
+      </c>
+      <c r="E121" s="85"/>
+    </row>
+    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="90"/>
+      <c r="B122" s="91" t="s">
+        <v>412</v>
+      </c>
+      <c r="C122" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="85" t="s">
+        <v>414</v>
+      </c>
+      <c r="E122" s="85"/>
+    </row>
+    <row r="123" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="103"/>
+      <c r="B123" s="104" t="s">
+        <v>415</v>
+      </c>
+      <c r="C123" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="105" t="s">
+        <v>416</v>
+      </c>
+      <c r="E123" s="105"/>
+    </row>
+    <row r="124" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="103"/>
+      <c r="B124" s="104" t="s">
+        <v>417</v>
+      </c>
+      <c r="C124" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="105" t="s">
+        <v>418</v>
+      </c>
+      <c r="E124" s="105"/>
+    </row>
+    <row r="125" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="103"/>
+      <c r="B125" s="104" t="s">
+        <v>419</v>
+      </c>
+      <c r="C125" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="105" t="s">
+        <v>463</v>
+      </c>
+      <c r="E125" s="105"/>
+    </row>
+    <row r="126" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="103"/>
+      <c r="B126" s="104" t="s">
+        <v>420</v>
+      </c>
+      <c r="C126" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="105" t="s">
+        <v>421</v>
+      </c>
+      <c r="E126" s="105"/>
+    </row>
+    <row r="127" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="103"/>
+      <c r="B127" s="104" t="s">
+        <v>422</v>
+      </c>
+      <c r="C127" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="105" t="s">
+        <v>423</v>
+      </c>
+      <c r="E127" s="105"/>
+    </row>
+    <row r="128" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="103"/>
+      <c r="B128" s="104" t="s">
+        <v>424</v>
+      </c>
+      <c r="C128" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="105" t="s">
+        <v>425</v>
+      </c>
+      <c r="E128" s="105"/>
+    </row>
+    <row r="129" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="103"/>
+      <c r="B129" s="104" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="105" t="s">
+        <v>426</v>
+      </c>
+      <c r="E129" s="105"/>
+    </row>
+    <row r="130" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="103"/>
+      <c r="B130" s="104" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="E130" s="105"/>
+    </row>
+    <row r="131" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="103"/>
+      <c r="B131" s="104" t="s">
+        <v>427</v>
+      </c>
+      <c r="C131" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="105" t="s">
+        <v>428</v>
+      </c>
+      <c r="E131" s="105"/>
+    </row>
+    <row r="132" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="103"/>
+      <c r="B132" s="104" t="s">
+        <v>429</v>
+      </c>
+      <c r="C132" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="105" t="s">
+        <v>430</v>
+      </c>
+      <c r="E132" s="105"/>
+    </row>
+    <row r="133" spans="1:5" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="103"/>
+      <c r="B133" s="104" t="s">
+        <v>431</v>
+      </c>
+      <c r="C133" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="105" t="s">
+        <v>465</v>
+      </c>
+      <c r="E133" s="105"/>
+    </row>
+    <row r="134" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="103"/>
+      <c r="B134" s="104" t="s">
+        <v>432</v>
+      </c>
+      <c r="C134" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D134" s="105" t="s">
+        <v>433</v>
+      </c>
+      <c r="E134" s="105"/>
+    </row>
+    <row r="135" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="103"/>
+      <c r="B135" s="104" t="s">
+        <v>434</v>
+      </c>
+      <c r="C135" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="105" t="s">
+        <v>435</v>
+      </c>
+      <c r="E135" s="105"/>
+    </row>
+    <row r="136" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="103"/>
+      <c r="B136" s="104" t="s">
+        <v>436</v>
+      </c>
+      <c r="C136" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="105" t="s">
+        <v>468</v>
+      </c>
+      <c r="E136" s="105"/>
+    </row>
+    <row r="137" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="103"/>
+      <c r="B137" s="104" t="s">
+        <v>437</v>
+      </c>
+      <c r="C137" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="105" t="s">
+        <v>467</v>
+      </c>
+      <c r="E137" s="105"/>
+    </row>
+    <row r="138" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="103"/>
+      <c r="B138" s="104" t="s">
+        <v>438</v>
+      </c>
+      <c r="C138" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="105" t="s">
+        <v>439</v>
+      </c>
+      <c r="E138" s="105"/>
+    </row>
+    <row r="139" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="103"/>
+      <c r="B139" s="104" t="s">
+        <v>440</v>
+      </c>
+      <c r="C139" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="105" t="s">
+        <v>469</v>
+      </c>
+      <c r="E139" s="105"/>
+    </row>
+    <row r="140" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="103"/>
+      <c r="B140" s="104" t="s">
+        <v>441</v>
+      </c>
+      <c r="C140" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D140" s="105" t="s">
+        <v>442</v>
+      </c>
+      <c r="E140" s="105"/>
+    </row>
+    <row r="141" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="103"/>
+      <c r="B141" s="104" t="s">
         <v>460</v>
       </c>
-      <c r="E103" s="98"/>
-    </row>
-    <row r="104" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="96"/>
-      <c r="B104" s="97" t="s">
-        <v>388</v>
-      </c>
-      <c r="C104" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="98" t="s">
+      <c r="C141" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D141" s="105" t="s">
         <v>461</v>
       </c>
-      <c r="E104" s="98"/>
-    </row>
-    <row r="105" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="96"/>
-      <c r="B105" s="97" t="s">
-        <v>389</v>
-      </c>
-      <c r="C105" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="98" t="s">
-        <v>462</v>
-      </c>
-      <c r="E105" s="98"/>
-    </row>
-    <row r="106" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="96"/>
-      <c r="B106" s="97" t="s">
-        <v>390</v>
-      </c>
-      <c r="C106" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="98" t="s">
-        <v>391</v>
-      </c>
-      <c r="E106" s="98"/>
-    </row>
-    <row r="107" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="96"/>
-      <c r="B107" s="97" t="s">
-        <v>392</v>
-      </c>
-      <c r="C107" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="98" t="s">
-        <v>393</v>
-      </c>
-      <c r="E107" s="98"/>
-    </row>
-    <row r="108" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="96"/>
-      <c r="B108" s="97" t="s">
-        <v>187</v>
-      </c>
-      <c r="C108" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="98" t="s">
-        <v>394</v>
-      </c>
-      <c r="E108" s="98"/>
-    </row>
-    <row r="109" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="96"/>
-      <c r="B109" s="97" t="s">
-        <v>395</v>
-      </c>
-      <c r="C109" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="98" t="s">
-        <v>464</v>
-      </c>
-      <c r="E109" s="98"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="83" t="s">
-        <v>379</v>
-      </c>
-      <c r="C110" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D110" s="84" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="83" t="s">
-        <v>380</v>
-      </c>
-      <c r="C111" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D111" s="84" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="83" t="s">
-        <v>399</v>
-      </c>
-      <c r="C112" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D112" s="84" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="83" t="s">
-        <v>401</v>
-      </c>
-      <c r="C113" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="84" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="83" t="s">
-        <v>403</v>
-      </c>
-      <c r="C114" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D114" s="84" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="83" t="s">
-        <v>405</v>
-      </c>
-      <c r="C115" s="84" t="s">
-        <v>282</v>
-      </c>
-      <c r="D115" s="84" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="83" t="s">
-        <v>407</v>
-      </c>
-      <c r="C116" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D116" s="84" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="83" t="s">
-        <v>409</v>
-      </c>
-      <c r="C117" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D117" s="84" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="83" t="s">
-        <v>411</v>
-      </c>
-      <c r="C118" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D118" s="84" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="83" t="s">
-        <v>413</v>
-      </c>
-      <c r="C119" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D119" s="84" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="83" t="s">
-        <v>188</v>
-      </c>
-      <c r="C120" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D120" s="84" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B121" s="83" t="s">
-        <v>416</v>
-      </c>
-      <c r="C121" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D121" s="84" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="83" t="s">
-        <v>417</v>
-      </c>
-      <c r="C122" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="84" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="96"/>
-      <c r="B123" s="97" t="s">
-        <v>420</v>
-      </c>
-      <c r="C123" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="98" t="s">
-        <v>421</v>
-      </c>
-      <c r="E123" s="98"/>
-    </row>
-    <row r="124" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="96"/>
-      <c r="B124" s="97" t="s">
-        <v>422</v>
-      </c>
-      <c r="C124" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="98" t="s">
-        <v>423</v>
-      </c>
-      <c r="E124" s="98"/>
-    </row>
-    <row r="125" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="96"/>
-      <c r="B125" s="97" t="s">
-        <v>424</v>
-      </c>
-      <c r="C125" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="98" t="s">
-        <v>468</v>
-      </c>
-      <c r="E125" s="98"/>
-    </row>
-    <row r="126" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="96"/>
-      <c r="B126" s="97" t="s">
-        <v>425</v>
-      </c>
-      <c r="C126" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="98" t="s">
-        <v>426</v>
-      </c>
-      <c r="E126" s="98"/>
-    </row>
-    <row r="127" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="96"/>
-      <c r="B127" s="97" t="s">
-        <v>427</v>
-      </c>
-      <c r="C127" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="98" t="s">
-        <v>428</v>
-      </c>
-      <c r="E127" s="98"/>
-    </row>
-    <row r="128" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="96"/>
-      <c r="B128" s="97" t="s">
-        <v>429</v>
-      </c>
-      <c r="C128" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="98" t="s">
-        <v>430</v>
-      </c>
-      <c r="E128" s="98"/>
-    </row>
-    <row r="129" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="96"/>
-      <c r="B129" s="97" t="s">
-        <v>189</v>
-      </c>
-      <c r="C129" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="98" t="s">
-        <v>431</v>
-      </c>
-      <c r="E129" s="98"/>
-    </row>
-    <row r="130" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="96"/>
-      <c r="B130" s="97" t="s">
-        <v>190</v>
-      </c>
-      <c r="C130" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="98" t="s">
-        <v>301</v>
-      </c>
-      <c r="E130" s="98"/>
-    </row>
-    <row r="131" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="96"/>
-      <c r="B131" s="97" t="s">
-        <v>432</v>
-      </c>
-      <c r="C131" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="98" t="s">
-        <v>433</v>
-      </c>
-      <c r="E131" s="98"/>
-    </row>
-    <row r="132" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="96"/>
-      <c r="B132" s="97" t="s">
-        <v>434</v>
-      </c>
-      <c r="C132" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="98" t="s">
-        <v>435</v>
-      </c>
-      <c r="E132" s="98"/>
-    </row>
-    <row r="133" spans="1:5" s="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="96"/>
-      <c r="B133" s="97" t="s">
-        <v>436</v>
-      </c>
-      <c r="C133" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="98" t="s">
-        <v>470</v>
-      </c>
-      <c r="E133" s="98"/>
-    </row>
-    <row r="134" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="96"/>
-      <c r="B134" s="97" t="s">
-        <v>437</v>
-      </c>
-      <c r="C134" s="98" t="s">
-        <v>275</v>
-      </c>
-      <c r="D134" s="98" t="s">
-        <v>438</v>
-      </c>
-      <c r="E134" s="98"/>
-    </row>
-    <row r="135" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="96"/>
-      <c r="B135" s="97" t="s">
-        <v>439</v>
-      </c>
-      <c r="C135" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D135" s="98" t="s">
-        <v>440</v>
-      </c>
-      <c r="E135" s="98"/>
-    </row>
-    <row r="136" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="96"/>
-      <c r="B136" s="97" t="s">
-        <v>441</v>
-      </c>
-      <c r="C136" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="98" t="s">
-        <v>473</v>
-      </c>
-      <c r="E136" s="98"/>
-    </row>
-    <row r="137" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="96"/>
-      <c r="B137" s="97" t="s">
-        <v>442</v>
-      </c>
-      <c r="C137" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="98" t="s">
+      <c r="E141" s="105"/>
+    </row>
+    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="90"/>
+      <c r="B142" s="91" t="s">
+        <v>471</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="D142" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="E137" s="98"/>
-    </row>
-    <row r="138" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="96"/>
-      <c r="B138" s="97" t="s">
-        <v>443</v>
-      </c>
-      <c r="C138" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="98" t="s">
-        <v>444</v>
-      </c>
-      <c r="E138" s="98"/>
-    </row>
-    <row r="139" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="96"/>
-      <c r="B139" s="97" t="s">
-        <v>445</v>
-      </c>
-      <c r="C139" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="98" t="s">
-        <v>474</v>
-      </c>
-      <c r="E139" s="98"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="83" t="s">
-        <v>446</v>
-      </c>
-      <c r="C140" s="84" t="s">
-        <v>275</v>
-      </c>
-      <c r="D140" s="84" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="96"/>
-      <c r="B141" s="97" t="s">
-        <v>465</v>
-      </c>
-      <c r="C141" s="98" t="s">
-        <v>275</v>
-      </c>
-      <c r="D141" s="98" t="s">
-        <v>466</v>
-      </c>
-      <c r="E141" s="98"/>
+      <c r="E142" s="85"/>
+    </row>
+    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="90"/>
+      <c r="B143" s="91" t="s">
+        <v>478</v>
+      </c>
+      <c r="C143" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D143" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="E143" s="85"/>
+    </row>
+    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="90"/>
+      <c r="B144" s="91" t="s">
+        <v>481</v>
+      </c>
+      <c r="C144" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D144" s="85" t="s">
+        <v>482</v>
+      </c>
+      <c r="E144" s="85"/>
+    </row>
+    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="90"/>
+      <c r="B145" s="91" t="s">
+        <v>483</v>
+      </c>
+      <c r="C145" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="E145" s="85"/>
+    </row>
+    <row r="146" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="98"/>
+      <c r="B146" s="100" t="s">
+        <v>485</v>
+      </c>
+      <c r="C146" s="101" t="s">
+        <v>339</v>
+      </c>
+      <c r="D146" s="101" t="s">
+        <v>486</v>
+      </c>
+      <c r="E146" s="101"/>
+    </row>
+    <row r="147" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="90"/>
+      <c r="B147" s="91" t="s">
+        <v>487</v>
+      </c>
+      <c r="C147" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D147" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="E147" s="85"/>
+    </row>
+    <row r="148" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="103"/>
+      <c r="B148" s="104" t="s">
+        <v>490</v>
+      </c>
+      <c r="C148" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D148" s="105" t="s">
+        <v>491</v>
+      </c>
+      <c r="E148" s="105"/>
+    </row>
+    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="90"/>
+      <c r="B149" s="91" t="s">
+        <v>492</v>
+      </c>
+      <c r="C149" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="85" t="s">
+        <v>493</v>
+      </c>
+      <c r="E149" s="85"/>
+    </row>
+    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="90"/>
+      <c r="B150" s="91" t="s">
+        <v>495</v>
+      </c>
+      <c r="C150" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D150" s="85" t="s">
+        <v>494</v>
+      </c>
+      <c r="E150" s="85"/>
+    </row>
+    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="90"/>
+      <c r="B151" s="91" t="s">
+        <v>496</v>
+      </c>
+      <c r="C151" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D151" s="85" t="s">
+        <v>497</v>
+      </c>
+      <c r="E151" s="85"/>
+    </row>
+    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="90"/>
+      <c r="B152" s="91"/>
+      <c r="C152" s="85"/>
+      <c r="D152" s="85"/>
+      <c r="E152" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated supporting docs and their links
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD3867F-D5E1-4513-A6E1-7C2474744C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16B014-E39A-4508-9433-16AC6FC2E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="30" windowWidth="14250" windowHeight="14475" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="1980" yWindow="210" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -2054,12 +2054,6 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,6 +2079,12 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2477,10 +2477,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="97"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5846,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5875,17 +5875,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
+      <c r="A2" s="105"/>
       <c r="B2" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="108" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="108" t="s">
+      <c r="C2" s="106" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="108"/>
+      <c r="E2" s="106"/>
     </row>
     <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92"/>
@@ -5952,44 +5952,44 @@
       </c>
       <c r="E7" s="94"/>
     </row>
-    <row r="8" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="109"/>
-      <c r="B8" s="110" t="s">
+    <row r="8" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
+      <c r="B8" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="111" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="111" t="s">
+      <c r="C8" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="109" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="111"/>
-    </row>
-    <row r="9" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
-      <c r="B9" s="110" t="s">
+      <c r="E8" s="109"/>
+    </row>
+    <row r="9" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
+      <c r="B9" s="108" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="111" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="111" t="s">
+      <c r="C9" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="109" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="111"/>
-    </row>
-    <row r="10" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="109"/>
-      <c r="B10" s="110" t="s">
+      <c r="E9" s="109"/>
+    </row>
+    <row r="10" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
+      <c r="B10" s="108" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="111" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="111" t="s">
+      <c r="C10" s="109" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="109" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="111"/>
+      <c r="E10" s="109"/>
     </row>
     <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92"/>
@@ -6056,83 +6056,83 @@
       </c>
       <c r="E15" s="85"/>
     </row>
-    <row r="16" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103"/>
-      <c r="B16" s="104" t="s">
+    <row r="16" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="101"/>
+      <c r="B16" s="102" t="s">
         <v>265</v>
       </c>
-      <c r="C16" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="105" t="s">
+      <c r="C16" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="103" t="s">
         <v>443</v>
       </c>
-      <c r="E16" s="105"/>
-    </row>
-    <row r="17" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="103"/>
-      <c r="B17" s="104" t="s">
+      <c r="E16" s="103"/>
+    </row>
+    <row r="17" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="101"/>
+      <c r="B17" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="105" t="s">
+      <c r="C17" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="103" t="s">
         <v>448</v>
       </c>
-      <c r="E17" s="105"/>
-    </row>
-    <row r="18" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="103"/>
-      <c r="B18" s="104" t="s">
+      <c r="E17" s="103"/>
+    </row>
+    <row r="18" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="102" t="s">
         <v>267</v>
       </c>
-      <c r="C18" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="105" t="s">
+      <c r="C18" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="103" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="105"/>
-    </row>
-    <row r="19" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103"/>
-      <c r="B19" s="104" t="s">
+      <c r="E18" s="103"/>
+    </row>
+    <row r="19" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="101"/>
+      <c r="B19" s="102" t="s">
         <v>268</v>
       </c>
-      <c r="C19" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="105" t="s">
+      <c r="C19" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="103" t="s">
         <v>462</v>
       </c>
-      <c r="E19" s="105"/>
-    </row>
-    <row r="20" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="103"/>
-      <c r="B20" s="104" t="s">
+      <c r="E19" s="103"/>
+    </row>
+    <row r="20" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101"/>
+      <c r="B20" s="102" t="s">
         <v>269</v>
       </c>
-      <c r="C20" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="105" t="s">
+      <c r="C20" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="103" t="s">
         <v>466</v>
       </c>
-      <c r="E20" s="105"/>
-    </row>
-    <row r="21" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="103"/>
-      <c r="B21" s="104" t="s">
+      <c r="E20" s="103"/>
+    </row>
+    <row r="21" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
+      <c r="B21" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="105" t="s">
+      <c r="C21" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="103" t="s">
         <v>445</v>
       </c>
-      <c r="E21" s="105"/>
+      <c r="E21" s="103"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="90"/>
@@ -6186,18 +6186,18 @@
       </c>
       <c r="E25" s="85"/>
     </row>
-    <row r="26" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
-      <c r="B26" s="104" t="s">
+    <row r="26" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="101"/>
+      <c r="B26" s="102" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="105" t="s">
+      <c r="C26" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="103" t="s">
         <v>464</v>
       </c>
-      <c r="E26" s="105"/>
+      <c r="E26" s="103"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="90"/>
@@ -6212,161 +6212,161 @@
       </c>
       <c r="E27" s="85"/>
     </row>
-    <row r="28" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="103"/>
-      <c r="B28" s="104" t="s">
+    <row r="28" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="101"/>
+      <c r="B28" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="C28" s="105" t="s">
+      <c r="C28" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="D28" s="105" t="s">
+      <c r="D28" s="103" t="s">
         <v>277</v>
       </c>
-      <c r="E28" s="105"/>
-    </row>
-    <row r="29" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="103"/>
-      <c r="B29" s="104" t="s">
+      <c r="E28" s="103"/>
+    </row>
+    <row r="29" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="101"/>
+      <c r="B29" s="102" t="s">
         <v>278</v>
       </c>
-      <c r="C29" s="105" t="s">
+      <c r="C29" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D29" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="E29" s="105"/>
-    </row>
-    <row r="30" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="103"/>
-      <c r="B30" s="104" t="s">
+      <c r="E29" s="103"/>
+    </row>
+    <row r="30" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="101"/>
+      <c r="B30" s="102" t="s">
         <v>280</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="105"/>
-    </row>
-    <row r="31" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
-      <c r="B31" s="104" t="s">
+      <c r="E30" s="103"/>
+    </row>
+    <row r="31" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="101"/>
+      <c r="B31" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="105" t="s">
+      <c r="C31" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="103" t="s">
         <v>444</v>
       </c>
-      <c r="E31" s="105"/>
-    </row>
-    <row r="32" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="104" t="s">
+      <c r="E31" s="103"/>
+    </row>
+    <row r="32" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="101"/>
+      <c r="B32" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="105" t="s">
+      <c r="C32" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="103" t="s">
         <v>447</v>
       </c>
-      <c r="E32" s="105"/>
-    </row>
-    <row r="33" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="104" t="s">
+      <c r="E32" s="103"/>
+    </row>
+    <row r="33" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="101"/>
+      <c r="B33" s="102" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="105" t="s">
+      <c r="C33" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="105"/>
-    </row>
-    <row r="34" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="104" t="s">
+      <c r="E33" s="103"/>
+    </row>
+    <row r="34" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="101"/>
+      <c r="B34" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="105" t="s">
+      <c r="C34" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="103" t="s">
         <v>452</v>
       </c>
-      <c r="E34" s="105"/>
-    </row>
-    <row r="35" spans="1:5" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="104" t="s">
+      <c r="E34" s="103"/>
+    </row>
+    <row r="35" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="101"/>
+      <c r="B35" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="105" t="s">
+      <c r="C35" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="103" t="s">
         <v>449</v>
       </c>
-      <c r="E35" s="105"/>
-    </row>
-    <row r="36" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="104" t="s">
+      <c r="E35" s="103"/>
+    </row>
+    <row r="36" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="101"/>
+      <c r="B36" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="105" t="s">
+      <c r="C36" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="103" t="s">
         <v>281</v>
       </c>
-      <c r="E36" s="105"/>
-    </row>
-    <row r="37" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="103"/>
-      <c r="B37" s="104" t="s">
+      <c r="E36" s="103"/>
+    </row>
+    <row r="37" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="101"/>
+      <c r="B37" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="105" t="s">
+      <c r="C37" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="103" t="s">
         <v>450</v>
       </c>
-      <c r="E37" s="105"/>
-    </row>
-    <row r="38" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="103"/>
-      <c r="B38" s="104" t="s">
+      <c r="E37" s="103"/>
+    </row>
+    <row r="38" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="101"/>
+      <c r="B38" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="105" t="s">
+      <c r="C38" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="103" t="s">
         <v>458</v>
       </c>
-      <c r="E38" s="105"/>
-    </row>
-    <row r="39" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
-      <c r="B39" s="104" t="s">
+      <c r="E38" s="103"/>
+    </row>
+    <row r="39" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="101"/>
+      <c r="B39" s="102" t="s">
         <v>282</v>
       </c>
-      <c r="C39" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="105" t="s">
+      <c r="C39" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="103" t="s">
         <v>451</v>
       </c>
-      <c r="E39" s="105"/>
+      <c r="E39" s="103"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="90"/>
@@ -6628,44 +6628,44 @@
       </c>
       <c r="E59" s="85"/>
     </row>
-    <row r="60" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="103"/>
-      <c r="B60" s="104" t="s">
+    <row r="60" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="101"/>
+      <c r="B60" s="102" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="105" t="s">
+      <c r="C60" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="103" t="s">
         <v>446</v>
       </c>
-      <c r="E60" s="105"/>
-    </row>
-    <row r="61" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="103"/>
-      <c r="B61" s="104" t="s">
+      <c r="E60" s="103"/>
+    </row>
+    <row r="61" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="101"/>
+      <c r="B61" s="102" t="s">
         <v>301</v>
       </c>
-      <c r="C61" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="105" t="s">
+      <c r="C61" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="103" t="s">
         <v>302</v>
       </c>
-      <c r="E61" s="105"/>
-    </row>
-    <row r="62" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="103"/>
-      <c r="B62" s="104" t="s">
+      <c r="E61" s="103"/>
+    </row>
+    <row r="62" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="101"/>
+      <c r="B62" s="102" t="s">
         <v>303</v>
       </c>
-      <c r="C62" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="105" t="s">
+      <c r="C62" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="E62" s="105"/>
+      <c r="E62" s="103"/>
     </row>
     <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="90"/>
@@ -6953,33 +6953,33 @@
       </c>
       <c r="E84" s="85"/>
     </row>
-    <row r="85" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="103"/>
-      <c r="B85" s="104" t="s">
+    <row r="85" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="101"/>
+      <c r="B85" s="102" t="s">
         <v>347</v>
       </c>
-      <c r="C85" s="105" t="s">
+      <c r="C85" s="103" t="s">
         <v>348</v>
       </c>
-      <c r="D85" s="105" t="s">
+      <c r="D85" s="103" t="s">
         <v>349</v>
       </c>
-      <c r="E85" s="105" t="s">
+      <c r="E85" s="103" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="103"/>
-      <c r="B86" s="104" t="s">
+    <row r="86" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="101"/>
+      <c r="B86" s="102" t="s">
         <v>350</v>
       </c>
-      <c r="C86" s="105" t="s">
+      <c r="C86" s="103" t="s">
         <v>348</v>
       </c>
-      <c r="D86" s="105" t="s">
+      <c r="D86" s="103" t="s">
         <v>351</v>
       </c>
-      <c r="E86" s="105" t="s">
+      <c r="E86" s="103" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6994,7 +6994,7 @@
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E87" s="99" t="s">
+      <c r="E87" s="97" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7009,7 +7009,7 @@
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="99" t="s">
+      <c r="E88" s="97" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7024,7 +7024,7 @@
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="E89" s="99" t="s">
+      <c r="E89" s="97" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7039,7 +7039,7 @@
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="E90" s="99" t="s">
+      <c r="E90" s="97" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7054,7 +7054,7 @@
       <c r="D91" s="85" t="s">
         <v>358</v>
       </c>
-      <c r="E91" s="99" t="s">
+      <c r="E91" s="97" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7069,230 +7069,230 @@
       <c r="D92" s="85" t="s">
         <v>361</v>
       </c>
-      <c r="E92" s="99" t="s">
+      <c r="E92" s="97" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="103"/>
-      <c r="B93" s="104" t="s">
+    <row r="93" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="101"/>
+      <c r="B93" s="102" t="s">
         <v>363</v>
       </c>
-      <c r="C93" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="105" t="s">
+      <c r="C93" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="103" t="s">
         <v>364</v>
       </c>
-      <c r="E93" s="105"/>
-    </row>
-    <row r="94" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="103"/>
-      <c r="B94" s="104" t="s">
+      <c r="E93" s="103"/>
+    </row>
+    <row r="94" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="101"/>
+      <c r="B94" s="102" t="s">
         <v>365</v>
       </c>
-      <c r="C94" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="105" t="s">
+      <c r="C94" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="103" t="s">
         <v>454</v>
       </c>
-      <c r="E94" s="105"/>
-    </row>
-    <row r="95" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="103"/>
-      <c r="B95" s="104" t="s">
+      <c r="E94" s="103"/>
+    </row>
+    <row r="95" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="101"/>
+      <c r="B95" s="102" t="s">
         <v>366</v>
       </c>
-      <c r="C95" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="105" t="s">
+      <c r="C95" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="103" t="s">
         <v>367</v>
       </c>
-      <c r="E95" s="105"/>
-    </row>
-    <row r="96" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="103"/>
-      <c r="B96" s="104" t="s">
+      <c r="E95" s="103"/>
+    </row>
+    <row r="96" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="101"/>
+      <c r="B96" s="102" t="s">
         <v>368</v>
       </c>
-      <c r="C96" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="105" t="s">
+      <c r="C96" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="103" t="s">
         <v>369</v>
       </c>
-      <c r="E96" s="105"/>
-    </row>
-    <row r="97" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="103"/>
-      <c r="B97" s="104" t="s">
+      <c r="E96" s="103"/>
+    </row>
+    <row r="97" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="101"/>
+      <c r="B97" s="102" t="s">
         <v>370</v>
       </c>
-      <c r="C97" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="105" t="s">
+      <c r="C97" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="103" t="s">
         <v>371</v>
       </c>
-      <c r="E97" s="105"/>
-    </row>
-    <row r="98" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="103"/>
-      <c r="B98" s="104" t="s">
+      <c r="E97" s="103"/>
+    </row>
+    <row r="98" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="101"/>
+      <c r="B98" s="102" t="s">
         <v>372</v>
       </c>
-      <c r="C98" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="105" t="s">
+      <c r="C98" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="103" t="s">
         <v>373</v>
       </c>
-      <c r="E98" s="105"/>
-    </row>
-    <row r="99" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="103"/>
-      <c r="B99" s="104" t="s">
+      <c r="E98" s="103"/>
+    </row>
+    <row r="99" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="101"/>
+      <c r="B99" s="102" t="s">
         <v>374</v>
       </c>
-      <c r="C99" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="105" t="s">
+      <c r="C99" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="103" t="s">
         <v>375</v>
       </c>
-      <c r="E99" s="105"/>
-    </row>
-    <row r="100" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="103"/>
-      <c r="B100" s="104" t="s">
+      <c r="E99" s="103"/>
+    </row>
+    <row r="100" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="101"/>
+      <c r="B100" s="102" t="s">
         <v>378</v>
       </c>
-      <c r="C100" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="105" t="s">
+      <c r="C100" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="103" t="s">
         <v>379</v>
       </c>
-      <c r="E100" s="105"/>
-    </row>
-    <row r="101" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="103"/>
-      <c r="B101" s="104" t="s">
+      <c r="E100" s="103"/>
+    </row>
+    <row r="101" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="101"/>
+      <c r="B101" s="102" t="s">
         <v>380</v>
       </c>
-      <c r="C101" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="105" t="s">
+      <c r="C101" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="103" t="s">
         <v>381</v>
       </c>
-      <c r="E101" s="105"/>
-    </row>
-    <row r="102" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="103"/>
-      <c r="B102" s="104" t="s">
+      <c r="E101" s="103"/>
+    </row>
+    <row r="102" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="101"/>
+      <c r="B102" s="102" t="s">
         <v>382</v>
       </c>
-      <c r="C102" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="105" t="s">
+      <c r="C102" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="103" t="s">
         <v>383</v>
       </c>
-      <c r="E102" s="105"/>
-    </row>
-    <row r="103" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="103"/>
-      <c r="B103" s="104" t="s">
+      <c r="E102" s="103"/>
+    </row>
+    <row r="103" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="101"/>
+      <c r="B103" s="102" t="s">
         <v>384</v>
       </c>
-      <c r="C103" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="105" t="s">
+      <c r="C103" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="103" t="s">
         <v>455</v>
       </c>
-      <c r="E103" s="105"/>
-    </row>
-    <row r="104" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="103"/>
-      <c r="B104" s="104" t="s">
+      <c r="E103" s="103"/>
+    </row>
+    <row r="104" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="101"/>
+      <c r="B104" s="102" t="s">
         <v>385</v>
       </c>
-      <c r="C104" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="105" t="s">
+      <c r="C104" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="103" t="s">
         <v>456</v>
       </c>
-      <c r="E104" s="105"/>
-    </row>
-    <row r="105" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="103"/>
-      <c r="B105" s="104" t="s">
+      <c r="E104" s="103"/>
+    </row>
+    <row r="105" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="101"/>
+      <c r="B105" s="102" t="s">
         <v>386</v>
       </c>
-      <c r="C105" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="105" t="s">
+      <c r="C105" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="103" t="s">
         <v>457</v>
       </c>
-      <c r="E105" s="105"/>
-    </row>
-    <row r="106" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="103"/>
-      <c r="B106" s="104" t="s">
+      <c r="E105" s="103"/>
+    </row>
+    <row r="106" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="101"/>
+      <c r="B106" s="102" t="s">
         <v>387</v>
       </c>
-      <c r="C106" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="105" t="s">
+      <c r="C106" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="E106" s="105"/>
-    </row>
-    <row r="107" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="103"/>
-      <c r="B107" s="104" t="s">
+      <c r="E106" s="103"/>
+    </row>
+    <row r="107" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="101"/>
+      <c r="B107" s="102" t="s">
         <v>389</v>
       </c>
-      <c r="C107" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="105" t="s">
+      <c r="C107" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="103" t="s">
         <v>390</v>
       </c>
-      <c r="E107" s="105"/>
-    </row>
-    <row r="108" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="103"/>
-      <c r="B108" s="104" t="s">
+      <c r="E107" s="103"/>
+    </row>
+    <row r="108" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="101"/>
+      <c r="B108" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="105" t="s">
+      <c r="C108" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="103" t="s">
         <v>391</v>
       </c>
-      <c r="E108" s="105"/>
-    </row>
-    <row r="109" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="103"/>
-      <c r="B109" s="104" t="s">
+      <c r="E108" s="103"/>
+    </row>
+    <row r="109" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="101"/>
+      <c r="B109" s="102" t="s">
         <v>392</v>
       </c>
-      <c r="C109" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="105" t="s">
+      <c r="C109" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="103" t="s">
         <v>459</v>
       </c>
-      <c r="E109" s="105"/>
+      <c r="E109" s="103"/>
     </row>
     <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="90"/>
@@ -7333,44 +7333,44 @@
       </c>
       <c r="E112" s="85"/>
     </row>
-    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="90"/>
-      <c r="B113" s="91" t="s">
+    <row r="113" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="101"/>
+      <c r="B113" s="102" t="s">
         <v>396</v>
       </c>
-      <c r="C113" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="85" t="s">
+      <c r="C113" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="103" t="s">
         <v>397</v>
       </c>
-      <c r="E113" s="85"/>
-    </row>
-    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="90"/>
-      <c r="B114" s="91" t="s">
+      <c r="E113" s="103"/>
+    </row>
+    <row r="114" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="101"/>
+      <c r="B114" s="102" t="s">
         <v>398</v>
       </c>
-      <c r="C114" s="85" t="s">
+      <c r="C114" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D114" s="85" t="s">
+      <c r="D114" s="103" t="s">
         <v>399</v>
       </c>
-      <c r="E114" s="85"/>
-    </row>
-    <row r="115" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="103"/>
-      <c r="B115" s="104" t="s">
+      <c r="E114" s="103"/>
+    </row>
+    <row r="115" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="101"/>
+      <c r="B115" s="102" t="s">
         <v>400</v>
       </c>
-      <c r="C115" s="105" t="s">
+      <c r="C115" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="D115" s="105" t="s">
+      <c r="D115" s="103" t="s">
         <v>401</v>
       </c>
-      <c r="E115" s="105"/>
+      <c r="E115" s="103"/>
     </row>
     <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="90"/>
@@ -7385,18 +7385,18 @@
       </c>
       <c r="E116" s="85"/>
     </row>
-    <row r="117" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="103"/>
-      <c r="B117" s="104" t="s">
+    <row r="117" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="101"/>
+      <c r="B117" s="102" t="s">
         <v>404</v>
       </c>
-      <c r="C117" s="105" t="s">
+      <c r="C117" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="D117" s="105" t="s">
+      <c r="D117" s="103" t="s">
         <v>405</v>
       </c>
-      <c r="E117" s="105"/>
+      <c r="E117" s="103"/>
     </row>
     <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="90"/>
@@ -7411,304 +7411,304 @@
       </c>
       <c r="E118" s="85"/>
     </row>
-    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="90"/>
-      <c r="B119" s="91" t="s">
+    <row r="119" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="101"/>
+      <c r="B119" s="102" t="s">
         <v>408</v>
       </c>
-      <c r="C119" s="85" t="s">
+      <c r="C119" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D119" s="85" t="s">
+      <c r="D119" s="103" t="s">
         <v>409</v>
       </c>
-      <c r="E119" s="85"/>
-    </row>
-    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="90"/>
-      <c r="B120" s="91" t="s">
+      <c r="E119" s="103"/>
+    </row>
+    <row r="120" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="101"/>
+      <c r="B120" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="C120" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D120" s="85" t="s">
+      <c r="C120" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="103" t="s">
         <v>410</v>
       </c>
-      <c r="E120" s="85"/>
-    </row>
-    <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="90"/>
-      <c r="B121" s="91" t="s">
+      <c r="E120" s="103"/>
+    </row>
+    <row r="121" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="101"/>
+      <c r="B121" s="102" t="s">
         <v>411</v>
       </c>
-      <c r="C121" s="85" t="s">
+      <c r="C121" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D121" s="85" t="s">
+      <c r="D121" s="103" t="s">
         <v>413</v>
       </c>
-      <c r="E121" s="85"/>
-    </row>
-    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="90"/>
-      <c r="B122" s="91" t="s">
+      <c r="E121" s="103"/>
+    </row>
+    <row r="122" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="101"/>
+      <c r="B122" s="102" t="s">
         <v>412</v>
       </c>
-      <c r="C122" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="85" t="s">
+      <c r="C122" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="103" t="s">
         <v>414</v>
       </c>
-      <c r="E122" s="85"/>
-    </row>
-    <row r="123" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="103"/>
-      <c r="B123" s="104" t="s">
+      <c r="E122" s="103"/>
+    </row>
+    <row r="123" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="101"/>
+      <c r="B123" s="102" t="s">
         <v>415</v>
       </c>
-      <c r="C123" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="105" t="s">
+      <c r="C123" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="103" t="s">
         <v>416</v>
       </c>
-      <c r="E123" s="105"/>
-    </row>
-    <row r="124" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="103"/>
-      <c r="B124" s="104" t="s">
+      <c r="E123" s="103"/>
+    </row>
+    <row r="124" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="101"/>
+      <c r="B124" s="102" t="s">
         <v>417</v>
       </c>
-      <c r="C124" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="105" t="s">
+      <c r="C124" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="103" t="s">
         <v>418</v>
       </c>
-      <c r="E124" s="105"/>
-    </row>
-    <row r="125" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="103"/>
-      <c r="B125" s="104" t="s">
+      <c r="E124" s="103"/>
+    </row>
+    <row r="125" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="101"/>
+      <c r="B125" s="102" t="s">
         <v>419</v>
       </c>
-      <c r="C125" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="105" t="s">
+      <c r="C125" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="103" t="s">
         <v>463</v>
       </c>
-      <c r="E125" s="105"/>
-    </row>
-    <row r="126" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="103"/>
-      <c r="B126" s="104" t="s">
+      <c r="E125" s="103"/>
+    </row>
+    <row r="126" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="101"/>
+      <c r="B126" s="102" t="s">
         <v>420</v>
       </c>
-      <c r="C126" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="105" t="s">
+      <c r="C126" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="103" t="s">
         <v>421</v>
       </c>
-      <c r="E126" s="105"/>
-    </row>
-    <row r="127" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="103"/>
-      <c r="B127" s="104" t="s">
+      <c r="E126" s="103"/>
+    </row>
+    <row r="127" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="101"/>
+      <c r="B127" s="102" t="s">
         <v>422</v>
       </c>
-      <c r="C127" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="105" t="s">
+      <c r="C127" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="103" t="s">
         <v>423</v>
       </c>
-      <c r="E127" s="105"/>
-    </row>
-    <row r="128" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="103"/>
-      <c r="B128" s="104" t="s">
+      <c r="E127" s="103"/>
+    </row>
+    <row r="128" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="101"/>
+      <c r="B128" s="102" t="s">
         <v>424</v>
       </c>
-      <c r="C128" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="105" t="s">
+      <c r="C128" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="103" t="s">
         <v>425</v>
       </c>
-      <c r="E128" s="105"/>
-    </row>
-    <row r="129" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="103"/>
-      <c r="B129" s="104" t="s">
+      <c r="E128" s="103"/>
+    </row>
+    <row r="129" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="101"/>
+      <c r="B129" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="C129" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="105" t="s">
+      <c r="C129" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="103" t="s">
         <v>426</v>
       </c>
-      <c r="E129" s="105"/>
-    </row>
-    <row r="130" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="103"/>
-      <c r="B130" s="104" t="s">
+      <c r="E129" s="103"/>
+    </row>
+    <row r="130" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="101"/>
+      <c r="B130" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="C130" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="105" t="s">
+      <c r="C130" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="103" t="s">
         <v>298</v>
       </c>
-      <c r="E130" s="105"/>
-    </row>
-    <row r="131" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="103"/>
-      <c r="B131" s="104" t="s">
+      <c r="E130" s="103"/>
+    </row>
+    <row r="131" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="101"/>
+      <c r="B131" s="102" t="s">
         <v>427</v>
       </c>
-      <c r="C131" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="105" t="s">
+      <c r="C131" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="103" t="s">
         <v>428</v>
       </c>
-      <c r="E131" s="105"/>
-    </row>
-    <row r="132" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="103"/>
-      <c r="B132" s="104" t="s">
+      <c r="E131" s="103"/>
+    </row>
+    <row r="132" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="101"/>
+      <c r="B132" s="102" t="s">
         <v>429</v>
       </c>
-      <c r="C132" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="105" t="s">
+      <c r="C132" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="103" t="s">
         <v>430</v>
       </c>
-      <c r="E132" s="105"/>
-    </row>
-    <row r="133" spans="1:5" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="103"/>
-      <c r="B133" s="104" t="s">
+      <c r="E132" s="103"/>
+    </row>
+    <row r="133" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="101"/>
+      <c r="B133" s="102" t="s">
         <v>431</v>
       </c>
-      <c r="C133" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="105" t="s">
+      <c r="C133" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="103" t="s">
         <v>465</v>
       </c>
-      <c r="E133" s="105"/>
-    </row>
-    <row r="134" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="103"/>
-      <c r="B134" s="104" t="s">
+      <c r="E133" s="103"/>
+    </row>
+    <row r="134" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="101"/>
+      <c r="B134" s="102" t="s">
         <v>432</v>
       </c>
-      <c r="C134" s="105" t="s">
+      <c r="C134" s="103" t="s">
         <v>272</v>
       </c>
-      <c r="D134" s="105" t="s">
+      <c r="D134" s="103" t="s">
         <v>433</v>
       </c>
-      <c r="E134" s="105"/>
-    </row>
-    <row r="135" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="103"/>
-      <c r="B135" s="104" t="s">
+      <c r="E134" s="103"/>
+    </row>
+    <row r="135" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="101"/>
+      <c r="B135" s="102" t="s">
         <v>434</v>
       </c>
-      <c r="C135" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D135" s="105" t="s">
+      <c r="C135" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="103" t="s">
         <v>435</v>
       </c>
-      <c r="E135" s="105"/>
-    </row>
-    <row r="136" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="103"/>
-      <c r="B136" s="104" t="s">
+      <c r="E135" s="103"/>
+    </row>
+    <row r="136" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="101"/>
+      <c r="B136" s="102" t="s">
         <v>436</v>
       </c>
-      <c r="C136" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="105" t="s">
+      <c r="C136" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="103" t="s">
         <v>468</v>
       </c>
-      <c r="E136" s="105"/>
-    </row>
-    <row r="137" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="103"/>
-      <c r="B137" s="104" t="s">
+      <c r="E136" s="103"/>
+    </row>
+    <row r="137" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="101"/>
+      <c r="B137" s="102" t="s">
         <v>437</v>
       </c>
-      <c r="C137" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="105" t="s">
+      <c r="C137" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="103" t="s">
         <v>467</v>
       </c>
-      <c r="E137" s="105"/>
-    </row>
-    <row r="138" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="103"/>
-      <c r="B138" s="104" t="s">
+      <c r="E137" s="103"/>
+    </row>
+    <row r="138" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="101"/>
+      <c r="B138" s="102" t="s">
         <v>438</v>
       </c>
-      <c r="C138" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="105" t="s">
+      <c r="C138" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="103" t="s">
         <v>439</v>
       </c>
-      <c r="E138" s="105"/>
-    </row>
-    <row r="139" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="103"/>
-      <c r="B139" s="104" t="s">
+      <c r="E138" s="103"/>
+    </row>
+    <row r="139" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="101"/>
+      <c r="B139" s="102" t="s">
         <v>440</v>
       </c>
-      <c r="C139" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="105" t="s">
+      <c r="C139" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="103" t="s">
         <v>469</v>
       </c>
-      <c r="E139" s="105"/>
-    </row>
-    <row r="140" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="103"/>
-      <c r="B140" s="104" t="s">
+      <c r="E139" s="103"/>
+    </row>
+    <row r="140" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="101"/>
+      <c r="B140" s="102" t="s">
         <v>441</v>
       </c>
-      <c r="C140" s="105" t="s">
+      <c r="C140" s="103" t="s">
         <v>272</v>
       </c>
-      <c r="D140" s="105" t="s">
+      <c r="D140" s="103" t="s">
         <v>442</v>
       </c>
-      <c r="E140" s="105"/>
-    </row>
-    <row r="141" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="103"/>
-      <c r="B141" s="104" t="s">
+      <c r="E140" s="103"/>
+    </row>
+    <row r="141" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="101"/>
+      <c r="B141" s="102" t="s">
         <v>460</v>
       </c>
-      <c r="C141" s="105" t="s">
+      <c r="C141" s="103" t="s">
         <v>272</v>
       </c>
-      <c r="D141" s="105" t="s">
+      <c r="D141" s="103" t="s">
         <v>461</v>
       </c>
-      <c r="E141" s="105"/>
+      <c r="E141" s="103"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="90"/>
@@ -7762,18 +7762,18 @@
       </c>
       <c r="E145" s="85"/>
     </row>
-    <row r="146" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="98"/>
-      <c r="B146" s="100" t="s">
+    <row r="146" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="96"/>
+      <c r="B146" s="98" t="s">
         <v>485</v>
       </c>
-      <c r="C146" s="101" t="s">
+      <c r="C146" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D146" s="101" t="s">
+      <c r="D146" s="99" t="s">
         <v>486</v>
       </c>
-      <c r="E146" s="101"/>
+      <c r="E146" s="99"/>
     </row>
     <row r="147" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="90"/>
@@ -7788,44 +7788,44 @@
       </c>
       <c r="E147" s="85"/>
     </row>
-    <row r="148" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="103"/>
-      <c r="B148" s="104" t="s">
+    <row r="148" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="101"/>
+      <c r="B148" s="102" t="s">
         <v>490</v>
       </c>
-      <c r="C148" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D148" s="105" t="s">
+      <c r="C148" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D148" s="103" t="s">
         <v>491</v>
       </c>
-      <c r="E148" s="105"/>
-    </row>
-    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="90"/>
-      <c r="B149" s="91" t="s">
+      <c r="E148" s="103"/>
+    </row>
+    <row r="149" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="101"/>
+      <c r="B149" s="102" t="s">
         <v>492</v>
       </c>
-      <c r="C149" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="85" t="s">
+      <c r="C149" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="103" t="s">
         <v>493</v>
       </c>
-      <c r="E149" s="85"/>
-    </row>
-    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="90"/>
-      <c r="B150" s="91" t="s">
+      <c r="E149" s="103"/>
+    </row>
+    <row r="150" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="101"/>
+      <c r="B150" s="102" t="s">
         <v>495</v>
       </c>
-      <c r="C150" s="85" t="s">
+      <c r="C150" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D150" s="85" t="s">
+      <c r="D150" s="103" t="s">
         <v>494</v>
       </c>
-      <c r="E150" s="85"/>
+      <c r="E150" s="103"/>
     </row>
     <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="90"/>

</xml_diff>

<commit_message>
Fixed alignment of listbox
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16B014-E39A-4508-9433-16AC6FC2E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05142C0-67BC-4AD4-9F12-BD20ADB445CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="210" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="4155" yWindow="555" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -5846,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6667,291 +6667,291 @@
       </c>
       <c r="E62" s="103"/>
     </row>
-    <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="90"/>
-      <c r="B63" s="91" t="s">
+    <row r="63" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="101"/>
+      <c r="B63" s="102" t="s">
         <v>304</v>
       </c>
-      <c r="C63" s="85" t="s">
+      <c r="C63" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D63" s="85" t="s">
+      <c r="D63" s="103" t="s">
         <v>306</v>
       </c>
-      <c r="E63" s="85"/>
-    </row>
-    <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="90"/>
-      <c r="B64" s="91" t="s">
+      <c r="E63" s="103"/>
+    </row>
+    <row r="64" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="101"/>
+      <c r="B64" s="102" t="s">
         <v>307</v>
       </c>
-      <c r="C64" s="85" t="s">
+      <c r="C64" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="85" t="s">
+      <c r="D64" s="103" t="s">
         <v>308</v>
       </c>
-      <c r="E64" s="85"/>
-    </row>
-    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="90"/>
-      <c r="B65" s="91" t="s">
+      <c r="E64" s="103"/>
+    </row>
+    <row r="65" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="101"/>
+      <c r="B65" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="C65" s="85" t="s">
+      <c r="C65" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D65" s="85" t="s">
+      <c r="D65" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="E65" s="85"/>
-    </row>
-    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="90"/>
-      <c r="B66" s="91" t="s">
+      <c r="E65" s="103"/>
+    </row>
+    <row r="66" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="101"/>
+      <c r="B66" s="102" t="s">
         <v>311</v>
       </c>
-      <c r="C66" s="85" t="s">
+      <c r="C66" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D66" s="85" t="s">
+      <c r="D66" s="103" t="s">
         <v>312</v>
       </c>
-      <c r="E66" s="85"/>
-    </row>
-    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="90"/>
-      <c r="B67" s="91" t="s">
+      <c r="E66" s="103"/>
+    </row>
+    <row r="67" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="101"/>
+      <c r="B67" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="C67" s="85" t="s">
+      <c r="C67" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D67" s="85" t="s">
+      <c r="D67" s="103" t="s">
         <v>314</v>
       </c>
-      <c r="E67" s="85"/>
-    </row>
-    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="90"/>
-      <c r="B68" s="91" t="s">
+      <c r="E67" s="103"/>
+    </row>
+    <row r="68" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="101"/>
+      <c r="B68" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="C68" s="85" t="s">
+      <c r="C68" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D68" s="85" t="s">
+      <c r="D68" s="103" t="s">
         <v>316</v>
       </c>
-      <c r="E68" s="85"/>
-    </row>
-    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="90"/>
-      <c r="B69" s="91" t="s">
+      <c r="E68" s="103"/>
+    </row>
+    <row r="69" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="101"/>
+      <c r="B69" s="102" t="s">
         <v>317</v>
       </c>
-      <c r="C69" s="85" t="s">
+      <c r="C69" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D69" s="85" t="s">
+      <c r="D69" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="E69" s="85"/>
-    </row>
-    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="90"/>
-      <c r="B70" s="91" t="s">
+      <c r="E69" s="103"/>
+    </row>
+    <row r="70" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="101"/>
+      <c r="B70" s="102" t="s">
         <v>319</v>
       </c>
-      <c r="C70" s="85" t="s">
+      <c r="C70" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D70" s="85" t="s">
+      <c r="D70" s="103" t="s">
         <v>320</v>
       </c>
-      <c r="E70" s="85"/>
-    </row>
-    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="90"/>
-      <c r="B71" s="91" t="s">
+      <c r="E70" s="103"/>
+    </row>
+    <row r="71" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="101"/>
+      <c r="B71" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="C71" s="85" t="s">
+      <c r="C71" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D71" s="85" t="s">
+      <c r="D71" s="103" t="s">
         <v>322</v>
       </c>
-      <c r="E71" s="85"/>
-    </row>
-    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="90"/>
-      <c r="B72" s="91" t="s">
+      <c r="E71" s="103"/>
+    </row>
+    <row r="72" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="101"/>
+      <c r="B72" s="102" t="s">
         <v>323</v>
       </c>
-      <c r="C72" s="85" t="s">
+      <c r="C72" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D72" s="85" t="s">
+      <c r="D72" s="103" t="s">
         <v>324</v>
       </c>
-      <c r="E72" s="85"/>
-    </row>
-    <row r="73" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="90"/>
-      <c r="B73" s="91" t="s">
+      <c r="E72" s="103"/>
+    </row>
+    <row r="73" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="101"/>
+      <c r="B73" s="102" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="85" t="s">
+      <c r="C73" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D73" s="85" t="s">
+      <c r="D73" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="85"/>
-    </row>
-    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="90"/>
-      <c r="B74" s="91" t="s">
+      <c r="E73" s="103"/>
+    </row>
+    <row r="74" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="101"/>
+      <c r="B74" s="102" t="s">
         <v>327</v>
       </c>
-      <c r="C74" s="85" t="s">
+      <c r="C74" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D74" s="85" t="s">
+      <c r="D74" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="E74" s="85"/>
-    </row>
-    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="90"/>
-      <c r="B75" s="91" t="s">
+      <c r="E74" s="103"/>
+    </row>
+    <row r="75" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="101"/>
+      <c r="B75" s="102" t="s">
         <v>328</v>
       </c>
-      <c r="C75" s="85" t="s">
+      <c r="C75" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D75" s="85" t="s">
+      <c r="D75" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="E75" s="85"/>
-    </row>
-    <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="90"/>
-      <c r="B76" s="91" t="s">
+      <c r="E75" s="103"/>
+    </row>
+    <row r="76" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="101"/>
+      <c r="B76" s="102" t="s">
         <v>330</v>
       </c>
-      <c r="C76" s="85" t="s">
+      <c r="C76" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D76" s="85" t="s">
+      <c r="D76" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="E76" s="85"/>
-    </row>
-    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="90"/>
-      <c r="B77" s="91" t="s">
+      <c r="E76" s="103"/>
+    </row>
+    <row r="77" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="101"/>
+      <c r="B77" s="102" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="85" t="s">
+      <c r="C77" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D77" s="85" t="s">
+      <c r="D77" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="E77" s="85"/>
-    </row>
-    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="90"/>
-      <c r="B78" s="91" t="s">
+      <c r="E77" s="103"/>
+    </row>
+    <row r="78" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="101"/>
+      <c r="B78" s="102" t="s">
         <v>334</v>
       </c>
-      <c r="C78" s="85" t="s">
+      <c r="C78" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="85" t="s">
+      <c r="D78" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="E78" s="85"/>
-    </row>
-    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="90"/>
-      <c r="B79" s="91" t="s">
+      <c r="E78" s="103"/>
+    </row>
+    <row r="79" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="101"/>
+      <c r="B79" s="102" t="s">
         <v>336</v>
       </c>
-      <c r="C79" s="85" t="s">
+      <c r="C79" s="103" t="s">
         <v>305</v>
       </c>
-      <c r="D79" s="85" t="s">
+      <c r="D79" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="E79" s="85"/>
-    </row>
-    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="90"/>
-      <c r="B80" s="91" t="s">
+      <c r="E79" s="103"/>
+    </row>
+    <row r="80" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="101"/>
+      <c r="B80" s="102" t="s">
         <v>338</v>
       </c>
-      <c r="C80" s="85" t="s">
+      <c r="C80" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D80" s="85" t="s">
+      <c r="D80" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="E80" s="85"/>
-    </row>
-    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="90"/>
-      <c r="B81" s="91" t="s">
+      <c r="E80" s="103"/>
+    </row>
+    <row r="81" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="101"/>
+      <c r="B81" s="102" t="s">
         <v>341</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="C81" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D81" s="85" t="s">
+      <c r="D81" s="103" t="s">
         <v>342</v>
       </c>
-      <c r="E81" s="85"/>
-    </row>
-    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="90"/>
-      <c r="B82" s="91" t="s">
+      <c r="E81" s="103"/>
+    </row>
+    <row r="82" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="101"/>
+      <c r="B82" s="102" t="s">
         <v>343</v>
       </c>
-      <c r="C82" s="85" t="s">
+      <c r="C82" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D82" s="85" t="s">
+      <c r="D82" s="103" t="s">
         <v>344</v>
       </c>
-      <c r="E82" s="85"/>
-    </row>
-    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="90"/>
-      <c r="B83" s="91" t="s">
+      <c r="E82" s="103"/>
+    </row>
+    <row r="83" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="101"/>
+      <c r="B83" s="102" t="s">
         <v>345</v>
       </c>
-      <c r="C83" s="85" t="s">
+      <c r="C83" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D83" s="85" t="s">
+      <c r="D83" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="E83" s="85"/>
-    </row>
-    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="90"/>
-      <c r="B84" s="91" t="s">
+      <c r="E83" s="103"/>
+    </row>
+    <row r="84" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="101"/>
+      <c r="B84" s="102" t="s">
         <v>346</v>
       </c>
-      <c r="C84" s="85" t="s">
+      <c r="C84" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="D84" s="85" t="s">
+      <c r="D84" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="E84" s="85"/>
+      <c r="E84" s="103"/>
     </row>
     <row r="85" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="101"/>

</xml_diff>

<commit_message>
Updated images for quality
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05142C0-67BC-4AD4-9F12-BD20ADB445CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D05A0B-3252-41A6-A6C8-F8852CB8CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="555" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="2010" yWindow="495" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -5846,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Button css and Noteboard saves
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D05A0B-3252-41A6-A6C8-F8852CB8CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD3014A-6E6B-4546-9576-1F0D89E3EEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="495" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-165" yWindow="90" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -5846,7 +5846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A136" workbookViewId="0">
       <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed image issues & added new wordcloud info
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD3014A-6E6B-4546-9576-1F0D89E3EEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADDDD4E-E464-4757-BC49-9F171FFCF7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="90" windowWidth="12030" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="522">
   <si>
     <t>ID</t>
   </si>
@@ -1533,6 +1533,78 @@
   </si>
   <si>
     <t>ERB Activity Chart</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>99 Small</t>
+  </si>
+  <si>
+    <t>100 Small</t>
+  </si>
+  <si>
+    <t>147 Small</t>
+  </si>
+  <si>
+    <t>113 Small</t>
+  </si>
+  <si>
+    <t>146 Small</t>
+  </si>
+  <si>
+    <t>148 Small</t>
+  </si>
+  <si>
+    <t>149 Small</t>
+  </si>
+  <si>
+    <t>150 Small</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>154 Small</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>79 Large</t>
+  </si>
+  <si>
+    <t>80 Large</t>
+  </si>
+  <si>
+    <t>81 Large</t>
   </si>
 </sst>
 </file>
@@ -2054,15 +2126,9 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,6 +2151,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2477,10 +2549,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="111" t="s">
+      <c r="G2" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="112"/>
+      <c r="H2" s="108"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5844,10 +5916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5875,17 +5947,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="105"/>
+      <c r="A2" s="101"/>
       <c r="B2" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="106" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="106" t="s">
+      <c r="C2" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="106"/>
+      <c r="E2" s="102"/>
     </row>
     <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92"/>
@@ -5952,44 +6024,44 @@
       </c>
       <c r="E7" s="94"/>
     </row>
-    <row r="8" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="108" t="s">
+    <row r="8" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="109" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="109" t="s">
+      <c r="C8" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="105" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="109"/>
-    </row>
-    <row r="9" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
-      <c r="B9" s="108" t="s">
+      <c r="E8" s="105"/>
+    </row>
+    <row r="9" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="103"/>
+      <c r="B9" s="104" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="109" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="109" t="s">
+      <c r="C9" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="105" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="109"/>
-    </row>
-    <row r="10" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="108" t="s">
+      <c r="E9" s="105"/>
+    </row>
+    <row r="10" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="103"/>
+      <c r="B10" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="109" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="109" t="s">
+      <c r="C10" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="105" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="109"/>
+      <c r="E10" s="105"/>
     </row>
     <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92"/>
@@ -6056,83 +6128,83 @@
       </c>
       <c r="E15" s="85"/>
     </row>
-    <row r="16" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
-      <c r="B16" s="102" t="s">
+    <row r="16" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="97"/>
+      <c r="B16" s="98" t="s">
         <v>265</v>
       </c>
-      <c r="C16" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="103" t="s">
+      <c r="C16" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="99" t="s">
         <v>443</v>
       </c>
-      <c r="E16" s="103"/>
-    </row>
-    <row r="17" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
-      <c r="B17" s="102" t="s">
+      <c r="E16" s="99"/>
+    </row>
+    <row r="17" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="97"/>
+      <c r="B17" s="98" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="103" t="s">
+      <c r="C17" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="99" t="s">
         <v>448</v>
       </c>
-      <c r="E17" s="103"/>
-    </row>
-    <row r="18" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="102" t="s">
+      <c r="E17" s="99"/>
+    </row>
+    <row r="18" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="97"/>
+      <c r="B18" s="98" t="s">
         <v>267</v>
       </c>
-      <c r="C18" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="103" t="s">
+      <c r="C18" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="99" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="103"/>
-    </row>
-    <row r="19" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="102" t="s">
+      <c r="E18" s="99"/>
+    </row>
+    <row r="19" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="97"/>
+      <c r="B19" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="C19" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="103" t="s">
+      <c r="C19" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="99" t="s">
         <v>462</v>
       </c>
-      <c r="E19" s="103"/>
-    </row>
-    <row r="20" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="102" t="s">
+      <c r="E19" s="99"/>
+    </row>
+    <row r="20" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="97"/>
+      <c r="B20" s="98" t="s">
         <v>269</v>
       </c>
-      <c r="C20" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="103" t="s">
+      <c r="C20" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="99" t="s">
         <v>466</v>
       </c>
-      <c r="E20" s="103"/>
-    </row>
-    <row r="21" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="102" t="s">
+      <c r="E20" s="99"/>
+    </row>
+    <row r="21" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="97"/>
+      <c r="B21" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="103" t="s">
+      <c r="C21" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="99" t="s">
         <v>445</v>
       </c>
-      <c r="E21" s="103"/>
+      <c r="E21" s="99"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="90"/>
@@ -6186,18 +6258,18 @@
       </c>
       <c r="E25" s="85"/>
     </row>
-    <row r="26" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
-      <c r="B26" s="102" t="s">
+    <row r="26" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="97"/>
+      <c r="B26" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="103" t="s">
+      <c r="C26" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="99" t="s">
         <v>464</v>
       </c>
-      <c r="E26" s="103"/>
+      <c r="E26" s="99"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="90"/>
@@ -6212,161 +6284,161 @@
       </c>
       <c r="E27" s="85"/>
     </row>
-    <row r="28" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
-      <c r="B28" s="102" t="s">
+    <row r="28" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="97"/>
+      <c r="B28" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="E28" s="103"/>
-    </row>
-    <row r="29" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
-      <c r="B29" s="102" t="s">
+      <c r="E28" s="99"/>
+    </row>
+    <row r="29" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="97"/>
+      <c r="B29" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="103" t="s">
+      <c r="D29" s="99" t="s">
         <v>233</v>
       </c>
-      <c r="E29" s="103"/>
-    </row>
-    <row r="30" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="101"/>
-      <c r="B30" s="102" t="s">
+      <c r="E29" s="99"/>
+    </row>
+    <row r="30" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="97"/>
+      <c r="B30" s="98" t="s">
         <v>280</v>
       </c>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="103" t="s">
+      <c r="D30" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="103"/>
-    </row>
-    <row r="31" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="101"/>
-      <c r="B31" s="102" t="s">
+      <c r="E30" s="99"/>
+    </row>
+    <row r="31" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="97"/>
+      <c r="B31" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="103" t="s">
+      <c r="C31" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="99" t="s">
         <v>444</v>
       </c>
-      <c r="E31" s="103"/>
-    </row>
-    <row r="32" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="101"/>
-      <c r="B32" s="102" t="s">
+      <c r="E31" s="99"/>
+    </row>
+    <row r="32" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="97"/>
+      <c r="B32" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="103" t="s">
+      <c r="C32" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="99" t="s">
         <v>447</v>
       </c>
-      <c r="E32" s="103"/>
-    </row>
-    <row r="33" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="101"/>
-      <c r="B33" s="102" t="s">
+      <c r="E32" s="99"/>
+    </row>
+    <row r="33" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="97"/>
+      <c r="B33" s="98" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="103" t="s">
+      <c r="C33" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="103"/>
-    </row>
-    <row r="34" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="101"/>
-      <c r="B34" s="102" t="s">
+      <c r="E33" s="99"/>
+    </row>
+    <row r="34" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="97"/>
+      <c r="B34" s="98" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="103" t="s">
+      <c r="C34" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="99" t="s">
         <v>452</v>
       </c>
-      <c r="E34" s="103"/>
-    </row>
-    <row r="35" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="101"/>
-      <c r="B35" s="102" t="s">
+      <c r="E34" s="99"/>
+    </row>
+    <row r="35" spans="1:5" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="97"/>
+      <c r="B35" s="98" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="103" t="s">
+      <c r="C35" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="99" t="s">
         <v>449</v>
       </c>
-      <c r="E35" s="103"/>
-    </row>
-    <row r="36" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
-      <c r="B36" s="102" t="s">
+      <c r="E35" s="99"/>
+    </row>
+    <row r="36" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="97"/>
+      <c r="B36" s="98" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="103" t="s">
+      <c r="C36" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="99" t="s">
         <v>281</v>
       </c>
-      <c r="E36" s="103"/>
-    </row>
-    <row r="37" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="101"/>
-      <c r="B37" s="102" t="s">
+      <c r="E36" s="99"/>
+    </row>
+    <row r="37" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="97"/>
+      <c r="B37" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="103" t="s">
+      <c r="C37" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="99" t="s">
         <v>450</v>
       </c>
-      <c r="E37" s="103"/>
-    </row>
-    <row r="38" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="101"/>
-      <c r="B38" s="102" t="s">
+      <c r="E37" s="99"/>
+    </row>
+    <row r="38" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="97"/>
+      <c r="B38" s="98" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="103" t="s">
+      <c r="C38" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="99" t="s">
         <v>458</v>
       </c>
-      <c r="E38" s="103"/>
-    </row>
-    <row r="39" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="101"/>
-      <c r="B39" s="102" t="s">
+      <c r="E38" s="99"/>
+    </row>
+    <row r="39" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="97"/>
+      <c r="B39" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="C39" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="103" t="s">
+      <c r="C39" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="99" t="s">
         <v>451</v>
       </c>
-      <c r="E39" s="103"/>
+      <c r="E39" s="99"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="90"/>
@@ -6628,358 +6700,358 @@
       </c>
       <c r="E59" s="85"/>
     </row>
-    <row r="60" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="101"/>
-      <c r="B60" s="102" t="s">
+    <row r="60" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="97"/>
+      <c r="B60" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="103" t="s">
+      <c r="C60" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="99" t="s">
         <v>446</v>
       </c>
-      <c r="E60" s="103"/>
-    </row>
-    <row r="61" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="101"/>
-      <c r="B61" s="102" t="s">
+      <c r="E60" s="99"/>
+    </row>
+    <row r="61" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="97"/>
+      <c r="B61" s="98" t="s">
         <v>301</v>
       </c>
-      <c r="C61" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="103" t="s">
+      <c r="C61" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="99" t="s">
         <v>302</v>
       </c>
-      <c r="E61" s="103"/>
-    </row>
-    <row r="62" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="101"/>
-      <c r="B62" s="102" t="s">
+      <c r="E61" s="99"/>
+    </row>
+    <row r="62" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="97"/>
+      <c r="B62" s="98" t="s">
         <v>303</v>
       </c>
-      <c r="C62" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="103" t="s">
+      <c r="C62" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="99" t="s">
         <v>230</v>
       </c>
-      <c r="E62" s="103"/>
-    </row>
-    <row r="63" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="101"/>
-      <c r="B63" s="102" t="s">
+      <c r="E62" s="99"/>
+    </row>
+    <row r="63" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="97"/>
+      <c r="B63" s="98" t="s">
         <v>304</v>
       </c>
-      <c r="C63" s="103" t="s">
+      <c r="C63" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D63" s="103" t="s">
+      <c r="D63" s="99" t="s">
         <v>306</v>
       </c>
-      <c r="E63" s="103"/>
-    </row>
-    <row r="64" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="101"/>
-      <c r="B64" s="102" t="s">
+      <c r="E63" s="99"/>
+    </row>
+    <row r="64" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="97"/>
+      <c r="B64" s="98" t="s">
         <v>307</v>
       </c>
-      <c r="C64" s="103" t="s">
+      <c r="C64" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="103" t="s">
+      <c r="D64" s="99" t="s">
         <v>308</v>
       </c>
-      <c r="E64" s="103"/>
-    </row>
-    <row r="65" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="101"/>
-      <c r="B65" s="102" t="s">
+      <c r="E64" s="99"/>
+    </row>
+    <row r="65" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="97"/>
+      <c r="B65" s="98" t="s">
         <v>309</v>
       </c>
-      <c r="C65" s="103" t="s">
+      <c r="C65" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D65" s="103" t="s">
+      <c r="D65" s="99" t="s">
         <v>310</v>
       </c>
-      <c r="E65" s="103"/>
-    </row>
-    <row r="66" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="101"/>
-      <c r="B66" s="102" t="s">
+      <c r="E65" s="99"/>
+    </row>
+    <row r="66" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="97"/>
+      <c r="B66" s="98" t="s">
         <v>311</v>
       </c>
-      <c r="C66" s="103" t="s">
+      <c r="C66" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D66" s="103" t="s">
+      <c r="D66" s="99" t="s">
         <v>312</v>
       </c>
-      <c r="E66" s="103"/>
-    </row>
-    <row r="67" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="101"/>
-      <c r="B67" s="102" t="s">
+      <c r="E66" s="99"/>
+    </row>
+    <row r="67" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="97"/>
+      <c r="B67" s="98" t="s">
         <v>313</v>
       </c>
-      <c r="C67" s="103" t="s">
+      <c r="C67" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D67" s="103" t="s">
+      <c r="D67" s="99" t="s">
         <v>314</v>
       </c>
-      <c r="E67" s="103"/>
-    </row>
-    <row r="68" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="101"/>
-      <c r="B68" s="102" t="s">
+      <c r="E67" s="99"/>
+    </row>
+    <row r="68" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="97"/>
+      <c r="B68" s="98" t="s">
         <v>315</v>
       </c>
-      <c r="C68" s="103" t="s">
+      <c r="C68" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D68" s="103" t="s">
+      <c r="D68" s="99" t="s">
         <v>316</v>
       </c>
-      <c r="E68" s="103"/>
-    </row>
-    <row r="69" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="101"/>
-      <c r="B69" s="102" t="s">
+      <c r="E68" s="99"/>
+    </row>
+    <row r="69" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="97"/>
+      <c r="B69" s="98" t="s">
         <v>317</v>
       </c>
-      <c r="C69" s="103" t="s">
+      <c r="C69" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D69" s="103" t="s">
+      <c r="D69" s="99" t="s">
         <v>318</v>
       </c>
-      <c r="E69" s="103"/>
-    </row>
-    <row r="70" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="101"/>
-      <c r="B70" s="102" t="s">
+      <c r="E69" s="99"/>
+    </row>
+    <row r="70" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="97"/>
+      <c r="B70" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="C70" s="103" t="s">
+      <c r="C70" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D70" s="103" t="s">
+      <c r="D70" s="99" t="s">
         <v>320</v>
       </c>
-      <c r="E70" s="103"/>
-    </row>
-    <row r="71" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="101"/>
-      <c r="B71" s="102" t="s">
+      <c r="E70" s="99"/>
+    </row>
+    <row r="71" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="97"/>
+      <c r="B71" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="C71" s="103" t="s">
+      <c r="C71" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D71" s="103" t="s">
+      <c r="D71" s="99" t="s">
         <v>322</v>
       </c>
-      <c r="E71" s="103"/>
-    </row>
-    <row r="72" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="101"/>
-      <c r="B72" s="102" t="s">
+      <c r="E71" s="99"/>
+    </row>
+    <row r="72" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="97"/>
+      <c r="B72" s="98" t="s">
         <v>323</v>
       </c>
-      <c r="C72" s="103" t="s">
+      <c r="C72" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D72" s="103" t="s">
+      <c r="D72" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="E72" s="103"/>
-    </row>
-    <row r="73" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="101"/>
-      <c r="B73" s="102" t="s">
+      <c r="E72" s="99"/>
+    </row>
+    <row r="73" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="97"/>
+      <c r="B73" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="103" t="s">
+      <c r="C73" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D73" s="103" t="s">
+      <c r="D73" s="99" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="103"/>
-    </row>
-    <row r="74" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="101"/>
-      <c r="B74" s="102" t="s">
+      <c r="E73" s="99"/>
+    </row>
+    <row r="74" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="97"/>
+      <c r="B74" s="98" t="s">
         <v>327</v>
       </c>
-      <c r="C74" s="103" t="s">
+      <c r="C74" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D74" s="103" t="s">
+      <c r="D74" s="99" t="s">
         <v>221</v>
       </c>
-      <c r="E74" s="103"/>
-    </row>
-    <row r="75" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="101"/>
-      <c r="B75" s="102" t="s">
+      <c r="E74" s="99"/>
+    </row>
+    <row r="75" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="97"/>
+      <c r="B75" s="98" t="s">
         <v>328</v>
       </c>
-      <c r="C75" s="103" t="s">
+      <c r="C75" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D75" s="103" t="s">
+      <c r="D75" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="E75" s="103"/>
-    </row>
-    <row r="76" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="101"/>
-      <c r="B76" s="102" t="s">
+      <c r="E75" s="99"/>
+    </row>
+    <row r="76" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="97"/>
+      <c r="B76" s="98" t="s">
         <v>330</v>
       </c>
-      <c r="C76" s="103" t="s">
+      <c r="C76" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D76" s="103" t="s">
+      <c r="D76" s="99" t="s">
         <v>331</v>
       </c>
-      <c r="E76" s="103"/>
-    </row>
-    <row r="77" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="101"/>
-      <c r="B77" s="102" t="s">
+      <c r="E76" s="99"/>
+    </row>
+    <row r="77" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="97"/>
+      <c r="B77" s="98" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="103" t="s">
+      <c r="C77" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D77" s="103" t="s">
+      <c r="D77" s="99" t="s">
         <v>333</v>
       </c>
-      <c r="E77" s="103"/>
-    </row>
-    <row r="78" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="101"/>
-      <c r="B78" s="102" t="s">
+      <c r="E77" s="99"/>
+    </row>
+    <row r="78" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="97"/>
+      <c r="B78" s="98" t="s">
         <v>334</v>
       </c>
-      <c r="C78" s="103" t="s">
+      <c r="C78" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="103" t="s">
+      <c r="D78" s="99" t="s">
         <v>335</v>
       </c>
-      <c r="E78" s="103"/>
-    </row>
-    <row r="79" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="101"/>
-      <c r="B79" s="102" t="s">
+      <c r="E78" s="99"/>
+    </row>
+    <row r="79" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="97"/>
+      <c r="B79" s="98" t="s">
         <v>336</v>
       </c>
-      <c r="C79" s="103" t="s">
+      <c r="C79" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="D79" s="103" t="s">
+      <c r="D79" s="99" t="s">
         <v>337</v>
       </c>
-      <c r="E79" s="103"/>
-    </row>
-    <row r="80" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="101"/>
-      <c r="B80" s="102" t="s">
+      <c r="E79" s="99"/>
+    </row>
+    <row r="80" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="97"/>
+      <c r="B80" s="98" t="s">
         <v>338</v>
       </c>
-      <c r="C80" s="103" t="s">
+      <c r="C80" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D80" s="103" t="s">
+      <c r="D80" s="99" t="s">
         <v>340</v>
       </c>
-      <c r="E80" s="103"/>
-    </row>
-    <row r="81" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="101"/>
-      <c r="B81" s="102" t="s">
+      <c r="E80" s="99"/>
+    </row>
+    <row r="81" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="97"/>
+      <c r="B81" s="98" t="s">
         <v>341</v>
       </c>
-      <c r="C81" s="103" t="s">
+      <c r="C81" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D81" s="103" t="s">
+      <c r="D81" s="99" t="s">
         <v>342</v>
       </c>
-      <c r="E81" s="103"/>
-    </row>
-    <row r="82" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="101"/>
-      <c r="B82" s="102" t="s">
+      <c r="E81" s="99"/>
+    </row>
+    <row r="82" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="97"/>
+      <c r="B82" s="98" t="s">
         <v>343</v>
       </c>
-      <c r="C82" s="103" t="s">
+      <c r="C82" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D82" s="103" t="s">
+      <c r="D82" s="99" t="s">
         <v>344</v>
       </c>
-      <c r="E82" s="103"/>
-    </row>
-    <row r="83" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="101"/>
-      <c r="B83" s="102" t="s">
+      <c r="E82" s="99"/>
+    </row>
+    <row r="83" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="97"/>
+      <c r="B83" s="98" t="s">
         <v>345</v>
       </c>
-      <c r="C83" s="103" t="s">
+      <c r="C83" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D83" s="103" t="s">
+      <c r="D83" s="99" t="s">
         <v>233</v>
       </c>
-      <c r="E83" s="103"/>
-    </row>
-    <row r="84" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="101"/>
-      <c r="B84" s="102" t="s">
+      <c r="E83" s="99"/>
+    </row>
+    <row r="84" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="97"/>
+      <c r="B84" s="98" t="s">
         <v>346</v>
       </c>
-      <c r="C84" s="103" t="s">
+      <c r="C84" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D84" s="103" t="s">
+      <c r="D84" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="E84" s="103"/>
-    </row>
-    <row r="85" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="101"/>
-      <c r="B85" s="102" t="s">
+      <c r="E84" s="99"/>
+    </row>
+    <row r="85" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="97"/>
+      <c r="B85" s="98" t="s">
         <v>347</v>
       </c>
-      <c r="C85" s="103" t="s">
+      <c r="C85" s="99" t="s">
         <v>348</v>
       </c>
-      <c r="D85" s="103" t="s">
+      <c r="D85" s="99" t="s">
         <v>349</v>
       </c>
-      <c r="E85" s="103" t="s">
+      <c r="E85" s="99" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="101"/>
-      <c r="B86" s="102" t="s">
+    <row r="86" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="97"/>
+      <c r="B86" s="98" t="s">
         <v>350</v>
       </c>
-      <c r="C86" s="103" t="s">
+      <c r="C86" s="99" t="s">
         <v>348</v>
       </c>
-      <c r="D86" s="103" t="s">
+      <c r="D86" s="99" t="s">
         <v>351</v>
       </c>
-      <c r="E86" s="103" t="s">
+      <c r="E86" s="99" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6994,7 +7066,7 @@
       <c r="D87" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E87" s="97" t="s">
+      <c r="E87" s="96" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7009,7 +7081,7 @@
       <c r="D88" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E88" s="97" t="s">
+      <c r="E88" s="96" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7024,7 +7096,7 @@
       <c r="D89" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="E89" s="97" t="s">
+      <c r="E89" s="96" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7039,7 +7111,7 @@
       <c r="D90" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="E90" s="97" t="s">
+      <c r="E90" s="96" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7054,7 +7126,7 @@
       <c r="D91" s="85" t="s">
         <v>358</v>
       </c>
-      <c r="E91" s="97" t="s">
+      <c r="E91" s="96" t="s">
         <v>393</v>
       </c>
     </row>
@@ -7069,308 +7141,308 @@
       <c r="D92" s="85" t="s">
         <v>361</v>
       </c>
-      <c r="E92" s="97" t="s">
+      <c r="E92" s="96" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="101"/>
-      <c r="B93" s="102" t="s">
+    <row r="93" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="97"/>
+      <c r="B93" s="98" t="s">
         <v>363</v>
       </c>
-      <c r="C93" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="103" t="s">
+      <c r="C93" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="99" t="s">
         <v>364</v>
       </c>
-      <c r="E93" s="103"/>
-    </row>
-    <row r="94" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="101"/>
-      <c r="B94" s="102" t="s">
+      <c r="E93" s="99"/>
+    </row>
+    <row r="94" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="97"/>
+      <c r="B94" s="98" t="s">
         <v>365</v>
       </c>
-      <c r="C94" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="103" t="s">
+      <c r="C94" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="99" t="s">
         <v>454</v>
       </c>
-      <c r="E94" s="103"/>
-    </row>
-    <row r="95" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="101"/>
-      <c r="B95" s="102" t="s">
+      <c r="E94" s="99"/>
+    </row>
+    <row r="95" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="97"/>
+      <c r="B95" s="98" t="s">
         <v>366</v>
       </c>
-      <c r="C95" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="103" t="s">
+      <c r="C95" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="99" t="s">
         <v>367</v>
       </c>
-      <c r="E95" s="103"/>
-    </row>
-    <row r="96" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="101"/>
-      <c r="B96" s="102" t="s">
+      <c r="E95" s="99"/>
+    </row>
+    <row r="96" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="97"/>
+      <c r="B96" s="98" t="s">
         <v>368</v>
       </c>
-      <c r="C96" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="103" t="s">
+      <c r="C96" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="E96" s="103"/>
-    </row>
-    <row r="97" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="101"/>
-      <c r="B97" s="102" t="s">
+      <c r="E96" s="99"/>
+    </row>
+    <row r="97" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="97"/>
+      <c r="B97" s="98" t="s">
         <v>370</v>
       </c>
-      <c r="C97" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="103" t="s">
+      <c r="C97" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="99" t="s">
         <v>371</v>
       </c>
-      <c r="E97" s="103"/>
-    </row>
-    <row r="98" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="101"/>
-      <c r="B98" s="102" t="s">
+      <c r="E97" s="99"/>
+    </row>
+    <row r="98" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="97"/>
+      <c r="B98" s="98" t="s">
         <v>372</v>
       </c>
-      <c r="C98" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="103" t="s">
+      <c r="C98" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="99" t="s">
         <v>373</v>
       </c>
-      <c r="E98" s="103"/>
-    </row>
-    <row r="99" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="101"/>
-      <c r="B99" s="102" t="s">
+      <c r="E98" s="99"/>
+    </row>
+    <row r="99" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="97"/>
+      <c r="B99" s="98" t="s">
         <v>374</v>
       </c>
-      <c r="C99" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="103" t="s">
+      <c r="C99" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="99" t="s">
         <v>375</v>
       </c>
-      <c r="E99" s="103"/>
-    </row>
-    <row r="100" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="101"/>
-      <c r="B100" s="102" t="s">
+      <c r="E99" s="99"/>
+    </row>
+    <row r="100" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="97"/>
+      <c r="B100" s="98" t="s">
         <v>378</v>
       </c>
-      <c r="C100" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="103" t="s">
+      <c r="C100" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="E100" s="103"/>
-    </row>
-    <row r="101" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="101"/>
-      <c r="B101" s="102" t="s">
+      <c r="E100" s="99"/>
+    </row>
+    <row r="101" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="97"/>
+      <c r="B101" s="98" t="s">
         <v>380</v>
       </c>
-      <c r="C101" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="103" t="s">
+      <c r="C101" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="99" t="s">
         <v>381</v>
       </c>
-      <c r="E101" s="103"/>
-    </row>
-    <row r="102" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="101"/>
-      <c r="B102" s="102" t="s">
+      <c r="E101" s="99"/>
+    </row>
+    <row r="102" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="97"/>
+      <c r="B102" s="98" t="s">
         <v>382</v>
       </c>
-      <c r="C102" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="103" t="s">
+      <c r="C102" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="99" t="s">
         <v>383</v>
       </c>
-      <c r="E102" s="103"/>
-    </row>
-    <row r="103" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="101"/>
-      <c r="B103" s="102" t="s">
+      <c r="E102" s="99"/>
+    </row>
+    <row r="103" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="97"/>
+      <c r="B103" s="98" t="s">
         <v>384</v>
       </c>
-      <c r="C103" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="103" t="s">
+      <c r="C103" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="99" t="s">
         <v>455</v>
       </c>
-      <c r="E103" s="103"/>
-    </row>
-    <row r="104" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="101"/>
-      <c r="B104" s="102" t="s">
+      <c r="E103" s="99"/>
+    </row>
+    <row r="104" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="97"/>
+      <c r="B104" s="98" t="s">
         <v>385</v>
       </c>
-      <c r="C104" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="103" t="s">
+      <c r="C104" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="99" t="s">
         <v>456</v>
       </c>
-      <c r="E104" s="103"/>
-    </row>
-    <row r="105" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="101"/>
-      <c r="B105" s="102" t="s">
+      <c r="E104" s="99"/>
+    </row>
+    <row r="105" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="97"/>
+      <c r="B105" s="98" t="s">
         <v>386</v>
       </c>
-      <c r="C105" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="103" t="s">
+      <c r="C105" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="99" t="s">
         <v>457</v>
       </c>
-      <c r="E105" s="103"/>
-    </row>
-    <row r="106" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="101"/>
-      <c r="B106" s="102" t="s">
+      <c r="E105" s="99"/>
+    </row>
+    <row r="106" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="97"/>
+      <c r="B106" s="98" t="s">
         <v>387</v>
       </c>
-      <c r="C106" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="103" t="s">
+      <c r="C106" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="99" t="s">
         <v>388</v>
       </c>
-      <c r="E106" s="103"/>
-    </row>
-    <row r="107" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="101"/>
-      <c r="B107" s="102" t="s">
+      <c r="E106" s="99"/>
+    </row>
+    <row r="107" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="97"/>
+      <c r="B107" s="98" t="s">
         <v>389</v>
       </c>
-      <c r="C107" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="103" t="s">
+      <c r="C107" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="99" t="s">
         <v>390</v>
       </c>
-      <c r="E107" s="103"/>
-    </row>
-    <row r="108" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="101"/>
-      <c r="B108" s="102" t="s">
+      <c r="E107" s="99"/>
+    </row>
+    <row r="108" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="97"/>
+      <c r="B108" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="103" t="s">
+      <c r="C108" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="99" t="s">
         <v>391</v>
       </c>
-      <c r="E108" s="103"/>
-    </row>
-    <row r="109" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="101"/>
-      <c r="B109" s="102" t="s">
+      <c r="E108" s="99"/>
+    </row>
+    <row r="109" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="97"/>
+      <c r="B109" s="98" t="s">
         <v>392</v>
       </c>
-      <c r="C109" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="103" t="s">
+      <c r="C109" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="E109" s="103"/>
-    </row>
-    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="90"/>
-      <c r="B110" s="91" t="s">
+      <c r="E109" s="99"/>
+    </row>
+    <row r="110" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="97"/>
+      <c r="B110" s="98" t="s">
         <v>376</v>
       </c>
-      <c r="C110" s="85" t="s">
+      <c r="C110" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D110" s="85" t="s">
+      <c r="D110" s="99" t="s">
         <v>394</v>
       </c>
-      <c r="E110" s="85"/>
-    </row>
-    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="90"/>
-      <c r="B111" s="91" t="s">
+      <c r="E110" s="99"/>
+    </row>
+    <row r="111" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="97"/>
+      <c r="B111" s="98" t="s">
         <v>377</v>
       </c>
-      <c r="C111" s="85" t="s">
+      <c r="C111" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D111" s="85" t="s">
+      <c r="D111" s="99" t="s">
         <v>474</v>
       </c>
-      <c r="E111" s="85"/>
-    </row>
-    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="90"/>
-      <c r="B112" s="91" t="s">
+      <c r="E111" s="99"/>
+    </row>
+    <row r="112" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="97"/>
+      <c r="B112" s="98" t="s">
         <v>395</v>
       </c>
-      <c r="C112" s="85" t="s">
+      <c r="C112" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D112" s="85" t="s">
+      <c r="D112" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="E112" s="85"/>
-    </row>
-    <row r="113" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="101"/>
-      <c r="B113" s="102" t="s">
+      <c r="E112" s="99"/>
+    </row>
+    <row r="113" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="97"/>
+      <c r="B113" s="98" t="s">
         <v>396</v>
       </c>
-      <c r="C113" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="103" t="s">
+      <c r="C113" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="99" t="s">
         <v>397</v>
       </c>
-      <c r="E113" s="103"/>
-    </row>
-    <row r="114" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="101"/>
-      <c r="B114" s="102" t="s">
+      <c r="E113" s="99"/>
+    </row>
+    <row r="114" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="97"/>
+      <c r="B114" s="98" t="s">
         <v>398</v>
       </c>
-      <c r="C114" s="103" t="s">
+      <c r="C114" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D114" s="103" t="s">
+      <c r="D114" s="99" t="s">
         <v>399</v>
       </c>
-      <c r="E114" s="103"/>
-    </row>
-    <row r="115" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="101"/>
-      <c r="B115" s="102" t="s">
+      <c r="E114" s="99"/>
+    </row>
+    <row r="115" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="97"/>
+      <c r="B115" s="98" t="s">
         <v>400</v>
       </c>
-      <c r="C115" s="103" t="s">
+      <c r="C115" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D115" s="103" t="s">
+      <c r="D115" s="99" t="s">
         <v>401</v>
       </c>
-      <c r="E115" s="103"/>
+      <c r="E115" s="99"/>
     </row>
     <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="90"/>
@@ -7385,330 +7457,330 @@
       </c>
       <c r="E116" s="85"/>
     </row>
-    <row r="117" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="101"/>
-      <c r="B117" s="102" t="s">
+    <row r="117" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="97"/>
+      <c r="B117" s="98" t="s">
         <v>404</v>
       </c>
-      <c r="C117" s="103" t="s">
+      <c r="C117" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D117" s="103" t="s">
+      <c r="D117" s="99" t="s">
         <v>405</v>
       </c>
-      <c r="E117" s="103"/>
-    </row>
-    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="90"/>
-      <c r="B118" s="91" t="s">
+      <c r="E117" s="99"/>
+    </row>
+    <row r="118" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="97"/>
+      <c r="B118" s="98" t="s">
         <v>406</v>
       </c>
-      <c r="C118" s="85" t="s">
+      <c r="C118" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D118" s="85" t="s">
+      <c r="D118" s="99" t="s">
         <v>407</v>
       </c>
-      <c r="E118" s="85"/>
-    </row>
-    <row r="119" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="101"/>
-      <c r="B119" s="102" t="s">
+      <c r="E118" s="99"/>
+    </row>
+    <row r="119" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="97"/>
+      <c r="B119" s="98" t="s">
         <v>408</v>
       </c>
-      <c r="C119" s="103" t="s">
+      <c r="C119" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D119" s="103" t="s">
+      <c r="D119" s="99" t="s">
         <v>409</v>
       </c>
-      <c r="E119" s="103"/>
-    </row>
-    <row r="120" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="101"/>
-      <c r="B120" s="102" t="s">
+      <c r="E119" s="99"/>
+    </row>
+    <row r="120" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="97"/>
+      <c r="B120" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="C120" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D120" s="103" t="s">
+      <c r="C120" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="99" t="s">
         <v>410</v>
       </c>
-      <c r="E120" s="103"/>
-    </row>
-    <row r="121" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="101"/>
-      <c r="B121" s="102" t="s">
+      <c r="E120" s="99"/>
+    </row>
+    <row r="121" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="97"/>
+      <c r="B121" s="98" t="s">
         <v>411</v>
       </c>
-      <c r="C121" s="103" t="s">
+      <c r="C121" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D121" s="103" t="s">
+      <c r="D121" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="E121" s="103"/>
-    </row>
-    <row r="122" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="101"/>
-      <c r="B122" s="102" t="s">
+      <c r="E121" s="99"/>
+    </row>
+    <row r="122" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="97"/>
+      <c r="B122" s="98" t="s">
         <v>412</v>
       </c>
-      <c r="C122" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="103" t="s">
+      <c r="C122" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="99" t="s">
         <v>414</v>
       </c>
-      <c r="E122" s="103"/>
-    </row>
-    <row r="123" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="101"/>
-      <c r="B123" s="102" t="s">
+      <c r="E122" s="99"/>
+    </row>
+    <row r="123" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="97"/>
+      <c r="B123" s="98" t="s">
         <v>415</v>
       </c>
-      <c r="C123" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="103" t="s">
+      <c r="C123" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="99" t="s">
         <v>416</v>
       </c>
-      <c r="E123" s="103"/>
-    </row>
-    <row r="124" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="101"/>
-      <c r="B124" s="102" t="s">
+      <c r="E123" s="99"/>
+    </row>
+    <row r="124" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="97"/>
+      <c r="B124" s="98" t="s">
         <v>417</v>
       </c>
-      <c r="C124" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="103" t="s">
+      <c r="C124" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="99" t="s">
         <v>418</v>
       </c>
-      <c r="E124" s="103"/>
-    </row>
-    <row r="125" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="101"/>
-      <c r="B125" s="102" t="s">
+      <c r="E124" s="99"/>
+    </row>
+    <row r="125" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="97"/>
+      <c r="B125" s="98" t="s">
         <v>419</v>
       </c>
-      <c r="C125" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="103" t="s">
+      <c r="C125" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="99" t="s">
         <v>463</v>
       </c>
-      <c r="E125" s="103"/>
-    </row>
-    <row r="126" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="101"/>
-      <c r="B126" s="102" t="s">
+      <c r="E125" s="99"/>
+    </row>
+    <row r="126" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="97"/>
+      <c r="B126" s="98" t="s">
         <v>420</v>
       </c>
-      <c r="C126" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="103" t="s">
+      <c r="C126" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="99" t="s">
         <v>421</v>
       </c>
-      <c r="E126" s="103"/>
-    </row>
-    <row r="127" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="101"/>
-      <c r="B127" s="102" t="s">
+      <c r="E126" s="99"/>
+    </row>
+    <row r="127" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="97"/>
+      <c r="B127" s="98" t="s">
         <v>422</v>
       </c>
-      <c r="C127" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="103" t="s">
+      <c r="C127" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="99" t="s">
         <v>423</v>
       </c>
-      <c r="E127" s="103"/>
-    </row>
-    <row r="128" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="101"/>
-      <c r="B128" s="102" t="s">
+      <c r="E127" s="99"/>
+    </row>
+    <row r="128" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="97"/>
+      <c r="B128" s="98" t="s">
         <v>424</v>
       </c>
-      <c r="C128" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="103" t="s">
+      <c r="C128" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="99" t="s">
         <v>425</v>
       </c>
-      <c r="E128" s="103"/>
-    </row>
-    <row r="129" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="101"/>
-      <c r="B129" s="102" t="s">
+      <c r="E128" s="99"/>
+    </row>
+    <row r="129" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="97"/>
+      <c r="B129" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="C129" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="103" t="s">
+      <c r="C129" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="99" t="s">
         <v>426</v>
       </c>
-      <c r="E129" s="103"/>
-    </row>
-    <row r="130" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="101"/>
-      <c r="B130" s="102" t="s">
+      <c r="E129" s="99"/>
+    </row>
+    <row r="130" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="97"/>
+      <c r="B130" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="C130" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="103" t="s">
+      <c r="C130" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="99" t="s">
         <v>298</v>
       </c>
-      <c r="E130" s="103"/>
-    </row>
-    <row r="131" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="101"/>
-      <c r="B131" s="102" t="s">
+      <c r="E130" s="99"/>
+    </row>
+    <row r="131" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="97"/>
+      <c r="B131" s="98" t="s">
         <v>427</v>
       </c>
-      <c r="C131" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="103" t="s">
+      <c r="C131" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="99" t="s">
         <v>428</v>
       </c>
-      <c r="E131" s="103"/>
-    </row>
-    <row r="132" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="101"/>
-      <c r="B132" s="102" t="s">
+      <c r="E131" s="99"/>
+    </row>
+    <row r="132" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="97"/>
+      <c r="B132" s="98" t="s">
         <v>429</v>
       </c>
-      <c r="C132" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="103" t="s">
+      <c r="C132" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="99" t="s">
         <v>430</v>
       </c>
-      <c r="E132" s="103"/>
-    </row>
-    <row r="133" spans="1:5" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="101"/>
-      <c r="B133" s="102" t="s">
+      <c r="E132" s="99"/>
+    </row>
+    <row r="133" spans="1:5" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="97"/>
+      <c r="B133" s="98" t="s">
         <v>431</v>
       </c>
-      <c r="C133" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="103" t="s">
+      <c r="C133" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="99" t="s">
         <v>465</v>
       </c>
-      <c r="E133" s="103"/>
-    </row>
-    <row r="134" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="101"/>
-      <c r="B134" s="102" t="s">
+      <c r="E133" s="99"/>
+    </row>
+    <row r="134" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="97"/>
+      <c r="B134" s="98" t="s">
         <v>432</v>
       </c>
-      <c r="C134" s="103" t="s">
+      <c r="C134" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="D134" s="103" t="s">
+      <c r="D134" s="99" t="s">
         <v>433</v>
       </c>
-      <c r="E134" s="103"/>
-    </row>
-    <row r="135" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="101"/>
-      <c r="B135" s="102" t="s">
+      <c r="E134" s="99"/>
+    </row>
+    <row r="135" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="97"/>
+      <c r="B135" s="98" t="s">
         <v>434</v>
       </c>
-      <c r="C135" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D135" s="103" t="s">
+      <c r="C135" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D135" s="99" t="s">
         <v>435</v>
       </c>
-      <c r="E135" s="103"/>
-    </row>
-    <row r="136" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="101"/>
-      <c r="B136" s="102" t="s">
+      <c r="E135" s="99"/>
+    </row>
+    <row r="136" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="97"/>
+      <c r="B136" s="98" t="s">
         <v>436</v>
       </c>
-      <c r="C136" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="103" t="s">
+      <c r="C136" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="E136" s="103"/>
-    </row>
-    <row r="137" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="101"/>
-      <c r="B137" s="102" t="s">
+      <c r="E136" s="99"/>
+    </row>
+    <row r="137" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="97"/>
+      <c r="B137" s="98" t="s">
         <v>437</v>
       </c>
-      <c r="C137" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="103" t="s">
+      <c r="C137" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="99" t="s">
         <v>467</v>
       </c>
-      <c r="E137" s="103"/>
-    </row>
-    <row r="138" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="101"/>
-      <c r="B138" s="102" t="s">
+      <c r="E137" s="99"/>
+    </row>
+    <row r="138" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="97"/>
+      <c r="B138" s="98" t="s">
         <v>438</v>
       </c>
-      <c r="C138" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="103" t="s">
+      <c r="C138" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="99" t="s">
         <v>439</v>
       </c>
-      <c r="E138" s="103"/>
-    </row>
-    <row r="139" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="101"/>
-      <c r="B139" s="102" t="s">
+      <c r="E138" s="99"/>
+    </row>
+    <row r="139" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="97"/>
+      <c r="B139" s="98" t="s">
         <v>440</v>
       </c>
-      <c r="C139" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="103" t="s">
+      <c r="C139" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="99" t="s">
         <v>469</v>
       </c>
-      <c r="E139" s="103"/>
-    </row>
-    <row r="140" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="101"/>
-      <c r="B140" s="102" t="s">
+      <c r="E139" s="99"/>
+    </row>
+    <row r="140" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="97"/>
+      <c r="B140" s="98" t="s">
         <v>441</v>
       </c>
-      <c r="C140" s="103" t="s">
+      <c r="C140" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="D140" s="103" t="s">
+      <c r="D140" s="99" t="s">
         <v>442</v>
       </c>
-      <c r="E140" s="103"/>
-    </row>
-    <row r="141" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="101"/>
-      <c r="B141" s="102" t="s">
+      <c r="E140" s="99"/>
+    </row>
+    <row r="141" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="97"/>
+      <c r="B141" s="98" t="s">
         <v>460</v>
       </c>
-      <c r="C141" s="103" t="s">
+      <c r="C141" s="99" t="s">
         <v>272</v>
       </c>
-      <c r="D141" s="103" t="s">
+      <c r="D141" s="99" t="s">
         <v>461</v>
       </c>
-      <c r="E141" s="103"/>
+      <c r="E141" s="99"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="90"/>
@@ -7723,109 +7795,109 @@
       </c>
       <c r="E142" s="85"/>
     </row>
-    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="90"/>
-      <c r="B143" s="91" t="s">
+    <row r="143" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="97"/>
+      <c r="B143" s="98" t="s">
         <v>478</v>
       </c>
-      <c r="C143" s="85" t="s">
+      <c r="C143" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D143" s="85" t="s">
+      <c r="D143" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="E143" s="85"/>
-    </row>
-    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="90"/>
-      <c r="B144" s="91" t="s">
+      <c r="E143" s="99"/>
+    </row>
+    <row r="144" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="97"/>
+      <c r="B144" s="98" t="s">
         <v>481</v>
       </c>
-      <c r="C144" s="85" t="s">
+      <c r="C144" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D144" s="85" t="s">
+      <c r="D144" s="99" t="s">
         <v>482</v>
       </c>
-      <c r="E144" s="85"/>
-    </row>
-    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="90"/>
-      <c r="B145" s="91" t="s">
+      <c r="E144" s="99"/>
+    </row>
+    <row r="145" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="97"/>
+      <c r="B145" s="98" t="s">
         <v>483</v>
       </c>
-      <c r="C145" s="85" t="s">
+      <c r="C145" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D145" s="85" t="s">
+      <c r="D145" s="99" t="s">
         <v>484</v>
       </c>
-      <c r="E145" s="85"/>
-    </row>
-    <row r="146" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="96"/>
-      <c r="B146" s="98" t="s">
+      <c r="E145" s="99"/>
+    </row>
+    <row r="146" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="109"/>
+      <c r="B146" s="110" t="s">
         <v>485</v>
       </c>
-      <c r="C146" s="99" t="s">
+      <c r="C146" s="111" t="s">
         <v>339</v>
       </c>
-      <c r="D146" s="99" t="s">
+      <c r="D146" s="111" t="s">
         <v>486</v>
       </c>
-      <c r="E146" s="99"/>
-    </row>
-    <row r="147" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="90"/>
-      <c r="B147" s="91" t="s">
+      <c r="E146" s="111"/>
+    </row>
+    <row r="147" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="97"/>
+      <c r="B147" s="98" t="s">
         <v>487</v>
       </c>
-      <c r="C147" s="85" t="s">
+      <c r="C147" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D147" s="85" t="s">
+      <c r="D147" s="99" t="s">
         <v>488</v>
       </c>
-      <c r="E147" s="85"/>
-    </row>
-    <row r="148" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="101"/>
-      <c r="B148" s="102" t="s">
+      <c r="E147" s="99"/>
+    </row>
+    <row r="148" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="97"/>
+      <c r="B148" s="98" t="s">
         <v>490</v>
       </c>
-      <c r="C148" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D148" s="103" t="s">
+      <c r="C148" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D148" s="99" t="s">
         <v>491</v>
       </c>
-      <c r="E148" s="103"/>
-    </row>
-    <row r="149" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="101"/>
-      <c r="B149" s="102" t="s">
+      <c r="E148" s="99"/>
+    </row>
+    <row r="149" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="97"/>
+      <c r="B149" s="98" t="s">
         <v>492</v>
       </c>
-      <c r="C149" s="103" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="103" t="s">
+      <c r="C149" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="99" t="s">
         <v>493</v>
       </c>
-      <c r="E149" s="103"/>
-    </row>
-    <row r="150" spans="1:5" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="101"/>
-      <c r="B150" s="102" t="s">
+      <c r="E149" s="99"/>
+    </row>
+    <row r="150" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="97"/>
+      <c r="B150" s="98" t="s">
         <v>495</v>
       </c>
-      <c r="C150" s="103" t="s">
+      <c r="C150" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="D150" s="103" t="s">
+      <c r="D150" s="99" t="s">
         <v>494</v>
       </c>
-      <c r="E150" s="103"/>
+      <c r="E150" s="99"/>
     </row>
     <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="90"/>
@@ -7842,10 +7914,137 @@
     </row>
     <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="90"/>
-      <c r="B152" s="91"/>
-      <c r="C152" s="85"/>
-      <c r="D152" s="85"/>
+      <c r="B152" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="C152" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D152" s="85" t="s">
+        <v>506</v>
+      </c>
       <c r="E152" s="85"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="83" t="s">
+        <v>499</v>
+      </c>
+      <c r="C153" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D153" s="84" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="83" t="s">
+        <v>500</v>
+      </c>
+      <c r="C154" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D154" s="84" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="83" t="s">
+        <v>501</v>
+      </c>
+      <c r="C155" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D155" s="84" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="83" t="s">
+        <v>502</v>
+      </c>
+      <c r="C156" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D156" s="84" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="83" t="s">
+        <v>503</v>
+      </c>
+      <c r="C157" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D157" s="84" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="C158" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D158" s="84" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="83" t="s">
+        <v>505</v>
+      </c>
+      <c r="C159" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D159" s="84" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="83" t="s">
+        <v>514</v>
+      </c>
+      <c r="C160" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D160" s="84" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="C161" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D161" s="84" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="83" t="s">
+        <v>517</v>
+      </c>
+      <c r="C162" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D162" s="84" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="83" t="s">
+        <v>518</v>
+      </c>
+      <c r="C163" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D163" s="84" t="s">
+        <v>521</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Disclaimer to About drop down in menu
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADDDD4E-E464-4757-BC49-9F171FFCF7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A05792-6273-4567-8E60-8980A35EEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15450" windowHeight="15315" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="524">
   <si>
     <t>ID</t>
   </si>
@@ -1605,6 +1605,12 @@
   </si>
   <si>
     <t>81 Large</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1686,12 +1692,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1949,7 +1949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2129,12 +2129,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2151,12 +2145,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2549,10 +2543,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="108"/>
+      <c r="H2" s="104"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5916,10 +5910,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5947,17 +5941,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="101"/>
+      <c r="A2" s="97"/>
       <c r="B2" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="102" t="s">
+      <c r="C2" s="98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="102"/>
+      <c r="E2" s="98"/>
     </row>
     <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92"/>
@@ -6024,44 +6018,44 @@
       </c>
       <c r="E7" s="94"/>
     </row>
-    <row r="8" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
-      <c r="B8" s="104" t="s">
+    <row r="8" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="99"/>
+      <c r="B8" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="105" t="s">
+      <c r="C8" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="101" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="105"/>
-    </row>
-    <row r="9" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="103"/>
-      <c r="B9" s="104" t="s">
+      <c r="E8" s="101"/>
+    </row>
+    <row r="9" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99"/>
+      <c r="B9" s="100" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="105" t="s">
+      <c r="C9" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="101" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="105"/>
-    </row>
-    <row r="10" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
-      <c r="B10" s="104" t="s">
+      <c r="E9" s="101"/>
+    </row>
+    <row r="10" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99"/>
+      <c r="B10" s="100" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="105" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="105" t="s">
+      <c r="C10" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="101" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="105"/>
+      <c r="E10" s="101"/>
     </row>
     <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92"/>
@@ -6076,1010 +6070,1008 @@
       </c>
       <c r="E11" s="94"/>
     </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
-      <c r="B12" s="91" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="85"/>
+    <row r="12" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100" t="s">
+        <v>522</v>
+      </c>
+      <c r="C12" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="101" t="s">
+        <v>523</v>
+      </c>
+      <c r="E12" s="101"/>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90"/>
       <c r="B13" s="91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D13" s="85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90"/>
       <c r="B14" s="91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>264</v>
+        <v>17</v>
       </c>
       <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="90"/>
       <c r="B15" s="91" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="E15" s="85"/>
+    </row>
+    <row r="16" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="90"/>
+      <c r="B16" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D15" s="85" t="s">
+      <c r="C16" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="85"/>
-    </row>
-    <row r="16" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="98" t="s">
+      <c r="E16" s="85"/>
+    </row>
+    <row r="17" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="90"/>
+      <c r="B17" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="C16" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="99" t="s">
+      <c r="C17" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="85" t="s">
         <v>443</v>
       </c>
-      <c r="E16" s="99"/>
-    </row>
-    <row r="17" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="98" t="s">
+      <c r="E17" s="85"/>
+    </row>
+    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="90"/>
+      <c r="B18" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="99" t="s">
+      <c r="C18" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="85" t="s">
         <v>448</v>
       </c>
-      <c r="E17" s="99"/>
-    </row>
-    <row r="18" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="97"/>
-      <c r="B18" s="98" t="s">
+      <c r="E18" s="85"/>
+    </row>
+    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="90"/>
+      <c r="B19" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="C18" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="99" t="s">
+      <c r="C19" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="85" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="99"/>
-    </row>
-    <row r="19" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="97"/>
-      <c r="B19" s="98" t="s">
+      <c r="E19" s="85"/>
+    </row>
+    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="90"/>
+      <c r="B20" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="C19" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="99" t="s">
+      <c r="C20" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="85" t="s">
         <v>462</v>
       </c>
-      <c r="E19" s="99"/>
-    </row>
-    <row r="20" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="97"/>
-      <c r="B20" s="98" t="s">
+      <c r="E20" s="85"/>
+    </row>
+    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="90"/>
+      <c r="B21" s="91" t="s">
         <v>269</v>
       </c>
-      <c r="C20" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="99" t="s">
+      <c r="C21" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>466</v>
       </c>
-      <c r="E20" s="99"/>
-    </row>
-    <row r="21" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="97"/>
-      <c r="B21" s="98" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>445</v>
-      </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="85"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="90"/>
       <c r="B22" s="91" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C22" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D22" s="85" t="s">
-        <v>270</v>
+        <v>445</v>
       </c>
       <c r="E22" s="85"/>
     </row>
     <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="90"/>
       <c r="B23" s="91" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="90"/>
       <c r="B24" s="91" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D24" s="85" t="s">
-        <v>8</v>
+        <v>271</v>
       </c>
       <c r="E24" s="85"/>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="90"/>
       <c r="B25" s="91" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D25" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="85"/>
+    </row>
+    <row r="26" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="90"/>
+      <c r="B26" s="91" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="85" t="s">
+      <c r="C26" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="D25" s="85" t="s">
+      <c r="D26" s="85" t="s">
         <v>273</v>
       </c>
-      <c r="E25" s="85"/>
-    </row>
-    <row r="26" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D26" s="99" t="s">
-        <v>464</v>
-      </c>
-      <c r="E26" s="99"/>
+      <c r="E26" s="85"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="90"/>
       <c r="B27" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27" s="85" t="s">
+        <v>464</v>
+      </c>
+      <c r="E27" s="85"/>
+    </row>
+    <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="90"/>
+      <c r="B28" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="C27" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="85" t="s">
+      <c r="C28" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="E27" s="85"/>
-    </row>
-    <row r="28" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="97"/>
-      <c r="B28" s="98" t="s">
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="90"/>
+      <c r="B29" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="C28" s="99" t="s">
+      <c r="C29" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="D28" s="99" t="s">
+      <c r="D29" s="85" t="s">
         <v>277</v>
       </c>
-      <c r="E28" s="99"/>
-    </row>
-    <row r="29" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="97"/>
-      <c r="B29" s="98" t="s">
+      <c r="E29" s="85"/>
+    </row>
+    <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="90"/>
+      <c r="B30" s="91" t="s">
         <v>278</v>
       </c>
-      <c r="C29" s="99" t="s">
+      <c r="C30" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="99" t="s">
+      <c r="D30" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="E29" s="99"/>
-    </row>
-    <row r="30" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="97"/>
-      <c r="B30" s="98" t="s">
+      <c r="E30" s="85"/>
+    </row>
+    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="90"/>
+      <c r="B31" s="91" t="s">
         <v>280</v>
       </c>
-      <c r="C30" s="99" t="s">
+      <c r="C31" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="99" t="s">
+      <c r="D31" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="99"/>
-    </row>
-    <row r="31" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="97"/>
-      <c r="B31" s="98" t="s">
+      <c r="E31" s="85"/>
+    </row>
+    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="90"/>
+      <c r="B32" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" s="99" t="s">
+      <c r="C32" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="E31" s="99"/>
-    </row>
-    <row r="32" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="97"/>
-      <c r="B32" s="98" t="s">
+      <c r="E32" s="85"/>
+    </row>
+    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="90"/>
+      <c r="B33" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="99" t="s">
+      <c r="C33" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="85" t="s">
         <v>447</v>
       </c>
-      <c r="E32" s="99"/>
-    </row>
-    <row r="33" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="97"/>
-      <c r="B33" s="98" t="s">
+      <c r="E33" s="85"/>
+    </row>
+    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="90"/>
+      <c r="B34" s="91" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="99" t="s">
+      <c r="C34" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="99"/>
-    </row>
-    <row r="34" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="97"/>
-      <c r="B34" s="98" t="s">
+      <c r="E34" s="85"/>
+    </row>
+    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="90"/>
+      <c r="B35" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="99" t="s">
+      <c r="C35" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="85" t="s">
         <v>452</v>
       </c>
-      <c r="E34" s="99"/>
-    </row>
-    <row r="35" spans="1:5" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="97"/>
-      <c r="B35" s="98" t="s">
+      <c r="E35" s="85"/>
+    </row>
+    <row r="36" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="90"/>
+      <c r="B36" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="99" t="s">
+      <c r="C36" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="85" t="s">
         <v>449</v>
       </c>
-      <c r="E35" s="99"/>
-    </row>
-    <row r="36" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="97"/>
-      <c r="B36" s="98" t="s">
+      <c r="E36" s="85"/>
+    </row>
+    <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="90"/>
+      <c r="B37" s="91" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="99" t="s">
+      <c r="C37" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="85" t="s">
         <v>281</v>
       </c>
-      <c r="E36" s="99"/>
-    </row>
-    <row r="37" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="97"/>
-      <c r="B37" s="98" t="s">
+      <c r="E37" s="85"/>
+    </row>
+    <row r="38" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="90"/>
+      <c r="B38" s="91" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="99" t="s">
+      <c r="C38" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="85" t="s">
         <v>450</v>
       </c>
-      <c r="E37" s="99"/>
-    </row>
-    <row r="38" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="97"/>
-      <c r="B38" s="98" t="s">
+      <c r="E38" s="85"/>
+    </row>
+    <row r="39" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="90"/>
+      <c r="B39" s="91" t="s">
         <v>172</v>
       </c>
-      <c r="C38" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="99" t="s">
+      <c r="C39" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" s="85" t="s">
         <v>458</v>
       </c>
-      <c r="E38" s="99"/>
-    </row>
-    <row r="39" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="97"/>
-      <c r="B39" s="98" t="s">
-        <v>282</v>
-      </c>
-      <c r="C39" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="99" t="s">
-        <v>451</v>
-      </c>
-      <c r="E39" s="99"/>
+      <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="90"/>
       <c r="B40" s="91" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C40" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D40" s="85" t="s">
-        <v>284</v>
+        <v>451</v>
       </c>
       <c r="E40" s="85"/>
     </row>
     <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="90"/>
       <c r="B41" s="91" t="s">
-        <v>155</v>
+        <v>283</v>
       </c>
       <c r="C41" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D41" s="85" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E41" s="85"/>
     </row>
     <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="90"/>
       <c r="B42" s="91" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C42" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D42" s="85" t="s">
-        <v>12</v>
+        <v>285</v>
       </c>
       <c r="E42" s="85"/>
     </row>
     <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="90"/>
       <c r="B43" s="91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D43" s="85" t="s">
-        <v>286</v>
+        <v>12</v>
       </c>
       <c r="E43" s="85"/>
     </row>
     <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="90"/>
       <c r="B44" s="91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D44" s="85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E44" s="85"/>
     </row>
     <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="90"/>
       <c r="B45" s="91" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D45" s="85" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E45" s="85"/>
     </row>
     <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="90"/>
       <c r="B46" s="91" t="s">
-        <v>289</v>
+        <v>177</v>
       </c>
       <c r="C46" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D46" s="85" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E46" s="85"/>
     </row>
     <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="90"/>
       <c r="B47" s="91" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C47" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D47" s="85" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E47" s="85"/>
     </row>
     <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="90"/>
       <c r="B48" s="91" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C48" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D48" s="85" t="s">
-        <v>15</v>
+        <v>292</v>
       </c>
       <c r="E48" s="85"/>
     </row>
     <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="90"/>
       <c r="B49" s="91" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C49" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D49" s="85" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E49" s="85"/>
     </row>
     <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="90"/>
       <c r="B50" s="91" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C50" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D50" s="85" t="s">
-        <v>296</v>
+        <v>24</v>
       </c>
       <c r="E50" s="85"/>
     </row>
     <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="90"/>
       <c r="B51" s="91" t="s">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="C51" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D51" s="85" t="s">
-        <v>27</v>
+        <v>296</v>
       </c>
       <c r="E51" s="85"/>
     </row>
     <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="90"/>
       <c r="B52" s="91" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C52" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D52" s="85" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E52" s="85"/>
     </row>
     <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="90"/>
       <c r="B53" s="91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D53" s="85" t="s">
-        <v>297</v>
+        <v>28</v>
       </c>
       <c r="E53" s="85"/>
     </row>
     <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="90"/>
       <c r="B54" s="91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C54" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D54" s="85" t="s">
-        <v>30</v>
+        <v>297</v>
       </c>
       <c r="E54" s="85"/>
     </row>
     <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="90"/>
       <c r="B55" s="91" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C55" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D55" s="85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E55" s="85"/>
     </row>
     <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="90"/>
       <c r="B56" s="91" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C56" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D56" s="85" t="s">
-        <v>298</v>
+        <v>31</v>
       </c>
       <c r="E56" s="85"/>
     </row>
     <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="90"/>
       <c r="B57" s="91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C57" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D57" s="85" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E57" s="85"/>
     </row>
     <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="90"/>
       <c r="B58" s="91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C58" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D58" s="85" t="s">
-        <v>34</v>
+        <v>299</v>
       </c>
       <c r="E58" s="85"/>
     </row>
     <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="90"/>
       <c r="B59" s="91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="85"/>
+    </row>
+    <row r="60" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="90"/>
+      <c r="B60" s="91" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="85" t="s">
+      <c r="C60" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="85" t="s">
         <v>300</v>
       </c>
-      <c r="E59" s="85"/>
-    </row>
-    <row r="60" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="97"/>
-      <c r="B60" s="98" t="s">
+      <c r="E60" s="85"/>
+    </row>
+    <row r="61" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="90"/>
+      <c r="B61" s="91" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="99" t="s">
+      <c r="C61" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" s="85" t="s">
         <v>446</v>
       </c>
-      <c r="E60" s="99"/>
-    </row>
-    <row r="61" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="97"/>
-      <c r="B61" s="98" t="s">
+      <c r="E61" s="85"/>
+    </row>
+    <row r="62" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="90"/>
+      <c r="B62" s="91" t="s">
         <v>301</v>
       </c>
-      <c r="C61" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="99" t="s">
+      <c r="C62" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="85" t="s">
         <v>302</v>
       </c>
-      <c r="E61" s="99"/>
-    </row>
-    <row r="62" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="97"/>
-      <c r="B62" s="98" t="s">
+      <c r="E62" s="85"/>
+    </row>
+    <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="90"/>
+      <c r="B63" s="91" t="s">
         <v>303</v>
       </c>
-      <c r="C62" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="99" t="s">
+      <c r="C63" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D63" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="E62" s="99"/>
-    </row>
-    <row r="63" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="97"/>
-      <c r="B63" s="98" t="s">
+      <c r="E63" s="85"/>
+    </row>
+    <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="90"/>
+      <c r="B64" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="C63" s="99" t="s">
+      <c r="C64" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D63" s="99" t="s">
+      <c r="D64" s="85" t="s">
         <v>306</v>
       </c>
-      <c r="E63" s="99"/>
-    </row>
-    <row r="64" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
-      <c r="B64" s="98" t="s">
+      <c r="E64" s="85"/>
+    </row>
+    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="90"/>
+      <c r="B65" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="C64" s="99" t="s">
+      <c r="C65" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="99" t="s">
+      <c r="D65" s="85" t="s">
         <v>308</v>
       </c>
-      <c r="E64" s="99"/>
-    </row>
-    <row r="65" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
-      <c r="B65" s="98" t="s">
+      <c r="E65" s="85"/>
+    </row>
+    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="90"/>
+      <c r="B66" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="C65" s="99" t="s">
+      <c r="C66" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D65" s="99" t="s">
+      <c r="D66" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="E65" s="99"/>
-    </row>
-    <row r="66" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
-      <c r="B66" s="98" t="s">
+      <c r="E66" s="85"/>
+    </row>
+    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="90"/>
+      <c r="B67" s="91" t="s">
         <v>311</v>
       </c>
-      <c r="C66" s="99" t="s">
+      <c r="C67" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D66" s="99" t="s">
+      <c r="D67" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="E66" s="99"/>
-    </row>
-    <row r="67" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
-      <c r="B67" s="98" t="s">
+      <c r="E67" s="85"/>
+    </row>
+    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="90"/>
+      <c r="B68" s="91" t="s">
         <v>313</v>
       </c>
-      <c r="C67" s="99" t="s">
+      <c r="C68" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D67" s="99" t="s">
+      <c r="D68" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="E67" s="99"/>
-    </row>
-    <row r="68" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
-      <c r="B68" s="98" t="s">
+      <c r="E68" s="85"/>
+    </row>
+    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="90"/>
+      <c r="B69" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="C68" s="99" t="s">
+      <c r="C69" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D68" s="99" t="s">
+      <c r="D69" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="E68" s="99"/>
-    </row>
-    <row r="69" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="97"/>
-      <c r="B69" s="98" t="s">
+      <c r="E69" s="85"/>
+    </row>
+    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="90"/>
+      <c r="B70" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="C69" s="99" t="s">
+      <c r="C70" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D69" s="99" t="s">
+      <c r="D70" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="E69" s="99"/>
-    </row>
-    <row r="70" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
-      <c r="B70" s="98" t="s">
+      <c r="E70" s="85"/>
+    </row>
+    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="90"/>
+      <c r="B71" s="91" t="s">
         <v>319</v>
       </c>
-      <c r="C70" s="99" t="s">
+      <c r="C71" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D70" s="99" t="s">
+      <c r="D71" s="85" t="s">
         <v>320</v>
       </c>
-      <c r="E70" s="99"/>
-    </row>
-    <row r="71" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
-      <c r="B71" s="98" t="s">
+      <c r="E71" s="85"/>
+    </row>
+    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="90"/>
+      <c r="B72" s="91" t="s">
         <v>321</v>
       </c>
-      <c r="C71" s="99" t="s">
+      <c r="C72" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D71" s="99" t="s">
+      <c r="D72" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="E71" s="99"/>
-    </row>
-    <row r="72" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="97"/>
-      <c r="B72" s="98" t="s">
+      <c r="E72" s="85"/>
+    </row>
+    <row r="73" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="90"/>
+      <c r="B73" s="91" t="s">
         <v>323</v>
       </c>
-      <c r="C72" s="99" t="s">
+      <c r="C73" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D72" s="99" t="s">
+      <c r="D73" s="85" t="s">
         <v>324</v>
       </c>
-      <c r="E72" s="99"/>
-    </row>
-    <row r="73" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="97"/>
-      <c r="B73" s="98" t="s">
+      <c r="E73" s="85"/>
+    </row>
+    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="90"/>
+      <c r="B74" s="91" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="99" t="s">
+      <c r="C74" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D73" s="99" t="s">
+      <c r="D74" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="99"/>
-    </row>
-    <row r="74" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="97"/>
-      <c r="B74" s="98" t="s">
+      <c r="E74" s="85"/>
+    </row>
+    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="90"/>
+      <c r="B75" s="91" t="s">
         <v>327</v>
       </c>
-      <c r="C74" s="99" t="s">
+      <c r="C75" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D74" s="99" t="s">
+      <c r="D75" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="E74" s="99"/>
-    </row>
-    <row r="75" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="97"/>
-      <c r="B75" s="98" t="s">
+      <c r="E75" s="85"/>
+    </row>
+    <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="90"/>
+      <c r="B76" s="91" t="s">
         <v>328</v>
       </c>
-      <c r="C75" s="99" t="s">
+      <c r="C76" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D75" s="99" t="s">
+      <c r="D76" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="E75" s="99"/>
-    </row>
-    <row r="76" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="97"/>
-      <c r="B76" s="98" t="s">
+      <c r="E76" s="85"/>
+    </row>
+    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="90"/>
+      <c r="B77" s="91" t="s">
         <v>330</v>
       </c>
-      <c r="C76" s="99" t="s">
+      <c r="C77" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D76" s="99" t="s">
+      <c r="D77" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="E76" s="99"/>
-    </row>
-    <row r="77" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="97"/>
-      <c r="B77" s="98" t="s">
+      <c r="E77" s="85"/>
+    </row>
+    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="90"/>
+      <c r="B78" s="91" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="99" t="s">
+      <c r="C78" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D77" s="99" t="s">
+      <c r="D78" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="E77" s="99"/>
-    </row>
-    <row r="78" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="97"/>
-      <c r="B78" s="98" t="s">
+      <c r="E78" s="85"/>
+    </row>
+    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="90"/>
+      <c r="B79" s="91" t="s">
         <v>334</v>
       </c>
-      <c r="C78" s="99" t="s">
+      <c r="C79" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="99" t="s">
+      <c r="D79" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="E78" s="99"/>
-    </row>
-    <row r="79" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="97"/>
-      <c r="B79" s="98" t="s">
+      <c r="E79" s="85"/>
+    </row>
+    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="90"/>
+      <c r="B80" s="91" t="s">
         <v>336</v>
       </c>
-      <c r="C79" s="99" t="s">
+      <c r="C80" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D79" s="99" t="s">
+      <c r="D80" s="85" t="s">
         <v>337</v>
       </c>
-      <c r="E79" s="99"/>
-    </row>
-    <row r="80" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="97"/>
-      <c r="B80" s="98" t="s">
+      <c r="E80" s="85"/>
+    </row>
+    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="90"/>
+      <c r="B81" s="91" t="s">
         <v>338</v>
       </c>
-      <c r="C80" s="99" t="s">
+      <c r="C81" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D80" s="99" t="s">
+      <c r="D81" s="85" t="s">
         <v>340</v>
       </c>
-      <c r="E80" s="99"/>
-    </row>
-    <row r="81" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="97"/>
-      <c r="B81" s="98" t="s">
+      <c r="E81" s="85"/>
+    </row>
+    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="90"/>
+      <c r="B82" s="91" t="s">
         <v>341</v>
       </c>
-      <c r="C81" s="99" t="s">
+      <c r="C82" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D81" s="99" t="s">
+      <c r="D82" s="85" t="s">
         <v>342</v>
       </c>
-      <c r="E81" s="99"/>
-    </row>
-    <row r="82" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="97"/>
-      <c r="B82" s="98" t="s">
+      <c r="E82" s="85"/>
+    </row>
+    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="90"/>
+      <c r="B83" s="91" t="s">
         <v>343</v>
       </c>
-      <c r="C82" s="99" t="s">
+      <c r="C83" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D82" s="99" t="s">
+      <c r="D83" s="85" t="s">
         <v>344</v>
       </c>
-      <c r="E82" s="99"/>
-    </row>
-    <row r="83" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="97"/>
-      <c r="B83" s="98" t="s">
+      <c r="E83" s="85"/>
+    </row>
+    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="90"/>
+      <c r="B84" s="91" t="s">
         <v>345</v>
       </c>
-      <c r="C83" s="99" t="s">
+      <c r="C84" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D83" s="99" t="s">
+      <c r="D84" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="E83" s="99"/>
-    </row>
-    <row r="84" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="97"/>
-      <c r="B84" s="98" t="s">
+      <c r="E84" s="85"/>
+    </row>
+    <row r="85" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="90"/>
+      <c r="B85" s="91" t="s">
         <v>346</v>
       </c>
-      <c r="C84" s="99" t="s">
+      <c r="C85" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D84" s="99" t="s">
+      <c r="D85" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E84" s="99"/>
-    </row>
-    <row r="85" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="97"/>
-      <c r="B85" s="98" t="s">
+      <c r="E85" s="85"/>
+    </row>
+    <row r="86" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="90"/>
+      <c r="B86" s="91" t="s">
         <v>347</v>
       </c>
-      <c r="C85" s="99" t="s">
+      <c r="C86" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D85" s="99" t="s">
+      <c r="D86" s="85" t="s">
         <v>349</v>
       </c>
-      <c r="E85" s="99" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="97"/>
-      <c r="B86" s="98" t="s">
-        <v>350</v>
-      </c>
-      <c r="C86" s="99" t="s">
-        <v>348</v>
-      </c>
-      <c r="D86" s="99" t="s">
-        <v>351</v>
-      </c>
-      <c r="E86" s="99" t="s">
+      <c r="E86" s="85" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="90"/>
       <c r="B87" s="91" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C87" s="85" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D87" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="E87" s="96" t="s">
-        <v>393</v>
+        <v>351</v>
+      </c>
+      <c r="E87" s="85" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="90"/>
       <c r="B88" s="91" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C88" s="85" t="s">
         <v>352</v>
       </c>
       <c r="D88" s="85" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="E88" s="96" t="s">
         <v>393</v>
@@ -7088,13 +7080,13 @@
     <row r="89" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="90"/>
       <c r="B89" s="91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C89" s="85" t="s">
         <v>352</v>
       </c>
       <c r="D89" s="85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E89" s="96" t="s">
         <v>393</v>
@@ -7103,13 +7095,13 @@
     <row r="90" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="90"/>
       <c r="B90" s="91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C90" s="85" t="s">
         <v>352</v>
       </c>
       <c r="D90" s="85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E90" s="96" t="s">
         <v>393</v>
@@ -7118,13 +7110,13 @@
     <row r="91" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="90"/>
       <c r="B91" s="91" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C91" s="85" t="s">
         <v>352</v>
       </c>
       <c r="D91" s="85" t="s">
-        <v>358</v>
+        <v>82</v>
       </c>
       <c r="E91" s="96" t="s">
         <v>393</v>
@@ -7133,918 +7125,955 @@
     <row r="92" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="90"/>
       <c r="B92" s="91" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C92" s="85" t="s">
         <v>352</v>
       </c>
       <c r="D92" s="85" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E92" s="96" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="97"/>
-      <c r="B93" s="98" t="s">
+    <row r="93" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="90"/>
+      <c r="B93" s="91" t="s">
+        <v>360</v>
+      </c>
+      <c r="C93" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="D93" s="85" t="s">
+        <v>361</v>
+      </c>
+      <c r="E93" s="96" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="90"/>
+      <c r="B94" s="91" t="s">
         <v>363</v>
       </c>
-      <c r="C93" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="99" t="s">
+      <c r="C94" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="85" t="s">
         <v>364</v>
       </c>
-      <c r="E93" s="99"/>
-    </row>
-    <row r="94" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="97"/>
-      <c r="B94" s="98" t="s">
+      <c r="E94" s="85"/>
+    </row>
+    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="90"/>
+      <c r="B95" s="91" t="s">
         <v>365</v>
       </c>
-      <c r="C94" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="99" t="s">
+      <c r="C95" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="85" t="s">
         <v>454</v>
       </c>
-      <c r="E94" s="99"/>
-    </row>
-    <row r="95" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="97"/>
-      <c r="B95" s="98" t="s">
+      <c r="E95" s="85"/>
+    </row>
+    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="90"/>
+      <c r="B96" s="91" t="s">
         <v>366</v>
       </c>
-      <c r="C95" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="99" t="s">
+      <c r="C96" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="E95" s="99"/>
-    </row>
-    <row r="96" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="97"/>
-      <c r="B96" s="98" t="s">
+      <c r="E96" s="85"/>
+    </row>
+    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="90"/>
+      <c r="B97" s="91" t="s">
         <v>368</v>
       </c>
-      <c r="C96" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="99" t="s">
+      <c r="C97" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="E96" s="99"/>
-    </row>
-    <row r="97" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="97"/>
-      <c r="B97" s="98" t="s">
+      <c r="E97" s="85"/>
+    </row>
+    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="90"/>
+      <c r="B98" s="91" t="s">
         <v>370</v>
       </c>
-      <c r="C97" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="99" t="s">
+      <c r="C98" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="E97" s="99"/>
-    </row>
-    <row r="98" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="97"/>
-      <c r="B98" s="98" t="s">
+      <c r="E98" s="85"/>
+    </row>
+    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="90"/>
+      <c r="B99" s="91" t="s">
         <v>372</v>
       </c>
-      <c r="C98" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="99" t="s">
+      <c r="C99" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="85" t="s">
         <v>373</v>
       </c>
-      <c r="E98" s="99"/>
-    </row>
-    <row r="99" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="97"/>
-      <c r="B99" s="98" t="s">
+      <c r="E99" s="85"/>
+    </row>
+    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="90"/>
+      <c r="B100" s="91" t="s">
         <v>374</v>
       </c>
-      <c r="C99" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="99" t="s">
+      <c r="C100" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="E99" s="99"/>
-    </row>
-    <row r="100" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="97"/>
-      <c r="B100" s="98" t="s">
+      <c r="E100" s="85"/>
+    </row>
+    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="90"/>
+      <c r="B101" s="91" t="s">
         <v>378</v>
       </c>
-      <c r="C100" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="99" t="s">
+      <c r="C101" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="85" t="s">
         <v>379</v>
       </c>
-      <c r="E100" s="99"/>
-    </row>
-    <row r="101" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="97"/>
-      <c r="B101" s="98" t="s">
+      <c r="E101" s="85"/>
+    </row>
+    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="90"/>
+      <c r="B102" s="91" t="s">
         <v>380</v>
       </c>
-      <c r="C101" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="99" t="s">
+      <c r="C102" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="85" t="s">
         <v>381</v>
       </c>
-      <c r="E101" s="99"/>
-    </row>
-    <row r="102" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="97"/>
-      <c r="B102" s="98" t="s">
+      <c r="E102" s="85"/>
+    </row>
+    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="90"/>
+      <c r="B103" s="91" t="s">
         <v>382</v>
       </c>
-      <c r="C102" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="99" t="s">
+      <c r="C103" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="85" t="s">
         <v>383</v>
       </c>
-      <c r="E102" s="99"/>
-    </row>
-    <row r="103" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="97"/>
-      <c r="B103" s="98" t="s">
+      <c r="E103" s="85"/>
+    </row>
+    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="90"/>
+      <c r="B104" s="91" t="s">
         <v>384</v>
       </c>
-      <c r="C103" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="99" t="s">
+      <c r="C104" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="85" t="s">
         <v>455</v>
       </c>
-      <c r="E103" s="99"/>
-    </row>
-    <row r="104" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="97"/>
-      <c r="B104" s="98" t="s">
+      <c r="E104" s="85"/>
+    </row>
+    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="90"/>
+      <c r="B105" s="91" t="s">
         <v>385</v>
       </c>
-      <c r="C104" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="99" t="s">
+      <c r="C105" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="85" t="s">
         <v>456</v>
       </c>
-      <c r="E104" s="99"/>
-    </row>
-    <row r="105" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="97"/>
-      <c r="B105" s="98" t="s">
+      <c r="E105" s="85"/>
+    </row>
+    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="90"/>
+      <c r="B106" s="91" t="s">
         <v>386</v>
       </c>
-      <c r="C105" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="99" t="s">
+      <c r="C106" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="85" t="s">
         <v>457</v>
       </c>
-      <c r="E105" s="99"/>
-    </row>
-    <row r="106" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="97"/>
-      <c r="B106" s="98" t="s">
+      <c r="E106" s="85"/>
+    </row>
+    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="90"/>
+      <c r="B107" s="91" t="s">
         <v>387</v>
       </c>
-      <c r="C106" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="99" t="s">
+      <c r="C107" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="85" t="s">
         <v>388</v>
       </c>
-      <c r="E106" s="99"/>
-    </row>
-    <row r="107" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="97"/>
-      <c r="B107" s="98" t="s">
+      <c r="E107" s="85"/>
+    </row>
+    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="90"/>
+      <c r="B108" s="91" t="s">
         <v>389</v>
       </c>
-      <c r="C107" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="99" t="s">
+      <c r="C108" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="85" t="s">
         <v>390</v>
       </c>
-      <c r="E107" s="99"/>
-    </row>
-    <row r="108" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="97"/>
-      <c r="B108" s="98" t="s">
+      <c r="E108" s="85"/>
+    </row>
+    <row r="109" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="90"/>
+      <c r="B109" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="99" t="s">
+      <c r="C109" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="85" t="s">
         <v>391</v>
       </c>
-      <c r="E108" s="99"/>
-    </row>
-    <row r="109" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="97"/>
-      <c r="B109" s="98" t="s">
+      <c r="E109" s="85"/>
+    </row>
+    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="90"/>
+      <c r="B110" s="91" t="s">
         <v>392</v>
       </c>
-      <c r="C109" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="99" t="s">
+      <c r="C110" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D110" s="85" t="s">
         <v>459</v>
       </c>
-      <c r="E109" s="99"/>
-    </row>
-    <row r="110" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="97"/>
-      <c r="B110" s="98" t="s">
+      <c r="E110" s="85"/>
+    </row>
+    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="90"/>
+      <c r="B111" s="91" t="s">
         <v>376</v>
       </c>
-      <c r="C110" s="99" t="s">
+      <c r="C111" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D110" s="99" t="s">
+      <c r="D111" s="85" t="s">
         <v>394</v>
       </c>
-      <c r="E110" s="99"/>
-    </row>
-    <row r="111" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="97"/>
-      <c r="B111" s="98" t="s">
+      <c r="E111" s="85"/>
+    </row>
+    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="90"/>
+      <c r="B112" s="91" t="s">
         <v>377</v>
       </c>
-      <c r="C111" s="99" t="s">
+      <c r="C112" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D111" s="99" t="s">
+      <c r="D112" s="85" t="s">
         <v>474</v>
       </c>
-      <c r="E111" s="99"/>
-    </row>
-    <row r="112" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="97"/>
-      <c r="B112" s="98" t="s">
+      <c r="E112" s="85"/>
+    </row>
+    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="90"/>
+      <c r="B113" s="91" t="s">
         <v>395</v>
       </c>
-      <c r="C112" s="99" t="s">
+      <c r="C113" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D112" s="99" t="s">
+      <c r="D113" s="85" t="s">
         <v>476</v>
       </c>
-      <c r="E112" s="99"/>
-    </row>
-    <row r="113" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="97"/>
-      <c r="B113" s="98" t="s">
+      <c r="E113" s="85"/>
+    </row>
+    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="90"/>
+      <c r="B114" s="91" t="s">
         <v>396</v>
       </c>
-      <c r="C113" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="99" t="s">
+      <c r="C114" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D114" s="85" t="s">
         <v>397</v>
       </c>
-      <c r="E113" s="99"/>
-    </row>
-    <row r="114" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="97"/>
-      <c r="B114" s="98" t="s">
+      <c r="E114" s="85"/>
+    </row>
+    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="90"/>
+      <c r="B115" s="91" t="s">
         <v>398</v>
       </c>
-      <c r="C114" s="99" t="s">
+      <c r="C115" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D114" s="99" t="s">
+      <c r="D115" s="85" t="s">
         <v>399</v>
       </c>
-      <c r="E114" s="99"/>
-    </row>
-    <row r="115" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="97"/>
-      <c r="B115" s="98" t="s">
-        <v>400</v>
-      </c>
-      <c r="C115" s="99" t="s">
-        <v>279</v>
-      </c>
-      <c r="D115" s="99" t="s">
-        <v>401</v>
-      </c>
-      <c r="E115" s="99"/>
+      <c r="E115" s="85"/>
     </row>
     <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="90"/>
       <c r="B116" s="91" t="s">
+        <v>400</v>
+      </c>
+      <c r="C116" s="85" t="s">
+        <v>279</v>
+      </c>
+      <c r="D116" s="85" t="s">
+        <v>401</v>
+      </c>
+      <c r="E116" s="85"/>
+    </row>
+    <row r="117" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="90"/>
+      <c r="B117" s="91" t="s">
         <v>402</v>
       </c>
-      <c r="C116" s="85" t="s">
+      <c r="C117" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D116" s="85" t="s">
+      <c r="D117" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="E116" s="85"/>
-    </row>
-    <row r="117" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="97"/>
-      <c r="B117" s="98" t="s">
+      <c r="E117" s="85"/>
+    </row>
+    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="90"/>
+      <c r="B118" s="91" t="s">
         <v>404</v>
       </c>
-      <c r="C117" s="99" t="s">
+      <c r="C118" s="85" t="s">
         <v>279</v>
       </c>
-      <c r="D117" s="99" t="s">
+      <c r="D118" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="E117" s="99"/>
-    </row>
-    <row r="118" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="97"/>
-      <c r="B118" s="98" t="s">
+      <c r="E118" s="85"/>
+    </row>
+    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="90"/>
+      <c r="B119" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="C118" s="99" t="s">
+      <c r="C119" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D118" s="99" t="s">
+      <c r="D119" s="85" t="s">
         <v>407</v>
       </c>
-      <c r="E118" s="99"/>
-    </row>
-    <row r="119" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="97"/>
-      <c r="B119" s="98" t="s">
+      <c r="E119" s="85"/>
+    </row>
+    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="90"/>
+      <c r="B120" s="91" t="s">
         <v>408</v>
       </c>
-      <c r="C119" s="99" t="s">
+      <c r="C120" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D119" s="99" t="s">
+      <c r="D120" s="85" t="s">
         <v>409</v>
       </c>
-      <c r="E119" s="99"/>
-    </row>
-    <row r="120" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="97"/>
-      <c r="B120" s="98" t="s">
+      <c r="E120" s="85"/>
+    </row>
+    <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="90"/>
+      <c r="B121" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="C120" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D120" s="99" t="s">
+      <c r="C121" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D121" s="85" t="s">
         <v>410</v>
       </c>
-      <c r="E120" s="99"/>
-    </row>
-    <row r="121" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="97"/>
-      <c r="B121" s="98" t="s">
+      <c r="E121" s="85"/>
+    </row>
+    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="90"/>
+      <c r="B122" s="91" t="s">
         <v>411</v>
       </c>
-      <c r="C121" s="99" t="s">
+      <c r="C122" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D121" s="99" t="s">
+      <c r="D122" s="85" t="s">
         <v>413</v>
       </c>
-      <c r="E121" s="99"/>
-    </row>
-    <row r="122" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="97"/>
-      <c r="B122" s="98" t="s">
+      <c r="E122" s="85"/>
+    </row>
+    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="90"/>
+      <c r="B123" s="91" t="s">
         <v>412</v>
       </c>
-      <c r="C122" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D122" s="99" t="s">
+      <c r="C123" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="85" t="s">
         <v>414</v>
       </c>
-      <c r="E122" s="99"/>
-    </row>
-    <row r="123" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="97"/>
-      <c r="B123" s="98" t="s">
+      <c r="E123" s="85"/>
+    </row>
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="90"/>
+      <c r="B124" s="91" t="s">
         <v>415</v>
       </c>
-      <c r="C123" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="99" t="s">
+      <c r="C124" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="85" t="s">
         <v>416</v>
       </c>
-      <c r="E123" s="99"/>
-    </row>
-    <row r="124" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="97"/>
-      <c r="B124" s="98" t="s">
+      <c r="E124" s="85"/>
+    </row>
+    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="90"/>
+      <c r="B125" s="91" t="s">
         <v>417</v>
       </c>
-      <c r="C124" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="99" t="s">
+      <c r="C125" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="85" t="s">
         <v>418</v>
       </c>
-      <c r="E124" s="99"/>
-    </row>
-    <row r="125" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="97"/>
-      <c r="B125" s="98" t="s">
+      <c r="E125" s="85"/>
+    </row>
+    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="90"/>
+      <c r="B126" s="91" t="s">
         <v>419</v>
       </c>
-      <c r="C125" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="99" t="s">
+      <c r="C126" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="85" t="s">
         <v>463</v>
       </c>
-      <c r="E125" s="99"/>
-    </row>
-    <row r="126" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="97"/>
-      <c r="B126" s="98" t="s">
+      <c r="E126" s="85"/>
+    </row>
+    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="90"/>
+      <c r="B127" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="C126" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="99" t="s">
+      <c r="C127" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="E126" s="99"/>
-    </row>
-    <row r="127" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="97"/>
-      <c r="B127" s="98" t="s">
+      <c r="E127" s="85"/>
+    </row>
+    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="90"/>
+      <c r="B128" s="91" t="s">
         <v>422</v>
       </c>
-      <c r="C127" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="99" t="s">
+      <c r="C128" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="85" t="s">
         <v>423</v>
       </c>
-      <c r="E127" s="99"/>
-    </row>
-    <row r="128" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="97"/>
-      <c r="B128" s="98" t="s">
+      <c r="E128" s="85"/>
+    </row>
+    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="90"/>
+      <c r="B129" s="91" t="s">
         <v>424</v>
       </c>
-      <c r="C128" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="99" t="s">
+      <c r="C129" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="85" t="s">
         <v>425</v>
       </c>
-      <c r="E128" s="99"/>
-    </row>
-    <row r="129" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="97"/>
-      <c r="B129" s="98" t="s">
+      <c r="E129" s="85"/>
+    </row>
+    <row r="130" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="90"/>
+      <c r="B130" s="91" t="s">
         <v>189</v>
       </c>
-      <c r="C129" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="99" t="s">
+      <c r="C130" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="85" t="s">
         <v>426</v>
       </c>
-      <c r="E129" s="99"/>
-    </row>
-    <row r="130" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="97"/>
-      <c r="B130" s="98" t="s">
+      <c r="E130" s="85"/>
+    </row>
+    <row r="131" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="90"/>
+      <c r="B131" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="C130" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="99" t="s">
+      <c r="C131" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="85" t="s">
         <v>298</v>
       </c>
-      <c r="E130" s="99"/>
-    </row>
-    <row r="131" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="97"/>
-      <c r="B131" s="98" t="s">
+      <c r="E131" s="85"/>
+    </row>
+    <row r="132" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="90"/>
+      <c r="B132" s="91" t="s">
         <v>427</v>
       </c>
-      <c r="C131" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="99" t="s">
+      <c r="C132" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="85" t="s">
         <v>428</v>
       </c>
-      <c r="E131" s="99"/>
-    </row>
-    <row r="132" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="97"/>
-      <c r="B132" s="98" t="s">
+      <c r="E132" s="85"/>
+    </row>
+    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="90"/>
+      <c r="B133" s="91" t="s">
         <v>429</v>
       </c>
-      <c r="C132" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="99" t="s">
+      <c r="C133" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="E132" s="99"/>
-    </row>
-    <row r="133" spans="1:5" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="97"/>
-      <c r="B133" s="98" t="s">
+      <c r="E133" s="85"/>
+    </row>
+    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="90"/>
+      <c r="B134" s="91" t="s">
         <v>431</v>
       </c>
-      <c r="C133" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="99" t="s">
+      <c r="C134" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D134" s="85" t="s">
         <v>465</v>
       </c>
-      <c r="E133" s="99"/>
-    </row>
-    <row r="134" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="97"/>
-      <c r="B134" s="98" t="s">
+      <c r="E134" s="85"/>
+    </row>
+    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="90"/>
+      <c r="B135" s="91" t="s">
         <v>432</v>
       </c>
-      <c r="C134" s="99" t="s">
+      <c r="C135" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="D134" s="99" t="s">
+      <c r="D135" s="85" t="s">
         <v>433</v>
       </c>
-      <c r="E134" s="99"/>
-    </row>
-    <row r="135" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="97"/>
-      <c r="B135" s="98" t="s">
+      <c r="E135" s="85"/>
+    </row>
+    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="90"/>
+      <c r="B136" s="91" t="s">
         <v>434</v>
       </c>
-      <c r="C135" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D135" s="99" t="s">
+      <c r="C136" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="E135" s="99"/>
-    </row>
-    <row r="136" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="97"/>
-      <c r="B136" s="98" t="s">
+      <c r="E136" s="85"/>
+    </row>
+    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="90"/>
+      <c r="B137" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="C136" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="99" t="s">
+      <c r="C137" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="85" t="s">
         <v>468</v>
       </c>
-      <c r="E136" s="99"/>
-    </row>
-    <row r="137" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="97"/>
-      <c r="B137" s="98" t="s">
+      <c r="E137" s="85"/>
+    </row>
+    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="90"/>
+      <c r="B138" s="91" t="s">
         <v>437</v>
       </c>
-      <c r="C137" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="99" t="s">
+      <c r="C138" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="85" t="s">
         <v>467</v>
       </c>
-      <c r="E137" s="99"/>
-    </row>
-    <row r="138" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="97"/>
-      <c r="B138" s="98" t="s">
+      <c r="E138" s="85"/>
+    </row>
+    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="90"/>
+      <c r="B139" s="91" t="s">
         <v>438</v>
       </c>
-      <c r="C138" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="99" t="s">
+      <c r="C139" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="85" t="s">
         <v>439</v>
       </c>
-      <c r="E138" s="99"/>
-    </row>
-    <row r="139" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="97"/>
-      <c r="B139" s="98" t="s">
+      <c r="E139" s="85"/>
+    </row>
+    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="90"/>
+      <c r="B140" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="C139" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="99" t="s">
+      <c r="C140" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D140" s="85" t="s">
         <v>469</v>
       </c>
-      <c r="E139" s="99"/>
-    </row>
-    <row r="140" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="97"/>
-      <c r="B140" s="98" t="s">
+      <c r="E140" s="85"/>
+    </row>
+    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="90"/>
+      <c r="B141" s="91" t="s">
         <v>441</v>
       </c>
-      <c r="C140" s="99" t="s">
+      <c r="C141" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="D140" s="99" t="s">
+      <c r="D141" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="E140" s="99"/>
-    </row>
-    <row r="141" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="97"/>
-      <c r="B141" s="98" t="s">
-        <v>460</v>
-      </c>
-      <c r="C141" s="99" t="s">
-        <v>272</v>
-      </c>
-      <c r="D141" s="99" t="s">
-        <v>461</v>
-      </c>
-      <c r="E141" s="99"/>
+      <c r="E141" s="85"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="90"/>
       <c r="B142" s="91" t="s">
+        <v>460</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>272</v>
+      </c>
+      <c r="D142" s="85" t="s">
+        <v>461</v>
+      </c>
+      <c r="E142" s="85"/>
+    </row>
+    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="90"/>
+      <c r="B143" s="91" t="s">
         <v>471</v>
       </c>
-      <c r="C142" s="85" t="s">
+      <c r="C143" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="D142" s="85" t="s">
+      <c r="D143" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="E142" s="85"/>
-    </row>
-    <row r="143" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="97"/>
-      <c r="B143" s="98" t="s">
+      <c r="E143" s="85"/>
+    </row>
+    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="90"/>
+      <c r="B144" s="91" t="s">
         <v>478</v>
       </c>
-      <c r="C143" s="99" t="s">
+      <c r="C144" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D143" s="99" t="s">
+      <c r="D144" s="85" t="s">
         <v>479</v>
       </c>
-      <c r="E143" s="99"/>
-    </row>
-    <row r="144" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="97"/>
-      <c r="B144" s="98" t="s">
+      <c r="E144" s="85"/>
+    </row>
+    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="90"/>
+      <c r="B145" s="91" t="s">
         <v>481</v>
       </c>
-      <c r="C144" s="99" t="s">
+      <c r="C145" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D144" s="99" t="s">
+      <c r="D145" s="85" t="s">
         <v>482</v>
       </c>
-      <c r="E144" s="99"/>
-    </row>
-    <row r="145" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="97"/>
-      <c r="B145" s="98" t="s">
+      <c r="E145" s="85"/>
+    </row>
+    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="90"/>
+      <c r="B146" s="91" t="s">
         <v>483</v>
       </c>
-      <c r="C145" s="99" t="s">
+      <c r="C146" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D145" s="99" t="s">
+      <c r="D146" s="85" t="s">
         <v>484</v>
       </c>
-      <c r="E145" s="99"/>
-    </row>
-    <row r="146" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="109"/>
-      <c r="B146" s="110" t="s">
+      <c r="E146" s="85"/>
+    </row>
+    <row r="147" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="105"/>
+      <c r="B147" s="106" t="s">
         <v>485</v>
       </c>
-      <c r="C146" s="111" t="s">
+      <c r="C147" s="107" t="s">
         <v>339</v>
       </c>
-      <c r="D146" s="111" t="s">
+      <c r="D147" s="107" t="s">
         <v>486</v>
       </c>
-      <c r="E146" s="111"/>
-    </row>
-    <row r="147" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="97"/>
-      <c r="B147" s="98" t="s">
+      <c r="E147" s="107"/>
+    </row>
+    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="90"/>
+      <c r="B148" s="91" t="s">
         <v>487</v>
       </c>
-      <c r="C147" s="99" t="s">
+      <c r="C148" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D147" s="99" t="s">
+      <c r="D148" s="85" t="s">
         <v>488</v>
       </c>
-      <c r="E147" s="99"/>
-    </row>
-    <row r="148" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="97"/>
-      <c r="B148" s="98" t="s">
+      <c r="E148" s="85"/>
+    </row>
+    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="90"/>
+      <c r="B149" s="91" t="s">
         <v>490</v>
       </c>
-      <c r="C148" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D148" s="99" t="s">
+      <c r="C149" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="85" t="s">
         <v>491</v>
       </c>
-      <c r="E148" s="99"/>
-    </row>
-    <row r="149" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="97"/>
-      <c r="B149" s="98" t="s">
+      <c r="E149" s="85"/>
+    </row>
+    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="90"/>
+      <c r="B150" s="91" t="s">
         <v>492</v>
       </c>
-      <c r="C149" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="99" t="s">
+      <c r="C150" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D150" s="85" t="s">
         <v>493</v>
       </c>
-      <c r="E149" s="99"/>
-    </row>
-    <row r="150" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="97"/>
-      <c r="B150" s="98" t="s">
-        <v>495</v>
-      </c>
-      <c r="C150" s="99" t="s">
-        <v>339</v>
-      </c>
-      <c r="D150" s="99" t="s">
-        <v>494</v>
-      </c>
-      <c r="E150" s="99"/>
+      <c r="E150" s="85"/>
     </row>
     <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="90"/>
       <c r="B151" s="91" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C151" s="85" t="s">
         <v>339</v>
       </c>
       <c r="D151" s="85" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E151" s="85"/>
     </row>
     <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="90"/>
       <c r="B152" s="91" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C152" s="85" t="s">
         <v>339</v>
       </c>
       <c r="D152" s="85" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="E152" s="85"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B153" s="83" t="s">
-        <v>499</v>
+    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="90"/>
+      <c r="B153" s="91" t="s">
+        <v>498</v>
       </c>
       <c r="C153" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D153" s="84" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="83" t="s">
-        <v>500</v>
+      <c r="D153" s="85" t="s">
+        <v>506</v>
+      </c>
+      <c r="E153" s="85"/>
+    </row>
+    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="90"/>
+      <c r="B154" s="91" t="s">
+        <v>499</v>
       </c>
       <c r="C154" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D154" s="84" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="83" t="s">
-        <v>501</v>
+      <c r="D154" s="85" t="s">
+        <v>507</v>
+      </c>
+      <c r="E154" s="85"/>
+    </row>
+    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="90"/>
+      <c r="B155" s="91" t="s">
+        <v>500</v>
       </c>
       <c r="C155" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D155" s="84" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="83" t="s">
-        <v>502</v>
+      <c r="D155" s="85" t="s">
+        <v>508</v>
+      </c>
+      <c r="E155" s="85"/>
+    </row>
+    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="90"/>
+      <c r="B156" s="91" t="s">
+        <v>501</v>
       </c>
       <c r="C156" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D156" s="84" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="83" t="s">
-        <v>503</v>
+      <c r="D156" s="85" t="s">
+        <v>509</v>
+      </c>
+      <c r="E156" s="85"/>
+    </row>
+    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="90"/>
+      <c r="B157" s="91" t="s">
+        <v>502</v>
       </c>
       <c r="C157" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D157" s="84" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B158" s="83" t="s">
-        <v>504</v>
+      <c r="D157" s="85" t="s">
+        <v>510</v>
+      </c>
+      <c r="E157" s="85"/>
+    </row>
+    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="90"/>
+      <c r="B158" s="91" t="s">
+        <v>503</v>
       </c>
       <c r="C158" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D158" s="84" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="83" t="s">
-        <v>505</v>
+      <c r="D158" s="85" t="s">
+        <v>511</v>
+      </c>
+      <c r="E158" s="85"/>
+    </row>
+    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="90"/>
+      <c r="B159" s="91" t="s">
+        <v>504</v>
       </c>
       <c r="C159" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D159" s="84" t="s">
+      <c r="D159" s="85" t="s">
+        <v>512</v>
+      </c>
+      <c r="E159" s="85"/>
+    </row>
+    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="90"/>
+      <c r="B160" s="91" t="s">
+        <v>505</v>
+      </c>
+      <c r="C160" s="85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D160" s="85" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B160" s="83" t="s">
+      <c r="E160" s="85"/>
+    </row>
+    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="90"/>
+      <c r="B161" s="91" t="s">
         <v>514</v>
       </c>
-      <c r="C160" s="84" t="s">
+      <c r="C161" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D160" s="84" t="s">
+      <c r="D161" s="85" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="83" t="s">
+      <c r="E161" s="85"/>
+    </row>
+    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="90"/>
+      <c r="B162" s="91" t="s">
         <v>516</v>
       </c>
-      <c r="C161" s="84" t="s">
+      <c r="C162" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D161" s="84" t="s">
+      <c r="D162" s="85" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="83" t="s">
+      <c r="E162" s="85"/>
+    </row>
+    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="90"/>
+      <c r="B163" s="91" t="s">
         <v>517</v>
       </c>
-      <c r="C162" s="84" t="s">
+      <c r="C163" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D162" s="84" t="s">
+      <c r="D163" s="85" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="83" t="s">
+      <c r="E163" s="85"/>
+    </row>
+    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="90"/>
+      <c r="B164" s="91" t="s">
         <v>518</v>
       </c>
-      <c r="C163" s="84" t="s">
+      <c r="C164" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="D163" s="84" t="s">
+      <c r="D164" s="85" t="s">
         <v>521</v>
       </c>
+      <c r="E164" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Actions Brainstorming Example
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A05792-6273-4567-8E60-8980A35EEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B46E9F-7B05-4B3C-8396-7D0329A65AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15450" windowHeight="15315" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="2340" yWindow="885" windowWidth="15450" windowHeight="15315" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="525">
   <si>
     <t>ID</t>
   </si>
@@ -1611,6 +1611,9 @@
   </si>
   <si>
     <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Actions Brainstorming Example Image</t>
   </si>
 </sst>
 </file>
@@ -2139,18 +2142,18 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2543,10 +2546,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="104"/>
+      <c r="H2" s="108"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5910,10 +5913,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7769,7 +7772,7 @@
         <v>441</v>
       </c>
       <c r="C141" s="85" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D141" s="85" t="s">
         <v>442</v>
@@ -7841,18 +7844,18 @@
       </c>
       <c r="E146" s="85"/>
     </row>
-    <row r="147" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="105"/>
-      <c r="B147" s="106" t="s">
+    <row r="147" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="103"/>
+      <c r="B147" s="104" t="s">
         <v>485</v>
       </c>
-      <c r="C147" s="107" t="s">
+      <c r="C147" s="105" t="s">
         <v>339</v>
       </c>
-      <c r="D147" s="107" t="s">
+      <c r="D147" s="105" t="s">
         <v>486</v>
       </c>
-      <c r="E147" s="107"/>
+      <c r="E147" s="105"/>
     </row>
     <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="90"/>
@@ -8074,6 +8077,17 @@
         <v>521</v>
       </c>
       <c r="E164" s="85"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="83" t="s">
+        <v>522</v>
+      </c>
+      <c r="C165" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D165" s="84" t="s">
+        <v>524</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Indicator cards list
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD57C1-6DAB-43F3-AE79-896E375E28F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A7E48-5A26-4706-B689-AE67048C2A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -5931,7 +5931,7 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B168" sqref="B168"/>
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adjusted scaling to fix window run off issue
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A7E48-5A26-4706-B689-AE67048C2A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C4F13D-0458-4DCA-8EBC-5B967220FCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -1967,7 +1967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2169,6 +2169,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5930,8 +5935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6309,44 +6314,44 @@
       </c>
       <c r="E28" s="85"/>
     </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91" t="s">
+    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="109"/>
+      <c r="B29" s="110" t="s">
         <v>276</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="111" t="s">
         <v>277</v>
       </c>
-      <c r="E29" s="85"/>
-    </row>
-    <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="90"/>
-      <c r="B30" s="91" t="s">
+      <c r="E29" s="111"/>
+    </row>
+    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="109"/>
+      <c r="B30" s="110" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="111" t="s">
         <v>233</v>
       </c>
-      <c r="E30" s="85"/>
-    </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="90"/>
-      <c r="B31" s="91" t="s">
+      <c r="E30" s="111"/>
+    </row>
+    <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="109"/>
+      <c r="B31" s="110" t="s">
         <v>280</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D31" s="85" t="s">
+      <c r="D31" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="85"/>
+      <c r="E31" s="111"/>
     </row>
     <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="90"/>
@@ -7456,18 +7461,18 @@
       </c>
       <c r="E115" s="85"/>
     </row>
-    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="90"/>
-      <c r="B116" s="91" t="s">
+    <row r="116" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="109"/>
+      <c r="B116" s="110" t="s">
         <v>400</v>
       </c>
-      <c r="C116" s="85" t="s">
+      <c r="C116" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D116" s="85" t="s">
+      <c r="D116" s="111" t="s">
         <v>401</v>
       </c>
-      <c r="E116" s="85"/>
+      <c r="E116" s="111"/>
     </row>
     <row r="117" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="90"/>
@@ -7482,18 +7487,18 @@
       </c>
       <c r="E117" s="85"/>
     </row>
-    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="90"/>
-      <c r="B118" s="91" t="s">
+    <row r="118" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="109"/>
+      <c r="B118" s="110" t="s">
         <v>404</v>
       </c>
-      <c r="C118" s="85" t="s">
+      <c r="C118" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D118" s="85" t="s">
+      <c r="D118" s="111" t="s">
         <v>405</v>
       </c>
-      <c r="E118" s="85"/>
+      <c r="E118" s="111"/>
     </row>
     <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="90"/>
@@ -7781,18 +7786,18 @@
       </c>
       <c r="E140" s="85"/>
     </row>
-    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="90"/>
-      <c r="B141" s="91" t="s">
+    <row r="141" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="109"/>
+      <c r="B141" s="110" t="s">
         <v>441</v>
       </c>
-      <c r="C141" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D141" s="85" t="s">
+      <c r="C141" s="111" t="s">
+        <v>279</v>
+      </c>
+      <c r="D141" s="111" t="s">
         <v>442</v>
       </c>
-      <c r="E141" s="85"/>
+      <c r="E141" s="111"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="90"/>

</xml_diff>

<commit_message>
Added content for new landing page headers and sub headers
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C4F13D-0458-4DCA-8EBC-5B967220FCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9532172-F2B3-4B22-BE5C-8CE0372CB4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="540">
   <si>
     <t>ID</t>
   </si>
@@ -1629,6 +1629,36 @@
   </si>
   <si>
     <t>169 Small</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>Quick Start Guide</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>Additional Resources</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>The 5 sections of ERB</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>The 5 sections of ERB image</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>How ERB centers equity</t>
   </si>
 </sst>
 </file>
@@ -2163,17 +2193,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2566,10 +2596,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="108"/>
+      <c r="H2" s="111"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5933,10 +5963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6315,43 +6345,43 @@
       <c r="E28" s="85"/>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
-      <c r="B29" s="110" t="s">
+      <c r="A29" s="107"/>
+      <c r="B29" s="108" t="s">
         <v>276</v>
       </c>
-      <c r="C29" s="111" t="s">
+      <c r="C29" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="109" t="s">
         <v>277</v>
       </c>
-      <c r="E29" s="111"/>
+      <c r="E29" s="109"/>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="109"/>
-      <c r="B30" s="110" t="s">
+      <c r="A30" s="107"/>
+      <c r="B30" s="108" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="111" t="s">
+      <c r="C30" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="111" t="s">
+      <c r="D30" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="E30" s="111"/>
+      <c r="E30" s="109"/>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="110" t="s">
+      <c r="A31" s="107"/>
+      <c r="B31" s="108" t="s">
         <v>280</v>
       </c>
-      <c r="C31" s="111" t="s">
+      <c r="C31" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D31" s="111" t="s">
+      <c r="D31" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="111"/>
+      <c r="E31" s="109"/>
     </row>
     <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="90"/>
@@ -7462,17 +7492,17 @@
       <c r="E115" s="85"/>
     </row>
     <row r="116" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="109"/>
-      <c r="B116" s="110" t="s">
+      <c r="A116" s="107"/>
+      <c r="B116" s="108" t="s">
         <v>400</v>
       </c>
-      <c r="C116" s="111" t="s">
+      <c r="C116" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D116" s="111" t="s">
+      <c r="D116" s="109" t="s">
         <v>401</v>
       </c>
-      <c r="E116" s="111"/>
+      <c r="E116" s="109"/>
     </row>
     <row r="117" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="90"/>
@@ -7488,17 +7518,17 @@
       <c r="E117" s="85"/>
     </row>
     <row r="118" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="109"/>
-      <c r="B118" s="110" t="s">
+      <c r="A118" s="107"/>
+      <c r="B118" s="108" t="s">
         <v>404</v>
       </c>
-      <c r="C118" s="111" t="s">
+      <c r="C118" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D118" s="111" t="s">
+      <c r="D118" s="109" t="s">
         <v>405</v>
       </c>
-      <c r="E118" s="111"/>
+      <c r="E118" s="109"/>
     </row>
     <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="90"/>
@@ -7787,17 +7817,17 @@
       <c r="E140" s="85"/>
     </row>
     <row r="141" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="109"/>
-      <c r="B141" s="110" t="s">
+      <c r="A141" s="107"/>
+      <c r="B141" s="108" t="s">
         <v>441</v>
       </c>
-      <c r="C141" s="111" t="s">
+      <c r="C141" s="109" t="s">
         <v>279</v>
       </c>
-      <c r="D141" s="111" t="s">
+      <c r="D141" s="109" t="s">
         <v>442</v>
       </c>
-      <c r="E141" s="111"/>
+      <c r="E141" s="109"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="90"/>
@@ -8129,6 +8159,61 @@
       </c>
       <c r="D167" s="84" t="s">
         <v>529</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B168" s="83" t="s">
+        <v>530</v>
+      </c>
+      <c r="C168" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D168" s="84" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="83" t="s">
+        <v>532</v>
+      </c>
+      <c r="C169" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D169" s="84" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B170" s="83" t="s">
+        <v>534</v>
+      </c>
+      <c r="C170" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D170" s="84" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B171" s="83" t="s">
+        <v>536</v>
+      </c>
+      <c r="C171" s="84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D171" s="84" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B172" s="83" t="s">
+        <v>538</v>
+      </c>
+      <c r="C172" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D172" s="84" t="s">
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added content for Instructions menu
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9532172-F2B3-4B22-BE5C-8CE0372CB4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7299FCA7-D83B-4EA8-8B91-C1A8B6D8063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-90" yWindow="45" windowWidth="13455" windowHeight="15465" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="542">
   <si>
     <t>ID</t>
   </si>
@@ -833,9 +833,6 @@
     <t>About ERB</t>
   </si>
   <si>
-    <t>What are indicators of Equitable Resilience?</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -851,12 +848,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>Goal Setting Scenario</t>
-  </si>
-  <si>
-    <t>Activity To Goal Matching Example</t>
-  </si>
-  <si>
     <t>OutputForm</t>
   </si>
   <si>
@@ -866,9 +857,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>Lay your cards on the table</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
@@ -1659,6 +1647,24 @@
   </si>
   <si>
     <t>How ERB centers equity</t>
+  </si>
+  <si>
+    <t>Supporting materials</t>
+  </si>
+  <si>
+    <t>Indicator card sorting</t>
+  </si>
+  <si>
+    <t>Reflection diary</t>
+  </si>
+  <si>
+    <t>Key takeaways</t>
+  </si>
+  <si>
+    <t>MyPortfolio</t>
+  </si>
+  <si>
+    <t>FAQ</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1688,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1740,6 +1746,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1997,7 +2021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2168,40 +2192,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2596,10 +2615,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="111"/>
+      <c r="H2" s="96"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5965,8 +5984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5990,154 +6009,154 @@
         <v>256</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
-      <c r="B2" s="93" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="106"/>
+      <c r="B2" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="98" t="s">
+      <c r="C2" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="98"/>
-    </row>
-    <row r="3" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="93" t="s">
+      <c r="E2" s="99"/>
+    </row>
+    <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="98"/>
+      <c r="B3" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="94" t="s">
-        <v>469</v>
-      </c>
-      <c r="E3" s="94"/>
-    </row>
-    <row r="4" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="93" t="s">
+      <c r="C3" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="85"/>
+    </row>
+    <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="98"/>
+      <c r="B4" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="94" t="s">
-        <v>474</v>
-      </c>
-      <c r="E4" s="94"/>
-    </row>
-    <row r="5" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93" t="s">
+      <c r="C4" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>470</v>
+      </c>
+      <c r="E4" s="85"/>
+    </row>
+    <row r="5" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="98"/>
+      <c r="B5" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="94" t="s">
+      <c r="C5" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>468</v>
+      </c>
+      <c r="E5" s="85"/>
+    </row>
+    <row r="6" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="98"/>
+      <c r="B6" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="E5" s="94"/>
-    </row>
-    <row r="6" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="94" t="s">
-        <v>476</v>
-      </c>
-      <c r="E6" s="94"/>
-    </row>
-    <row r="7" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
-      <c r="B7" s="93" t="s">
+      <c r="E6" s="85"/>
+    </row>
+    <row r="7" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="98"/>
+      <c r="B7" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>479</v>
-      </c>
-      <c r="E7" s="94"/>
-    </row>
-    <row r="8" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
-      <c r="B8" s="100" t="s">
+      <c r="C7" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="85" t="s">
+        <v>475</v>
+      </c>
+      <c r="E7" s="85"/>
+    </row>
+    <row r="8" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="98"/>
+      <c r="B8" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="101" t="s">
+      <c r="C8" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="85" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="101"/>
-    </row>
-    <row r="9" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="100" t="s">
+      <c r="E8" s="85"/>
+    </row>
+    <row r="9" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="98"/>
+      <c r="B9" s="91" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="101" t="s">
+      <c r="C9" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="85" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="101"/>
-    </row>
-    <row r="10" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="100" t="s">
+      <c r="E9" s="85"/>
+    </row>
+    <row r="10" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="98"/>
+      <c r="B10" s="91" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="101" t="s">
+      <c r="C10" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="101"/>
-    </row>
-    <row r="11" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
-      <c r="B11" s="93" t="s">
+      <c r="E10" s="85"/>
+    </row>
+    <row r="11" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="98"/>
+      <c r="B11" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>488</v>
-      </c>
-      <c r="E11" s="94"/>
-    </row>
-    <row r="12" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100" t="s">
-        <v>521</v>
-      </c>
-      <c r="C12" s="101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="101" t="s">
-        <v>522</v>
-      </c>
-      <c r="E12" s="101"/>
+      <c r="C11" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="E11" s="85"/>
+    </row>
+    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="98"/>
+      <c r="B12" s="91" t="s">
+        <v>517</v>
+      </c>
+      <c r="C12" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>518</v>
+      </c>
+      <c r="E12" s="85"/>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="91" t="s">
         <v>157</v>
       </c>
@@ -6145,12 +6164,12 @@
         <v>258</v>
       </c>
       <c r="D13" s="85" t="s">
-        <v>16</v>
+        <v>536</v>
       </c>
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="91" t="s">
         <v>158</v>
       </c>
@@ -6158,12 +6177,12 @@
         <v>258</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
+      <c r="A15" s="98"/>
       <c r="B15" s="91" t="s">
         <v>159</v>
       </c>
@@ -6171,12 +6190,12 @@
         <v>258</v>
       </c>
       <c r="D15" s="85" t="s">
-        <v>264</v>
+        <v>537</v>
       </c>
       <c r="E15" s="85"/>
     </row>
     <row r="16" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="91" t="s">
         <v>160</v>
       </c>
@@ -6189,72 +6208,72 @@
       <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="91" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="85" t="s">
+        <v>439</v>
+      </c>
+      <c r="E17" s="85"/>
+    </row>
+    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="98"/>
+      <c r="B18" s="91" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="85" t="s">
-        <v>443</v>
-      </c>
-      <c r="E17" s="85"/>
-    </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="90"/>
-      <c r="B18" s="91" t="s">
+      <c r="C18" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>444</v>
+      </c>
+      <c r="E18" s="85"/>
+    </row>
+    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98"/>
+      <c r="B19" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="85" t="s">
-        <v>448</v>
-      </c>
-      <c r="E18" s="85"/>
-    </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91" t="s">
+      <c r="C19" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="85" t="s">
+        <v>449</v>
+      </c>
+      <c r="E19" s="85"/>
+    </row>
+    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="98"/>
+      <c r="B20" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="C19" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="85" t="s">
-        <v>453</v>
-      </c>
-      <c r="E19" s="85"/>
-    </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="90"/>
-      <c r="B20" s="91" t="s">
+      <c r="C20" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="85" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="85"/>
+    </row>
+    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="98"/>
+      <c r="B21" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="85" t="s">
+      <c r="C21" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="85" t="s">
         <v>462</v>
       </c>
-      <c r="E20" s="85"/>
-    </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91" t="s">
-        <v>269</v>
-      </c>
-      <c r="C21" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="85" t="s">
-        <v>466</v>
-      </c>
       <c r="E21" s="85"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="90"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="91" t="s">
         <v>153</v>
       </c>
@@ -6262,12 +6281,12 @@
         <v>258</v>
       </c>
       <c r="D22" s="85" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E22" s="85"/>
     </row>
     <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="90"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="91" t="s">
         <v>161</v>
       </c>
@@ -6275,12 +6294,12 @@
         <v>258</v>
       </c>
       <c r="D23" s="85" t="s">
-        <v>270</v>
+        <v>538</v>
       </c>
       <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="90"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="91" t="s">
         <v>162</v>
       </c>
@@ -6288,12 +6307,12 @@
         <v>258</v>
       </c>
       <c r="D24" s="85" t="s">
-        <v>271</v>
+        <v>539</v>
       </c>
       <c r="E24" s="85"/>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="91" t="s">
         <v>163</v>
       </c>
@@ -6301,25 +6320,25 @@
         <v>258</v>
       </c>
       <c r="D25" s="85" t="s">
-        <v>8</v>
+        <v>540</v>
       </c>
       <c r="E25" s="85"/>
     </row>
     <row r="26" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="90"/>
+      <c r="A26" s="98"/>
       <c r="B26" s="91" t="s">
         <v>164</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D26" s="85" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E26" s="85"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="90"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="91" t="s">
         <v>165</v>
       </c>
@@ -6327,64 +6346,64 @@
         <v>258</v>
       </c>
       <c r="D27" s="85" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E27" s="85"/>
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90"/>
+      <c r="A28" s="98"/>
       <c r="B28" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="85" t="s">
+        <v>541</v>
+      </c>
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="98"/>
+      <c r="B29" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="85"/>
+    </row>
+    <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="98"/>
+      <c r="B30" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="C28" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D28" s="85" t="s">
+      <c r="C30" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="E28" s="85"/>
-    </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
-      <c r="B29" s="108" t="s">
+      <c r="D30" s="85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="85"/>
+    </row>
+    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="98"/>
+      <c r="B31" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="C29" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D29" s="109" t="s">
-        <v>277</v>
-      </c>
-      <c r="E29" s="109"/>
-    </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="108" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D30" s="109" t="s">
-        <v>233</v>
-      </c>
-      <c r="E30" s="109"/>
-    </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="108" t="s">
-        <v>280</v>
-      </c>
-      <c r="C31" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D31" s="109" t="s">
+      <c r="C31" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="109"/>
+      <c r="E31" s="85"/>
     </row>
     <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="90"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="91" t="s">
         <v>154</v>
       </c>
@@ -6392,12 +6411,12 @@
         <v>258</v>
       </c>
       <c r="D32" s="85" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E32" s="85"/>
     </row>
     <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
+      <c r="A33" s="98"/>
       <c r="B33" s="91" t="s">
         <v>166</v>
       </c>
@@ -6405,12 +6424,12 @@
         <v>258</v>
       </c>
       <c r="D33" s="85" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E33" s="85"/>
     </row>
     <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90"/>
+      <c r="A34" s="98"/>
       <c r="B34" s="91" t="s">
         <v>167</v>
       </c>
@@ -6423,7 +6442,7 @@
       <c r="E34" s="85"/>
     </row>
     <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="90"/>
+      <c r="A35" s="98"/>
       <c r="B35" s="91" t="s">
         <v>168</v>
       </c>
@@ -6431,12 +6450,12 @@
         <v>258</v>
       </c>
       <c r="D35" s="85" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E35" s="85"/>
     </row>
     <row r="36" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="90"/>
+      <c r="A36" s="98"/>
       <c r="B36" s="91" t="s">
         <v>169</v>
       </c>
@@ -6444,12 +6463,12 @@
         <v>258</v>
       </c>
       <c r="D36" s="85" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E36" s="85"/>
     </row>
     <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="90"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="91" t="s">
         <v>170</v>
       </c>
@@ -6457,12 +6476,12 @@
         <v>258</v>
       </c>
       <c r="D37" s="85" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E37" s="85"/>
     </row>
     <row r="38" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="90"/>
+      <c r="A38" s="98"/>
       <c r="B38" s="91" t="s">
         <v>171</v>
       </c>
@@ -6470,12 +6489,12 @@
         <v>258</v>
       </c>
       <c r="D38" s="85" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E38" s="85"/>
     </row>
     <row r="39" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="90"/>
+      <c r="A39" s="98"/>
       <c r="B39" s="91" t="s">
         <v>172</v>
       </c>
@@ -6483,285 +6502,285 @@
         <v>258</v>
       </c>
       <c r="D39" s="85" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="90"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>447</v>
+      </c>
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="100"/>
+      <c r="B41" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="102" t="s">
+        <v>280</v>
+      </c>
+      <c r="E41" s="102"/>
+    </row>
+    <row r="42" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="100"/>
+      <c r="B42" s="101" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="102" t="s">
+        <v>281</v>
+      </c>
+      <c r="E42" s="102"/>
+    </row>
+    <row r="43" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="100"/>
+      <c r="B43" s="101" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="102"/>
+    </row>
+    <row r="44" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="100"/>
+      <c r="B44" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="102" t="s">
         <v>282</v>
       </c>
-      <c r="C40" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="85" t="s">
-        <v>451</v>
-      </c>
-      <c r="E40" s="85"/>
-    </row>
-    <row r="41" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
-      <c r="B41" s="91" t="s">
+      <c r="E44" s="102"/>
+    </row>
+    <row r="45" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="100"/>
+      <c r="B45" s="101" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="102" t="s">
         <v>283</v>
       </c>
-      <c r="C41" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="85" t="s">
+      <c r="E45" s="102"/>
+    </row>
+    <row r="46" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="100"/>
+      <c r="B46" s="101" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="E41" s="85"/>
-    </row>
-    <row r="42" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
-      <c r="B42" s="91" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="85" t="s">
+      <c r="E46" s="102"/>
+    </row>
+    <row r="47" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="100"/>
+      <c r="B47" s="101" t="s">
         <v>285</v>
       </c>
-      <c r="E42" s="85"/>
-    </row>
-    <row r="43" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="85" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="85"/>
-    </row>
-    <row r="44" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="90"/>
-      <c r="B44" s="91" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="85" t="s">
+      <c r="C47" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="102" t="s">
         <v>286</v>
       </c>
-      <c r="E44" s="85"/>
-    </row>
-    <row r="45" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="91" t="s">
-        <v>176</v>
-      </c>
-      <c r="C45" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="85" t="s">
+      <c r="E47" s="102"/>
+    </row>
+    <row r="48" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="100"/>
+      <c r="B48" s="101" t="s">
         <v>287</v>
       </c>
-      <c r="E45" s="85"/>
-    </row>
-    <row r="46" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="90"/>
-      <c r="B46" s="91" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="85" t="s">
+      <c r="C48" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="102" t="s">
         <v>288</v>
       </c>
-      <c r="E46" s="85"/>
-    </row>
-    <row r="47" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="90"/>
-      <c r="B47" s="91" t="s">
+      <c r="E48" s="102"/>
+    </row>
+    <row r="49" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="100"/>
+      <c r="B49" s="101" t="s">
         <v>289</v>
       </c>
-      <c r="C47" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="85" t="s">
+      <c r="C49" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="102"/>
+    </row>
+    <row r="50" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="100"/>
+      <c r="B50" s="101" t="s">
         <v>290</v>
       </c>
-      <c r="E47" s="85"/>
-    </row>
-    <row r="48" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="90"/>
-      <c r="B48" s="91" t="s">
+      <c r="C50" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="102"/>
+    </row>
+    <row r="51" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="100"/>
+      <c r="B51" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="C48" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="85" t="s">
+      <c r="C51" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="102" t="s">
         <v>292</v>
       </c>
-      <c r="E48" s="85"/>
-    </row>
-    <row r="49" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="90"/>
-      <c r="B49" s="91" t="s">
+      <c r="E51" s="102"/>
+    </row>
+    <row r="52" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="100"/>
+      <c r="B52" s="101" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="102"/>
+    </row>
+    <row r="53" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="100"/>
+      <c r="B53" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="102"/>
+    </row>
+    <row r="54" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="100"/>
+      <c r="B54" s="101" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="102" t="s">
         <v>293</v>
       </c>
-      <c r="C49" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="85"/>
-    </row>
-    <row r="50" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="90"/>
-      <c r="B50" s="91" t="s">
+      <c r="E54" s="102"/>
+    </row>
+    <row r="55" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="100"/>
+      <c r="B55" s="101" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="102"/>
+    </row>
+    <row r="56" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="100"/>
+      <c r="B56" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="102"/>
+    </row>
+    <row r="57" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="100"/>
+      <c r="B57" s="101" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="102" t="s">
         <v>294</v>
       </c>
-      <c r="C50" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="85"/>
-    </row>
-    <row r="51" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="90"/>
-      <c r="B51" s="91" t="s">
+      <c r="E57" s="102"/>
+    </row>
+    <row r="58" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="100"/>
+      <c r="B58" s="101" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="102" t="s">
         <v>295</v>
       </c>
-      <c r="C51" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="85" t="s">
+      <c r="E58" s="102"/>
+    </row>
+    <row r="59" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="100"/>
+      <c r="B59" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="102" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="102"/>
+    </row>
+    <row r="60" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="100"/>
+      <c r="B60" s="101" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="102" t="s">
         <v>296</v>
       </c>
-      <c r="E51" s="85"/>
-    </row>
-    <row r="52" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="90"/>
-      <c r="B52" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="85" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="85"/>
-    </row>
-    <row r="53" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="90"/>
-      <c r="B53" s="91" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="85"/>
-    </row>
-    <row r="54" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="90"/>
-      <c r="B54" s="91" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="85" t="s">
-        <v>297</v>
-      </c>
-      <c r="E54" s="85"/>
-    </row>
-    <row r="55" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="90"/>
-      <c r="B55" s="91" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="85"/>
-    </row>
-    <row r="56" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="90"/>
-      <c r="B56" s="91" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="85"/>
-    </row>
-    <row r="57" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="90"/>
-      <c r="B57" s="91" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="85" t="s">
-        <v>298</v>
-      </c>
-      <c r="E57" s="85"/>
-    </row>
-    <row r="58" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="90"/>
-      <c r="B58" s="91" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="85" t="s">
-        <v>299</v>
-      </c>
-      <c r="E58" s="85"/>
-    </row>
-    <row r="59" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="90"/>
-      <c r="B59" s="91" t="s">
-        <v>184</v>
-      </c>
-      <c r="C59" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="85"/>
-    </row>
-    <row r="60" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="90"/>
-      <c r="B60" s="91" t="s">
-        <v>185</v>
-      </c>
-      <c r="C60" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="85" t="s">
-        <v>300</v>
-      </c>
-      <c r="E60" s="85"/>
+      <c r="E60" s="102"/>
     </row>
     <row r="61" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="90"/>
+      <c r="A61" s="98"/>
       <c r="B61" s="91" t="s">
         <v>186</v>
       </c>
@@ -6769,27 +6788,27 @@
         <v>258</v>
       </c>
       <c r="D61" s="85" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E61" s="85"/>
     </row>
     <row r="62" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="90"/>
+      <c r="A62" s="98"/>
       <c r="B62" s="91" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C62" s="85" t="s">
         <v>258</v>
       </c>
       <c r="D62" s="85" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E62" s="85"/>
     </row>
     <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="90"/>
+      <c r="A63" s="98"/>
       <c r="B63" s="91" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C63" s="85" t="s">
         <v>258</v>
@@ -6800,155 +6819,155 @@
       <c r="E63" s="85"/>
     </row>
     <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="90"/>
+      <c r="A64" s="97"/>
       <c r="B64" s="91" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D64" s="85" t="s">
+        <v>302</v>
+      </c>
+      <c r="E64" s="85"/>
+    </row>
+    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="97"/>
+      <c r="B65" s="91" t="s">
+        <v>303</v>
+      </c>
+      <c r="C65" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D65" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="C64" s="85" t="s">
+      <c r="E65" s="85"/>
+    </row>
+    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="97"/>
+      <c r="B66" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="85" t="s">
+      <c r="C66" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D66" s="85" t="s">
         <v>306</v>
       </c>
-      <c r="E64" s="85"/>
-    </row>
-    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="90"/>
-      <c r="B65" s="91" t="s">
+      <c r="E66" s="85"/>
+    </row>
+    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="97"/>
+      <c r="B67" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="C65" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D65" s="85" t="s">
+      <c r="C67" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D67" s="85" t="s">
         <v>308</v>
       </c>
-      <c r="E65" s="85"/>
-    </row>
-    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="90"/>
-      <c r="B66" s="91" t="s">
+      <c r="E67" s="85"/>
+    </row>
+    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="97"/>
+      <c r="B68" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="C66" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D66" s="85" t="s">
+      <c r="C68" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D68" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="E66" s="85"/>
-    </row>
-    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="90"/>
-      <c r="B67" s="91" t="s">
+      <c r="E68" s="85"/>
+    </row>
+    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="97"/>
+      <c r="B69" s="91" t="s">
         <v>311</v>
       </c>
-      <c r="C67" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D67" s="85" t="s">
+      <c r="C69" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D69" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="E67" s="85"/>
-    </row>
-    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="90"/>
-      <c r="B68" s="91" t="s">
+      <c r="E69" s="85"/>
+    </row>
+    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="97"/>
+      <c r="B70" s="91" t="s">
         <v>313</v>
       </c>
-      <c r="C68" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D68" s="85" t="s">
+      <c r="C70" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="E68" s="85"/>
-    </row>
-    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="90"/>
-      <c r="B69" s="91" t="s">
+      <c r="E70" s="85"/>
+    </row>
+    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="97"/>
+      <c r="B71" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="C69" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D69" s="85" t="s">
+      <c r="C71" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D71" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="E69" s="85"/>
-    </row>
-    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="90"/>
-      <c r="B70" s="91" t="s">
+      <c r="E71" s="85"/>
+    </row>
+    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="97"/>
+      <c r="B72" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D70" s="85" t="s">
+      <c r="C72" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D72" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="E70" s="85"/>
-    </row>
-    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="90"/>
-      <c r="B71" s="91" t="s">
+      <c r="E72" s="85"/>
+    </row>
+    <row r="73" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="100"/>
+      <c r="B73" s="101" t="s">
         <v>319</v>
       </c>
-      <c r="C71" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D71" s="85" t="s">
+      <c r="C73" s="102" t="s">
+        <v>301</v>
+      </c>
+      <c r="D73" s="102" t="s">
         <v>320</v>
       </c>
-      <c r="E71" s="85"/>
-    </row>
-    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="90"/>
-      <c r="B72" s="91" t="s">
+      <c r="E73" s="102"/>
+    </row>
+    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="97"/>
+      <c r="B74" s="91" t="s">
         <v>321</v>
       </c>
-      <c r="C72" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D72" s="85" t="s">
+      <c r="C74" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D74" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="E72" s="85"/>
-    </row>
-    <row r="73" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="90"/>
-      <c r="B73" s="91" t="s">
+      <c r="E74" s="85"/>
+    </row>
+    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="97"/>
+      <c r="B75" s="91" t="s">
         <v>323</v>
       </c>
-      <c r="C73" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D73" s="85" t="s">
-        <v>324</v>
-      </c>
-      <c r="E73" s="85"/>
-    </row>
-    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="90"/>
-      <c r="B74" s="91" t="s">
-        <v>325</v>
-      </c>
-      <c r="C74" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D74" s="85" t="s">
-        <v>326</v>
-      </c>
-      <c r="E74" s="85"/>
-    </row>
-    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="90"/>
-      <c r="B75" s="91" t="s">
-        <v>327</v>
-      </c>
       <c r="C75" s="85" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D75" s="85" t="s">
         <v>221</v>
@@ -6956,116 +6975,116 @@
       <c r="E75" s="85"/>
     </row>
     <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="90"/>
+      <c r="A76" s="97"/>
       <c r="B76" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="C76" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D76" s="85" t="s">
+        <v>325</v>
+      </c>
+      <c r="E76" s="85"/>
+    </row>
+    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="97"/>
+      <c r="B77" s="91" t="s">
+        <v>326</v>
+      </c>
+      <c r="C77" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" s="85" t="s">
+        <v>327</v>
+      </c>
+      <c r="E77" s="85"/>
+    </row>
+    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="97"/>
+      <c r="B78" s="91" t="s">
         <v>328</v>
       </c>
-      <c r="C76" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D76" s="85" t="s">
+      <c r="C78" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D78" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="E76" s="85"/>
-    </row>
-    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="90"/>
-      <c r="B77" s="91" t="s">
+      <c r="E78" s="85"/>
+    </row>
+    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="97"/>
+      <c r="B79" s="91" t="s">
         <v>330</v>
       </c>
-      <c r="C77" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D77" s="85" t="s">
+      <c r="C79" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D79" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="E77" s="85"/>
-    </row>
-    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="90"/>
-      <c r="B78" s="91" t="s">
+      <c r="E79" s="85"/>
+    </row>
+    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="97"/>
+      <c r="B80" s="91" t="s">
         <v>332</v>
       </c>
-      <c r="C78" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D78" s="85" t="s">
+      <c r="C80" s="85" t="s">
+        <v>301</v>
+      </c>
+      <c r="D80" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="E78" s="85"/>
-    </row>
-    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="90"/>
-      <c r="B79" s="91" t="s">
+      <c r="E80" s="85"/>
+    </row>
+    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="97"/>
+      <c r="B81" s="91" t="s">
         <v>334</v>
       </c>
-      <c r="C79" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D79" s="85" t="s">
+      <c r="C81" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="E79" s="85"/>
-    </row>
-    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="90"/>
-      <c r="B80" s="91" t="s">
+      <c r="D81" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C80" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D80" s="85" t="s">
+      <c r="E81" s="85"/>
+    </row>
+    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="97"/>
+      <c r="B82" s="91" t="s">
         <v>337</v>
       </c>
-      <c r="E80" s="85"/>
-    </row>
-    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="90"/>
-      <c r="B81" s="91" t="s">
+      <c r="C82" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D82" s="85" t="s">
         <v>338</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="E82" s="85"/>
+    </row>
+    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="97"/>
+      <c r="B83" s="91" t="s">
         <v>339</v>
       </c>
-      <c r="D81" s="85" t="s">
+      <c r="C83" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D83" s="85" t="s">
         <v>340</v>
       </c>
-      <c r="E81" s="85"/>
-    </row>
-    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="90"/>
-      <c r="B82" s="91" t="s">
+      <c r="E83" s="85"/>
+    </row>
+    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="97"/>
+      <c r="B84" s="91" t="s">
         <v>341</v>
       </c>
-      <c r="C82" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D82" s="85" t="s">
-        <v>342</v>
-      </c>
-      <c r="E82" s="85"/>
-    </row>
-    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="90"/>
-      <c r="B83" s="91" t="s">
-        <v>343</v>
-      </c>
-      <c r="C83" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D83" s="85" t="s">
-        <v>344</v>
-      </c>
-      <c r="E83" s="85"/>
-    </row>
-    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="90"/>
-      <c r="B84" s="91" t="s">
-        <v>345</v>
-      </c>
       <c r="C84" s="85" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D84" s="85" t="s">
         <v>233</v>
@@ -7073,12 +7092,12 @@
       <c r="E84" s="85"/>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="90"/>
+      <c r="A85" s="97"/>
       <c r="B85" s="91" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C85" s="85" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D85" s="85" t="s">
         <v>234</v>
@@ -7086,322 +7105,322 @@
       <c r="E85" s="85"/>
     </row>
     <row r="86" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="90"/>
+      <c r="A86" s="97"/>
       <c r="B86" s="91" t="s">
+        <v>343</v>
+      </c>
+      <c r="C86" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="D86" s="85" t="s">
+        <v>345</v>
+      </c>
+      <c r="E86" s="85" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="97"/>
+      <c r="B87" s="91" t="s">
+        <v>346</v>
+      </c>
+      <c r="C87" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="D87" s="85" t="s">
         <v>347</v>
       </c>
-      <c r="C86" s="85" t="s">
+      <c r="E87" s="85" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="100"/>
+      <c r="B88" s="101" t="s">
+        <v>349</v>
+      </c>
+      <c r="C88" s="102" t="s">
         <v>348</v>
       </c>
-      <c r="D86" s="85" t="s">
-        <v>349</v>
-      </c>
-      <c r="E86" s="85" t="s">
+      <c r="D88" s="102" t="s">
+        <v>193</v>
+      </c>
+      <c r="E88" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="100"/>
+      <c r="B89" s="101" t="s">
+        <v>350</v>
+      </c>
+      <c r="C89" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D89" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="100"/>
+      <c r="B90" s="101" t="s">
+        <v>351</v>
+      </c>
+      <c r="C90" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D90" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="100"/>
+      <c r="B91" s="101" t="s">
+        <v>352</v>
+      </c>
+      <c r="C91" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D91" s="102" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="100"/>
+      <c r="B92" s="101" t="s">
+        <v>353</v>
+      </c>
+      <c r="C92" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D92" s="102" t="s">
+        <v>354</v>
+      </c>
+      <c r="E92" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="100"/>
+      <c r="B93" s="101" t="s">
+        <v>356</v>
+      </c>
+      <c r="C93" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D93" s="102" t="s">
+        <v>357</v>
+      </c>
+      <c r="E93" s="104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="98"/>
+      <c r="B94" s="91" t="s">
+        <v>359</v>
+      </c>
+      <c r="C94" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="E94" s="85"/>
+    </row>
+    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="98"/>
+      <c r="B95" s="91" t="s">
+        <v>361</v>
+      </c>
+      <c r="C95" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="85" t="s">
+        <v>450</v>
+      </c>
+      <c r="E95" s="85"/>
+    </row>
+    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="98"/>
+      <c r="B96" s="91" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="90"/>
-      <c r="B87" s="91" t="s">
-        <v>350</v>
-      </c>
-      <c r="C87" s="85" t="s">
-        <v>348</v>
-      </c>
-      <c r="D87" s="85" t="s">
-        <v>351</v>
-      </c>
-      <c r="E87" s="85" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="90"/>
-      <c r="B88" s="91" t="s">
-        <v>353</v>
-      </c>
-      <c r="C88" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D88" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="E88" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="90"/>
-      <c r="B89" s="91" t="s">
-        <v>354</v>
-      </c>
-      <c r="C89" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D89" s="85" t="s">
-        <v>80</v>
-      </c>
-      <c r="E89" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="90"/>
-      <c r="B90" s="91" t="s">
-        <v>355</v>
-      </c>
-      <c r="C90" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D90" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="E90" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="90"/>
-      <c r="B91" s="91" t="s">
-        <v>356</v>
-      </c>
-      <c r="C91" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D91" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="E91" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="90"/>
-      <c r="B92" s="91" t="s">
-        <v>357</v>
-      </c>
-      <c r="C92" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D92" s="85" t="s">
-        <v>358</v>
-      </c>
-      <c r="E92" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="90"/>
-      <c r="B93" s="91" t="s">
-        <v>360</v>
-      </c>
-      <c r="C93" s="85" t="s">
-        <v>352</v>
-      </c>
-      <c r="D93" s="85" t="s">
-        <v>361</v>
-      </c>
-      <c r="E93" s="96" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="90"/>
-      <c r="B94" s="91" t="s">
+      <c r="C96" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D96" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="C94" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="85" t="s">
+      <c r="E96" s="85"/>
+    </row>
+    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="98"/>
+      <c r="B97" s="91" t="s">
         <v>364</v>
       </c>
-      <c r="E94" s="85"/>
-    </row>
-    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="90"/>
-      <c r="B95" s="91" t="s">
+      <c r="C97" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D97" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="C95" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="85" t="s">
-        <v>454</v>
-      </c>
-      <c r="E95" s="85"/>
-    </row>
-    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="90"/>
-      <c r="B96" s="91" t="s">
+      <c r="E97" s="85"/>
+    </row>
+    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="98"/>
+      <c r="B98" s="91" t="s">
         <v>366</v>
       </c>
-      <c r="C96" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="85" t="s">
+      <c r="C98" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="E96" s="85"/>
-    </row>
-    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="90"/>
-      <c r="B97" s="91" t="s">
+      <c r="E98" s="85"/>
+    </row>
+    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="98"/>
+      <c r="B99" s="91" t="s">
         <v>368</v>
       </c>
-      <c r="C97" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="85" t="s">
+      <c r="C99" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="E97" s="85"/>
-    </row>
-    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="90"/>
-      <c r="B98" s="91" t="s">
+      <c r="E99" s="85"/>
+    </row>
+    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="98"/>
+      <c r="B100" s="91" t="s">
         <v>370</v>
       </c>
-      <c r="C98" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="85" t="s">
+      <c r="C100" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="E98" s="85"/>
-    </row>
-    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="90"/>
-      <c r="B99" s="91" t="s">
-        <v>372</v>
-      </c>
-      <c r="C99" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="85" t="s">
-        <v>373</v>
-      </c>
-      <c r="E99" s="85"/>
-    </row>
-    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="90"/>
-      <c r="B100" s="91" t="s">
+      <c r="E100" s="85"/>
+    </row>
+    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="98"/>
+      <c r="B101" s="91" t="s">
         <v>374</v>
       </c>
-      <c r="C100" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="85" t="s">
+      <c r="C101" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="E100" s="85"/>
-    </row>
-    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="90"/>
-      <c r="B101" s="91" t="s">
+      <c r="E101" s="85"/>
+    </row>
+    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="98"/>
+      <c r="B102" s="91" t="s">
+        <v>376</v>
+      </c>
+      <c r="C102" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" s="85" t="s">
+        <v>377</v>
+      </c>
+      <c r="E102" s="85"/>
+    </row>
+    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="98"/>
+      <c r="B103" s="91" t="s">
         <v>378</v>
       </c>
-      <c r="C101" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="85" t="s">
+      <c r="C103" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="85" t="s">
         <v>379</v>
       </c>
-      <c r="E101" s="85"/>
-    </row>
-    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="90"/>
-      <c r="B102" s="91" t="s">
+      <c r="E103" s="85"/>
+    </row>
+    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="98"/>
+      <c r="B104" s="91" t="s">
         <v>380</v>
       </c>
-      <c r="C102" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="85" t="s">
+      <c r="C104" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D104" s="85" t="s">
+        <v>451</v>
+      </c>
+      <c r="E104" s="85"/>
+    </row>
+    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="98"/>
+      <c r="B105" s="91" t="s">
         <v>381</v>
       </c>
-      <c r="E102" s="85"/>
-    </row>
-    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="90"/>
-      <c r="B103" s="91" t="s">
+      <c r="C105" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="85" t="s">
+        <v>452</v>
+      </c>
+      <c r="E105" s="85"/>
+    </row>
+    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="98"/>
+      <c r="B106" s="91" t="s">
         <v>382</v>
       </c>
-      <c r="C103" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="85" t="s">
+      <c r="C106" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D106" s="85" t="s">
+        <v>453</v>
+      </c>
+      <c r="E106" s="85"/>
+    </row>
+    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="98"/>
+      <c r="B107" s="91" t="s">
         <v>383</v>
       </c>
-      <c r="E103" s="85"/>
-    </row>
-    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="90"/>
-      <c r="B104" s="91" t="s">
+      <c r="C107" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="85" t="s">
         <v>384</v>
       </c>
-      <c r="C104" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="85" t="s">
-        <v>455</v>
-      </c>
-      <c r="E104" s="85"/>
-    </row>
-    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="90"/>
-      <c r="B105" s="91" t="s">
+      <c r="E107" s="85"/>
+    </row>
+    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="98"/>
+      <c r="B108" s="91" t="s">
         <v>385</v>
       </c>
-      <c r="C105" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="85" t="s">
-        <v>456</v>
-      </c>
-      <c r="E105" s="85"/>
-    </row>
-    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="90"/>
-      <c r="B106" s="91" t="s">
+      <c r="C108" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="85" t="s">
         <v>386</v>
       </c>
-      <c r="C106" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="85" t="s">
-        <v>457</v>
-      </c>
-      <c r="E106" s="85"/>
-    </row>
-    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="90"/>
-      <c r="B107" s="91" t="s">
-        <v>387</v>
-      </c>
-      <c r="C107" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="85" t="s">
-        <v>388</v>
-      </c>
-      <c r="E107" s="85"/>
-    </row>
-    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="90"/>
-      <c r="B108" s="91" t="s">
-        <v>389</v>
-      </c>
-      <c r="C108" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="85" t="s">
-        <v>390</v>
-      </c>
       <c r="E108" s="85"/>
     </row>
     <row r="109" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="90"/>
+      <c r="A109" s="98"/>
       <c r="B109" s="91" t="s">
         <v>187</v>
       </c>
@@ -7409,155 +7428,155 @@
         <v>258</v>
       </c>
       <c r="D109" s="85" t="s">
+        <v>387</v>
+      </c>
+      <c r="E109" s="85"/>
+    </row>
+    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="98"/>
+      <c r="B110" s="91" t="s">
+        <v>388</v>
+      </c>
+      <c r="C110" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D110" s="85" t="s">
+        <v>455</v>
+      </c>
+      <c r="E110" s="85"/>
+    </row>
+    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="98"/>
+      <c r="B111" s="91" t="s">
+        <v>372</v>
+      </c>
+      <c r="C111" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D111" s="85" t="s">
+        <v>390</v>
+      </c>
+      <c r="E111" s="85"/>
+    </row>
+    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="98"/>
+      <c r="B112" s="91" t="s">
+        <v>373</v>
+      </c>
+      <c r="C112" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D112" s="85" t="s">
+        <v>469</v>
+      </c>
+      <c r="E112" s="85"/>
+    </row>
+    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="98"/>
+      <c r="B113" s="91" t="s">
         <v>391</v>
       </c>
-      <c r="E109" s="85"/>
-    </row>
-    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="90"/>
-      <c r="B110" s="91" t="s">
+      <c r="C113" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D113" s="85" t="s">
+        <v>471</v>
+      </c>
+      <c r="E113" s="85"/>
+    </row>
+    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="97"/>
+      <c r="B114" s="91" t="s">
         <v>392</v>
       </c>
-      <c r="C110" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D110" s="85" t="s">
-        <v>459</v>
-      </c>
-      <c r="E110" s="85"/>
-    </row>
-    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="90"/>
-      <c r="B111" s="91" t="s">
-        <v>376</v>
-      </c>
-      <c r="C111" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D111" s="85" t="s">
+      <c r="C114" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D114" s="85" t="s">
+        <v>393</v>
+      </c>
+      <c r="E114" s="85"/>
+    </row>
+    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="97"/>
+      <c r="B115" s="91" t="s">
         <v>394</v>
       </c>
-      <c r="E111" s="85"/>
-    </row>
-    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="90"/>
-      <c r="B112" s="91" t="s">
-        <v>377</v>
-      </c>
-      <c r="C112" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D112" s="85" t="s">
-        <v>473</v>
-      </c>
-      <c r="E112" s="85"/>
-    </row>
-    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="90"/>
-      <c r="B113" s="91" t="s">
+      <c r="C115" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D115" s="85" t="s">
         <v>395</v>
       </c>
-      <c r="C113" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D113" s="85" t="s">
-        <v>475</v>
-      </c>
-      <c r="E113" s="85"/>
-    </row>
-    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="90"/>
-      <c r="B114" s="91" t="s">
+      <c r="E115" s="85"/>
+    </row>
+    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="98"/>
+      <c r="B116" s="91" t="s">
         <v>396</v>
       </c>
-      <c r="C114" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="85" t="s">
+      <c r="C116" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D116" s="85" t="s">
         <v>397</v>
       </c>
-      <c r="E114" s="85"/>
-    </row>
-    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="90"/>
-      <c r="B115" s="91" t="s">
+      <c r="E116" s="85"/>
+    </row>
+    <row r="117" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="100"/>
+      <c r="B117" s="101" t="s">
         <v>398</v>
       </c>
-      <c r="C115" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D115" s="85" t="s">
+      <c r="C117" s="102" t="s">
+        <v>335</v>
+      </c>
+      <c r="D117" s="102" t="s">
         <v>399</v>
       </c>
-      <c r="E115" s="85"/>
-    </row>
-    <row r="116" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="107"/>
-      <c r="B116" s="108" t="s">
+      <c r="E117" s="102"/>
+    </row>
+    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="98"/>
+      <c r="B118" s="91" t="s">
         <v>400</v>
       </c>
-      <c r="C116" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D116" s="109" t="s">
+      <c r="C118" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D118" s="85" t="s">
         <v>401</v>
       </c>
-      <c r="E116" s="109"/>
-    </row>
-    <row r="117" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="90"/>
-      <c r="B117" s="91" t="s">
+      <c r="E118" s="85"/>
+    </row>
+    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="97"/>
+      <c r="B119" s="91" t="s">
         <v>402</v>
       </c>
-      <c r="C117" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D117" s="85" t="s">
+      <c r="C119" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D119" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="E117" s="85"/>
-    </row>
-    <row r="118" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="107"/>
-      <c r="B118" s="108" t="s">
+      <c r="E119" s="85"/>
+    </row>
+    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="97"/>
+      <c r="B120" s="91" t="s">
         <v>404</v>
       </c>
-      <c r="C118" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D118" s="109" t="s">
+      <c r="C120" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D120" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="E118" s="109"/>
-    </row>
-    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="90"/>
-      <c r="B119" s="91" t="s">
-        <v>406</v>
-      </c>
-      <c r="C119" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D119" s="85" t="s">
-        <v>407</v>
-      </c>
-      <c r="E119" s="85"/>
-    </row>
-    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="90"/>
-      <c r="B120" s="91" t="s">
-        <v>408</v>
-      </c>
-      <c r="C120" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D120" s="85" t="s">
-        <v>409</v>
-      </c>
       <c r="E120" s="85"/>
     </row>
     <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="90"/>
+      <c r="A121" s="97"/>
       <c r="B121" s="91" t="s">
         <v>188</v>
       </c>
@@ -7565,116 +7584,116 @@
         <v>258</v>
       </c>
       <c r="D121" s="85" t="s">
+        <v>406</v>
+      </c>
+      <c r="E121" s="85"/>
+    </row>
+    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="97"/>
+      <c r="B122" s="91" t="s">
+        <v>407</v>
+      </c>
+      <c r="C122" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D122" s="85" t="s">
+        <v>409</v>
+      </c>
+      <c r="E122" s="85"/>
+    </row>
+    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="97"/>
+      <c r="B123" s="91" t="s">
+        <v>408</v>
+      </c>
+      <c r="C123" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="85" t="s">
         <v>410</v>
       </c>
-      <c r="E121" s="85"/>
-    </row>
-    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="90"/>
-      <c r="B122" s="91" t="s">
+      <c r="E123" s="85"/>
+    </row>
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="98"/>
+      <c r="B124" s="91" t="s">
         <v>411</v>
       </c>
-      <c r="C122" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D122" s="85" t="s">
+      <c r="C124" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" s="85" t="s">
+        <v>412</v>
+      </c>
+      <c r="E124" s="85"/>
+    </row>
+    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="98"/>
+      <c r="B125" s="91" t="s">
         <v>413</v>
       </c>
-      <c r="E122" s="85"/>
-    </row>
-    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="90"/>
-      <c r="B123" s="91" t="s">
-        <v>412</v>
-      </c>
-      <c r="C123" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="85" t="s">
+      <c r="C125" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D125" s="85" t="s">
         <v>414</v>
       </c>
-      <c r="E123" s="85"/>
-    </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="90"/>
-      <c r="B124" s="91" t="s">
+      <c r="E125" s="85"/>
+    </row>
+    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="98"/>
+      <c r="B126" s="91" t="s">
         <v>415</v>
       </c>
-      <c r="C124" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="85" t="s">
+      <c r="C126" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="85" t="s">
+        <v>459</v>
+      </c>
+      <c r="E126" s="85"/>
+    </row>
+    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="98"/>
+      <c r="B127" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="E124" s="85"/>
-    </row>
-    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="90"/>
-      <c r="B125" s="91" t="s">
+      <c r="C127" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="85" t="s">
         <v>417</v>
       </c>
-      <c r="C125" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="85" t="s">
+      <c r="E127" s="85"/>
+    </row>
+    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="98"/>
+      <c r="B128" s="91" t="s">
         <v>418</v>
       </c>
-      <c r="E125" s="85"/>
-    </row>
-    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="90"/>
-      <c r="B126" s="91" t="s">
+      <c r="C128" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" s="85" t="s">
         <v>419</v>
       </c>
-      <c r="C126" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="85" t="s">
-        <v>463</v>
-      </c>
-      <c r="E126" s="85"/>
-    </row>
-    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="90"/>
-      <c r="B127" s="91" t="s">
+      <c r="E128" s="85"/>
+    </row>
+    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="98"/>
+      <c r="B129" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="C127" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="85" t="s">
+      <c r="C129" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D129" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="E127" s="85"/>
-    </row>
-    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="90"/>
-      <c r="B128" s="91" t="s">
-        <v>422</v>
-      </c>
-      <c r="C128" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="85" t="s">
-        <v>423</v>
-      </c>
-      <c r="E128" s="85"/>
-    </row>
-    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="90"/>
-      <c r="B129" s="91" t="s">
-        <v>424</v>
-      </c>
-      <c r="C129" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="85" t="s">
-        <v>425</v>
-      </c>
       <c r="E129" s="85"/>
     </row>
     <row r="130" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="90"/>
+      <c r="A130" s="98"/>
       <c r="B130" s="91" t="s">
         <v>189</v>
       </c>
@@ -7682,12 +7701,12 @@
         <v>258</v>
       </c>
       <c r="D130" s="85" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E130" s="85"/>
     </row>
     <row r="131" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="90"/>
+      <c r="A131" s="98"/>
       <c r="B131" s="91" t="s">
         <v>190</v>
       </c>
@@ -7695,526 +7714,539 @@
         <v>258</v>
       </c>
       <c r="D131" s="85" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E131" s="85"/>
     </row>
     <row r="132" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="90"/>
+      <c r="A132" s="98"/>
       <c r="B132" s="91" t="s">
+        <v>423</v>
+      </c>
+      <c r="C132" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" s="85" t="s">
+        <v>424</v>
+      </c>
+      <c r="E132" s="85"/>
+    </row>
+    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="98"/>
+      <c r="B133" s="91" t="s">
+        <v>425</v>
+      </c>
+      <c r="C133" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D133" s="85" t="s">
+        <v>426</v>
+      </c>
+      <c r="E133" s="85"/>
+    </row>
+    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="98"/>
+      <c r="B134" s="91" t="s">
         <v>427</v>
       </c>
-      <c r="C132" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="85" t="s">
+      <c r="C134" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D134" s="85" t="s">
+        <v>461</v>
+      </c>
+      <c r="E134" s="85"/>
+    </row>
+    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="98"/>
+      <c r="B135" s="91" t="s">
         <v>428</v>
       </c>
-      <c r="E132" s="85"/>
-    </row>
-    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="90"/>
-      <c r="B133" s="91" t="s">
+      <c r="C135" s="85" t="s">
+        <v>269</v>
+      </c>
+      <c r="D135" s="85" t="s">
         <v>429</v>
       </c>
-      <c r="C133" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="85" t="s">
+      <c r="E135" s="85"/>
+    </row>
+    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="98"/>
+      <c r="B136" s="91" t="s">
         <v>430</v>
       </c>
-      <c r="E133" s="85"/>
-    </row>
-    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="90"/>
-      <c r="B134" s="91" t="s">
+      <c r="C136" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D136" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="C134" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D134" s="85" t="s">
-        <v>465</v>
-      </c>
-      <c r="E134" s="85"/>
-    </row>
-    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="90"/>
-      <c r="B135" s="91" t="s">
+      <c r="E136" s="85"/>
+    </row>
+    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="98"/>
+      <c r="B137" s="91" t="s">
         <v>432</v>
       </c>
-      <c r="C135" s="85" t="s">
-        <v>272</v>
-      </c>
-      <c r="D135" s="85" t="s">
+      <c r="C137" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D137" s="85" t="s">
+        <v>520</v>
+      </c>
+      <c r="E137" s="85"/>
+    </row>
+    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="98"/>
+      <c r="B138" s="91" t="s">
         <v>433</v>
       </c>
-      <c r="E135" s="85"/>
-    </row>
-    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="90"/>
-      <c r="B136" s="91" t="s">
+      <c r="C138" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D138" s="85" t="s">
+        <v>463</v>
+      </c>
+      <c r="E138" s="85"/>
+    </row>
+    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="98"/>
+      <c r="B139" s="91" t="s">
         <v>434</v>
       </c>
-      <c r="C136" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="85" t="s">
+      <c r="C139" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="E136" s="85"/>
-    </row>
-    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="90"/>
-      <c r="B137" s="91" t="s">
+      <c r="E139" s="85"/>
+    </row>
+    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="98"/>
+      <c r="B140" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="C137" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="85" t="s">
+      <c r="C140" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D140" s="85" t="s">
+        <v>464</v>
+      </c>
+      <c r="E140" s="85"/>
+    </row>
+    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="98"/>
+      <c r="B141" s="91" t="s">
+        <v>437</v>
+      </c>
+      <c r="C141" s="85" t="s">
+        <v>275</v>
+      </c>
+      <c r="D141" s="85" t="s">
+        <v>438</v>
+      </c>
+      <c r="E141" s="85"/>
+    </row>
+    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="97"/>
+      <c r="B142" s="91" t="s">
+        <v>456</v>
+      </c>
+      <c r="C142" s="85" t="s">
+        <v>269</v>
+      </c>
+      <c r="D142" s="85" t="s">
+        <v>457</v>
+      </c>
+      <c r="E142" s="85"/>
+    </row>
+    <row r="143" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="100"/>
+      <c r="B143" s="101" t="s">
+        <v>466</v>
+      </c>
+      <c r="C143" s="102" t="s">
+        <v>301</v>
+      </c>
+      <c r="D143" s="102" t="s">
+        <v>467</v>
+      </c>
+      <c r="E143" s="102"/>
+    </row>
+    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="98"/>
+      <c r="B144" s="91" t="s">
+        <v>473</v>
+      </c>
+      <c r="C144" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D144" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="E144" s="85"/>
+    </row>
+    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="98"/>
+      <c r="B145" s="91" t="s">
+        <v>476</v>
+      </c>
+      <c r="C145" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D145" s="85" t="s">
+        <v>477</v>
+      </c>
+      <c r="E145" s="85"/>
+    </row>
+    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="98"/>
+      <c r="B146" s="91" t="s">
+        <v>478</v>
+      </c>
+      <c r="C146" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D146" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="E146" s="85"/>
+    </row>
+    <row r="147" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="105"/>
+      <c r="B147" s="92" t="s">
+        <v>480</v>
+      </c>
+      <c r="C147" s="93" t="s">
+        <v>335</v>
+      </c>
+      <c r="D147" s="93" t="s">
+        <v>481</v>
+      </c>
+      <c r="E147" s="93"/>
+    </row>
+    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="98"/>
+      <c r="B148" s="91" t="s">
+        <v>482</v>
+      </c>
+      <c r="C148" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D148" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="E148" s="85"/>
+    </row>
+    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="98"/>
+      <c r="B149" s="91" t="s">
+        <v>485</v>
+      </c>
+      <c r="C149" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D149" s="85" t="s">
+        <v>486</v>
+      </c>
+      <c r="E149" s="85"/>
+    </row>
+    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="98"/>
+      <c r="B150" s="91" t="s">
+        <v>487</v>
+      </c>
+      <c r="C150" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D150" s="85" t="s">
+        <v>488</v>
+      </c>
+      <c r="E150" s="85"/>
+    </row>
+    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="98"/>
+      <c r="B151" s="91" t="s">
+        <v>490</v>
+      </c>
+      <c r="C151" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D151" s="85" t="s">
+        <v>489</v>
+      </c>
+      <c r="E151" s="85"/>
+    </row>
+    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="98"/>
+      <c r="B152" s="91" t="s">
+        <v>491</v>
+      </c>
+      <c r="C152" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D152" s="85" t="s">
+        <v>492</v>
+      </c>
+      <c r="E152" s="85"/>
+    </row>
+    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="98"/>
+      <c r="B153" s="91" t="s">
+        <v>493</v>
+      </c>
+      <c r="C153" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D153" s="85" t="s">
+        <v>501</v>
+      </c>
+      <c r="E153" s="85"/>
+    </row>
+    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="97"/>
+      <c r="B154" s="91" t="s">
+        <v>494</v>
+      </c>
+      <c r="C154" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D154" s="85" t="s">
+        <v>502</v>
+      </c>
+      <c r="E154" s="85"/>
+    </row>
+    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="97"/>
+      <c r="B155" s="91" t="s">
+        <v>495</v>
+      </c>
+      <c r="C155" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D155" s="85" t="s">
+        <v>503</v>
+      </c>
+      <c r="E155" s="85"/>
+    </row>
+    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="97"/>
+      <c r="B156" s="91" t="s">
+        <v>496</v>
+      </c>
+      <c r="C156" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D156" s="85" t="s">
+        <v>504</v>
+      </c>
+      <c r="E156" s="85"/>
+    </row>
+    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="97"/>
+      <c r="B157" s="91" t="s">
+        <v>497</v>
+      </c>
+      <c r="C157" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D157" s="85" t="s">
+        <v>505</v>
+      </c>
+      <c r="E157" s="85"/>
+    </row>
+    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="97"/>
+      <c r="B158" s="91" t="s">
+        <v>498</v>
+      </c>
+      <c r="C158" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D158" s="85" t="s">
+        <v>506</v>
+      </c>
+      <c r="E158" s="85"/>
+    </row>
+    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="97"/>
+      <c r="B159" s="91" t="s">
+        <v>499</v>
+      </c>
+      <c r="C159" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D159" s="85" t="s">
+        <v>507</v>
+      </c>
+      <c r="E159" s="85"/>
+    </row>
+    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="97"/>
+      <c r="B160" s="91" t="s">
+        <v>500</v>
+      </c>
+      <c r="C160" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D160" s="85" t="s">
+        <v>508</v>
+      </c>
+      <c r="E160" s="85"/>
+    </row>
+    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="97"/>
+      <c r="B161" s="91" t="s">
+        <v>509</v>
+      </c>
+      <c r="C161" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D161" s="85" t="s">
+        <v>510</v>
+      </c>
+      <c r="E161" s="85"/>
+    </row>
+    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="98"/>
+      <c r="B162" s="91" t="s">
+        <v>511</v>
+      </c>
+      <c r="C162" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D162" s="85" t="s">
+        <v>514</v>
+      </c>
+      <c r="E162" s="85"/>
+    </row>
+    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="98"/>
+      <c r="B163" s="91" t="s">
+        <v>512</v>
+      </c>
+      <c r="C163" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D163" s="85" t="s">
+        <v>515</v>
+      </c>
+      <c r="E163" s="85"/>
+    </row>
+    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="98"/>
+      <c r="B164" s="91" t="s">
+        <v>513</v>
+      </c>
+      <c r="C164" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D164" s="85" t="s">
+        <v>516</v>
+      </c>
+      <c r="E164" s="85"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="98"/>
+      <c r="B165" s="83" t="s">
+        <v>521</v>
+      </c>
+      <c r="C165" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D165" s="84" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="98"/>
+      <c r="B166" s="91" t="s">
+        <v>522</v>
+      </c>
+      <c r="C166" s="85" t="s">
+        <v>335</v>
+      </c>
+      <c r="D166" s="85" t="s">
+        <v>523</v>
+      </c>
+      <c r="E166" s="85"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="98"/>
+      <c r="B167" s="83" t="s">
         <v>524</v>
       </c>
-      <c r="E137" s="85"/>
-    </row>
-    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="90"/>
-      <c r="B138" s="91" t="s">
-        <v>437</v>
-      </c>
-      <c r="C138" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="85" t="s">
-        <v>467</v>
-      </c>
-      <c r="E138" s="85"/>
-    </row>
-    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="90"/>
-      <c r="B139" s="91" t="s">
-        <v>438</v>
-      </c>
-      <c r="C139" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="85" t="s">
-        <v>439</v>
-      </c>
-      <c r="E139" s="85"/>
-    </row>
-    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="90"/>
-      <c r="B140" s="91" t="s">
-        <v>440</v>
-      </c>
-      <c r="C140" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D140" s="85" t="s">
-        <v>468</v>
-      </c>
-      <c r="E140" s="85"/>
-    </row>
-    <row r="141" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="107"/>
-      <c r="B141" s="108" t="s">
-        <v>441</v>
-      </c>
-      <c r="C141" s="109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D141" s="109" t="s">
-        <v>442</v>
-      </c>
-      <c r="E141" s="109"/>
-    </row>
-    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="90"/>
-      <c r="B142" s="91" t="s">
-        <v>460</v>
-      </c>
-      <c r="C142" s="85" t="s">
-        <v>272</v>
-      </c>
-      <c r="D142" s="85" t="s">
-        <v>461</v>
-      </c>
-      <c r="E142" s="85"/>
-    </row>
-    <row r="143" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="90"/>
-      <c r="B143" s="91" t="s">
-        <v>470</v>
-      </c>
-      <c r="C143" s="85" t="s">
-        <v>305</v>
-      </c>
-      <c r="D143" s="85" t="s">
-        <v>471</v>
-      </c>
-      <c r="E143" s="85"/>
-    </row>
-    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="90"/>
-      <c r="B144" s="91" t="s">
-        <v>477</v>
-      </c>
-      <c r="C144" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D144" s="85" t="s">
-        <v>478</v>
-      </c>
-      <c r="E144" s="85"/>
-    </row>
-    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="90"/>
-      <c r="B145" s="91" t="s">
-        <v>480</v>
-      </c>
-      <c r="C145" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D145" s="85" t="s">
-        <v>481</v>
-      </c>
-      <c r="E145" s="85"/>
-    </row>
-    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="90"/>
-      <c r="B146" s="91" t="s">
-        <v>482</v>
-      </c>
-      <c r="C146" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D146" s="85" t="s">
-        <v>483</v>
-      </c>
-      <c r="E146" s="85"/>
-    </row>
-    <row r="147" spans="1:5" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="103"/>
-      <c r="B147" s="104" t="s">
-        <v>484</v>
-      </c>
-      <c r="C147" s="105" t="s">
-        <v>339</v>
-      </c>
-      <c r="D147" s="105" t="s">
-        <v>485</v>
-      </c>
-      <c r="E147" s="105"/>
-    </row>
-    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="90"/>
-      <c r="B148" s="91" t="s">
-        <v>486</v>
-      </c>
-      <c r="C148" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D148" s="85" t="s">
-        <v>487</v>
-      </c>
-      <c r="E148" s="85"/>
-    </row>
-    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="90"/>
-      <c r="B149" s="91" t="s">
-        <v>489</v>
-      </c>
-      <c r="C149" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="85" t="s">
-        <v>490</v>
-      </c>
-      <c r="E149" s="85"/>
-    </row>
-    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="90"/>
-      <c r="B150" s="91" t="s">
-        <v>491</v>
-      </c>
-      <c r="C150" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D150" s="85" t="s">
-        <v>492</v>
-      </c>
-      <c r="E150" s="85"/>
-    </row>
-    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="90"/>
-      <c r="B151" s="91" t="s">
-        <v>494</v>
-      </c>
-      <c r="C151" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D151" s="85" t="s">
-        <v>493</v>
-      </c>
-      <c r="E151" s="85"/>
-    </row>
-    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="90"/>
-      <c r="B152" s="91" t="s">
-        <v>495</v>
-      </c>
-      <c r="C152" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D152" s="85" t="s">
-        <v>496</v>
-      </c>
-      <c r="E152" s="85"/>
-    </row>
-    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="90"/>
-      <c r="B153" s="91" t="s">
-        <v>497</v>
-      </c>
-      <c r="C153" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D153" s="85" t="s">
-        <v>505</v>
-      </c>
-      <c r="E153" s="85"/>
-    </row>
-    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="90"/>
-      <c r="B154" s="91" t="s">
-        <v>498</v>
-      </c>
-      <c r="C154" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D154" s="85" t="s">
-        <v>506</v>
-      </c>
-      <c r="E154" s="85"/>
-    </row>
-    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="90"/>
-      <c r="B155" s="91" t="s">
-        <v>499</v>
-      </c>
-      <c r="C155" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D155" s="85" t="s">
-        <v>507</v>
-      </c>
-      <c r="E155" s="85"/>
-    </row>
-    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="90"/>
-      <c r="B156" s="91" t="s">
-        <v>500</v>
-      </c>
-      <c r="C156" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D156" s="85" t="s">
-        <v>508</v>
-      </c>
-      <c r="E156" s="85"/>
-    </row>
-    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="90"/>
-      <c r="B157" s="91" t="s">
-        <v>501</v>
-      </c>
-      <c r="C157" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D157" s="85" t="s">
-        <v>509</v>
-      </c>
-      <c r="E157" s="85"/>
-    </row>
-    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="90"/>
-      <c r="B158" s="91" t="s">
-        <v>502</v>
-      </c>
-      <c r="C158" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D158" s="85" t="s">
-        <v>510</v>
-      </c>
-      <c r="E158" s="85"/>
-    </row>
-    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="90"/>
-      <c r="B159" s="91" t="s">
-        <v>503</v>
-      </c>
-      <c r="C159" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D159" s="85" t="s">
-        <v>511</v>
-      </c>
-      <c r="E159" s="85"/>
-    </row>
-    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="90"/>
-      <c r="B160" s="91" t="s">
-        <v>504</v>
-      </c>
-      <c r="C160" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D160" s="85" t="s">
-        <v>512</v>
-      </c>
-      <c r="E160" s="85"/>
-    </row>
-    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="90"/>
-      <c r="B161" s="91" t="s">
-        <v>513</v>
-      </c>
-      <c r="C161" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D161" s="85" t="s">
-        <v>514</v>
-      </c>
-      <c r="E161" s="85"/>
-    </row>
-    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="90"/>
-      <c r="B162" s="91" t="s">
-        <v>515</v>
-      </c>
-      <c r="C162" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D162" s="85" t="s">
-        <v>518</v>
-      </c>
-      <c r="E162" s="85"/>
-    </row>
-    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="90"/>
-      <c r="B163" s="91" t="s">
-        <v>516</v>
-      </c>
-      <c r="C163" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D163" s="85" t="s">
-        <v>519</v>
-      </c>
-      <c r="E163" s="85"/>
-    </row>
-    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="90"/>
-      <c r="B164" s="91" t="s">
-        <v>517</v>
-      </c>
-      <c r="C164" s="85" t="s">
-        <v>339</v>
-      </c>
-      <c r="D164" s="85" t="s">
-        <v>520</v>
-      </c>
-      <c r="E164" s="85"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="83" t="s">
+      <c r="C167" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D167" s="84" t="s">
         <v>525</v>
       </c>
-      <c r="C165" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D165" s="84" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="83" t="s">
+    </row>
+    <row r="168" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="98"/>
+      <c r="B168" s="91" t="s">
         <v>526</v>
       </c>
-      <c r="C166" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D166" s="84" t="s">
+      <c r="C168" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D168" s="85" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="83" t="s">
+      <c r="E168" s="85"/>
+    </row>
+    <row r="169" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="98"/>
+      <c r="B169" s="91" t="s">
         <v>528</v>
       </c>
-      <c r="C167" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D167" s="84" t="s">
+      <c r="C169" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D169" s="85" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="83" t="s">
+      <c r="E169" s="85"/>
+    </row>
+    <row r="170" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="98"/>
+      <c r="B170" s="91" t="s">
         <v>530</v>
       </c>
-      <c r="C168" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D168" s="84" t="s">
+      <c r="C170" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D170" s="85" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B169" s="83" t="s">
+      <c r="E170" s="85"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="97"/>
+      <c r="B171" s="83" t="s">
         <v>532</v>
       </c>
-      <c r="C169" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D169" s="84" t="s">
+      <c r="C171" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D171" s="84" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="83" t="s">
+    <row r="172" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="98"/>
+      <c r="B172" s="91" t="s">
         <v>534</v>
       </c>
-      <c r="C170" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D170" s="84" t="s">
+      <c r="C172" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="D172" s="85" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="83" t="s">
-        <v>536</v>
-      </c>
-      <c r="C171" s="84" t="s">
-        <v>339</v>
-      </c>
-      <c r="D171" s="84" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B172" s="83" t="s">
-        <v>538</v>
-      </c>
-      <c r="C172" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D172" s="84" t="s">
-        <v>539</v>
-      </c>
+      <c r="E172" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added code to read from indicator list & print indicator cards
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7299FCA7-D83B-4EA8-8B91-C1A8B6D8063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331CB209-DDED-40D7-BEFA-8E80C463C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="45" windowWidth="13455" windowHeight="15465" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -5984,7 +5984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated worksheets and erbpedia docs
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331CB209-DDED-40D7-BEFA-8E80C463C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DDDBA7-70A9-49F0-A6A8-24DC351D5287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="550">
   <si>
     <t>ID</t>
   </si>
@@ -1665,6 +1665,30 @@
   </si>
   <si>
     <t>FAQ</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Facilitation Tips</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Capacity Considerations</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Additional Resources 2</t>
+  </si>
+  <si>
+    <t>Youth Engagement Image: Additional Resources 1</t>
   </si>
 </sst>
 </file>
@@ -2195,12 +2219,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2221,6 +2239,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2615,10 +2639,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="95" t="s">
+      <c r="G2" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="96"/>
+      <c r="H2" s="106"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5982,10 +6006,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6013,20 +6037,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106"/>
+      <c r="A2" s="104"/>
       <c r="B2" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="99" t="s">
+      <c r="C2" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="99"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="98"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="91" t="s">
         <v>60</v>
       </c>
@@ -6039,7 +6063,7 @@
       <c r="E3" s="85"/>
     </row>
     <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="91" t="s">
         <v>61</v>
       </c>
@@ -6052,7 +6076,7 @@
       <c r="E4" s="85"/>
     </row>
     <row r="5" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="91" t="s">
         <v>62</v>
       </c>
@@ -6065,7 +6089,7 @@
       <c r="E5" s="85"/>
     </row>
     <row r="6" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="98"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="91" t="s">
         <v>63</v>
       </c>
@@ -6078,7 +6102,7 @@
       <c r="E6" s="85"/>
     </row>
     <row r="7" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="91" t="s">
         <v>64</v>
       </c>
@@ -6091,7 +6115,7 @@
       <c r="E7" s="85"/>
     </row>
     <row r="8" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
+      <c r="A8" s="96"/>
       <c r="B8" s="91" t="s">
         <v>65</v>
       </c>
@@ -6104,7 +6128,7 @@
       <c r="E8" s="85"/>
     </row>
     <row r="9" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="91" t="s">
         <v>260</v>
       </c>
@@ -6117,7 +6141,7 @@
       <c r="E9" s="85"/>
     </row>
     <row r="10" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
+      <c r="A10" s="96"/>
       <c r="B10" s="91" t="s">
         <v>262</v>
       </c>
@@ -6130,7 +6154,7 @@
       <c r="E10" s="85"/>
     </row>
     <row r="11" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="98"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="91" t="s">
         <v>152</v>
       </c>
@@ -6143,7 +6167,7 @@
       <c r="E11" s="85"/>
     </row>
     <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
+      <c r="A12" s="96"/>
       <c r="B12" s="91" t="s">
         <v>517</v>
       </c>
@@ -6156,7 +6180,7 @@
       <c r="E12" s="85"/>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="91" t="s">
         <v>157</v>
       </c>
@@ -6169,7 +6193,7 @@
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="91" t="s">
         <v>158</v>
       </c>
@@ -6182,7 +6206,7 @@
       <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="98"/>
+      <c r="A15" s="96"/>
       <c r="B15" s="91" t="s">
         <v>159</v>
       </c>
@@ -6195,7 +6219,7 @@
       <c r="E15" s="85"/>
     </row>
     <row r="16" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="91" t="s">
         <v>160</v>
       </c>
@@ -6208,7 +6232,7 @@
       <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="91" t="s">
         <v>264</v>
       </c>
@@ -6221,7 +6245,7 @@
       <c r="E17" s="85"/>
     </row>
     <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
+      <c r="A18" s="96"/>
       <c r="B18" s="91" t="s">
         <v>265</v>
       </c>
@@ -6234,7 +6258,7 @@
       <c r="E18" s="85"/>
     </row>
     <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
+      <c r="A19" s="96"/>
       <c r="B19" s="91" t="s">
         <v>266</v>
       </c>
@@ -6247,7 +6271,7 @@
       <c r="E19" s="85"/>
     </row>
     <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="98"/>
+      <c r="A20" s="96"/>
       <c r="B20" s="91" t="s">
         <v>267</v>
       </c>
@@ -6260,7 +6284,7 @@
       <c r="E20" s="85"/>
     </row>
     <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="91" t="s">
         <v>268</v>
       </c>
@@ -6273,7 +6297,7 @@
       <c r="E21" s="85"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
+      <c r="A22" s="96"/>
       <c r="B22" s="91" t="s">
         <v>153</v>
       </c>
@@ -6286,7 +6310,7 @@
       <c r="E22" s="85"/>
     </row>
     <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
+      <c r="A23" s="96"/>
       <c r="B23" s="91" t="s">
         <v>161</v>
       </c>
@@ -6299,7 +6323,7 @@
       <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
+      <c r="A24" s="96"/>
       <c r="B24" s="91" t="s">
         <v>162</v>
       </c>
@@ -6312,7 +6336,7 @@
       <c r="E24" s="85"/>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="91" t="s">
         <v>163</v>
       </c>
@@ -6325,7 +6349,7 @@
       <c r="E25" s="85"/>
     </row>
     <row r="26" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="98"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="91" t="s">
         <v>164</v>
       </c>
@@ -6338,7 +6362,7 @@
       <c r="E26" s="85"/>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="91" t="s">
         <v>165</v>
       </c>
@@ -6351,7 +6375,7 @@
       <c r="E27" s="85"/>
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="98"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="91" t="s">
         <v>271</v>
       </c>
@@ -6364,7 +6388,7 @@
       <c r="E28" s="85"/>
     </row>
     <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="98"/>
+      <c r="A29" s="96"/>
       <c r="B29" s="91" t="s">
         <v>272</v>
       </c>
@@ -6377,7 +6401,7 @@
       <c r="E29" s="85"/>
     </row>
     <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="98"/>
+      <c r="A30" s="96"/>
       <c r="B30" s="91" t="s">
         <v>274</v>
       </c>
@@ -6390,7 +6414,7 @@
       <c r="E30" s="85"/>
     </row>
     <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="98"/>
+      <c r="A31" s="96"/>
       <c r="B31" s="91" t="s">
         <v>276</v>
       </c>
@@ -6403,7 +6427,7 @@
       <c r="E31" s="85"/>
     </row>
     <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="98"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="91" t="s">
         <v>154</v>
       </c>
@@ -6416,7 +6440,7 @@
       <c r="E32" s="85"/>
     </row>
     <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="98"/>
+      <c r="A33" s="96"/>
       <c r="B33" s="91" t="s">
         <v>166</v>
       </c>
@@ -6429,7 +6453,7 @@
       <c r="E33" s="85"/>
     </row>
     <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="98"/>
+      <c r="A34" s="96"/>
       <c r="B34" s="91" t="s">
         <v>167</v>
       </c>
@@ -6442,7 +6466,7 @@
       <c r="E34" s="85"/>
     </row>
     <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="98"/>
+      <c r="A35" s="96"/>
       <c r="B35" s="91" t="s">
         <v>168</v>
       </c>
@@ -6455,7 +6479,7 @@
       <c r="E35" s="85"/>
     </row>
     <row r="36" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="98"/>
+      <c r="A36" s="96"/>
       <c r="B36" s="91" t="s">
         <v>169</v>
       </c>
@@ -6468,7 +6492,7 @@
       <c r="E36" s="85"/>
     </row>
     <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="98"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="91" t="s">
         <v>170</v>
       </c>
@@ -6481,7 +6505,7 @@
       <c r="E37" s="85"/>
     </row>
     <row r="38" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="98"/>
+      <c r="A38" s="96"/>
       <c r="B38" s="91" t="s">
         <v>171</v>
       </c>
@@ -6494,7 +6518,7 @@
       <c r="E38" s="85"/>
     </row>
     <row r="39" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="98"/>
+      <c r="A39" s="96"/>
       <c r="B39" s="91" t="s">
         <v>172</v>
       </c>
@@ -6507,7 +6531,7 @@
       <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="98"/>
+      <c r="A40" s="96"/>
       <c r="B40" s="91" t="s">
         <v>278</v>
       </c>
@@ -6519,268 +6543,268 @@
       </c>
       <c r="E40" s="85"/>
     </row>
-    <row r="41" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="100"/>
-      <c r="B41" s="101" t="s">
+    <row r="41" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="98"/>
+      <c r="B41" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="C41" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="102" t="s">
+      <c r="C41" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="100" t="s">
         <v>280</v>
       </c>
-      <c r="E41" s="102"/>
-    </row>
-    <row r="42" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="100"/>
-      <c r="B42" s="101" t="s">
+      <c r="E41" s="100"/>
+    </row>
+    <row r="42" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="98"/>
+      <c r="B42" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="102" t="s">
+      <c r="C42" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="E42" s="102"/>
-    </row>
-    <row r="43" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="100"/>
-      <c r="B43" s="101" t="s">
+      <c r="E42" s="100"/>
+    </row>
+    <row r="43" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="98"/>
+      <c r="B43" s="99" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="102" t="s">
+      <c r="C43" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="102"/>
-    </row>
-    <row r="44" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="100"/>
-      <c r="B44" s="101" t="s">
+      <c r="E43" s="100"/>
+    </row>
+    <row r="44" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="98"/>
+      <c r="B44" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="102" t="s">
+      <c r="C44" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" s="100" t="s">
         <v>282</v>
       </c>
-      <c r="E44" s="102"/>
-    </row>
-    <row r="45" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="100"/>
-      <c r="B45" s="101" t="s">
+      <c r="E44" s="100"/>
+    </row>
+    <row r="45" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="98"/>
+      <c r="B45" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="102" t="s">
+      <c r="C45" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="E45" s="102"/>
-    </row>
-    <row r="46" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="100"/>
-      <c r="B46" s="101" t="s">
+      <c r="E45" s="100"/>
+    </row>
+    <row r="46" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="98"/>
+      <c r="B46" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="102" t="s">
+      <c r="C46" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="E46" s="102"/>
-    </row>
-    <row r="47" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="100"/>
-      <c r="B47" s="101" t="s">
+      <c r="E46" s="100"/>
+    </row>
+    <row r="47" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="98"/>
+      <c r="B47" s="99" t="s">
         <v>285</v>
       </c>
-      <c r="C47" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="102" t="s">
+      <c r="C47" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="100" t="s">
         <v>286</v>
       </c>
-      <c r="E47" s="102"/>
-    </row>
-    <row r="48" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="100"/>
-      <c r="B48" s="101" t="s">
+      <c r="E47" s="100"/>
+    </row>
+    <row r="48" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="98"/>
+      <c r="B48" s="99" t="s">
         <v>287</v>
       </c>
-      <c r="C48" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="102" t="s">
+      <c r="C48" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="E48" s="102"/>
-    </row>
-    <row r="49" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="100"/>
-      <c r="B49" s="101" t="s">
+      <c r="E48" s="100"/>
+    </row>
+    <row r="49" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="98"/>
+      <c r="B49" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="C49" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="102" t="s">
+      <c r="C49" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="102"/>
-    </row>
-    <row r="50" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="100"/>
-      <c r="B50" s="101" t="s">
+      <c r="E49" s="100"/>
+    </row>
+    <row r="50" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="98"/>
+      <c r="B50" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="C50" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="102" t="s">
+      <c r="C50" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="102"/>
-    </row>
-    <row r="51" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="100"/>
-      <c r="B51" s="101" t="s">
+      <c r="E50" s="100"/>
+    </row>
+    <row r="51" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="98"/>
+      <c r="B51" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="C51" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="102" t="s">
+      <c r="C51" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="E51" s="102"/>
-    </row>
-    <row r="52" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="100"/>
-      <c r="B52" s="101" t="s">
+      <c r="E51" s="100"/>
+    </row>
+    <row r="52" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="98"/>
+      <c r="B52" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="102" t="s">
+      <c r="C52" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="102"/>
-    </row>
-    <row r="53" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="100"/>
-      <c r="B53" s="101" t="s">
+      <c r="E52" s="100"/>
+    </row>
+    <row r="53" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="98"/>
+      <c r="B53" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="102" t="s">
+      <c r="C53" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="102"/>
-    </row>
-    <row r="54" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="100"/>
-      <c r="B54" s="101" t="s">
+      <c r="E53" s="100"/>
+    </row>
+    <row r="54" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="98"/>
+      <c r="B54" s="99" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="102" t="s">
+      <c r="C54" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D54" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="E54" s="102"/>
-    </row>
-    <row r="55" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="100"/>
-      <c r="B55" s="101" t="s">
+      <c r="E54" s="100"/>
+    </row>
+    <row r="55" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="98"/>
+      <c r="B55" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="102" t="s">
+      <c r="C55" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="102"/>
-    </row>
-    <row r="56" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="100"/>
-      <c r="B56" s="101" t="s">
+      <c r="E55" s="100"/>
+    </row>
+    <row r="56" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="98"/>
+      <c r="B56" s="99" t="s">
         <v>181</v>
       </c>
-      <c r="C56" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="102" t="s">
+      <c r="C56" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="102"/>
-    </row>
-    <row r="57" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="100"/>
-      <c r="B57" s="101" t="s">
+      <c r="E56" s="100"/>
+    </row>
+    <row r="57" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="98"/>
+      <c r="B57" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="102" t="s">
+      <c r="C57" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="E57" s="102"/>
-    </row>
-    <row r="58" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="100"/>
-      <c r="B58" s="101" t="s">
+      <c r="E57" s="100"/>
+    </row>
+    <row r="58" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="98"/>
+      <c r="B58" s="99" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="102" t="s">
+      <c r="C58" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="E58" s="102"/>
-    </row>
-    <row r="59" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="100"/>
-      <c r="B59" s="101" t="s">
+      <c r="E58" s="100"/>
+    </row>
+    <row r="59" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="98"/>
+      <c r="B59" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="C59" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="102" t="s">
+      <c r="C59" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="102"/>
-    </row>
-    <row r="60" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="100"/>
-      <c r="B60" s="101" t="s">
+      <c r="E59" s="100"/>
+    </row>
+    <row r="60" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="98"/>
+      <c r="B60" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="102" t="s">
+      <c r="C60" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="E60" s="102"/>
+      <c r="E60" s="100"/>
     </row>
     <row r="61" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="98"/>
+      <c r="A61" s="96"/>
       <c r="B61" s="91" t="s">
         <v>186</v>
       </c>
@@ -6793,7 +6817,7 @@
       <c r="E61" s="85"/>
     </row>
     <row r="62" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="98"/>
+      <c r="A62" s="96"/>
       <c r="B62" s="91" t="s">
         <v>297</v>
       </c>
@@ -6806,7 +6830,7 @@
       <c r="E62" s="85"/>
     </row>
     <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="98"/>
+      <c r="A63" s="96"/>
       <c r="B63" s="91" t="s">
         <v>299</v>
       </c>
@@ -6819,7 +6843,7 @@
       <c r="E63" s="85"/>
     </row>
     <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
+      <c r="A64" s="95"/>
       <c r="B64" s="91" t="s">
         <v>300</v>
       </c>
@@ -6832,7 +6856,7 @@
       <c r="E64" s="85"/>
     </row>
     <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
+      <c r="A65" s="95"/>
       <c r="B65" s="91" t="s">
         <v>303</v>
       </c>
@@ -6845,7 +6869,7 @@
       <c r="E65" s="85"/>
     </row>
     <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
+      <c r="A66" s="95"/>
       <c r="B66" s="91" t="s">
         <v>305</v>
       </c>
@@ -6858,7 +6882,7 @@
       <c r="E66" s="85"/>
     </row>
     <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="97"/>
+      <c r="A67" s="95"/>
       <c r="B67" s="91" t="s">
         <v>307</v>
       </c>
@@ -6871,7 +6895,7 @@
       <c r="E67" s="85"/>
     </row>
     <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="97"/>
+      <c r="A68" s="95"/>
       <c r="B68" s="91" t="s">
         <v>309</v>
       </c>
@@ -6884,7 +6908,7 @@
       <c r="E68" s="85"/>
     </row>
     <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="97"/>
+      <c r="A69" s="95"/>
       <c r="B69" s="91" t="s">
         <v>311</v>
       </c>
@@ -6897,7 +6921,7 @@
       <c r="E69" s="85"/>
     </row>
     <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="97"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="91" t="s">
         <v>313</v>
       </c>
@@ -6910,7 +6934,7 @@
       <c r="E70" s="85"/>
     </row>
     <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="97"/>
+      <c r="A71" s="95"/>
       <c r="B71" s="91" t="s">
         <v>315</v>
       </c>
@@ -6923,7 +6947,7 @@
       <c r="E71" s="85"/>
     </row>
     <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="97"/>
+      <c r="A72" s="95"/>
       <c r="B72" s="91" t="s">
         <v>317</v>
       </c>
@@ -6935,21 +6959,21 @@
       </c>
       <c r="E72" s="85"/>
     </row>
-    <row r="73" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="100"/>
-      <c r="B73" s="101" t="s">
+    <row r="73" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="98"/>
+      <c r="B73" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="C73" s="102" t="s">
+      <c r="C73" s="100" t="s">
         <v>301</v>
       </c>
-      <c r="D73" s="102" t="s">
+      <c r="D73" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="E73" s="102"/>
+      <c r="E73" s="100"/>
     </row>
     <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="97"/>
+      <c r="A74" s="95"/>
       <c r="B74" s="91" t="s">
         <v>321</v>
       </c>
@@ -6962,7 +6986,7 @@
       <c r="E74" s="85"/>
     </row>
     <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="97"/>
+      <c r="A75" s="95"/>
       <c r="B75" s="91" t="s">
         <v>323</v>
       </c>
@@ -6975,7 +6999,7 @@
       <c r="E75" s="85"/>
     </row>
     <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="97"/>
+      <c r="A76" s="95"/>
       <c r="B76" s="91" t="s">
         <v>324</v>
       </c>
@@ -6988,7 +7012,7 @@
       <c r="E76" s="85"/>
     </row>
     <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="97"/>
+      <c r="A77" s="95"/>
       <c r="B77" s="91" t="s">
         <v>326</v>
       </c>
@@ -7001,7 +7025,7 @@
       <c r="E77" s="85"/>
     </row>
     <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="97"/>
+      <c r="A78" s="95"/>
       <c r="B78" s="91" t="s">
         <v>328</v>
       </c>
@@ -7014,7 +7038,7 @@
       <c r="E78" s="85"/>
     </row>
     <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="97"/>
+      <c r="A79" s="95"/>
       <c r="B79" s="91" t="s">
         <v>330</v>
       </c>
@@ -7027,7 +7051,7 @@
       <c r="E79" s="85"/>
     </row>
     <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="97"/>
+      <c r="A80" s="95"/>
       <c r="B80" s="91" t="s">
         <v>332</v>
       </c>
@@ -7040,7 +7064,7 @@
       <c r="E80" s="85"/>
     </row>
     <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="97"/>
+      <c r="A81" s="95"/>
       <c r="B81" s="91" t="s">
         <v>334</v>
       </c>
@@ -7053,7 +7077,7 @@
       <c r="E81" s="85"/>
     </row>
     <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="97"/>
+      <c r="A82" s="95"/>
       <c r="B82" s="91" t="s">
         <v>337</v>
       </c>
@@ -7066,7 +7090,7 @@
       <c r="E82" s="85"/>
     </row>
     <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="97"/>
+      <c r="A83" s="95"/>
       <c r="B83" s="91" t="s">
         <v>339</v>
       </c>
@@ -7079,7 +7103,7 @@
       <c r="E83" s="85"/>
     </row>
     <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="97"/>
+      <c r="A84" s="95"/>
       <c r="B84" s="91" t="s">
         <v>341</v>
       </c>
@@ -7092,7 +7116,7 @@
       <c r="E84" s="85"/>
     </row>
     <row r="85" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="97"/>
+      <c r="A85" s="95"/>
       <c r="B85" s="91" t="s">
         <v>342</v>
       </c>
@@ -7105,7 +7129,7 @@
       <c r="E85" s="85"/>
     </row>
     <row r="86" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="97"/>
+      <c r="A86" s="95"/>
       <c r="B86" s="91" t="s">
         <v>343</v>
       </c>
@@ -7120,7 +7144,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="97"/>
+      <c r="A87" s="95"/>
       <c r="B87" s="91" t="s">
         <v>346</v>
       </c>
@@ -7134,98 +7158,98 @@
         <v>358</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="100"/>
-      <c r="B88" s="101" t="s">
+    <row r="88" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="98"/>
+      <c r="B88" s="99" t="s">
         <v>349</v>
       </c>
-      <c r="C88" s="102" t="s">
+      <c r="C88" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D88" s="102" t="s">
+      <c r="D88" s="100" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="104" t="s">
+      <c r="E88" s="102" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="100"/>
-      <c r="B89" s="101" t="s">
+    <row r="89" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="98"/>
+      <c r="B89" s="99" t="s">
         <v>350</v>
       </c>
-      <c r="C89" s="102" t="s">
+      <c r="C89" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D89" s="102" t="s">
+      <c r="D89" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="E89" s="104" t="s">
+      <c r="E89" s="102" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="100"/>
-      <c r="B90" s="101" t="s">
+    <row r="90" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="98"/>
+      <c r="B90" s="99" t="s">
         <v>351</v>
       </c>
-      <c r="C90" s="102" t="s">
+      <c r="C90" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D90" s="102" t="s">
+      <c r="D90" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="E90" s="104" t="s">
+      <c r="E90" s="102" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="100"/>
-      <c r="B91" s="101" t="s">
+    <row r="91" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="98"/>
+      <c r="B91" s="99" t="s">
         <v>352</v>
       </c>
-      <c r="C91" s="102" t="s">
+      <c r="C91" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D91" s="102" t="s">
+      <c r="D91" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E91" s="104" t="s">
+      <c r="E91" s="102" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="100"/>
-      <c r="B92" s="101" t="s">
+    <row r="92" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="98"/>
+      <c r="B92" s="99" t="s">
         <v>353</v>
       </c>
-      <c r="C92" s="102" t="s">
+      <c r="C92" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D92" s="102" t="s">
+      <c r="D92" s="100" t="s">
         <v>354</v>
       </c>
-      <c r="E92" s="104" t="s">
+      <c r="E92" s="102" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="100"/>
-      <c r="B93" s="101" t="s">
+    <row r="93" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="98"/>
+      <c r="B93" s="99" t="s">
         <v>356</v>
       </c>
-      <c r="C93" s="102" t="s">
+      <c r="C93" s="100" t="s">
         <v>348</v>
       </c>
-      <c r="D93" s="102" t="s">
+      <c r="D93" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="E93" s="104" t="s">
+      <c r="E93" s="102" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="98"/>
+      <c r="A94" s="96"/>
       <c r="B94" s="91" t="s">
         <v>359</v>
       </c>
@@ -7238,7 +7262,7 @@
       <c r="E94" s="85"/>
     </row>
     <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="98"/>
+      <c r="A95" s="96"/>
       <c r="B95" s="91" t="s">
         <v>361</v>
       </c>
@@ -7251,7 +7275,7 @@
       <c r="E95" s="85"/>
     </row>
     <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="98"/>
+      <c r="A96" s="96"/>
       <c r="B96" s="91" t="s">
         <v>362</v>
       </c>
@@ -7264,7 +7288,7 @@
       <c r="E96" s="85"/>
     </row>
     <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="98"/>
+      <c r="A97" s="96"/>
       <c r="B97" s="91" t="s">
         <v>364</v>
       </c>
@@ -7277,7 +7301,7 @@
       <c r="E97" s="85"/>
     </row>
     <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="98"/>
+      <c r="A98" s="96"/>
       <c r="B98" s="91" t="s">
         <v>366</v>
       </c>
@@ -7290,7 +7314,7 @@
       <c r="E98" s="85"/>
     </row>
     <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="98"/>
+      <c r="A99" s="96"/>
       <c r="B99" s="91" t="s">
         <v>368</v>
       </c>
@@ -7303,7 +7327,7 @@
       <c r="E99" s="85"/>
     </row>
     <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="98"/>
+      <c r="A100" s="96"/>
       <c r="B100" s="91" t="s">
         <v>370</v>
       </c>
@@ -7316,7 +7340,7 @@
       <c r="E100" s="85"/>
     </row>
     <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="98"/>
+      <c r="A101" s="96"/>
       <c r="B101" s="91" t="s">
         <v>374</v>
       </c>
@@ -7329,7 +7353,7 @@
       <c r="E101" s="85"/>
     </row>
     <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="98"/>
+      <c r="A102" s="96"/>
       <c r="B102" s="91" t="s">
         <v>376</v>
       </c>
@@ -7342,7 +7366,7 @@
       <c r="E102" s="85"/>
     </row>
     <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="98"/>
+      <c r="A103" s="96"/>
       <c r="B103" s="91" t="s">
         <v>378</v>
       </c>
@@ -7355,7 +7379,7 @@
       <c r="E103" s="85"/>
     </row>
     <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="98"/>
+      <c r="A104" s="96"/>
       <c r="B104" s="91" t="s">
         <v>380</v>
       </c>
@@ -7368,7 +7392,7 @@
       <c r="E104" s="85"/>
     </row>
     <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="98"/>
+      <c r="A105" s="96"/>
       <c r="B105" s="91" t="s">
         <v>381</v>
       </c>
@@ -7381,7 +7405,7 @@
       <c r="E105" s="85"/>
     </row>
     <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="98"/>
+      <c r="A106" s="96"/>
       <c r="B106" s="91" t="s">
         <v>382</v>
       </c>
@@ -7394,7 +7418,7 @@
       <c r="E106" s="85"/>
     </row>
     <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="98"/>
+      <c r="A107" s="96"/>
       <c r="B107" s="91" t="s">
         <v>383</v>
       </c>
@@ -7407,7 +7431,7 @@
       <c r="E107" s="85"/>
     </row>
     <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="98"/>
+      <c r="A108" s="96"/>
       <c r="B108" s="91" t="s">
         <v>385</v>
       </c>
@@ -7420,7 +7444,7 @@
       <c r="E108" s="85"/>
     </row>
     <row r="109" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="98"/>
+      <c r="A109" s="96"/>
       <c r="B109" s="91" t="s">
         <v>187</v>
       </c>
@@ -7433,7 +7457,7 @@
       <c r="E109" s="85"/>
     </row>
     <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="98"/>
+      <c r="A110" s="96"/>
       <c r="B110" s="91" t="s">
         <v>388</v>
       </c>
@@ -7446,7 +7470,7 @@
       <c r="E110" s="85"/>
     </row>
     <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="98"/>
+      <c r="A111" s="96"/>
       <c r="B111" s="91" t="s">
         <v>372</v>
       </c>
@@ -7459,7 +7483,7 @@
       <c r="E111" s="85"/>
     </row>
     <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="98"/>
+      <c r="A112" s="96"/>
       <c r="B112" s="91" t="s">
         <v>373</v>
       </c>
@@ -7472,7 +7496,7 @@
       <c r="E112" s="85"/>
     </row>
     <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="98"/>
+      <c r="A113" s="96"/>
       <c r="B113" s="91" t="s">
         <v>391</v>
       </c>
@@ -7485,7 +7509,7 @@
       <c r="E113" s="85"/>
     </row>
     <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="97"/>
+      <c r="A114" s="95"/>
       <c r="B114" s="91" t="s">
         <v>392</v>
       </c>
@@ -7498,7 +7522,7 @@
       <c r="E114" s="85"/>
     </row>
     <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="97"/>
+      <c r="A115" s="95"/>
       <c r="B115" s="91" t="s">
         <v>394</v>
       </c>
@@ -7511,7 +7535,7 @@
       <c r="E115" s="85"/>
     </row>
     <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="98"/>
+      <c r="A116" s="96"/>
       <c r="B116" s="91" t="s">
         <v>396</v>
       </c>
@@ -7523,21 +7547,21 @@
       </c>
       <c r="E116" s="85"/>
     </row>
-    <row r="117" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="100"/>
-      <c r="B117" s="101" t="s">
+    <row r="117" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="98"/>
+      <c r="B117" s="99" t="s">
         <v>398</v>
       </c>
-      <c r="C117" s="102" t="s">
+      <c r="C117" s="100" t="s">
         <v>335</v>
       </c>
-      <c r="D117" s="102" t="s">
+      <c r="D117" s="100" t="s">
         <v>399</v>
       </c>
-      <c r="E117" s="102"/>
+      <c r="E117" s="100"/>
     </row>
     <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="98"/>
+      <c r="A118" s="96"/>
       <c r="B118" s="91" t="s">
         <v>400</v>
       </c>
@@ -7550,7 +7574,7 @@
       <c r="E118" s="85"/>
     </row>
     <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="97"/>
+      <c r="A119" s="95"/>
       <c r="B119" s="91" t="s">
         <v>402</v>
       </c>
@@ -7563,7 +7587,7 @@
       <c r="E119" s="85"/>
     </row>
     <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="97"/>
+      <c r="A120" s="95"/>
       <c r="B120" s="91" t="s">
         <v>404</v>
       </c>
@@ -7576,7 +7600,7 @@
       <c r="E120" s="85"/>
     </row>
     <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="97"/>
+      <c r="A121" s="95"/>
       <c r="B121" s="91" t="s">
         <v>188</v>
       </c>
@@ -7589,7 +7613,7 @@
       <c r="E121" s="85"/>
     </row>
     <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="97"/>
+      <c r="A122" s="95"/>
       <c r="B122" s="91" t="s">
         <v>407</v>
       </c>
@@ -7602,7 +7626,7 @@
       <c r="E122" s="85"/>
     </row>
     <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="97"/>
+      <c r="A123" s="95"/>
       <c r="B123" s="91" t="s">
         <v>408</v>
       </c>
@@ -7615,7 +7639,7 @@
       <c r="E123" s="85"/>
     </row>
     <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="98"/>
+      <c r="A124" s="96"/>
       <c r="B124" s="91" t="s">
         <v>411</v>
       </c>
@@ -7628,7 +7652,7 @@
       <c r="E124" s="85"/>
     </row>
     <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="98"/>
+      <c r="A125" s="96"/>
       <c r="B125" s="91" t="s">
         <v>413</v>
       </c>
@@ -7641,7 +7665,7 @@
       <c r="E125" s="85"/>
     </row>
     <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="98"/>
+      <c r="A126" s="96"/>
       <c r="B126" s="91" t="s">
         <v>415</v>
       </c>
@@ -7654,7 +7678,7 @@
       <c r="E126" s="85"/>
     </row>
     <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="98"/>
+      <c r="A127" s="96"/>
       <c r="B127" s="91" t="s">
         <v>416</v>
       </c>
@@ -7667,7 +7691,7 @@
       <c r="E127" s="85"/>
     </row>
     <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="98"/>
+      <c r="A128" s="96"/>
       <c r="B128" s="91" t="s">
         <v>418</v>
       </c>
@@ -7680,7 +7704,7 @@
       <c r="E128" s="85"/>
     </row>
     <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="98"/>
+      <c r="A129" s="96"/>
       <c r="B129" s="91" t="s">
         <v>420</v>
       </c>
@@ -7693,7 +7717,7 @@
       <c r="E129" s="85"/>
     </row>
     <row r="130" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="98"/>
+      <c r="A130" s="96"/>
       <c r="B130" s="91" t="s">
         <v>189</v>
       </c>
@@ -7706,7 +7730,7 @@
       <c r="E130" s="85"/>
     </row>
     <row r="131" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="98"/>
+      <c r="A131" s="96"/>
       <c r="B131" s="91" t="s">
         <v>190</v>
       </c>
@@ -7719,7 +7743,7 @@
       <c r="E131" s="85"/>
     </row>
     <row r="132" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="98"/>
+      <c r="A132" s="96"/>
       <c r="B132" s="91" t="s">
         <v>423</v>
       </c>
@@ -7732,7 +7756,7 @@
       <c r="E132" s="85"/>
     </row>
     <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="98"/>
+      <c r="A133" s="96"/>
       <c r="B133" s="91" t="s">
         <v>425</v>
       </c>
@@ -7745,7 +7769,7 @@
       <c r="E133" s="85"/>
     </row>
     <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="98"/>
+      <c r="A134" s="96"/>
       <c r="B134" s="91" t="s">
         <v>427</v>
       </c>
@@ -7758,7 +7782,7 @@
       <c r="E134" s="85"/>
     </row>
     <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="98"/>
+      <c r="A135" s="96"/>
       <c r="B135" s="91" t="s">
         <v>428</v>
       </c>
@@ -7771,7 +7795,7 @@
       <c r="E135" s="85"/>
     </row>
     <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="98"/>
+      <c r="A136" s="96"/>
       <c r="B136" s="91" t="s">
         <v>430</v>
       </c>
@@ -7784,7 +7808,7 @@
       <c r="E136" s="85"/>
     </row>
     <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="98"/>
+      <c r="A137" s="96"/>
       <c r="B137" s="91" t="s">
         <v>432</v>
       </c>
@@ -7797,7 +7821,7 @@
       <c r="E137" s="85"/>
     </row>
     <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="98"/>
+      <c r="A138" s="96"/>
       <c r="B138" s="91" t="s">
         <v>433</v>
       </c>
@@ -7810,7 +7834,7 @@
       <c r="E138" s="85"/>
     </row>
     <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="98"/>
+      <c r="A139" s="96"/>
       <c r="B139" s="91" t="s">
         <v>434</v>
       </c>
@@ -7823,7 +7847,7 @@
       <c r="E139" s="85"/>
     </row>
     <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="98"/>
+      <c r="A140" s="96"/>
       <c r="B140" s="91" t="s">
         <v>436</v>
       </c>
@@ -7836,7 +7860,7 @@
       <c r="E140" s="85"/>
     </row>
     <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="98"/>
+      <c r="A141" s="96"/>
       <c r="B141" s="91" t="s">
         <v>437</v>
       </c>
@@ -7849,7 +7873,7 @@
       <c r="E141" s="85"/>
     </row>
     <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="97"/>
+      <c r="A142" s="95"/>
       <c r="B142" s="91" t="s">
         <v>456</v>
       </c>
@@ -7861,21 +7885,21 @@
       </c>
       <c r="E142" s="85"/>
     </row>
-    <row r="143" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="100"/>
-      <c r="B143" s="101" t="s">
+    <row r="143" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="98"/>
+      <c r="B143" s="99" t="s">
         <v>466</v>
       </c>
-      <c r="C143" s="102" t="s">
+      <c r="C143" s="100" t="s">
         <v>301</v>
       </c>
-      <c r="D143" s="102" t="s">
+      <c r="D143" s="100" t="s">
         <v>467</v>
       </c>
-      <c r="E143" s="102"/>
+      <c r="E143" s="100"/>
     </row>
     <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="98"/>
+      <c r="A144" s="96"/>
       <c r="B144" s="91" t="s">
         <v>473</v>
       </c>
@@ -7888,7 +7912,7 @@
       <c r="E144" s="85"/>
     </row>
     <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="98"/>
+      <c r="A145" s="96"/>
       <c r="B145" s="91" t="s">
         <v>476</v>
       </c>
@@ -7901,7 +7925,7 @@
       <c r="E145" s="85"/>
     </row>
     <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="98"/>
+      <c r="A146" s="96"/>
       <c r="B146" s="91" t="s">
         <v>478</v>
       </c>
@@ -7914,7 +7938,7 @@
       <c r="E146" s="85"/>
     </row>
     <row r="147" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="105"/>
+      <c r="A147" s="103"/>
       <c r="B147" s="92" t="s">
         <v>480</v>
       </c>
@@ -7927,7 +7951,7 @@
       <c r="E147" s="93"/>
     </row>
     <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="98"/>
+      <c r="A148" s="96"/>
       <c r="B148" s="91" t="s">
         <v>482</v>
       </c>
@@ -7940,7 +7964,7 @@
       <c r="E148" s="85"/>
     </row>
     <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="98"/>
+      <c r="A149" s="96"/>
       <c r="B149" s="91" t="s">
         <v>485</v>
       </c>
@@ -7953,7 +7977,7 @@
       <c r="E149" s="85"/>
     </row>
     <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="98"/>
+      <c r="A150" s="96"/>
       <c r="B150" s="91" t="s">
         <v>487</v>
       </c>
@@ -7966,7 +7990,7 @@
       <c r="E150" s="85"/>
     </row>
     <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="98"/>
+      <c r="A151" s="96"/>
       <c r="B151" s="91" t="s">
         <v>490</v>
       </c>
@@ -7979,7 +8003,7 @@
       <c r="E151" s="85"/>
     </row>
     <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="98"/>
+      <c r="A152" s="96"/>
       <c r="B152" s="91" t="s">
         <v>491</v>
       </c>
@@ -7992,7 +8016,7 @@
       <c r="E152" s="85"/>
     </row>
     <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="98"/>
+      <c r="A153" s="96"/>
       <c r="B153" s="91" t="s">
         <v>493</v>
       </c>
@@ -8005,7 +8029,7 @@
       <c r="E153" s="85"/>
     </row>
     <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="97"/>
+      <c r="A154" s="95"/>
       <c r="B154" s="91" t="s">
         <v>494</v>
       </c>
@@ -8018,7 +8042,7 @@
       <c r="E154" s="85"/>
     </row>
     <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="97"/>
+      <c r="A155" s="95"/>
       <c r="B155" s="91" t="s">
         <v>495</v>
       </c>
@@ -8031,7 +8055,7 @@
       <c r="E155" s="85"/>
     </row>
     <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="97"/>
+      <c r="A156" s="95"/>
       <c r="B156" s="91" t="s">
         <v>496</v>
       </c>
@@ -8044,7 +8068,7 @@
       <c r="E156" s="85"/>
     </row>
     <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="97"/>
+      <c r="A157" s="95"/>
       <c r="B157" s="91" t="s">
         <v>497</v>
       </c>
@@ -8057,7 +8081,7 @@
       <c r="E157" s="85"/>
     </row>
     <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="97"/>
+      <c r="A158" s="95"/>
       <c r="B158" s="91" t="s">
         <v>498</v>
       </c>
@@ -8070,7 +8094,7 @@
       <c r="E158" s="85"/>
     </row>
     <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="97"/>
+      <c r="A159" s="95"/>
       <c r="B159" s="91" t="s">
         <v>499</v>
       </c>
@@ -8083,7 +8107,7 @@
       <c r="E159" s="85"/>
     </row>
     <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="97"/>
+      <c r="A160" s="95"/>
       <c r="B160" s="91" t="s">
         <v>500</v>
       </c>
@@ -8096,7 +8120,7 @@
       <c r="E160" s="85"/>
     </row>
     <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="97"/>
+      <c r="A161" s="95"/>
       <c r="B161" s="91" t="s">
         <v>509</v>
       </c>
@@ -8109,7 +8133,7 @@
       <c r="E161" s="85"/>
     </row>
     <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="98"/>
+      <c r="A162" s="96"/>
       <c r="B162" s="91" t="s">
         <v>511</v>
       </c>
@@ -8122,7 +8146,7 @@
       <c r="E162" s="85"/>
     </row>
     <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="98"/>
+      <c r="A163" s="96"/>
       <c r="B163" s="91" t="s">
         <v>512</v>
       </c>
@@ -8135,7 +8159,7 @@
       <c r="E163" s="85"/>
     </row>
     <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="98"/>
+      <c r="A164" s="96"/>
       <c r="B164" s="91" t="s">
         <v>513</v>
       </c>
@@ -8148,7 +8172,7 @@
       <c r="E164" s="85"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="98"/>
+      <c r="A165" s="96"/>
       <c r="B165" s="83" t="s">
         <v>521</v>
       </c>
@@ -8160,7 +8184,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="98"/>
+      <c r="A166" s="96"/>
       <c r="B166" s="91" t="s">
         <v>522</v>
       </c>
@@ -8173,7 +8197,7 @@
       <c r="E166" s="85"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="98"/>
+      <c r="A167" s="96"/>
       <c r="B167" s="83" t="s">
         <v>524</v>
       </c>
@@ -8185,7 +8209,7 @@
       </c>
     </row>
     <row r="168" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="98"/>
+      <c r="A168" s="96"/>
       <c r="B168" s="91" t="s">
         <v>526</v>
       </c>
@@ -8198,7 +8222,7 @@
       <c r="E168" s="85"/>
     </row>
     <row r="169" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="98"/>
+      <c r="A169" s="96"/>
       <c r="B169" s="91" t="s">
         <v>528</v>
       </c>
@@ -8211,7 +8235,7 @@
       <c r="E169" s="85"/>
     </row>
     <row r="170" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="98"/>
+      <c r="A170" s="96"/>
       <c r="B170" s="91" t="s">
         <v>530</v>
       </c>
@@ -8224,7 +8248,7 @@
       <c r="E170" s="85"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="97"/>
+      <c r="A171" s="95"/>
       <c r="B171" s="83" t="s">
         <v>532</v>
       </c>
@@ -8236,7 +8260,7 @@
       </c>
     </row>
     <row r="172" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="98"/>
+      <c r="A172" s="96"/>
       <c r="B172" s="91" t="s">
         <v>534</v>
       </c>
@@ -8247,6 +8271,54 @@
         <v>535</v>
       </c>
       <c r="E172" s="85"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="96"/>
+      <c r="B173" s="83" t="s">
+        <v>542</v>
+      </c>
+      <c r="C173" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D173" s="84" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="96"/>
+      <c r="B174" s="83" t="s">
+        <v>544</v>
+      </c>
+      <c r="C174" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D174" s="84" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="96"/>
+      <c r="B175" s="83" t="s">
+        <v>545</v>
+      </c>
+      <c r="C175" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D175" s="84" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="96"/>
+      <c r="B176" s="83" t="s">
+        <v>547</v>
+      </c>
+      <c r="C176" s="84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D176" s="84" t="s">
+        <v>548</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated content and grammer issues
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DDDBA7-70A9-49F0-A6A8-24DC351D5287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C9CF86-02C9-46AD-817F-6F58F99B60EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -6008,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Key Takeaways dynamic field functionality
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607D771A-691F-46C8-BFE4-36B3FA7CAA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC94D78-E1FE-41B2-8701-7243EA587646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -1760,7 +1760,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1823,24 +1823,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -2051,17 +2039,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2093,7 +2070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2255,39 +2232,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2687,10 +2643,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="106"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -6054,2405 +6010,2229 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="90" customWidth="1"/>
-    <col min="2" max="2" width="4" style="83" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="84" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" style="84" customWidth="1"/>
+    <col min="1" max="1" width="4" style="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="84" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89"/>
-      <c r="B1" s="87" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="B2" s="88" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="C2" s="88" t="s">
         <v>256</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="D2" s="88" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
-      <c r="B2" s="91" t="s">
+    <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="97" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="97" t="s">
+      <c r="B3" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="97"/>
-    </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96"/>
-      <c r="B3" s="91" t="s">
+      <c r="D3" s="93"/>
+    </row>
+    <row r="4" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="85" t="s">
+      <c r="B4" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="85" t="s">
         <v>465</v>
       </c>
-      <c r="E3" s="85"/>
-    </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96"/>
-      <c r="B4" s="91" t="s">
+      <c r="D4" s="85"/>
+    </row>
+    <row r="5" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="85" t="s">
+      <c r="B5" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="85" t="s">
         <v>470</v>
       </c>
-      <c r="E4" s="85"/>
-    </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="91" t="s">
+      <c r="D5" s="85"/>
+    </row>
+    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="85" t="s">
+      <c r="B6" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="85" t="s">
         <v>468</v>
       </c>
-      <c r="E5" s="85"/>
-    </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
-      <c r="B6" s="91" t="s">
+      <c r="D6" s="85"/>
+    </row>
+    <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="85" t="s">
+      <c r="B7" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="E6" s="85"/>
-    </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="91" t="s">
+      <c r="D7" s="85"/>
+    </row>
+    <row r="8" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D7" s="85" t="s">
+      <c r="B8" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" s="85" t="s">
         <v>475</v>
       </c>
-      <c r="E7" s="85"/>
-    </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="91" t="s">
+      <c r="D8" s="85"/>
+    </row>
+    <row r="9" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="85" t="s">
+      <c r="B9" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="85" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="85"/>
-    </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="96"/>
-      <c r="B9" s="91" t="s">
+      <c r="D9" s="85"/>
+    </row>
+    <row r="10" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="85" t="s">
+      <c r="B10" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="85" t="s">
         <v>261</v>
       </c>
-      <c r="E9" s="85"/>
-    </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="96"/>
-      <c r="B10" s="91" t="s">
+      <c r="D10" s="85"/>
+    </row>
+    <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="89" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="85" t="s">
+      <c r="B11" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="E10" s="85"/>
-    </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96"/>
-      <c r="B11" s="91" t="s">
+      <c r="D11" s="85"/>
+    </row>
+    <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="85" t="s">
+      <c r="B12" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="85" t="s">
         <v>484</v>
       </c>
-      <c r="E11" s="85"/>
-    </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="96"/>
-      <c r="B12" s="91" t="s">
+      <c r="D12" s="85"/>
+    </row>
+    <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89" t="s">
         <v>517</v>
       </c>
-      <c r="C12" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="85" t="s">
+      <c r="B13" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="85" t="s">
         <v>518</v>
       </c>
-      <c r="E12" s="85"/>
-    </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="91" t="s">
+      <c r="D13" s="85"/>
+    </row>
+    <row r="14" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" s="85" t="s">
+      <c r="B14" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="85" t="s">
         <v>536</v>
       </c>
-      <c r="E13" s="85"/>
-    </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="96"/>
-      <c r="B14" s="91" t="s">
+      <c r="D14" s="85"/>
+    </row>
+    <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D14" s="85" t="s">
+      <c r="B15" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="E14" s="85"/>
-    </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="91" t="s">
+      <c r="D15" s="85"/>
+    </row>
+    <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D15" s="85" t="s">
+      <c r="B16" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="85" t="s">
         <v>537</v>
       </c>
-      <c r="E15" s="85"/>
-    </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="96"/>
-      <c r="B16" s="91" t="s">
+      <c r="D16" s="85"/>
+    </row>
+    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D16" s="85" t="s">
+      <c r="B17" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="85"/>
-    </row>
-    <row r="17" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="91" t="s">
+      <c r="D17" s="85"/>
+    </row>
+    <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89" t="s">
         <v>264</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" s="85" t="s">
+      <c r="B18" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="85" t="s">
         <v>439</v>
       </c>
-      <c r="E17" s="85"/>
-    </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="91" t="s">
+      <c r="D18" s="85"/>
+    </row>
+    <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89" t="s">
         <v>265</v>
       </c>
-      <c r="C18" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="85" t="s">
+      <c r="B19" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="E18" s="85"/>
-    </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="91" t="s">
+      <c r="D19" s="85"/>
+    </row>
+    <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
         <v>266</v>
       </c>
-      <c r="C19" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" s="85" t="s">
+      <c r="B20" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="85" t="s">
         <v>449</v>
       </c>
-      <c r="E19" s="85"/>
-    </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="91" t="s">
+      <c r="D20" s="85"/>
+    </row>
+    <row r="21" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="C20" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="85" t="s">
+      <c r="B21" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" s="85" t="s">
         <v>458</v>
       </c>
-      <c r="E20" s="85"/>
-    </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
-      <c r="B21" s="91" t="s">
+      <c r="D21" s="85"/>
+    </row>
+    <row r="22" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
         <v>268</v>
       </c>
-      <c r="C21" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="85" t="s">
+      <c r="B22" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="85" t="s">
         <v>462</v>
       </c>
-      <c r="E21" s="85"/>
-    </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
-      <c r="B22" s="91" t="s">
+      <c r="D22" s="85"/>
+    </row>
+    <row r="23" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="85" t="s">
+      <c r="B23" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="85" t="s">
         <v>441</v>
       </c>
-      <c r="E22" s="85"/>
-    </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="96"/>
-      <c r="B23" s="91" t="s">
+      <c r="D23" s="85"/>
+    </row>
+    <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89" t="s">
         <v>161</v>
       </c>
-      <c r="C23" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="85" t="s">
+      <c r="B24" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" s="85" t="s">
         <v>538</v>
       </c>
-      <c r="E23" s="85"/>
-    </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
-      <c r="B24" s="91" t="s">
+      <c r="D24" s="85"/>
+    </row>
+    <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="85" t="s">
+      <c r="B25" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="85" t="s">
         <v>539</v>
       </c>
-      <c r="E24" s="85"/>
-    </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="96"/>
-      <c r="B25" s="91" t="s">
+      <c r="D25" s="85"/>
+    </row>
+    <row r="26" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D25" s="85" t="s">
+      <c r="B26" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="85" t="s">
         <v>540</v>
       </c>
-      <c r="E25" s="85"/>
-    </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
-      <c r="B26" s="91" t="s">
+      <c r="D26" s="85"/>
+    </row>
+    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="C26" s="85" t="s">
+      <c r="B27" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="85" t="s">
+      <c r="C27" s="85" t="s">
         <v>270</v>
       </c>
-      <c r="E26" s="85"/>
-    </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="96"/>
-      <c r="B27" s="91" t="s">
+      <c r="D27" s="85"/>
+    </row>
+    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="C27" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" s="85" t="s">
+      <c r="B28" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="85" t="s">
         <v>460</v>
       </c>
-      <c r="E27" s="85"/>
-    </row>
-    <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96"/>
-      <c r="B28" s="91" t="s">
+      <c r="D28" s="85"/>
+    </row>
+    <row r="29" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="89" t="s">
         <v>271</v>
       </c>
-      <c r="C28" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D28" s="85" t="s">
+      <c r="B29" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C29" s="85" t="s">
         <v>541</v>
       </c>
-      <c r="E28" s="85"/>
-    </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="96"/>
-      <c r="B29" s="91" t="s">
+      <c r="D29" s="85"/>
+    </row>
+    <row r="30" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="89" t="s">
         <v>272</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="B30" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="C30" s="85" t="s">
         <v>273</v>
       </c>
-      <c r="E29" s="85"/>
-    </row>
-    <row r="30" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="96"/>
-      <c r="B30" s="91" t="s">
+      <c r="D30" s="85"/>
+    </row>
+    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="89" t="s">
         <v>274</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="B31" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D30" s="85" t="s">
+      <c r="C31" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="E30" s="85"/>
-    </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="96"/>
-      <c r="B31" s="91" t="s">
+      <c r="D31" s="85"/>
+    </row>
+    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="89" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="B32" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D31" s="85" t="s">
+      <c r="C32" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="85"/>
-    </row>
-    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="96"/>
-      <c r="B32" s="91" t="s">
+      <c r="D32" s="85"/>
+    </row>
+    <row r="33" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="C32" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D32" s="85" t="s">
+      <c r="B33" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" s="85" t="s">
         <v>440</v>
       </c>
-      <c r="E32" s="85"/>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="96"/>
-      <c r="B33" s="91" t="s">
+      <c r="D33" s="85"/>
+    </row>
+    <row r="34" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="C33" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D33" s="85" t="s">
+      <c r="B34" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C34" s="85" t="s">
         <v>443</v>
       </c>
-      <c r="E33" s="85"/>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="96"/>
-      <c r="B34" s="91" t="s">
+      <c r="D34" s="85"/>
+    </row>
+    <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D34" s="85" t="s">
+      <c r="B35" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="85"/>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="96"/>
-      <c r="B35" s="91" t="s">
+      <c r="D35" s="85"/>
+    </row>
+    <row r="36" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" s="85" t="s">
+      <c r="B36" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" s="85" t="s">
         <v>448</v>
       </c>
-      <c r="E35" s="85"/>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="96"/>
-      <c r="B36" s="91" t="s">
+      <c r="D36" s="85"/>
+    </row>
+    <row r="37" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="85" t="s">
+      <c r="B37" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="E36" s="85"/>
-    </row>
-    <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="96"/>
-      <c r="B37" s="91" t="s">
+      <c r="D37" s="85"/>
+    </row>
+    <row r="38" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="89" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="85" t="s">
+      <c r="B38" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" s="85" t="s">
         <v>277</v>
       </c>
-      <c r="E37" s="85"/>
-    </row>
-    <row r="38" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="96"/>
-      <c r="B38" s="91" t="s">
+      <c r="D38" s="85"/>
+    </row>
+    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="85" t="s">
+      <c r="B39" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" s="85" t="s">
         <v>446</v>
       </c>
-      <c r="E38" s="85"/>
-    </row>
-    <row r="39" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="96"/>
-      <c r="B39" s="91" t="s">
+      <c r="D39" s="85"/>
+    </row>
+    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="85" t="s">
+      <c r="B40" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C40" s="85" t="s">
         <v>454</v>
       </c>
-      <c r="E39" s="85"/>
-    </row>
-    <row r="40" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="96"/>
-      <c r="B40" s="91" t="s">
+      <c r="D40" s="85"/>
+    </row>
+    <row r="41" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="89" t="s">
         <v>278</v>
       </c>
-      <c r="C40" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D40" s="85" t="s">
+      <c r="B41" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" s="85" t="s">
         <v>447</v>
       </c>
-      <c r="E40" s="85"/>
-    </row>
-    <row r="41" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="98"/>
-      <c r="B41" s="99" t="s">
+      <c r="D41" s="85"/>
+    </row>
+    <row r="42" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="94" t="s">
         <v>279</v>
       </c>
-      <c r="C41" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D41" s="100" t="s">
+      <c r="B42" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" s="95" t="s">
         <v>280</v>
       </c>
-      <c r="E41" s="100"/>
-    </row>
-    <row r="42" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="98"/>
-      <c r="B42" s="99" t="s">
+      <c r="D42" s="95"/>
+    </row>
+    <row r="43" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="100" t="s">
+      <c r="B43" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C43" s="95" t="s">
         <v>281</v>
       </c>
-      <c r="E42" s="100"/>
-    </row>
-    <row r="43" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="98"/>
-      <c r="B43" s="99" t="s">
+      <c r="D43" s="95"/>
+    </row>
+    <row r="44" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" s="100" t="s">
+      <c r="B44" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="100"/>
-    </row>
-    <row r="44" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="98"/>
-      <c r="B44" s="99" t="s">
+      <c r="D44" s="95"/>
+    </row>
+    <row r="45" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="94" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D44" s="100" t="s">
+      <c r="B45" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C45" s="95" t="s">
         <v>282</v>
       </c>
-      <c r="E44" s="100"/>
-    </row>
-    <row r="45" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="98"/>
-      <c r="B45" s="99" t="s">
+      <c r="D45" s="95"/>
+    </row>
+    <row r="46" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D45" s="100" t="s">
+      <c r="B46" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" s="95" t="s">
         <v>283</v>
       </c>
-      <c r="E45" s="100"/>
-    </row>
-    <row r="46" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="98"/>
-      <c r="B46" s="99" t="s">
+      <c r="D46" s="95"/>
+    </row>
+    <row r="47" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="94" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" s="100" t="s">
+      <c r="B47" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="95" t="s">
         <v>284</v>
       </c>
-      <c r="E46" s="100"/>
-    </row>
-    <row r="47" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="98"/>
-      <c r="B47" s="99" t="s">
+      <c r="D47" s="95"/>
+    </row>
+    <row r="48" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="94" t="s">
         <v>285</v>
       </c>
-      <c r="C47" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="100" t="s">
+      <c r="B48" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C48" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="E47" s="100"/>
-    </row>
-    <row r="48" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="98"/>
-      <c r="B48" s="99" t="s">
+      <c r="D48" s="95"/>
+    </row>
+    <row r="49" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="94" t="s">
         <v>287</v>
       </c>
-      <c r="C48" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D48" s="100" t="s">
+      <c r="B49" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" s="95" t="s">
         <v>288</v>
       </c>
-      <c r="E48" s="100"/>
-    </row>
-    <row r="49" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="98"/>
-      <c r="B49" s="99" t="s">
+      <c r="D49" s="95"/>
+    </row>
+    <row r="50" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="94" t="s">
         <v>289</v>
       </c>
-      <c r="C49" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D49" s="100" t="s">
+      <c r="B50" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="100"/>
-    </row>
-    <row r="50" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="98"/>
-      <c r="B50" s="99" t="s">
+      <c r="D50" s="95"/>
+    </row>
+    <row r="51" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="94" t="s">
         <v>290</v>
       </c>
-      <c r="C50" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D50" s="100" t="s">
+      <c r="B51" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="100"/>
-    </row>
-    <row r="51" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="98"/>
-      <c r="B51" s="99" t="s">
+      <c r="D51" s="95"/>
+    </row>
+    <row r="52" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="94" t="s">
         <v>291</v>
       </c>
-      <c r="C51" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D51" s="100" t="s">
+      <c r="B52" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" s="95" t="s">
         <v>292</v>
       </c>
-      <c r="E51" s="100"/>
-    </row>
-    <row r="52" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="98"/>
-      <c r="B52" s="99" t="s">
+      <c r="D52" s="95"/>
+    </row>
+    <row r="53" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="100" t="s">
+      <c r="B53" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="100"/>
-    </row>
-    <row r="53" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="98"/>
-      <c r="B53" s="99" t="s">
+      <c r="D53" s="95"/>
+    </row>
+    <row r="54" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="94" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D53" s="100" t="s">
+      <c r="B54" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C54" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="100"/>
-    </row>
-    <row r="54" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="98"/>
-      <c r="B54" s="99" t="s">
+      <c r="D54" s="95"/>
+    </row>
+    <row r="55" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D54" s="100" t="s">
+      <c r="B55" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C55" s="95" t="s">
         <v>293</v>
       </c>
-      <c r="E54" s="100"/>
-    </row>
-    <row r="55" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="98"/>
-      <c r="B55" s="99" t="s">
+      <c r="D55" s="95"/>
+    </row>
+    <row r="56" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="100" t="s">
+      <c r="B56" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C56" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="100"/>
-    </row>
-    <row r="56" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="98"/>
-      <c r="B56" s="99" t="s">
+      <c r="D56" s="95"/>
+    </row>
+    <row r="57" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="94" t="s">
         <v>181</v>
       </c>
-      <c r="C56" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D56" s="100" t="s">
+      <c r="B57" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C57" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="100"/>
-    </row>
-    <row r="57" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="98"/>
-      <c r="B57" s="99" t="s">
+      <c r="D57" s="95"/>
+    </row>
+    <row r="58" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="94" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="100" t="s">
+      <c r="B58" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" s="95" t="s">
         <v>294</v>
       </c>
-      <c r="E57" s="100"/>
-    </row>
-    <row r="58" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="98"/>
-      <c r="B58" s="99" t="s">
+      <c r="D58" s="95"/>
+    </row>
+    <row r="59" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" s="100" t="s">
+      <c r="B59" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="95" t="s">
         <v>295</v>
       </c>
-      <c r="E58" s="100"/>
-    </row>
-    <row r="59" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="98"/>
-      <c r="B59" s="99" t="s">
+      <c r="D59" s="95"/>
+    </row>
+    <row r="60" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="94" t="s">
         <v>184</v>
       </c>
-      <c r="C59" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="100" t="s">
+      <c r="B60" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="100"/>
-    </row>
-    <row r="60" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="98"/>
-      <c r="B60" s="99" t="s">
+      <c r="D60" s="95"/>
+    </row>
+    <row r="61" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="100" t="s">
-        <v>258</v>
-      </c>
-      <c r="D60" s="100" t="s">
+      <c r="B61" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" s="95" t="s">
         <v>296</v>
       </c>
-      <c r="E60" s="100"/>
-    </row>
-    <row r="61" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="96"/>
-      <c r="B61" s="91" t="s">
+      <c r="D61" s="95"/>
+    </row>
+    <row r="62" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="89" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D61" s="85" t="s">
+      <c r="B62" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="E61" s="85"/>
-    </row>
-    <row r="62" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="96"/>
-      <c r="B62" s="91" t="s">
+      <c r="D62" s="85"/>
+    </row>
+    <row r="63" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="89" t="s">
         <v>297</v>
       </c>
-      <c r="C62" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="85" t="s">
+      <c r="B63" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" s="85" t="s">
         <v>298</v>
       </c>
-      <c r="E62" s="85"/>
-    </row>
-    <row r="63" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="96"/>
-      <c r="B63" s="91" t="s">
+      <c r="D63" s="85"/>
+    </row>
+    <row r="64" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="89" t="s">
         <v>299</v>
       </c>
-      <c r="C63" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D63" s="85" t="s">
+      <c r="B64" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="E63" s="85"/>
-    </row>
-    <row r="64" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="95"/>
-      <c r="B64" s="91" t="s">
+      <c r="D64" s="85"/>
+    </row>
+    <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="89" t="s">
         <v>300</v>
       </c>
-      <c r="C64" s="85" t="s">
+      <c r="B65" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D64" s="85" t="s">
+      <c r="C65" s="85" t="s">
         <v>302</v>
       </c>
-      <c r="E64" s="85"/>
-    </row>
-    <row r="65" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
-      <c r="B65" s="91" t="s">
+      <c r="D65" s="85"/>
+    </row>
+    <row r="66" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="89" t="s">
         <v>303</v>
       </c>
-      <c r="C65" s="85" t="s">
+      <c r="B66" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D65" s="85" t="s">
+      <c r="C66" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="E65" s="85"/>
-    </row>
-    <row r="66" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
-      <c r="B66" s="91" t="s">
+      <c r="D66" s="85"/>
+    </row>
+    <row r="67" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="89" t="s">
         <v>305</v>
       </c>
-      <c r="C66" s="85" t="s">
+      <c r="B67" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D66" s="85" t="s">
+      <c r="C67" s="85" t="s">
         <v>306</v>
       </c>
-      <c r="E66" s="85"/>
-    </row>
-    <row r="67" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
-      <c r="B67" s="91" t="s">
+      <c r="D67" s="85"/>
+    </row>
+    <row r="68" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="89" t="s">
         <v>307</v>
       </c>
-      <c r="C67" s="85" t="s">
+      <c r="B68" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D67" s="85" t="s">
+      <c r="C68" s="85" t="s">
         <v>308</v>
       </c>
-      <c r="E67" s="85"/>
-    </row>
-    <row r="68" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
-      <c r="B68" s="91" t="s">
+      <c r="D68" s="85"/>
+    </row>
+    <row r="69" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="89" t="s">
         <v>309</v>
       </c>
-      <c r="C68" s="85" t="s">
+      <c r="B69" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D68" s="85" t="s">
+      <c r="C69" s="85" t="s">
         <v>310</v>
       </c>
-      <c r="E68" s="85"/>
-    </row>
-    <row r="69" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
-      <c r="B69" s="91" t="s">
+      <c r="D69" s="85"/>
+    </row>
+    <row r="70" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="89" t="s">
         <v>311</v>
       </c>
-      <c r="C69" s="85" t="s">
+      <c r="B70" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D69" s="85" t="s">
+      <c r="C70" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="E69" s="85"/>
-    </row>
-    <row r="70" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="95"/>
-      <c r="B70" s="91" t="s">
+      <c r="D70" s="85"/>
+    </row>
+    <row r="71" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="C70" s="85" t="s">
+      <c r="B71" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D70" s="85" t="s">
+      <c r="C71" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="E70" s="85"/>
-    </row>
-    <row r="71" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="95"/>
-      <c r="B71" s="91" t="s">
+      <c r="D71" s="85"/>
+    </row>
+    <row r="72" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="89" t="s">
         <v>315</v>
       </c>
-      <c r="C71" s="85" t="s">
+      <c r="B72" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D71" s="85" t="s">
+      <c r="C72" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="E71" s="85"/>
-    </row>
-    <row r="72" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="95"/>
-      <c r="B72" s="91" t="s">
+      <c r="D72" s="85"/>
+    </row>
+    <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="89" t="s">
         <v>317</v>
       </c>
-      <c r="C72" s="85" t="s">
+      <c r="B73" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D72" s="85" t="s">
+      <c r="C73" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="E72" s="85"/>
-    </row>
-    <row r="73" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="98"/>
-      <c r="B73" s="99" t="s">
+      <c r="D73" s="85"/>
+    </row>
+    <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="94" t="s">
         <v>319</v>
       </c>
-      <c r="C73" s="100" t="s">
+      <c r="B74" s="95" t="s">
         <v>301</v>
       </c>
-      <c r="D73" s="100" t="s">
+      <c r="C74" s="95" t="s">
         <v>320</v>
       </c>
-      <c r="E73" s="100"/>
-    </row>
-    <row r="74" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="95"/>
-      <c r="B74" s="91" t="s">
+      <c r="D74" s="95"/>
+    </row>
+    <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="89" t="s">
         <v>321</v>
       </c>
-      <c r="C74" s="85" t="s">
+      <c r="B75" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D74" s="85" t="s">
+      <c r="C75" s="85" t="s">
         <v>322</v>
       </c>
-      <c r="E74" s="85"/>
-    </row>
-    <row r="75" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="95"/>
-      <c r="B75" s="91" t="s">
+      <c r="D75" s="85"/>
+    </row>
+    <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="89" t="s">
         <v>323</v>
       </c>
-      <c r="C75" s="85" t="s">
+      <c r="B76" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D75" s="85" t="s">
+      <c r="C76" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="E75" s="85"/>
-    </row>
-    <row r="76" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="95"/>
-      <c r="B76" s="91" t="s">
+      <c r="D76" s="85"/>
+    </row>
+    <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="89" t="s">
         <v>324</v>
       </c>
-      <c r="C76" s="85" t="s">
+      <c r="B77" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D76" s="85" t="s">
+      <c r="C77" s="85" t="s">
         <v>325</v>
       </c>
-      <c r="E76" s="85"/>
-    </row>
-    <row r="77" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="95"/>
-      <c r="B77" s="91" t="s">
+      <c r="D77" s="85"/>
+    </row>
+    <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="89" t="s">
         <v>326</v>
       </c>
-      <c r="C77" s="85" t="s">
+      <c r="B78" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D77" s="85" t="s">
+      <c r="C78" s="85" t="s">
         <v>327</v>
       </c>
-      <c r="E77" s="85"/>
-    </row>
-    <row r="78" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="95"/>
-      <c r="B78" s="91" t="s">
+      <c r="D78" s="85"/>
+    </row>
+    <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="89" t="s">
         <v>328</v>
       </c>
-      <c r="C78" s="85" t="s">
+      <c r="B79" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D78" s="85" t="s">
+      <c r="C79" s="85" t="s">
         <v>329</v>
       </c>
-      <c r="E78" s="85"/>
-    </row>
-    <row r="79" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="95"/>
-      <c r="B79" s="91" t="s">
+      <c r="D79" s="85"/>
+    </row>
+    <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="89" t="s">
         <v>330</v>
       </c>
-      <c r="C79" s="85" t="s">
+      <c r="B80" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D79" s="85" t="s">
+      <c r="C80" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="E79" s="85"/>
-    </row>
-    <row r="80" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="95"/>
-      <c r="B80" s="91" t="s">
+      <c r="D80" s="85"/>
+    </row>
+    <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="89" t="s">
         <v>332</v>
       </c>
-      <c r="C80" s="85" t="s">
+      <c r="B81" s="85" t="s">
         <v>301</v>
       </c>
-      <c r="D80" s="85" t="s">
+      <c r="C81" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="E80" s="85"/>
-    </row>
-    <row r="81" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="95"/>
-      <c r="B81" s="91" t="s">
+      <c r="D81" s="85"/>
+    </row>
+    <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="89" t="s">
         <v>334</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="B82" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D81" s="85" t="s">
+      <c r="C82" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="E81" s="85"/>
-    </row>
-    <row r="82" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="95"/>
-      <c r="B82" s="91" t="s">
+      <c r="D82" s="85"/>
+    </row>
+    <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="89" t="s">
         <v>337</v>
       </c>
-      <c r="C82" s="85" t="s">
+      <c r="B83" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="85" t="s">
+      <c r="C83" s="85" t="s">
         <v>338</v>
       </c>
-      <c r="E82" s="85"/>
-    </row>
-    <row r="83" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="95"/>
-      <c r="B83" s="91" t="s">
+      <c r="D83" s="85"/>
+    </row>
+    <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="89" t="s">
         <v>339</v>
       </c>
-      <c r="C83" s="85" t="s">
+      <c r="B84" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D83" s="85" t="s">
+      <c r="C84" s="85" t="s">
         <v>340</v>
       </c>
-      <c r="E83" s="85"/>
-    </row>
-    <row r="84" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="95"/>
-      <c r="B84" s="91" t="s">
+      <c r="D84" s="85"/>
+    </row>
+    <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="89" t="s">
         <v>341</v>
       </c>
-      <c r="C84" s="85" t="s">
+      <c r="B85" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D84" s="85" t="s">
+      <c r="C85" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="E84" s="85"/>
-    </row>
-    <row r="85" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="95"/>
-      <c r="B85" s="91" t="s">
+      <c r="D85" s="85"/>
+    </row>
+    <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="89" t="s">
         <v>342</v>
       </c>
-      <c r="C85" s="85" t="s">
+      <c r="B86" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D85" s="85" t="s">
+      <c r="C86" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="E85" s="85"/>
-    </row>
-    <row r="86" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="95"/>
-      <c r="B86" s="91" t="s">
+      <c r="D86" s="85"/>
+    </row>
+    <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="89" t="s">
         <v>343</v>
       </c>
-      <c r="C86" s="85" t="s">
+      <c r="B87" s="85" t="s">
         <v>344</v>
       </c>
-      <c r="D86" s="85" t="s">
+      <c r="C87" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="E86" s="85" t="s">
+      <c r="D87" s="85" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="95"/>
-      <c r="B87" s="91" t="s">
+    <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="89" t="s">
         <v>346</v>
       </c>
-      <c r="C87" s="85" t="s">
+      <c r="B88" s="85" t="s">
         <v>344</v>
       </c>
-      <c r="D87" s="85" t="s">
+      <c r="C88" s="85" t="s">
         <v>347</v>
       </c>
-      <c r="E87" s="85" t="s">
+      <c r="D88" s="85" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="98"/>
-      <c r="B88" s="99" t="s">
+    <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="94" t="s">
         <v>349</v>
       </c>
-      <c r="C88" s="100" t="s">
+      <c r="B89" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D88" s="100" t="s">
+      <c r="C89" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="102" t="s">
+      <c r="D89" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="98"/>
-      <c r="B89" s="99" t="s">
+    <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="94" t="s">
         <v>350</v>
       </c>
-      <c r="C89" s="100" t="s">
+      <c r="B90" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D89" s="100" t="s">
+      <c r="C90" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="E89" s="102" t="s">
+      <c r="D90" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="98"/>
-      <c r="B90" s="99" t="s">
+    <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="94" t="s">
         <v>351</v>
       </c>
-      <c r="C90" s="100" t="s">
+      <c r="B91" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D90" s="100" t="s">
+      <c r="C91" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="E90" s="102" t="s">
+      <c r="D91" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="98"/>
-      <c r="B91" s="99" t="s">
+    <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="94" t="s">
         <v>352</v>
       </c>
-      <c r="C91" s="100" t="s">
+      <c r="B92" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D91" s="100" t="s">
+      <c r="C92" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="E91" s="102" t="s">
+      <c r="D92" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="98"/>
-      <c r="B92" s="99" t="s">
+    <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="94" t="s">
         <v>353</v>
       </c>
-      <c r="C92" s="100" t="s">
+      <c r="B93" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D92" s="100" t="s">
+      <c r="C93" s="95" t="s">
         <v>354</v>
       </c>
-      <c r="E92" s="102" t="s">
+      <c r="D93" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="98"/>
-      <c r="B93" s="99" t="s">
+    <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="94" t="s">
         <v>356</v>
       </c>
-      <c r="C93" s="100" t="s">
+      <c r="B94" s="95" t="s">
         <v>348</v>
       </c>
-      <c r="D93" s="100" t="s">
+      <c r="C94" s="95" t="s">
         <v>357</v>
       </c>
-      <c r="E93" s="102" t="s">
+      <c r="D94" s="97" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="96"/>
-      <c r="B94" s="91" t="s">
+    <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="89" t="s">
         <v>359</v>
       </c>
-      <c r="C94" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="85" t="s">
+      <c r="B95" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C95" s="85" t="s">
         <v>360</v>
       </c>
-      <c r="E94" s="85"/>
-    </row>
-    <row r="95" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="96"/>
-      <c r="B95" s="91" t="s">
+      <c r="D95" s="85"/>
+    </row>
+    <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="89" t="s">
         <v>361</v>
       </c>
-      <c r="C95" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="85" t="s">
+      <c r="B96" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C96" s="85" t="s">
         <v>450</v>
       </c>
-      <c r="E95" s="85"/>
-    </row>
-    <row r="96" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="96"/>
-      <c r="B96" s="91" t="s">
+      <c r="D96" s="85"/>
+    </row>
+    <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="89" t="s">
         <v>362</v>
       </c>
-      <c r="C96" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D96" s="85" t="s">
+      <c r="B97" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C97" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="E96" s="85"/>
-    </row>
-    <row r="97" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="96"/>
-      <c r="B97" s="91" t="s">
+      <c r="D97" s="85"/>
+    </row>
+    <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="89" t="s">
         <v>364</v>
       </c>
-      <c r="C97" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D97" s="85" t="s">
+      <c r="B98" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C98" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="E97" s="85"/>
-    </row>
-    <row r="98" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="96"/>
-      <c r="B98" s="91" t="s">
+      <c r="D98" s="85"/>
+    </row>
+    <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="89" t="s">
         <v>366</v>
       </c>
-      <c r="C98" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D98" s="85" t="s">
+      <c r="B99" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C99" s="85" t="s">
         <v>367</v>
       </c>
-      <c r="E98" s="85"/>
-    </row>
-    <row r="99" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="96"/>
-      <c r="B99" s="91" t="s">
+      <c r="D99" s="85"/>
+    </row>
+    <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="89" t="s">
         <v>368</v>
       </c>
-      <c r="C99" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D99" s="85" t="s">
+      <c r="B100" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C100" s="85" t="s">
         <v>369</v>
       </c>
-      <c r="E99" s="85"/>
-    </row>
-    <row r="100" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="96"/>
-      <c r="B100" s="91" t="s">
+      <c r="D100" s="85"/>
+    </row>
+    <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="89" t="s">
         <v>370</v>
       </c>
-      <c r="C100" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D100" s="85" t="s">
+      <c r="B101" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C101" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="E100" s="85"/>
-    </row>
-    <row r="101" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="96"/>
-      <c r="B101" s="91" t="s">
+      <c r="D101" s="85"/>
+    </row>
+    <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="89" t="s">
         <v>374</v>
       </c>
-      <c r="C101" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" s="85" t="s">
+      <c r="B102" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C102" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="E101" s="85"/>
-    </row>
-    <row r="102" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="96"/>
-      <c r="B102" s="91" t="s">
+      <c r="D102" s="85"/>
+    </row>
+    <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="89" t="s">
         <v>376</v>
       </c>
-      <c r="C102" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D102" s="85" t="s">
+      <c r="B103" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C103" s="85" t="s">
         <v>377</v>
       </c>
-      <c r="E102" s="85"/>
-    </row>
-    <row r="103" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="96"/>
-      <c r="B103" s="91" t="s">
+      <c r="D103" s="85"/>
+    </row>
+    <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="89" t="s">
         <v>378</v>
       </c>
-      <c r="C103" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D103" s="85" t="s">
+      <c r="B104" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" s="85" t="s">
         <v>379</v>
       </c>
-      <c r="E103" s="85"/>
-    </row>
-    <row r="104" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="96"/>
-      <c r="B104" s="91" t="s">
+      <c r="D104" s="85"/>
+    </row>
+    <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="89" t="s">
         <v>380</v>
       </c>
-      <c r="C104" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D104" s="85" t="s">
+      <c r="B105" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C105" s="85" t="s">
         <v>451</v>
       </c>
-      <c r="E104" s="85"/>
-    </row>
-    <row r="105" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="96"/>
-      <c r="B105" s="91" t="s">
+      <c r="D105" s="85"/>
+    </row>
+    <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="89" t="s">
         <v>381</v>
       </c>
-      <c r="C105" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="85" t="s">
+      <c r="B106" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C106" s="85" t="s">
         <v>452</v>
       </c>
-      <c r="E105" s="85"/>
-    </row>
-    <row r="106" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="96"/>
-      <c r="B106" s="91" t="s">
+      <c r="D106" s="85"/>
+    </row>
+    <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="89" t="s">
         <v>382</v>
       </c>
-      <c r="C106" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D106" s="85" t="s">
+      <c r="B107" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C107" s="85" t="s">
         <v>453</v>
       </c>
-      <c r="E106" s="85"/>
-    </row>
-    <row r="107" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="96"/>
-      <c r="B107" s="91" t="s">
+      <c r="D107" s="85"/>
+    </row>
+    <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="89" t="s">
         <v>383</v>
       </c>
-      <c r="C107" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D107" s="85" t="s">
+      <c r="B108" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C108" s="85" t="s">
         <v>384</v>
       </c>
-      <c r="E107" s="85"/>
-    </row>
-    <row r="108" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="96"/>
-      <c r="B108" s="91" t="s">
+      <c r="D108" s="85"/>
+    </row>
+    <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="89" t="s">
         <v>385</v>
       </c>
-      <c r="C108" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D108" s="85" t="s">
+      <c r="B109" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" s="85" t="s">
         <v>386</v>
       </c>
-      <c r="E108" s="85"/>
-    </row>
-    <row r="109" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="96"/>
-      <c r="B109" s="91" t="s">
+      <c r="D109" s="85"/>
+    </row>
+    <row r="110" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="C109" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" s="85" t="s">
+      <c r="B110" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C110" s="85" t="s">
         <v>387</v>
       </c>
-      <c r="E109" s="85"/>
-    </row>
-    <row r="110" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="96"/>
-      <c r="B110" s="91" t="s">
+      <c r="D110" s="85"/>
+    </row>
+    <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="89" t="s">
         <v>388</v>
       </c>
-      <c r="C110" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D110" s="85" t="s">
+      <c r="B111" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C111" s="85" t="s">
         <v>455</v>
       </c>
-      <c r="E110" s="85"/>
-    </row>
-    <row r="111" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="96"/>
-      <c r="B111" s="91" t="s">
+      <c r="D111" s="85"/>
+    </row>
+    <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="89" t="s">
         <v>372</v>
       </c>
-      <c r="C111" s="85" t="s">
+      <c r="B112" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D111" s="85" t="s">
+      <c r="C112" s="85" t="s">
         <v>390</v>
       </c>
-      <c r="E111" s="85"/>
-    </row>
-    <row r="112" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="96"/>
-      <c r="B112" s="91" t="s">
+      <c r="D112" s="85"/>
+    </row>
+    <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="89" t="s">
         <v>373</v>
       </c>
-      <c r="C112" s="85" t="s">
+      <c r="B113" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D112" s="85" t="s">
+      <c r="C113" s="85" t="s">
         <v>469</v>
       </c>
-      <c r="E112" s="85"/>
-    </row>
-    <row r="113" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="96"/>
-      <c r="B113" s="91" t="s">
+      <c r="D113" s="85"/>
+    </row>
+    <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="89" t="s">
         <v>391</v>
       </c>
-      <c r="C113" s="85" t="s">
+      <c r="B114" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D113" s="85" t="s">
+      <c r="C114" s="85" t="s">
         <v>471</v>
       </c>
-      <c r="E113" s="85"/>
-    </row>
-    <row r="114" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="95"/>
-      <c r="B114" s="91" t="s">
+      <c r="D114" s="85"/>
+    </row>
+    <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="89" t="s">
         <v>392</v>
       </c>
-      <c r="C114" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="85" t="s">
+      <c r="B115" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C115" s="85" t="s">
         <v>393</v>
       </c>
-      <c r="E114" s="85"/>
-    </row>
-    <row r="115" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="95"/>
-      <c r="B115" s="91" t="s">
+      <c r="D115" s="85"/>
+    </row>
+    <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="89" t="s">
         <v>394</v>
       </c>
-      <c r="C115" s="85" t="s">
+      <c r="B116" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D115" s="85" t="s">
+      <c r="C116" s="85" t="s">
         <v>395</v>
       </c>
-      <c r="E115" s="85"/>
-    </row>
-    <row r="116" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="96"/>
-      <c r="B116" s="91" t="s">
+      <c r="D116" s="85"/>
+    </row>
+    <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="89" t="s">
         <v>396</v>
       </c>
-      <c r="C116" s="85" t="s">
+      <c r="B117" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D116" s="85" t="s">
+      <c r="C117" s="85" t="s">
         <v>397</v>
       </c>
-      <c r="E116" s="85"/>
-    </row>
-    <row r="117" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="98"/>
-      <c r="B117" s="99" t="s">
+      <c r="D117" s="85"/>
+    </row>
+    <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="94" t="s">
         <v>398</v>
       </c>
-      <c r="C117" s="100" t="s">
+      <c r="B118" s="95" t="s">
         <v>335</v>
       </c>
-      <c r="D117" s="100" t="s">
+      <c r="C118" s="95" t="s">
         <v>399</v>
       </c>
-      <c r="E117" s="100"/>
-    </row>
-    <row r="118" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="96"/>
-      <c r="B118" s="91" t="s">
+      <c r="D118" s="95"/>
+    </row>
+    <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="89" t="s">
         <v>400</v>
       </c>
-      <c r="C118" s="85" t="s">
+      <c r="B119" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D118" s="85" t="s">
+      <c r="C119" s="85" t="s">
         <v>401</v>
       </c>
-      <c r="E118" s="85"/>
-    </row>
-    <row r="119" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="95"/>
-      <c r="B119" s="91" t="s">
+      <c r="D119" s="85"/>
+    </row>
+    <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="89" t="s">
         <v>402</v>
       </c>
-      <c r="C119" s="85" t="s">
+      <c r="B120" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D119" s="85" t="s">
+      <c r="C120" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="E119" s="85"/>
-    </row>
-    <row r="120" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="95"/>
-      <c r="B120" s="91" t="s">
+      <c r="D120" s="85"/>
+    </row>
+    <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="89" t="s">
         <v>404</v>
       </c>
-      <c r="C120" s="85" t="s">
+      <c r="B121" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D120" s="85" t="s">
+      <c r="C121" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="E120" s="85"/>
-    </row>
-    <row r="121" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="95"/>
-      <c r="B121" s="91" t="s">
+      <c r="D121" s="85"/>
+    </row>
+    <row r="122" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="C121" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D121" s="85" t="s">
+      <c r="B122" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C122" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="E121" s="85"/>
-    </row>
-    <row r="122" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="95"/>
-      <c r="B122" s="91" t="s">
+      <c r="D122" s="85"/>
+    </row>
+    <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="89" t="s">
         <v>407</v>
       </c>
-      <c r="C122" s="85" t="s">
+      <c r="B123" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D122" s="85" t="s">
+      <c r="C123" s="85" t="s">
         <v>409</v>
       </c>
-      <c r="E122" s="85"/>
-    </row>
-    <row r="123" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="95"/>
-      <c r="B123" s="91" t="s">
+      <c r="D123" s="85"/>
+    </row>
+    <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="89" t="s">
         <v>408</v>
       </c>
-      <c r="C123" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D123" s="85" t="s">
+      <c r="B124" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C124" s="85" t="s">
         <v>410</v>
       </c>
-      <c r="E123" s="85"/>
-    </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="96"/>
-      <c r="B124" s="91" t="s">
+      <c r="D124" s="85"/>
+    </row>
+    <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="89" t="s">
         <v>411</v>
       </c>
-      <c r="C124" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D124" s="85" t="s">
+      <c r="B125" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C125" s="85" t="s">
         <v>412</v>
       </c>
-      <c r="E124" s="85"/>
-    </row>
-    <row r="125" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="96"/>
-      <c r="B125" s="91" t="s">
+      <c r="D125" s="85"/>
+    </row>
+    <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="89" t="s">
         <v>413</v>
       </c>
-      <c r="C125" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="85" t="s">
+      <c r="B126" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C126" s="85" t="s">
         <v>414</v>
       </c>
-      <c r="E125" s="85"/>
-    </row>
-    <row r="126" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="96"/>
-      <c r="B126" s="91" t="s">
+      <c r="D126" s="85"/>
+    </row>
+    <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="89" t="s">
         <v>415</v>
       </c>
-      <c r="C126" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D126" s="85" t="s">
+      <c r="B127" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C127" s="85" t="s">
         <v>459</v>
       </c>
-      <c r="E126" s="85"/>
-    </row>
-    <row r="127" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="96"/>
-      <c r="B127" s="91" t="s">
+      <c r="D127" s="85"/>
+    </row>
+    <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="89" t="s">
         <v>416</v>
       </c>
-      <c r="C127" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D127" s="85" t="s">
+      <c r="B128" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C128" s="85" t="s">
         <v>417</v>
       </c>
-      <c r="E127" s="85"/>
-    </row>
-    <row r="128" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="96"/>
-      <c r="B128" s="91" t="s">
+      <c r="D128" s="85"/>
+    </row>
+    <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="89" t="s">
         <v>418</v>
       </c>
-      <c r="C128" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="85" t="s">
+      <c r="B129" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C129" s="85" t="s">
         <v>419</v>
       </c>
-      <c r="E128" s="85"/>
-    </row>
-    <row r="129" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="96"/>
-      <c r="B129" s="91" t="s">
+      <c r="D129" s="85"/>
+    </row>
+    <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="89" t="s">
         <v>420</v>
       </c>
-      <c r="C129" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D129" s="85" t="s">
+      <c r="B130" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C130" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="E129" s="85"/>
-    </row>
-    <row r="130" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="96"/>
-      <c r="B130" s="91" t="s">
+      <c r="D130" s="85"/>
+    </row>
+    <row r="131" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C130" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D130" s="85" t="s">
+      <c r="B131" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C131" s="85" t="s">
         <v>422</v>
       </c>
-      <c r="E130" s="85"/>
-    </row>
-    <row r="131" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="96"/>
-      <c r="B131" s="91" t="s">
+      <c r="D131" s="85"/>
+    </row>
+    <row r="132" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="89" t="s">
         <v>190</v>
       </c>
-      <c r="C131" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D131" s="85" t="s">
+      <c r="B132" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C132" s="85" t="s">
         <v>294</v>
       </c>
-      <c r="E131" s="85"/>
-    </row>
-    <row r="132" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="96"/>
-      <c r="B132" s="91" t="s">
+      <c r="D132" s="85"/>
+    </row>
+    <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="89" t="s">
         <v>423</v>
       </c>
-      <c r="C132" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D132" s="85" t="s">
+      <c r="B133" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C133" s="85" t="s">
         <v>424</v>
       </c>
-      <c r="E132" s="85"/>
-    </row>
-    <row r="133" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="96"/>
-      <c r="B133" s="91" t="s">
+      <c r="D133" s="85"/>
+    </row>
+    <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="89" t="s">
         <v>425</v>
       </c>
-      <c r="C133" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D133" s="85" t="s">
+      <c r="B134" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C134" s="85" t="s">
         <v>426</v>
       </c>
-      <c r="E133" s="85"/>
-    </row>
-    <row r="134" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="96"/>
-      <c r="B134" s="91" t="s">
+      <c r="D134" s="85"/>
+    </row>
+    <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="89" t="s">
         <v>427</v>
       </c>
-      <c r="C134" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D134" s="85" t="s">
+      <c r="B135" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C135" s="85" t="s">
         <v>461</v>
       </c>
-      <c r="E134" s="85"/>
-    </row>
-    <row r="135" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="96"/>
-      <c r="B135" s="91" t="s">
+      <c r="D135" s="85"/>
+    </row>
+    <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="89" t="s">
         <v>428</v>
       </c>
-      <c r="C135" s="85" t="s">
+      <c r="B136" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="D135" s="85" t="s">
+      <c r="C136" s="85" t="s">
         <v>429</v>
       </c>
-      <c r="E135" s="85"/>
-    </row>
-    <row r="136" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="96"/>
-      <c r="B136" s="91" t="s">
+      <c r="D136" s="85"/>
+    </row>
+    <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="89" t="s">
         <v>430</v>
       </c>
-      <c r="C136" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D136" s="85" t="s">
+      <c r="B137" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C137" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="E136" s="85"/>
-    </row>
-    <row r="137" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="96"/>
-      <c r="B137" s="91" t="s">
+      <c r="D137" s="85"/>
+    </row>
+    <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="89" t="s">
         <v>432</v>
       </c>
-      <c r="C137" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="85" t="s">
+      <c r="B138" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C138" s="85" t="s">
         <v>520</v>
       </c>
-      <c r="E137" s="85"/>
-    </row>
-    <row r="138" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="96"/>
-      <c r="B138" s="91" t="s">
+      <c r="D138" s="85"/>
+    </row>
+    <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="89" t="s">
         <v>433</v>
       </c>
-      <c r="C138" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D138" s="85" t="s">
+      <c r="B139" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C139" s="85" t="s">
         <v>463</v>
       </c>
-      <c r="E138" s="85"/>
-    </row>
-    <row r="139" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="96"/>
-      <c r="B139" s="91" t="s">
+      <c r="D139" s="85"/>
+    </row>
+    <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="89" t="s">
         <v>434</v>
       </c>
-      <c r="C139" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D139" s="85" t="s">
+      <c r="B140" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C140" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="E139" s="85"/>
-    </row>
-    <row r="140" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="96"/>
-      <c r="B140" s="91" t="s">
+      <c r="D140" s="85"/>
+    </row>
+    <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="89" t="s">
         <v>436</v>
       </c>
-      <c r="C140" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D140" s="85" t="s">
+      <c r="B141" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C141" s="85" t="s">
         <v>464</v>
       </c>
-      <c r="E140" s="85"/>
-    </row>
-    <row r="141" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="96"/>
-      <c r="B141" s="91" t="s">
+      <c r="D141" s="85"/>
+    </row>
+    <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="89" t="s">
         <v>437</v>
       </c>
-      <c r="C141" s="85" t="s">
+      <c r="B142" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="D141" s="85" t="s">
+      <c r="C142" s="85" t="s">
         <v>438</v>
       </c>
-      <c r="E141" s="85"/>
-    </row>
-    <row r="142" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="95"/>
-      <c r="B142" s="91" t="s">
+      <c r="D142" s="85"/>
+    </row>
+    <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="89" t="s">
         <v>456</v>
       </c>
-      <c r="C142" s="85" t="s">
+      <c r="B143" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="D142" s="85" t="s">
+      <c r="C143" s="85" t="s">
         <v>457</v>
       </c>
-      <c r="E142" s="85"/>
-    </row>
-    <row r="143" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="98"/>
-      <c r="B143" s="99" t="s">
+      <c r="D143" s="85"/>
+    </row>
+    <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="94" t="s">
         <v>466</v>
       </c>
-      <c r="C143" s="100" t="s">
+      <c r="B144" s="95" t="s">
         <v>301</v>
       </c>
-      <c r="D143" s="100" t="s">
+      <c r="C144" s="95" t="s">
         <v>467</v>
       </c>
-      <c r="E143" s="100"/>
-    </row>
-    <row r="144" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="96"/>
-      <c r="B144" s="91" t="s">
+      <c r="D144" s="95"/>
+    </row>
+    <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="89" t="s">
         <v>473</v>
       </c>
-      <c r="C144" s="85" t="s">
+      <c r="B145" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D144" s="85" t="s">
+      <c r="C145" s="85" t="s">
         <v>474</v>
       </c>
-      <c r="E144" s="85"/>
-    </row>
-    <row r="145" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="96"/>
-      <c r="B145" s="91" t="s">
+      <c r="D145" s="85"/>
+    </row>
+    <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="89" t="s">
         <v>476</v>
       </c>
-      <c r="C145" s="85" t="s">
+      <c r="B146" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D145" s="85" t="s">
+      <c r="C146" s="85" t="s">
         <v>477</v>
       </c>
-      <c r="E145" s="85"/>
-    </row>
-    <row r="146" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="96"/>
-      <c r="B146" s="91" t="s">
+      <c r="D146" s="85"/>
+    </row>
+    <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="89" t="s">
         <v>478</v>
       </c>
-      <c r="C146" s="85" t="s">
+      <c r="B147" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D146" s="85" t="s">
+      <c r="C147" s="85" t="s">
         <v>479</v>
       </c>
-      <c r="E146" s="85"/>
-    </row>
-    <row r="147" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="103"/>
-      <c r="B147" s="92" t="s">
+      <c r="D147" s="85"/>
+    </row>
+    <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="90" t="s">
         <v>480</v>
       </c>
-      <c r="C147" s="93" t="s">
+      <c r="B148" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="D147" s="93" t="s">
+      <c r="C148" s="91" t="s">
         <v>481</v>
       </c>
-      <c r="E147" s="93"/>
-    </row>
-    <row r="148" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="96"/>
-      <c r="B148" s="91" t="s">
+      <c r="D148" s="91"/>
+    </row>
+    <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="89" t="s">
         <v>482</v>
       </c>
-      <c r="C148" s="85" t="s">
+      <c r="B149" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D148" s="85" t="s">
+      <c r="C149" s="85" t="s">
         <v>483</v>
       </c>
-      <c r="E148" s="85"/>
-    </row>
-    <row r="149" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="96"/>
-      <c r="B149" s="91" t="s">
+      <c r="D149" s="85"/>
+    </row>
+    <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="89" t="s">
         <v>485</v>
       </c>
-      <c r="C149" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D149" s="85" t="s">
+      <c r="B150" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C150" s="85" t="s">
         <v>486</v>
       </c>
-      <c r="E149" s="85"/>
-    </row>
-    <row r="150" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="96"/>
-      <c r="B150" s="91" t="s">
+      <c r="D150" s="85"/>
+    </row>
+    <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="89" t="s">
         <v>487</v>
       </c>
-      <c r="C150" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D150" s="85" t="s">
+      <c r="B151" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C151" s="85" t="s">
         <v>488</v>
       </c>
-      <c r="E150" s="85"/>
-    </row>
-    <row r="151" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="96"/>
-      <c r="B151" s="91" t="s">
+      <c r="D151" s="85"/>
+    </row>
+    <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="89" t="s">
         <v>490</v>
       </c>
-      <c r="C151" s="85" t="s">
+      <c r="B152" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D151" s="85" t="s">
+      <c r="C152" s="85" t="s">
         <v>489</v>
       </c>
-      <c r="E151" s="85"/>
-    </row>
-    <row r="152" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="96"/>
-      <c r="B152" s="91" t="s">
+      <c r="D152" s="85"/>
+    </row>
+    <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="89" t="s">
         <v>491</v>
       </c>
-      <c r="C152" s="85" t="s">
+      <c r="B153" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D152" s="85" t="s">
+      <c r="C153" s="85" t="s">
         <v>492</v>
       </c>
-      <c r="E152" s="85"/>
-    </row>
-    <row r="153" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="96"/>
-      <c r="B153" s="91" t="s">
+      <c r="D153" s="85"/>
+    </row>
+    <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="C153" s="85" t="s">
+      <c r="B154" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D153" s="85" t="s">
+      <c r="C154" s="85" t="s">
         <v>501</v>
       </c>
-      <c r="E153" s="85"/>
-    </row>
-    <row r="154" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="95"/>
-      <c r="B154" s="91" t="s">
+      <c r="D154" s="85"/>
+    </row>
+    <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="89" t="s">
         <v>494</v>
       </c>
-      <c r="C154" s="85" t="s">
+      <c r="B155" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D154" s="85" t="s">
+      <c r="C155" s="85" t="s">
         <v>502</v>
       </c>
-      <c r="E154" s="85"/>
-    </row>
-    <row r="155" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="95"/>
-      <c r="B155" s="91" t="s">
+      <c r="D155" s="85"/>
+    </row>
+    <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="89" t="s">
         <v>495</v>
       </c>
-      <c r="C155" s="85" t="s">
+      <c r="B156" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D155" s="85" t="s">
+      <c r="C156" s="85" t="s">
         <v>503</v>
       </c>
-      <c r="E155" s="85"/>
-    </row>
-    <row r="156" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="95"/>
-      <c r="B156" s="91" t="s">
+      <c r="D156" s="85"/>
+    </row>
+    <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="89" t="s">
         <v>496</v>
       </c>
-      <c r="C156" s="85" t="s">
+      <c r="B157" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D156" s="85" t="s">
+      <c r="C157" s="85" t="s">
         <v>504</v>
       </c>
-      <c r="E156" s="85"/>
-    </row>
-    <row r="157" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="95"/>
-      <c r="B157" s="91" t="s">
+      <c r="D157" s="85"/>
+    </row>
+    <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="89" t="s">
         <v>497</v>
       </c>
-      <c r="C157" s="85" t="s">
+      <c r="B158" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D157" s="85" t="s">
+      <c r="C158" s="85" t="s">
         <v>505</v>
       </c>
-      <c r="E157" s="85"/>
-    </row>
-    <row r="158" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="95"/>
-      <c r="B158" s="91" t="s">
+      <c r="D158" s="85"/>
+    </row>
+    <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="89" t="s">
         <v>498</v>
       </c>
-      <c r="C158" s="85" t="s">
+      <c r="B159" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D158" s="85" t="s">
+      <c r="C159" s="85" t="s">
         <v>506</v>
       </c>
-      <c r="E158" s="85"/>
-    </row>
-    <row r="159" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="95"/>
-      <c r="B159" s="91" t="s">
+      <c r="D159" s="85"/>
+    </row>
+    <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="89" t="s">
         <v>499</v>
       </c>
-      <c r="C159" s="85" t="s">
+      <c r="B160" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D159" s="85" t="s">
+      <c r="C160" s="85" t="s">
         <v>507</v>
       </c>
-      <c r="E159" s="85"/>
-    </row>
-    <row r="160" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="95"/>
-      <c r="B160" s="91" t="s">
+      <c r="D160" s="85"/>
+    </row>
+    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="89" t="s">
         <v>500</v>
       </c>
-      <c r="C160" s="85" t="s">
+      <c r="B161" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D160" s="85" t="s">
+      <c r="C161" s="85" t="s">
         <v>508</v>
       </c>
-      <c r="E160" s="85"/>
-    </row>
-    <row r="161" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="95"/>
-      <c r="B161" s="91" t="s">
+      <c r="D161" s="85"/>
+    </row>
+    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="89" t="s">
         <v>509</v>
       </c>
-      <c r="C161" s="85" t="s">
+      <c r="B162" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D161" s="85" t="s">
+      <c r="C162" s="85" t="s">
         <v>510</v>
       </c>
-      <c r="E161" s="85"/>
-    </row>
-    <row r="162" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="96"/>
-      <c r="B162" s="91" t="s">
+      <c r="D162" s="85"/>
+    </row>
+    <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="89" t="s">
         <v>511</v>
       </c>
-      <c r="C162" s="85" t="s">
+      <c r="B163" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D162" s="85" t="s">
+      <c r="C163" s="85" t="s">
         <v>514</v>
       </c>
-      <c r="E162" s="85"/>
-    </row>
-    <row r="163" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="96"/>
-      <c r="B163" s="91" t="s">
+      <c r="D163" s="85"/>
+    </row>
+    <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="89" t="s">
         <v>512</v>
       </c>
-      <c r="C163" s="85" t="s">
+      <c r="B164" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D163" s="85" t="s">
+      <c r="C164" s="85" t="s">
         <v>515</v>
       </c>
-      <c r="E163" s="85"/>
-    </row>
-    <row r="164" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="96"/>
-      <c r="B164" s="91" t="s">
+      <c r="D164" s="85"/>
+    </row>
+    <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="89" t="s">
         <v>513</v>
       </c>
-      <c r="C164" s="85" t="s">
+      <c r="B165" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D164" s="85" t="s">
+      <c r="C165" s="85" t="s">
         <v>516</v>
       </c>
-      <c r="E164" s="85"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="96"/>
-      <c r="B165" s="83" t="s">
+      <c r="D165" s="85"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="83" t="s">
         <v>521</v>
       </c>
-      <c r="C165" s="84" t="s">
+      <c r="B166" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D165" s="84" t="s">
+      <c r="C166" s="84" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="96"/>
-      <c r="B166" s="91" t="s">
+    <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="89" t="s">
         <v>522</v>
       </c>
-      <c r="C166" s="85" t="s">
+      <c r="B167" s="85" t="s">
         <v>335</v>
       </c>
-      <c r="D166" s="85" t="s">
+      <c r="C167" s="85" t="s">
         <v>523</v>
       </c>
-      <c r="E166" s="85"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="96"/>
-      <c r="B167" s="83" t="s">
+      <c r="D167" s="85"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="83" t="s">
         <v>524</v>
       </c>
-      <c r="C167" s="84" t="s">
+      <c r="B168" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D167" s="84" t="s">
+      <c r="C168" s="84" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="96"/>
-      <c r="B168" s="91" t="s">
+    <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="89" t="s">
         <v>526</v>
       </c>
-      <c r="C168" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D168" s="85" t="s">
+      <c r="B169" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C169" s="85" t="s">
         <v>527</v>
       </c>
-      <c r="E168" s="85"/>
-    </row>
-    <row r="169" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="96"/>
-      <c r="B169" s="91" t="s">
+      <c r="D169" s="85"/>
+    </row>
+    <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="89" t="s">
         <v>528</v>
       </c>
-      <c r="C169" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D169" s="85" t="s">
+      <c r="B170" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C170" s="85" t="s">
         <v>529</v>
       </c>
-      <c r="E169" s="85"/>
-    </row>
-    <row r="170" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="96"/>
-      <c r="B170" s="91" t="s">
+      <c r="D170" s="85"/>
+    </row>
+    <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="89" t="s">
         <v>530</v>
       </c>
-      <c r="C170" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D170" s="85" t="s">
+      <c r="B171" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C171" s="85" t="s">
         <v>531</v>
       </c>
-      <c r="E170" s="85"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="95"/>
-      <c r="B171" s="83" t="s">
+      <c r="D171" s="85"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="83" t="s">
         <v>532</v>
       </c>
-      <c r="C171" s="84" t="s">
+      <c r="B172" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D171" s="84" t="s">
+      <c r="C172" s="84" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="96"/>
-      <c r="B172" s="91" t="s">
+    <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="89" t="s">
         <v>534</v>
       </c>
-      <c r="C172" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="D172" s="85" t="s">
+      <c r="B173" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C173" s="85" t="s">
         <v>535</v>
       </c>
-      <c r="E172" s="85"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="96"/>
-      <c r="B173" s="83" t="s">
+      <c r="D173" s="85"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="83" t="s">
         <v>542</v>
       </c>
-      <c r="C173" s="84" t="s">
+      <c r="B174" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D173" s="84" t="s">
+      <c r="C174" s="84" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="96"/>
-      <c r="B174" s="83" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="83" t="s">
         <v>544</v>
       </c>
-      <c r="C174" s="84" t="s">
+      <c r="B175" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D174" s="84" t="s">
+      <c r="C175" s="84" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="96"/>
-      <c r="B175" s="83" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="83" t="s">
         <v>545</v>
       </c>
-      <c r="C175" s="84" t="s">
+      <c r="B176" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D175" s="84" t="s">
+      <c r="C176" s="84" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="96"/>
-      <c r="B176" s="83" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="83" t="s">
         <v>547</v>
       </c>
-      <c r="C176" s="84" t="s">
+      <c r="B177" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D176" s="84" t="s">
+      <c r="C177" s="84" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="83" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="83" t="s">
         <v>550</v>
       </c>
-      <c r="C177" s="84" t="s">
+      <c r="B178" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D177" s="84" t="s">
+      <c r="C178" s="84" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="83" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="83" t="s">
         <v>552</v>
       </c>
-      <c r="C178" s="84" t="s">
+      <c r="B179" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D178" s="84" t="s">
+      <c r="C179" s="84" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="83" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="83" t="s">
         <v>553</v>
       </c>
-      <c r="C179" s="84" t="s">
+      <c r="B180" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D179" s="84" t="s">
+      <c r="C180" s="84" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="83" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="83" t="s">
         <v>555</v>
       </c>
-      <c r="C180" s="84" t="s">
+      <c r="B181" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D180" s="84" t="s">
+      <c r="C181" s="84" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="83" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="83" t="s">
         <v>557</v>
       </c>
-      <c r="C181" s="84" t="s">
+      <c r="B182" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D181" s="84" t="s">
+      <c r="C182" s="84" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="83" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="83" t="s">
         <v>560</v>
       </c>
-      <c r="C182" s="84" t="s">
+      <c r="B183" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D182" s="84" t="s">
+      <c r="C183" s="84" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="83" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="83" t="s">
         <v>562</v>
       </c>
-      <c r="C183" s="84" t="s">
+      <c r="B184" s="84" t="s">
         <v>335</v>
       </c>
-      <c r="D183" s="84" t="s">
+      <c r="C184" s="84" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="83" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="83" t="s">
         <v>564</v>
       </c>
-      <c r="C184" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="D184" s="84" t="s">
+      <c r="B185" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C185" s="84" t="s">
         <v>565</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increased border spacing on popup windows
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC94D78-E1FE-41B2-8701-7243EA587646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65AA990-7920-42CE-A11B-B32B1F9E811A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -6012,8 +6012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the icons for vulnerability and local knowledge
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65AA990-7920-42CE-A11B-B32B1F9E811A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEEA9B1-54C7-4362-B088-09B1CD29CE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-55020" yWindow="600" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -989,9 +989,6 @@
     <t>69</t>
   </si>
   <si>
-    <t>Teacher at board point w/ students</t>
-  </si>
-  <si>
     <t>70</t>
   </si>
   <si>
@@ -1007,9 +1004,6 @@
     <t>72</t>
   </si>
   <si>
-    <t>Person balancing</t>
-  </si>
-  <si>
     <t>73</t>
   </si>
   <si>
@@ -1737,6 +1731,12 @@
   </si>
   <si>
     <t>Equity Principles for Resilience Planning</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Umbrella</t>
   </si>
 </sst>
 </file>
@@ -6012,8 +6012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6036,7 +6036,7 @@
         <v>256</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -6059,7 +6059,7 @@
         <v>258</v>
       </c>
       <c r="C4" s="85" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D4" s="85"/>
     </row>
@@ -6071,7 +6071,7 @@
         <v>258</v>
       </c>
       <c r="C5" s="85" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D5" s="85"/>
     </row>
@@ -6083,7 +6083,7 @@
         <v>258</v>
       </c>
       <c r="C6" s="85" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D6" s="85"/>
     </row>
@@ -6095,7 +6095,7 @@
         <v>258</v>
       </c>
       <c r="C7" s="85" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D7" s="85"/>
     </row>
@@ -6107,7 +6107,7 @@
         <v>258</v>
       </c>
       <c r="C8" s="85" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D8" s="85"/>
     </row>
@@ -6155,19 +6155,19 @@
         <v>258</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D12" s="85"/>
     </row>
     <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B13" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D13" s="85"/>
     </row>
@@ -6179,7 +6179,7 @@
         <v>258</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D14" s="85"/>
     </row>
@@ -6203,7 +6203,7 @@
         <v>258</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D16" s="85"/>
     </row>
@@ -6227,7 +6227,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="85" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D18" s="85"/>
     </row>
@@ -6239,7 +6239,7 @@
         <v>258</v>
       </c>
       <c r="C19" s="85" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D19" s="85"/>
     </row>
@@ -6251,7 +6251,7 @@
         <v>258</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D20" s="85"/>
     </row>
@@ -6263,7 +6263,7 @@
         <v>258</v>
       </c>
       <c r="C21" s="85" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D21" s="85"/>
     </row>
@@ -6275,7 +6275,7 @@
         <v>258</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D22" s="85"/>
     </row>
@@ -6287,7 +6287,7 @@
         <v>258</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D23" s="85"/>
     </row>
@@ -6299,7 +6299,7 @@
         <v>258</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D24" s="85"/>
     </row>
@@ -6311,7 +6311,7 @@
         <v>258</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D25" s="85"/>
     </row>
@@ -6323,7 +6323,7 @@
         <v>258</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D26" s="85"/>
     </row>
@@ -6347,7 +6347,7 @@
         <v>258</v>
       </c>
       <c r="C28" s="85" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D28" s="85"/>
     </row>
@@ -6359,7 +6359,7 @@
         <v>258</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D29" s="85"/>
     </row>
@@ -6407,7 +6407,7 @@
         <v>258</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D33" s="85"/>
     </row>
@@ -6419,7 +6419,7 @@
         <v>258</v>
       </c>
       <c r="C34" s="85" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D34" s="85"/>
     </row>
@@ -6443,7 +6443,7 @@
         <v>258</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D36" s="85"/>
     </row>
@@ -6455,7 +6455,7 @@
         <v>258</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D37" s="85"/>
     </row>
@@ -6479,7 +6479,7 @@
         <v>258</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D39" s="85"/>
     </row>
@@ -6491,7 +6491,7 @@
         <v>258</v>
       </c>
       <c r="C40" s="85" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D40" s="85"/>
     </row>
@@ -6503,7 +6503,7 @@
         <v>258</v>
       </c>
       <c r="C41" s="85" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D41" s="85"/>
     </row>
@@ -6755,7 +6755,7 @@
         <v>258</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D62" s="85"/>
     </row>
@@ -6875,49 +6875,49 @@
         <v>301</v>
       </c>
       <c r="C72" s="85" t="s">
-        <v>316</v>
+        <v>564</v>
       </c>
       <c r="D72" s="85"/>
     </row>
     <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="89" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B73" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C73" s="85" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D73" s="85"/>
     </row>
     <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="94" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B74" s="95" t="s">
         <v>301</v>
       </c>
       <c r="C74" s="95" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D74" s="95"/>
     </row>
     <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="89" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B75" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C75" s="85" t="s">
-        <v>322</v>
+        <v>565</v>
       </c>
       <c r="D75" s="85"/>
     </row>
     <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="89" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B76" s="85" t="s">
         <v>301</v>
@@ -6929,106 +6929,106 @@
     </row>
     <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="89" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B77" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C77" s="85" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D77" s="85"/>
     </row>
     <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="89" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B78" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C78" s="85" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D78" s="85"/>
     </row>
     <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="89" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B79" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C79" s="85" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D79" s="85"/>
     </row>
     <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="89" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B80" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C80" s="85" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D80" s="85"/>
     </row>
     <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="89" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B81" s="85" t="s">
         <v>301</v>
       </c>
       <c r="C81" s="85" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D81" s="85"/>
     </row>
     <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="89" t="s">
+        <v>332</v>
+      </c>
+      <c r="B82" s="85" t="s">
+        <v>333</v>
+      </c>
+      <c r="C82" s="85" t="s">
         <v>334</v>
-      </c>
-      <c r="B82" s="85" t="s">
-        <v>335</v>
-      </c>
-      <c r="C82" s="85" t="s">
-        <v>336</v>
       </c>
       <c r="D82" s="85"/>
     </row>
     <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="89" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B83" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C83" s="85" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D83" s="85"/>
     </row>
     <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="89" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B84" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C84" s="85" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D84" s="85"/>
     </row>
     <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="89" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B85" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C85" s="85" t="s">
         <v>233</v>
@@ -7037,10 +7037,10 @@
     </row>
     <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="89" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B86" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C86" s="85" t="s">
         <v>234</v>
@@ -7049,293 +7049,293 @@
     </row>
     <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="89" t="s">
+        <v>341</v>
+      </c>
+      <c r="B87" s="85" t="s">
+        <v>342</v>
+      </c>
+      <c r="C87" s="85" t="s">
         <v>343</v>
       </c>
-      <c r="B87" s="85" t="s">
-        <v>344</v>
-      </c>
-      <c r="C87" s="85" t="s">
-        <v>345</v>
-      </c>
       <c r="D87" s="85" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="89" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B88" s="85" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C88" s="85" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D88" s="85" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="94" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B89" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C89" s="95" t="s">
         <v>193</v>
       </c>
       <c r="D89" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="94" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B90" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C90" s="95" t="s">
         <v>80</v>
       </c>
       <c r="D90" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="94" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B91" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C91" s="95" t="s">
         <v>81</v>
       </c>
       <c r="D91" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="94" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B92" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C92" s="95" t="s">
         <v>82</v>
       </c>
       <c r="D92" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="94" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B93" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C93" s="95" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D93" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="94" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B94" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C94" s="95" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D94" s="97" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="89" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B95" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C95" s="85" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D95" s="85"/>
     </row>
     <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="89" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B96" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C96" s="85" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D96" s="85"/>
     </row>
     <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="89" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B97" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C97" s="85" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D97" s="85"/>
     </row>
     <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="89" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B98" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C98" s="85" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D98" s="85"/>
     </row>
     <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="89" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B99" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C99" s="85" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D99" s="85"/>
     </row>
     <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="89" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B100" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C100" s="85" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D100" s="85"/>
     </row>
     <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="89" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B101" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C101" s="85" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D101" s="85"/>
     </row>
     <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="89" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B102" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C102" s="85" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D102" s="85"/>
     </row>
     <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="89" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B103" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C103" s="85" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D103" s="85"/>
     </row>
     <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="89" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B104" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C104" s="85" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D104" s="85"/>
     </row>
     <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="89" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B105" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C105" s="85" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D105" s="85"/>
     </row>
     <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="89" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B106" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C106" s="85" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D106" s="85"/>
     </row>
     <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="89" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B107" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C107" s="85" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D107" s="85"/>
     </row>
     <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="89" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B108" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C108" s="85" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D108" s="85"/>
     </row>
     <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="89" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B109" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C109" s="85" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D109" s="85"/>
     </row>
@@ -7347,139 +7347,139 @@
         <v>258</v>
       </c>
       <c r="C110" s="85" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D110" s="85"/>
     </row>
     <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="89" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B111" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C111" s="85" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D111" s="85"/>
     </row>
     <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="89" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B112" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C112" s="85" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D112" s="85"/>
     </row>
     <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="89" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B113" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C113" s="85" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D113" s="85"/>
     </row>
     <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="89" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B114" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C114" s="85" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D114" s="85"/>
     </row>
     <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="89" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B115" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C115" s="85" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D115" s="85"/>
     </row>
     <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="89" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B116" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C116" s="85" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D116" s="85"/>
     </row>
     <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="89" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B117" s="85" t="s">
         <v>275</v>
       </c>
       <c r="C117" s="85" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D117" s="85"/>
     </row>
     <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="94" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B118" s="95" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C118" s="95" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D118" s="95"/>
     </row>
     <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="89" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B119" s="85" t="s">
         <v>275</v>
       </c>
       <c r="C119" s="85" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D119" s="85"/>
     </row>
     <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="89" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B120" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C120" s="85" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D120" s="85"/>
     </row>
     <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="89" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B121" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C121" s="85" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D121" s="85"/>
     </row>
@@ -7491,103 +7491,103 @@
         <v>258</v>
       </c>
       <c r="C122" s="85" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D122" s="85"/>
     </row>
     <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="89" t="s">
+        <v>405</v>
+      </c>
+      <c r="B123" s="85" t="s">
+        <v>333</v>
+      </c>
+      <c r="C123" s="85" t="s">
         <v>407</v>
-      </c>
-      <c r="B123" s="85" t="s">
-        <v>335</v>
-      </c>
-      <c r="C123" s="85" t="s">
-        <v>409</v>
       </c>
       <c r="D123" s="85"/>
     </row>
     <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="89" t="s">
+        <v>406</v>
+      </c>
+      <c r="B124" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C124" s="85" t="s">
         <v>408</v>
-      </c>
-      <c r="B124" s="85" t="s">
-        <v>258</v>
-      </c>
-      <c r="C124" s="85" t="s">
-        <v>410</v>
       </c>
       <c r="D124" s="85"/>
     </row>
     <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="89" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B125" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C125" s="85" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D125" s="85"/>
     </row>
     <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="89" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B126" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C126" s="85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D126" s="85"/>
     </row>
     <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="89" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B127" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C127" s="85" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D127" s="85"/>
     </row>
     <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="89" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B128" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C128" s="85" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D128" s="85"/>
     </row>
     <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="89" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B129" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C129" s="85" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D129" s="85"/>
     </row>
     <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="89" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B130" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C130" s="85" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D130" s="85"/>
     </row>
@@ -7599,7 +7599,7 @@
         <v>258</v>
       </c>
       <c r="C131" s="85" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D131" s="85"/>
     </row>
@@ -7617,623 +7617,623 @@
     </row>
     <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="89" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B133" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C133" s="85" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D133" s="85"/>
     </row>
     <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="89" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B134" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C134" s="85" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D134" s="85"/>
     </row>
     <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="89" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B135" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C135" s="85" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D135" s="85"/>
     </row>
     <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="89" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B136" s="85" t="s">
         <v>269</v>
       </c>
       <c r="C136" s="85" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D136" s="85"/>
     </row>
     <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="89" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B137" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C137" s="85" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D137" s="85"/>
     </row>
     <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="89" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B138" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C138" s="85" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D138" s="85"/>
     </row>
     <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="89" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B139" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C139" s="85" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D139" s="85"/>
     </row>
     <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="89" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B140" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C140" s="85" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D140" s="85"/>
     </row>
     <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="89" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B141" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C141" s="85" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D141" s="85"/>
     </row>
     <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="89" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B142" s="85" t="s">
         <v>275</v>
       </c>
       <c r="C142" s="85" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D142" s="85"/>
     </row>
     <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="89" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B143" s="85" t="s">
         <v>269</v>
       </c>
       <c r="C143" s="85" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D143" s="85"/>
     </row>
     <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="94" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B144" s="95" t="s">
         <v>301</v>
       </c>
       <c r="C144" s="95" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D144" s="95"/>
     </row>
     <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="89" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B145" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C145" s="85" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D145" s="85"/>
     </row>
     <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="89" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B146" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C146" s="85" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D146" s="85"/>
     </row>
     <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="89" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B147" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C147" s="85" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D147" s="85"/>
     </row>
     <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="90" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B148" s="91" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C148" s="91" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D148" s="91"/>
     </row>
     <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="89" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B149" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C149" s="85" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D149" s="85"/>
     </row>
     <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="89" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B150" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C150" s="85" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D150" s="85"/>
     </row>
     <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="89" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B151" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C151" s="85" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D151" s="85"/>
     </row>
     <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="89" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B152" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C152" s="85" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D152" s="85"/>
     </row>
     <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="89" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B153" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C153" s="85" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D153" s="85"/>
     </row>
     <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="89" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B154" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C154" s="85" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D154" s="85"/>
     </row>
     <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="89" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B155" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C155" s="85" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D155" s="85"/>
     </row>
     <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="89" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B156" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C156" s="85" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D156" s="85"/>
     </row>
     <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="89" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B157" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C157" s="85" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D157" s="85"/>
     </row>
     <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="89" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B158" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C158" s="85" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D158" s="85"/>
     </row>
     <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="89" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B159" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C159" s="85" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D159" s="85"/>
     </row>
     <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="89" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B160" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C160" s="85" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D160" s="85"/>
     </row>
     <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="89" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B161" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C161" s="85" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D161" s="85"/>
     </row>
     <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="89" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B162" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C162" s="85" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D162" s="85"/>
     </row>
     <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="89" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B163" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C163" s="85" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D163" s="85"/>
     </row>
     <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="89" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B164" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C164" s="85" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D164" s="85"/>
     </row>
     <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="89" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B165" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C165" s="85" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D165" s="85"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="83" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B166" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C166" s="84" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="89" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B167" s="85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C167" s="85" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D167" s="85"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="83" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B168" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C168" s="84" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="89" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B169" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C169" s="85" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D169" s="85"/>
     </row>
     <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="89" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B170" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C170" s="85" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D170" s="85"/>
     </row>
     <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="89" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B171" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C171" s="85" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D171" s="85"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="83" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B172" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C172" s="84" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="89" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B173" s="85" t="s">
         <v>258</v>
       </c>
       <c r="C173" s="85" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D173" s="85"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="83" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B174" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C174" s="84" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="83" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B175" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C175" s="84" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="83" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B176" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C176" s="84" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="83" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B177" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C177" s="84" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="83" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B178" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C178" s="84" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="83" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B179" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C179" s="84" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="83" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B180" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C180" s="84" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="83" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B181" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C181" s="84" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="83" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B182" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C182" s="84" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="83" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B183" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C183" s="84" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="83" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B184" s="84" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C184" s="84" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="83" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B185" s="84" t="s">
         <v>258</v>
       </c>
       <c r="C185" s="84" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added images to chapter home pages
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEEA9B1-54C7-4362-B088-09B1CD29CE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E82DC8-47FC-4EE1-BC48-5550B3DEB996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55020" yWindow="600" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="576">
   <si>
     <t>ID</t>
   </si>
@@ -1737,6 +1737,36 @@
   </si>
   <si>
     <t>Umbrella</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>Chapter 1 Landing Image</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>Chapter 2 Landing Image</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>Chapter 3 Landing Image</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>Chapter 4 Landing Image</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>Chapter 5 Landing Image</t>
   </si>
 </sst>
 </file>
@@ -6010,10 +6040,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8236,6 +8266,61 @@
         <v>563</v>
       </c>
     </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="83" t="s">
+        <v>566</v>
+      </c>
+      <c r="B186" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C186" s="84" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="83" t="s">
+        <v>568</v>
+      </c>
+      <c r="B187" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C187" s="84" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="83" t="s">
+        <v>570</v>
+      </c>
+      <c r="B188" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C188" s="84" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="83" t="s">
+        <v>572</v>
+      </c>
+      <c r="B189" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C189" s="84" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="83" t="s">
+        <v>574</v>
+      </c>
+      <c r="B190" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C190" s="84" t="s">
+        <v>575</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Indicator Center to treeview
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E82DC8-47FC-4EE1-BC48-5550B3DEB996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CBDF1E-9BF8-4349-9E33-6CEEFD0E9823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="578">
   <si>
     <t>ID</t>
   </si>
@@ -1767,6 +1767,12 @@
   </si>
   <si>
     <t>Chapter 5 Landing Image</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>Indicator Center</t>
   </si>
 </sst>
 </file>
@@ -6040,10 +6046,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D190"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8321,6 +8327,17 @@
         <v>575</v>
       </c>
     </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="83" t="s">
+        <v>576</v>
+      </c>
+      <c r="B191" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="C191" s="84" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated chapter home page images when clicked
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CBDF1E-9BF8-4349-9E33-6CEEFD0E9823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C251EF-59BD-4A11-91A6-8D983DB7B024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="588">
   <si>
     <t>ID</t>
   </si>
@@ -1773,6 +1773,36 @@
   </si>
   <si>
     <t>Indicator Center</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>Chapter 1 Landing Image Large</t>
+  </si>
+  <si>
+    <t>Chapter 2 Landing Image Large</t>
+  </si>
+  <si>
+    <t>Chapter 3 Landing Image Large</t>
+  </si>
+  <si>
+    <t>Chapter 4 Landing Image Large</t>
+  </si>
+  <si>
+    <t>Chapter 5 Landing Image Large</t>
   </si>
 </sst>
 </file>
@@ -6046,10 +6076,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8338,6 +8368,61 @@
         <v>577</v>
       </c>
     </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="83" t="s">
+        <v>578</v>
+      </c>
+      <c r="B192" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C192" s="84" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="83" t="s">
+        <v>579</v>
+      </c>
+      <c r="B193" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C193" s="84" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="83" t="s">
+        <v>580</v>
+      </c>
+      <c r="B194" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C194" s="84" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="83" t="s">
+        <v>581</v>
+      </c>
+      <c r="B195" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C195" s="84" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="83" t="s">
+        <v>582</v>
+      </c>
+      <c r="B196" s="84" t="s">
+        <v>333</v>
+      </c>
+      <c r="C196" s="84" t="s">
+        <v>587</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 3 new pages
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C251EF-59BD-4A11-91A6-8D983DB7B024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE840E59-8372-4D17-BD9C-DD768618C143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="593">
   <si>
     <t>ID</t>
   </si>
@@ -1803,6 +1803,21 @@
   </si>
   <si>
     <t>Chapter 5 Landing Image Large</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Core team kickoff</t>
+  </si>
+  <si>
+    <t>Explore Equitable Resilience</t>
+  </si>
+  <si>
+    <t>Finding Funding to Support Taking Action</t>
   </si>
 </sst>
 </file>
@@ -6076,10 +6091,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D196"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8423,6 +8438,39 @@
         <v>587</v>
       </c>
     </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="83" t="s">
+        <v>588</v>
+      </c>
+      <c r="B197" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C197" s="84" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="83" t="s">
+        <v>589</v>
+      </c>
+      <c r="B198" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C198" s="84" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="83" t="s">
+        <v>148</v>
+      </c>
+      <c r="B199" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C199" s="84" t="s">
+        <v>592</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edited project creation and selection text, capitalized text of instuction entries and headers in XML files, and updated text in ID chart and available content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cromanow\MetroCERIRepo\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE840E59-8372-4D17-BD9C-DD768618C143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2B989-C8E1-4FB5-AF90-8D7FDE656563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4335" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10080" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -1643,18 +1643,6 @@
     <t>How ERB centers equity</t>
   </si>
   <si>
-    <t>Supporting materials</t>
-  </si>
-  <si>
-    <t>Indicator card sorting</t>
-  </si>
-  <si>
-    <t>Reflection diary</t>
-  </si>
-  <si>
-    <t>Key takeaways</t>
-  </si>
-  <si>
     <t>MyPortfolio</t>
   </si>
   <si>
@@ -1818,6 +1806,18 @@
   </si>
   <si>
     <t>Finding Funding to Support Taking Action</t>
+  </si>
+  <si>
+    <t>Supporting Materials</t>
+  </si>
+  <si>
+    <t>Indicator Card Sorting</t>
+  </si>
+  <si>
+    <t>Reflection Diary</t>
+  </si>
+  <si>
+    <t>Key Takeaways</t>
   </si>
 </sst>
 </file>
@@ -2661,19 +2661,19 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="24"/>
-    <col min="8" max="8" width="15.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="8.85546875" style="24"/>
+    <col min="1" max="1" width="5.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.81640625" style="24"/>
+    <col min="8" max="8" width="15.453125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="8.81640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="56" t="s">
         <v>76</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
     </row>
-    <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="75" t="s">
         <v>98</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
     </row>
-    <row r="4" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
     </row>
-    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>48</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
     </row>
-    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>49</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="U6" s="24"/>
       <c r="V6" s="24"/>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>73</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="U7" s="24"/>
       <c r="V7" s="24"/>
     </row>
-    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>59</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
     </row>
-    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>61</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="U10" s="24"/>
       <c r="V10" s="24"/>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>62</v>
       </c>
@@ -3053,7 +3053,7 @@
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>63</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
     </row>
-    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>64</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
     </row>
-    <row r="14" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>65</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
     </row>
-    <row r="15" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33">
         <v>10</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
     </row>
-    <row r="16" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34">
         <v>11</v>
       </c>
@@ -3215,7 +3215,7 @@
       <c r="U16" s="24"/>
       <c r="V16" s="24"/>
     </row>
-    <row r="17" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="35">
         <v>111</v>
       </c>
@@ -3249,7 +3249,7 @@
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
     </row>
-    <row r="18" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34">
         <v>12</v>
       </c>
@@ -3283,7 +3283,7 @@
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
     </row>
-    <row r="19" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="35">
         <v>121</v>
       </c>
@@ -3317,7 +3317,7 @@
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
     </row>
-    <row r="20" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="34">
         <v>13</v>
       </c>
@@ -3351,7 +3351,7 @@
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
     </row>
-    <row r="21" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="35">
         <v>131</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
     </row>
-    <row r="22" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35">
         <v>132</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
     </row>
-    <row r="23" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34">
         <v>14</v>
       </c>
@@ -3453,7 +3453,7 @@
       <c r="U23" s="24"/>
       <c r="V23" s="24"/>
     </row>
-    <row r="24" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="36">
         <v>20</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="U24" s="24"/>
       <c r="V24" s="24"/>
     </row>
-    <row r="25" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="37">
         <v>201</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
     </row>
-    <row r="26" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="37">
         <v>202</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
     </row>
-    <row r="27" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34">
         <v>21</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="U27" s="24"/>
       <c r="V27" s="24"/>
     </row>
-    <row r="28" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="34">
         <v>22</v>
       </c>
@@ -3621,7 +3621,7 @@
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
     </row>
-    <row r="29" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="34">
         <v>23</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
     </row>
-    <row r="30" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="34">
         <v>24</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="U30" s="24"/>
       <c r="V30" s="24"/>
     </row>
-    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="34">
         <v>25</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="U31" s="24"/>
       <c r="V31" s="24"/>
     </row>
-    <row r="32" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="36">
         <v>30</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
     </row>
-    <row r="33" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="34">
         <v>301</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="U33" s="24"/>
       <c r="V33" s="24"/>
     </row>
-    <row r="34" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34">
         <v>31</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="U34" s="24"/>
       <c r="V34" s="24"/>
     </row>
-    <row r="35" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="34">
         <v>32</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="U35" s="24"/>
       <c r="V35" s="24"/>
     </row>
-    <row r="36" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="34">
         <v>33</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="U36" s="24"/>
       <c r="V36" s="24"/>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34">
         <v>34</v>
       </c>
@@ -3925,7 +3925,7 @@
       <c r="U37" s="24"/>
       <c r="V37" s="24"/>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="34">
         <v>35</v>
       </c>
@@ -3959,7 +3959,7 @@
       <c r="U38" s="24"/>
       <c r="V38" s="24"/>
     </row>
-    <row r="39" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34">
         <v>36</v>
       </c>
@@ -3993,7 +3993,7 @@
       <c r="U39" s="24"/>
       <c r="V39" s="24"/>
     </row>
-    <row r="40" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34">
         <v>37</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="U40" s="24"/>
       <c r="V40" s="24"/>
     </row>
-    <row r="41" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="36">
         <v>40</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="U41" s="24"/>
       <c r="V41" s="24"/>
     </row>
-    <row r="42" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="37">
         <v>401</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="U42" s="24"/>
       <c r="V42" s="24"/>
     </row>
-    <row r="43" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="34">
         <v>41</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="U43" s="24"/>
       <c r="V43" s="24"/>
     </row>
-    <row r="44" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="34">
         <v>42</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="U44" s="24"/>
       <c r="V44" s="24"/>
     </row>
-    <row r="45" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="37">
         <v>421</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="U45" s="24"/>
       <c r="V45" s="24"/>
     </row>
-    <row r="46" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34">
         <v>43</v>
       </c>
@@ -4229,7 +4229,7 @@
       <c r="U46" s="24"/>
       <c r="V46" s="24"/>
     </row>
-    <row r="47" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="35">
         <v>431</v>
       </c>
@@ -4263,7 +4263,7 @@
       <c r="U47" s="24"/>
       <c r="V47" s="24"/>
     </row>
-    <row r="48" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="35">
         <v>432</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="U48" s="24"/>
       <c r="V48" s="24"/>
     </row>
-    <row r="49" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="34">
         <v>44</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="U49" s="24"/>
       <c r="V49" s="24"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50" s="36">
         <v>50</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51" s="34">
         <v>51</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52" s="34">
         <v>52</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" s="34">
         <v>53</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" s="34">
         <v>54</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55" s="34">
         <v>55</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" s="34">
         <v>56</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A57" s="34">
         <v>57</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" s="34">
         <v>58</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" s="34">
         <v>59</v>
       </c>
@@ -4516,26 +4516,26 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" customWidth="1"/>
-    <col min="14" max="14" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" customWidth="1"/>
+    <col min="12" max="12" width="86.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7265625" customWidth="1"/>
+    <col min="14" max="14" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="65" t="s">
         <v>93</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="I1" s="77"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="63" t="s">
         <v>93</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>94</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="63" t="s">
         <v>95</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="63" t="s">
         <v>96</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="63" t="s">
         <v>97</v>
       </c>
@@ -4672,7 +4672,7 @@
       <c r="C6" s="80"/>
       <c r="D6" s="59"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="63" t="s">
         <v>114</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="C7" s="80"/>
       <c r="D7" s="59"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="64" t="s">
         <v>115</v>
       </c>
@@ -4692,7 +4692,7 @@
       <c r="C8" s="80"/>
       <c r="D8" s="59"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
         <v>97</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="63" t="s">
         <v>101</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="63" t="s">
         <v>102</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="63" t="s">
         <v>103</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="63" t="s">
         <v>104</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="64" t="s">
         <v>105</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C17" s="63" t="s">
         <v>122</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C18" s="63" t="s">
         <v>123</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C19" s="63" t="s">
         <v>124</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C20" s="63" t="s">
         <v>125</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C21" s="63" t="s">
         <v>126</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C22" s="63" t="s">
         <v>127</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="63" t="s">
         <v>128</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C24" s="63" t="s">
         <v>129</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C25" s="63" t="s">
         <v>130</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C26" s="63" t="s">
         <v>131</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C27" s="63" t="s">
         <v>132</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C28" s="63" t="s">
         <v>133</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C29" s="63" t="s">
         <v>134</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C30" s="63" t="s">
         <v>135</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C31" s="63" t="s">
         <v>136</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C32" s="63" t="s">
         <v>137</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C33" s="63" t="s">
         <v>138</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C34" s="63" t="s">
         <v>139</v>
       </c>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="E34" s="67"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C35" s="63" t="s">
         <v>140</v>
       </c>
@@ -5164,7 +5164,7 @@
       </c>
       <c r="E35" s="67"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C36" s="63" t="s">
         <v>141</v>
       </c>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="E36" s="67"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C37" s="63" t="s">
         <v>142</v>
       </c>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="E37" s="67"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C38" s="63" t="s">
         <v>143</v>
       </c>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="E38" s="67"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C39" s="63" t="s">
         <v>144</v>
       </c>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="E39" s="67"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C40" s="63" t="s">
         <v>145</v>
       </c>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="E40" s="67"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C41" s="64" t="s">
         <v>146</v>
       </c>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="E41" s="67"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C42" s="76" t="s">
         <v>224</v>
       </c>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="E42" s="67"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C43" s="76" t="s">
         <v>228</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C44" s="76" t="s">
         <v>229</v>
       </c>
@@ -5257,22 +5257,22 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="24" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.54296875" style="24" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.453125" style="24" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
         <v>93</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="71" t="s">
         <v>93</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="71" t="s">
         <v>94</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="71" t="s">
         <v>95</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="71" t="s">
         <v>96</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="71" t="s">
         <v>97</v>
       </c>
@@ -5430,7 +5430,7 @@
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="71" t="s">
         <v>114</v>
       </c>
@@ -5447,7 +5447,7 @@
       <c r="J7" s="73"/>
       <c r="K7" s="73"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="71" t="s">
         <v>115</v>
       </c>
@@ -5464,7 +5464,7 @@
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="73"/>
       <c r="B9" s="73"/>
       <c r="C9" s="74"/>
@@ -5477,7 +5477,7 @@
       <c r="J9" s="73"/>
       <c r="K9" s="73"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="73"/>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
@@ -5490,7 +5490,7 @@
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="68" t="s">
         <v>97</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="71" t="s">
         <v>101</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="71" t="s">
         <v>102</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="71" t="s">
         <v>103</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="71" t="s">
         <v>104</v>
       </c>
@@ -5627,7 +5627,7 @@
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="71" t="s">
         <v>105</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="73"/>
       <c r="B17" s="73"/>
       <c r="C17" s="74"/>
@@ -5673,7 +5673,7 @@
       <c r="J17" s="73"/>
       <c r="K17" s="73"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="73"/>
       <c r="B18" s="73"/>
       <c r="C18" s="74"/>
@@ -5694,7 +5694,7 @@
       <c r="J18" s="73"/>
       <c r="K18" s="73"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="73"/>
       <c r="B19" s="73"/>
       <c r="C19" s="74"/>
@@ -5711,7 +5711,7 @@
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="73"/>
       <c r="B20" s="73"/>
       <c r="C20" s="74"/>
@@ -5728,7 +5728,7 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="73"/>
       <c r="B21" s="73"/>
       <c r="C21" s="74"/>
@@ -5745,7 +5745,7 @@
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="73"/>
       <c r="B22" s="73"/>
       <c r="C22" s="74"/>
@@ -5762,7 +5762,7 @@
       <c r="J22" s="73"/>
       <c r="K22" s="73"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="73"/>
       <c r="B23" s="73"/>
       <c r="C23" s="74"/>
@@ -5779,7 +5779,7 @@
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="73"/>
       <c r="B24" s="73"/>
       <c r="C24" s="74"/>
@@ -5796,7 +5796,7 @@
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="73"/>
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
@@ -5813,7 +5813,7 @@
       <c r="J25" s="73"/>
       <c r="K25" s="73"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="73"/>
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
@@ -5830,7 +5830,7 @@
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="73"/>
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
@@ -5847,7 +5847,7 @@
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="73"/>
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
@@ -5864,7 +5864,7 @@
       <c r="J28" s="73"/>
       <c r="K28" s="73"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="73"/>
       <c r="B29" s="73"/>
       <c r="C29" s="74"/>
@@ -5881,7 +5881,7 @@
       <c r="J29" s="73"/>
       <c r="K29" s="73"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="73"/>
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
@@ -5898,7 +5898,7 @@
       <c r="J30" s="73"/>
       <c r="K30" s="73"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="73"/>
       <c r="B31" s="73"/>
       <c r="C31" s="74"/>
@@ -5915,7 +5915,7 @@
       <c r="J31" s="73"/>
       <c r="K31" s="73"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="73"/>
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
@@ -5932,7 +5932,7 @@
       <c r="J32" s="73"/>
       <c r="K32" s="73"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="73"/>
       <c r="B33" s="73"/>
       <c r="C33" s="74"/>
@@ -5949,7 +5949,7 @@
       <c r="J33" s="73"/>
       <c r="K33" s="73"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="73"/>
       <c r="B34" s="73"/>
       <c r="C34" s="74"/>
@@ -5966,7 +5966,7 @@
       <c r="J34" s="73"/>
       <c r="K34" s="73"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="73"/>
       <c r="B35" s="73"/>
       <c r="C35" s="74"/>
@@ -5983,7 +5983,7 @@
       <c r="J35" s="73"/>
       <c r="K35" s="73"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="73"/>
       <c r="B36" s="73"/>
       <c r="C36" s="74"/>
@@ -6000,7 +6000,7 @@
       <c r="J36" s="73"/>
       <c r="K36" s="73"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="73"/>
       <c r="B37" s="73"/>
       <c r="C37" s="74"/>
@@ -6017,7 +6017,7 @@
       <c r="J37" s="73"/>
       <c r="K37" s="73"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="73"/>
       <c r="B38" s="73"/>
       <c r="C38" s="74"/>
@@ -6034,7 +6034,7 @@
       <c r="J38" s="73"/>
       <c r="K38" s="73"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="73"/>
       <c r="B39" s="73"/>
       <c r="C39" s="74"/>
@@ -6051,7 +6051,7 @@
       <c r="J39" s="73"/>
       <c r="K39" s="73"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="73"/>
       <c r="B40" s="73"/>
       <c r="C40" s="74"/>
@@ -6068,7 +6068,7 @@
       <c r="J40" s="73"/>
       <c r="K40" s="73"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="59"/>
       <c r="B41" s="59"/>
       <c r="C41" s="32"/>
@@ -6081,7 +6081,7 @@
       <c r="J41" s="59"/>
       <c r="K41" s="59"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G42" s="67"/>
     </row>
   </sheetData>
@@ -6093,20 +6093,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="84" customWidth="1"/>
-    <col min="3" max="3" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" style="84" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="84" customWidth="1"/>
+    <col min="3" max="3" width="80.81640625" style="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7265625" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:4" s="86" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="89" t="s">
         <v>59</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="D3" s="93"/>
     </row>
-    <row r="4" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="89" t="s">
         <v>60</v>
       </c>
@@ -6144,7 +6144,7 @@
       </c>
       <c r="D4" s="85"/>
     </row>
-    <row r="5" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="89" t="s">
         <v>61</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="D5" s="85"/>
     </row>
-    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="89" t="s">
         <v>62</v>
       </c>
@@ -6168,7 +6168,7 @@
       </c>
       <c r="D6" s="85"/>
     </row>
-    <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
         <v>63</v>
       </c>
@@ -6180,7 +6180,7 @@
       </c>
       <c r="D7" s="85"/>
     </row>
-    <row r="8" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
         <v>64</v>
       </c>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="D8" s="85"/>
     </row>
-    <row r="9" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="89" t="s">
         <v>65</v>
       </c>
@@ -6204,7 +6204,7 @@
       </c>
       <c r="D9" s="85"/>
     </row>
-    <row r="10" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="89" t="s">
         <v>260</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="D10" s="85"/>
     </row>
-    <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="89" t="s">
         <v>262</v>
       </c>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="D11" s="85"/>
     </row>
-    <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="89" t="s">
         <v>152</v>
       </c>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="D12" s="85"/>
     </row>
-    <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="89" t="s">
         <v>515</v>
       </c>
@@ -6252,7 +6252,7 @@
       </c>
       <c r="D13" s="85"/>
     </row>
-    <row r="14" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
         <v>157</v>
       </c>
@@ -6260,11 +6260,11 @@
         <v>258</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>534</v>
+        <v>589</v>
       </c>
       <c r="D14" s="85"/>
     </row>
-    <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="89" t="s">
         <v>158</v>
       </c>
@@ -6272,11 +6272,11 @@
         <v>258</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D15" s="85"/>
     </row>
-    <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="89" t="s">
         <v>159</v>
       </c>
@@ -6284,11 +6284,11 @@
         <v>258</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>535</v>
+        <v>590</v>
       </c>
       <c r="D16" s="85"/>
     </row>
-    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="89" t="s">
         <v>160</v>
       </c>
@@ -6300,7 +6300,7 @@
       </c>
       <c r="D17" s="85"/>
     </row>
-    <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="89" t="s">
         <v>264</v>
       </c>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="D18" s="85"/>
     </row>
-    <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="89" t="s">
         <v>265</v>
       </c>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="D19" s="85"/>
     </row>
-    <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="89" t="s">
         <v>266</v>
       </c>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="D20" s="85"/>
     </row>
-    <row r="21" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="89" t="s">
         <v>267</v>
       </c>
@@ -6348,7 +6348,7 @@
       </c>
       <c r="D21" s="85"/>
     </row>
-    <row r="22" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="89" t="s">
         <v>268</v>
       </c>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="D22" s="85"/>
     </row>
-    <row r="23" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="89" t="s">
         <v>153</v>
       </c>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="D23" s="85"/>
     </row>
-    <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="89" t="s">
         <v>161</v>
       </c>
@@ -6380,11 +6380,11 @@
         <v>258</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>536</v>
+        <v>591</v>
       </c>
       <c r="D24" s="85"/>
     </row>
-    <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="89" t="s">
         <v>162</v>
       </c>
@@ -6392,11 +6392,11 @@
         <v>258</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>537</v>
+        <v>592</v>
       </c>
       <c r="D25" s="85"/>
     </row>
-    <row r="26" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="89" t="s">
         <v>163</v>
       </c>
@@ -6404,11 +6404,11 @@
         <v>258</v>
       </c>
       <c r="C26" s="85" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D26" s="85"/>
     </row>
-    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="89" t="s">
         <v>164</v>
       </c>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="D27" s="85"/>
     </row>
-    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="89" t="s">
         <v>165</v>
       </c>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="D28" s="85"/>
     </row>
-    <row r="29" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="89" t="s">
         <v>271</v>
       </c>
@@ -6440,11 +6440,11 @@
         <v>258</v>
       </c>
       <c r="C29" s="85" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D29" s="85"/>
     </row>
-    <row r="30" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="89" t="s">
         <v>272</v>
       </c>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="D30" s="85"/>
     </row>
-    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="89" t="s">
         <v>274</v>
       </c>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="D31" s="85"/>
     </row>
-    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="89" t="s">
         <v>276</v>
       </c>
@@ -6480,7 +6480,7 @@
       </c>
       <c r="D32" s="85"/>
     </row>
-    <row r="33" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="89" t="s">
         <v>154</v>
       </c>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="D33" s="85"/>
     </row>
-    <row r="34" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="89" t="s">
         <v>166</v>
       </c>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="D34" s="85"/>
     </row>
-    <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="89" t="s">
         <v>167</v>
       </c>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="D35" s="85"/>
     </row>
-    <row r="36" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="89" t="s">
         <v>168</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="D36" s="85"/>
     </row>
-    <row r="37" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="89" t="s">
         <v>169</v>
       </c>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="D37" s="85"/>
     </row>
-    <row r="38" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="89" t="s">
         <v>170</v>
       </c>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="D38" s="85"/>
     </row>
-    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="89" t="s">
         <v>171</v>
       </c>
@@ -6564,7 +6564,7 @@
       </c>
       <c r="D39" s="85"/>
     </row>
-    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="89" t="s">
         <v>172</v>
       </c>
@@ -6576,7 +6576,7 @@
       </c>
       <c r="D40" s="85"/>
     </row>
-    <row r="41" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="89" t="s">
         <v>278</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="D41" s="85"/>
     </row>
-    <row r="42" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="94" t="s">
         <v>279</v>
       </c>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="D42" s="95"/>
     </row>
-    <row r="43" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="94" t="s">
         <v>155</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
       <c r="D43" s="95"/>
     </row>
-    <row r="44" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="94" t="s">
         <v>174</v>
       </c>
@@ -6624,7 +6624,7 @@
       </c>
       <c r="D44" s="95"/>
     </row>
-    <row r="45" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="94" t="s">
         <v>175</v>
       </c>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="D45" s="95"/>
     </row>
-    <row r="46" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="94" t="s">
         <v>176</v>
       </c>
@@ -6648,7 +6648,7 @@
       </c>
       <c r="D46" s="95"/>
     </row>
-    <row r="47" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="94" t="s">
         <v>177</v>
       </c>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="D47" s="95"/>
     </row>
-    <row r="48" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="94" t="s">
         <v>285</v>
       </c>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="D48" s="95"/>
     </row>
-    <row r="49" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="94" t="s">
         <v>287</v>
       </c>
@@ -6684,7 +6684,7 @@
       </c>
       <c r="D49" s="95"/>
     </row>
-    <row r="50" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="94" t="s">
         <v>289</v>
       </c>
@@ -6696,7 +6696,7 @@
       </c>
       <c r="D50" s="95"/>
     </row>
-    <row r="51" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="94" t="s">
         <v>290</v>
       </c>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="D51" s="95"/>
     </row>
-    <row r="52" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="94" t="s">
         <v>291</v>
       </c>
@@ -6720,7 +6720,7 @@
       </c>
       <c r="D52" s="95"/>
     </row>
-    <row r="53" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="94" t="s">
         <v>156</v>
       </c>
@@ -6732,7 +6732,7 @@
       </c>
       <c r="D53" s="95"/>
     </row>
-    <row r="54" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="94" t="s">
         <v>178</v>
       </c>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="D54" s="95"/>
     </row>
-    <row r="55" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="94" t="s">
         <v>179</v>
       </c>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="D55" s="95"/>
     </row>
-    <row r="56" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="94" t="s">
         <v>180</v>
       </c>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="D56" s="95"/>
     </row>
-    <row r="57" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="94" t="s">
         <v>181</v>
       </c>
@@ -6780,7 +6780,7 @@
       </c>
       <c r="D57" s="95"/>
     </row>
-    <row r="58" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="94" t="s">
         <v>182</v>
       </c>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="D58" s="95"/>
     </row>
-    <row r="59" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="94" t="s">
         <v>183</v>
       </c>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="D59" s="95"/>
     </row>
-    <row r="60" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="94" t="s">
         <v>184</v>
       </c>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="D60" s="95"/>
     </row>
-    <row r="61" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="94" t="s">
         <v>185</v>
       </c>
@@ -6828,7 +6828,7 @@
       </c>
       <c r="D61" s="95"/>
     </row>
-    <row r="62" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="89" t="s">
         <v>186</v>
       </c>
@@ -6840,7 +6840,7 @@
       </c>
       <c r="D62" s="85"/>
     </row>
-    <row r="63" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="89" t="s">
         <v>297</v>
       </c>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="D63" s="85"/>
     </row>
-    <row r="64" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="89" t="s">
         <v>299</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="D64" s="85"/>
     </row>
-    <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="89" t="s">
         <v>300</v>
       </c>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="D65" s="85"/>
     </row>
-    <row r="66" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="89" t="s">
         <v>303</v>
       </c>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="D66" s="85"/>
     </row>
-    <row r="67" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="89" t="s">
         <v>305</v>
       </c>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="D67" s="85"/>
     </row>
-    <row r="68" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="89" t="s">
         <v>307</v>
       </c>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="D68" s="85"/>
     </row>
-    <row r="69" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="89" t="s">
         <v>309</v>
       </c>
@@ -6924,7 +6924,7 @@
       </c>
       <c r="D69" s="85"/>
     </row>
-    <row r="70" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="89" t="s">
         <v>311</v>
       </c>
@@ -6936,7 +6936,7 @@
       </c>
       <c r="D70" s="85"/>
     </row>
-    <row r="71" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="89" t="s">
         <v>313</v>
       </c>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="D71" s="85"/>
     </row>
-    <row r="72" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="89" t="s">
         <v>315</v>
       </c>
@@ -6956,11 +6956,11 @@
         <v>301</v>
       </c>
       <c r="C72" s="85" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D72" s="85"/>
     </row>
-    <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="89" t="s">
         <v>316</v>
       </c>
@@ -6972,7 +6972,7 @@
       </c>
       <c r="D73" s="85"/>
     </row>
-    <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="94" t="s">
         <v>318</v>
       </c>
@@ -6984,7 +6984,7 @@
       </c>
       <c r="D74" s="95"/>
     </row>
-    <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="89" t="s">
         <v>320</v>
       </c>
@@ -6992,11 +6992,11 @@
         <v>301</v>
       </c>
       <c r="C75" s="85" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D75" s="85"/>
     </row>
-    <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="89" t="s">
         <v>321</v>
       </c>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="D76" s="85"/>
     </row>
-    <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="89" t="s">
         <v>322</v>
       </c>
@@ -7020,7 +7020,7 @@
       </c>
       <c r="D77" s="85"/>
     </row>
-    <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="89" t="s">
         <v>324</v>
       </c>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="D78" s="85"/>
     </row>
-    <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="89" t="s">
         <v>326</v>
       </c>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="D79" s="85"/>
     </row>
-    <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="89" t="s">
         <v>328</v>
       </c>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="D80" s="85"/>
     </row>
-    <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="89" t="s">
         <v>330</v>
       </c>
@@ -7068,7 +7068,7 @@
       </c>
       <c r="D81" s="85"/>
     </row>
-    <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="89" t="s">
         <v>332</v>
       </c>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="D82" s="85"/>
     </row>
-    <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="89" t="s">
         <v>335</v>
       </c>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="D83" s="85"/>
     </row>
-    <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="89" t="s">
         <v>337</v>
       </c>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="D84" s="85"/>
     </row>
-    <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="89" t="s">
         <v>339</v>
       </c>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="D85" s="85"/>
     </row>
-    <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="89" t="s">
         <v>340</v>
       </c>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="D86" s="85"/>
     </row>
-    <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="89" t="s">
         <v>341</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="89" t="s">
         <v>344</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="94" t="s">
         <v>347</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="94" t="s">
         <v>348</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="94" t="s">
         <v>349</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="94" t="s">
         <v>350</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="94" t="s">
         <v>351</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="94" t="s">
         <v>354</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="89" t="s">
         <v>357</v>
       </c>
@@ -7252,7 +7252,7 @@
       </c>
       <c r="D95" s="85"/>
     </row>
-    <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="89" t="s">
         <v>359</v>
       </c>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="D96" s="85"/>
     </row>
-    <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="89" t="s">
         <v>360</v>
       </c>
@@ -7276,7 +7276,7 @@
       </c>
       <c r="D97" s="85"/>
     </row>
-    <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="89" t="s">
         <v>362</v>
       </c>
@@ -7288,7 +7288,7 @@
       </c>
       <c r="D98" s="85"/>
     </row>
-    <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="89" t="s">
         <v>364</v>
       </c>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="D99" s="85"/>
     </row>
-    <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="89" t="s">
         <v>366</v>
       </c>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="D100" s="85"/>
     </row>
-    <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="89" t="s">
         <v>368</v>
       </c>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="D101" s="85"/>
     </row>
-    <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="89" t="s">
         <v>372</v>
       </c>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="D102" s="85"/>
     </row>
-    <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="89" t="s">
         <v>374</v>
       </c>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="D103" s="85"/>
     </row>
-    <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="89" t="s">
         <v>376</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="D104" s="85"/>
     </row>
-    <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="89" t="s">
         <v>378</v>
       </c>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="D105" s="85"/>
     </row>
-    <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="89" t="s">
         <v>379</v>
       </c>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="D106" s="85"/>
     </row>
-    <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="89" t="s">
         <v>380</v>
       </c>
@@ -7396,7 +7396,7 @@
       </c>
       <c r="D107" s="85"/>
     </row>
-    <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="89" t="s">
         <v>381</v>
       </c>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="D108" s="85"/>
     </row>
-    <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="89" t="s">
         <v>383</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="D109" s="85"/>
     </row>
-    <row r="110" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="89" t="s">
         <v>187</v>
       </c>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="D110" s="85"/>
     </row>
-    <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="89" t="s">
         <v>386</v>
       </c>
@@ -7444,7 +7444,7 @@
       </c>
       <c r="D111" s="85"/>
     </row>
-    <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="89" t="s">
         <v>370</v>
       </c>
@@ -7456,7 +7456,7 @@
       </c>
       <c r="D112" s="85"/>
     </row>
-    <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="89" t="s">
         <v>371</v>
       </c>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="D113" s="85"/>
     </row>
-    <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="89" t="s">
         <v>389</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="D114" s="85"/>
     </row>
-    <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="89" t="s">
         <v>390</v>
       </c>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="D115" s="85"/>
     </row>
-    <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="89" t="s">
         <v>392</v>
       </c>
@@ -7504,7 +7504,7 @@
       </c>
       <c r="D116" s="85"/>
     </row>
-    <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="89" t="s">
         <v>394</v>
       </c>
@@ -7516,7 +7516,7 @@
       </c>
       <c r="D117" s="85"/>
     </row>
-    <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="94" t="s">
         <v>396</v>
       </c>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="D118" s="95"/>
     </row>
-    <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="89" t="s">
         <v>398</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="D119" s="85"/>
     </row>
-    <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="89" t="s">
         <v>400</v>
       </c>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="D120" s="85"/>
     </row>
-    <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="89" t="s">
         <v>402</v>
       </c>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="D121" s="85"/>
     </row>
-    <row r="122" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="89" t="s">
         <v>188</v>
       </c>
@@ -7576,7 +7576,7 @@
       </c>
       <c r="D122" s="85"/>
     </row>
-    <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" s="89" t="s">
         <v>405</v>
       </c>
@@ -7588,7 +7588,7 @@
       </c>
       <c r="D123" s="85"/>
     </row>
-    <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A124" s="89" t="s">
         <v>406</v>
       </c>
@@ -7600,7 +7600,7 @@
       </c>
       <c r="D124" s="85"/>
     </row>
-    <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="89" t="s">
         <v>409</v>
       </c>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="D125" s="85"/>
     </row>
-    <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" s="89" t="s">
         <v>411</v>
       </c>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="D126" s="85"/>
     </row>
-    <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A127" s="89" t="s">
         <v>413</v>
       </c>
@@ -7636,7 +7636,7 @@
       </c>
       <c r="D127" s="85"/>
     </row>
-    <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A128" s="89" t="s">
         <v>414</v>
       </c>
@@ -7648,7 +7648,7 @@
       </c>
       <c r="D128" s="85"/>
     </row>
-    <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A129" s="89" t="s">
         <v>416</v>
       </c>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="D129" s="85"/>
     </row>
-    <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="89" t="s">
         <v>418</v>
       </c>
@@ -7672,7 +7672,7 @@
       </c>
       <c r="D130" s="85"/>
     </row>
-    <row r="131" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="89" t="s">
         <v>189</v>
       </c>
@@ -7684,7 +7684,7 @@
       </c>
       <c r="D131" s="85"/>
     </row>
-    <row r="132" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="89" t="s">
         <v>190</v>
       </c>
@@ -7696,7 +7696,7 @@
       </c>
       <c r="D132" s="85"/>
     </row>
-    <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="89" t="s">
         <v>421</v>
       </c>
@@ -7708,7 +7708,7 @@
       </c>
       <c r="D133" s="85"/>
     </row>
-    <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="89" t="s">
         <v>423</v>
       </c>
@@ -7720,7 +7720,7 @@
       </c>
       <c r="D134" s="85"/>
     </row>
-    <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="89" t="s">
         <v>425</v>
       </c>
@@ -7732,7 +7732,7 @@
       </c>
       <c r="D135" s="85"/>
     </row>
-    <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="89" t="s">
         <v>426</v>
       </c>
@@ -7744,7 +7744,7 @@
       </c>
       <c r="D136" s="85"/>
     </row>
-    <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="89" t="s">
         <v>428</v>
       </c>
@@ -7756,7 +7756,7 @@
       </c>
       <c r="D137" s="85"/>
     </row>
-    <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="89" t="s">
         <v>430</v>
       </c>
@@ -7768,7 +7768,7 @@
       </c>
       <c r="D138" s="85"/>
     </row>
-    <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="89" t="s">
         <v>431</v>
       </c>
@@ -7780,7 +7780,7 @@
       </c>
       <c r="D139" s="85"/>
     </row>
-    <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="89" t="s">
         <v>432</v>
       </c>
@@ -7792,7 +7792,7 @@
       </c>
       <c r="D140" s="85"/>
     </row>
-    <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="89" t="s">
         <v>434</v>
       </c>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="D141" s="85"/>
     </row>
-    <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="89" t="s">
         <v>435</v>
       </c>
@@ -7816,7 +7816,7 @@
       </c>
       <c r="D142" s="85"/>
     </row>
-    <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="89" t="s">
         <v>454</v>
       </c>
@@ -7828,7 +7828,7 @@
       </c>
       <c r="D143" s="85"/>
     </row>
-    <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A144" s="94" t="s">
         <v>464</v>
       </c>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="D144" s="95"/>
     </row>
-    <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="89" t="s">
         <v>471</v>
       </c>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="D145" s="85"/>
     </row>
-    <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="89" t="s">
         <v>474</v>
       </c>
@@ -7864,7 +7864,7 @@
       </c>
       <c r="D146" s="85"/>
     </row>
-    <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="89" t="s">
         <v>476</v>
       </c>
@@ -7876,7 +7876,7 @@
       </c>
       <c r="D147" s="85"/>
     </row>
-    <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="90" t="s">
         <v>478</v>
       </c>
@@ -7888,7 +7888,7 @@
       </c>
       <c r="D148" s="91"/>
     </row>
-    <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="89" t="s">
         <v>480</v>
       </c>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="D149" s="85"/>
     </row>
-    <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="89" t="s">
         <v>483</v>
       </c>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="D150" s="85"/>
     </row>
-    <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="89" t="s">
         <v>485</v>
       </c>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="D151" s="85"/>
     </row>
-    <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="89" t="s">
         <v>488</v>
       </c>
@@ -7936,7 +7936,7 @@
       </c>
       <c r="D152" s="85"/>
     </row>
-    <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="89" t="s">
         <v>489</v>
       </c>
@@ -7948,7 +7948,7 @@
       </c>
       <c r="D153" s="85"/>
     </row>
-    <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A154" s="89" t="s">
         <v>491</v>
       </c>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="D154" s="85"/>
     </row>
-    <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A155" s="89" t="s">
         <v>492</v>
       </c>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="D155" s="85"/>
     </row>
-    <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A156" s="89" t="s">
         <v>493</v>
       </c>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="D156" s="85"/>
     </row>
-    <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A157" s="89" t="s">
         <v>494</v>
       </c>
@@ -7996,7 +7996,7 @@
       </c>
       <c r="D157" s="85"/>
     </row>
-    <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A158" s="89" t="s">
         <v>495</v>
       </c>
@@ -8008,7 +8008,7 @@
       </c>
       <c r="D158" s="85"/>
     </row>
-    <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A159" s="89" t="s">
         <v>496</v>
       </c>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="D159" s="85"/>
     </row>
-    <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A160" s="89" t="s">
         <v>497</v>
       </c>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="D160" s="85"/>
     </row>
-    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A161" s="89" t="s">
         <v>498</v>
       </c>
@@ -8044,7 +8044,7 @@
       </c>
       <c r="D161" s="85"/>
     </row>
-    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A162" s="89" t="s">
         <v>507</v>
       </c>
@@ -8056,7 +8056,7 @@
       </c>
       <c r="D162" s="85"/>
     </row>
-    <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A163" s="89" t="s">
         <v>509</v>
       </c>
@@ -8068,7 +8068,7 @@
       </c>
       <c r="D163" s="85"/>
     </row>
-    <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A164" s="89" t="s">
         <v>510</v>
       </c>
@@ -8080,7 +8080,7 @@
       </c>
       <c r="D164" s="85"/>
     </row>
-    <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A165" s="89" t="s">
         <v>511</v>
       </c>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="D165" s="85"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="83" t="s">
         <v>519</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A167" s="89" t="s">
         <v>520</v>
       </c>
@@ -8115,7 +8115,7 @@
       </c>
       <c r="D167" s="85"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="83" t="s">
         <v>522</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A169" s="89" t="s">
         <v>524</v>
       </c>
@@ -8138,7 +8138,7 @@
       </c>
       <c r="D169" s="85"/>
     </row>
-    <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A170" s="89" t="s">
         <v>526</v>
       </c>
@@ -8150,7 +8150,7 @@
       </c>
       <c r="D170" s="85"/>
     </row>
-    <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A171" s="89" t="s">
         <v>528</v>
       </c>
@@ -8162,7 +8162,7 @@
       </c>
       <c r="D171" s="85"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" s="83" t="s">
         <v>530</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A173" s="89" t="s">
         <v>532</v>
       </c>
@@ -8185,282 +8185,282 @@
       </c>
       <c r="D173" s="85"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="83" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B174" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C174" s="84" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="83" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B175" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C175" s="84" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" s="83" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B176" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C176" s="84" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="83" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B177" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C177" s="84" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="83" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B178" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C178" s="84" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="83" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B179" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C179" s="84" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="83" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B180" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C180" s="84" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="83" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B181" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C181" s="84" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="83" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B182" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C182" s="84" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="83" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B183" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C183" s="84" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="83" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B184" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C184" s="84" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="83" t="s">
+        <v>558</v>
+      </c>
+      <c r="B185" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C185" s="84" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="83" t="s">
         <v>562</v>
-      </c>
-      <c r="B185" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="C185" s="84" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="83" t="s">
-        <v>566</v>
       </c>
       <c r="B186" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C186" s="84" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="83" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B187" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C187" s="84" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="83" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B188" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C188" s="84" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="83" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B189" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C189" s="84" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="83" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B190" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C190" s="84" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="83" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B191" s="84" t="s">
         <v>342</v>
       </c>
       <c r="C191" s="84" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="83" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B192" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C192" s="84" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="83" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B193" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C193" s="84" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="83" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B194" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C194" s="84" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="83" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B195" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C195" s="84" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="83" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B196" s="84" t="s">
         <v>333</v>
       </c>
       <c r="C196" s="84" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="83" t="s">
+        <v>584</v>
+      </c>
+      <c r="B197" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C197" s="84" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" s="83" t="s">
+        <v>585</v>
+      </c>
+      <c r="B198" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C198" s="84" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="83" t="s">
-        <v>588</v>
-      </c>
-      <c r="B197" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="C197" s="84" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="83" t="s">
-        <v>589</v>
-      </c>
-      <c r="B198" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="C198" s="84" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="83" t="s">
         <v>148</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>258</v>
       </c>
       <c r="C199" s="84" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated links and images from Sept 1 pass off in content pages
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cromanow\MetroCERIRepo\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2B989-C8E1-4FB5-AF90-8D7FDE656563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A270B-9517-44EE-BA2D-46C772DE9EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10080" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="240" yWindow="1920" windowWidth="14235" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -2661,19 +2661,19 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.81640625" style="24"/>
-    <col min="8" max="8" width="15.453125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="8.81640625" style="24"/>
+    <col min="1" max="1" width="5.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="24"/>
+    <col min="8" max="8" width="15.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="22" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
     </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>76</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
     </row>
-    <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
         <v>98</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
     </row>
-    <row r="4" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
     </row>
-    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>48</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
     </row>
-    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>49</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="U6" s="24"/>
       <c r="V6" s="24"/>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>73</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="U7" s="24"/>
       <c r="V7" s="24"/>
     </row>
-    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>59</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
     </row>
-    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>61</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="U10" s="24"/>
       <c r="V10" s="24"/>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>62</v>
       </c>
@@ -3053,7 +3053,7 @@
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>63</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
     </row>
-    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>64</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
     </row>
-    <row r="14" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>65</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
     </row>
-    <row r="15" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
         <v>10</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
     </row>
-    <row r="16" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>11</v>
       </c>
@@ -3215,7 +3215,7 @@
       <c r="U16" s="24"/>
       <c r="V16" s="24"/>
     </row>
-    <row r="17" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>111</v>
       </c>
@@ -3249,7 +3249,7 @@
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
     </row>
-    <row r="18" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>12</v>
       </c>
@@ -3283,7 +3283,7 @@
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
     </row>
-    <row r="19" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>121</v>
       </c>
@@ -3317,7 +3317,7 @@
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
     </row>
-    <row r="20" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>13</v>
       </c>
@@ -3351,7 +3351,7 @@
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
     </row>
-    <row r="21" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>131</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
     </row>
-    <row r="22" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>132</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
     </row>
-    <row r="23" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34">
         <v>14</v>
       </c>
@@ -3453,7 +3453,7 @@
       <c r="U23" s="24"/>
       <c r="V23" s="24"/>
     </row>
-    <row r="24" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <v>20</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="U24" s="24"/>
       <c r="V24" s="24"/>
     </row>
-    <row r="25" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
         <v>201</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
     </row>
-    <row r="26" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37">
         <v>202</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
     </row>
-    <row r="27" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34">
         <v>21</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="U27" s="24"/>
       <c r="V27" s="24"/>
     </row>
-    <row r="28" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34">
         <v>22</v>
       </c>
@@ -3621,7 +3621,7 @@
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
     </row>
-    <row r="29" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <v>23</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
     </row>
-    <row r="30" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34">
         <v>24</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="U30" s="24"/>
       <c r="V30" s="24"/>
     </row>
-    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34">
         <v>25</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="U31" s="24"/>
       <c r="V31" s="24"/>
     </row>
-    <row r="32" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="36">
         <v>30</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
     </row>
-    <row r="33" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34">
         <v>301</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="U33" s="24"/>
       <c r="V33" s="24"/>
     </row>
-    <row r="34" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34">
         <v>31</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="U34" s="24"/>
       <c r="V34" s="24"/>
     </row>
-    <row r="35" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34">
         <v>32</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="U35" s="24"/>
       <c r="V35" s="24"/>
     </row>
-    <row r="36" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34">
         <v>33</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="U36" s="24"/>
       <c r="V36" s="24"/>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34">
         <v>34</v>
       </c>
@@ -3925,7 +3925,7 @@
       <c r="U37" s="24"/>
       <c r="V37" s="24"/>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34">
         <v>35</v>
       </c>
@@ -3959,7 +3959,7 @@
       <c r="U38" s="24"/>
       <c r="V38" s="24"/>
     </row>
-    <row r="39" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34">
         <v>36</v>
       </c>
@@ -3993,7 +3993,7 @@
       <c r="U39" s="24"/>
       <c r="V39" s="24"/>
     </row>
-    <row r="40" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34">
         <v>37</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="U40" s="24"/>
       <c r="V40" s="24"/>
     </row>
-    <row r="41" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>40</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="U41" s="24"/>
       <c r="V41" s="24"/>
     </row>
-    <row r="42" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37">
         <v>401</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="U42" s="24"/>
       <c r="V42" s="24"/>
     </row>
-    <row r="43" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34">
         <v>41</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="U43" s="24"/>
       <c r="V43" s="24"/>
     </row>
-    <row r="44" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="34">
         <v>42</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="U44" s="24"/>
       <c r="V44" s="24"/>
     </row>
-    <row r="45" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="37">
         <v>421</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="U45" s="24"/>
       <c r="V45" s="24"/>
     </row>
-    <row r="46" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34">
         <v>43</v>
       </c>
@@ -4229,7 +4229,7 @@
       <c r="U46" s="24"/>
       <c r="V46" s="24"/>
     </row>
-    <row r="47" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>431</v>
       </c>
@@ -4263,7 +4263,7 @@
       <c r="U47" s="24"/>
       <c r="V47" s="24"/>
     </row>
-    <row r="48" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="35">
         <v>432</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="U48" s="24"/>
       <c r="V48" s="24"/>
     </row>
-    <row r="49" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34">
         <v>44</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="U49" s="24"/>
       <c r="V49" s="24"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <v>50</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="34">
         <v>51</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="34">
         <v>52</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="34">
         <v>53</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="34">
         <v>54</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="34">
         <v>55</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="34">
         <v>56</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="34">
         <v>57</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="34">
         <v>58</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="34">
         <v>59</v>
       </c>
@@ -4516,26 +4516,26 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" customWidth="1"/>
-    <col min="12" max="12" width="86.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7265625" customWidth="1"/>
-    <col min="14" max="14" width="35.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>93</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="I1" s="77"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>93</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>94</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>95</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>96</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
         <v>97</v>
       </c>
@@ -4672,7 +4672,7 @@
       <c r="C6" s="80"/>
       <c r="D6" s="59"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
         <v>114</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="C7" s="80"/>
       <c r="D7" s="59"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>115</v>
       </c>
@@ -4692,7 +4692,7 @@
       <c r="C8" s="80"/>
       <c r="D8" s="59"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>97</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>101</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>102</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
         <v>103</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
         <v>104</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>105</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="63" t="s">
         <v>122</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="63" t="s">
         <v>123</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="63" t="s">
         <v>124</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="63" t="s">
         <v>125</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="63" t="s">
         <v>126</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="63" t="s">
         <v>127</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="63" t="s">
         <v>128</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="63" t="s">
         <v>129</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="63" t="s">
         <v>130</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="63" t="s">
         <v>131</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="s">
         <v>132</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="63" t="s">
         <v>133</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="63" t="s">
         <v>134</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="63" t="s">
         <v>135</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="63" t="s">
         <v>136</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="63" t="s">
         <v>137</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="63" t="s">
         <v>138</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="63" t="s">
         <v>139</v>
       </c>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="E34" s="67"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="63" t="s">
         <v>140</v>
       </c>
@@ -5164,7 +5164,7 @@
       </c>
       <c r="E35" s="67"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="63" t="s">
         <v>141</v>
       </c>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="E36" s="67"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="63" t="s">
         <v>142</v>
       </c>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="E37" s="67"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="63" t="s">
         <v>143</v>
       </c>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="E38" s="67"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="63" t="s">
         <v>144</v>
       </c>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="E39" s="67"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="63" t="s">
         <v>145</v>
       </c>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="E40" s="67"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="64" t="s">
         <v>146</v>
       </c>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="E41" s="67"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="76" t="s">
         <v>224</v>
       </c>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="E42" s="67"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="76" t="s">
         <v>228</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C44" s="76" t="s">
         <v>229</v>
       </c>
@@ -5257,22 +5257,22 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="24" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.54296875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="24" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.453125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="24" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>93</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
         <v>93</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">
         <v>94</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>95</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="71" t="s">
         <v>96</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="71" t="s">
         <v>97</v>
       </c>
@@ -5430,7 +5430,7 @@
       <c r="J6" s="73"/>
       <c r="K6" s="73"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="71" t="s">
         <v>114</v>
       </c>
@@ -5447,7 +5447,7 @@
       <c r="J7" s="73"/>
       <c r="K7" s="73"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="71" t="s">
         <v>115</v>
       </c>
@@ -5464,7 +5464,7 @@
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="73"/>
       <c r="B9" s="73"/>
       <c r="C9" s="74"/>
@@ -5477,7 +5477,7 @@
       <c r="J9" s="73"/>
       <c r="K9" s="73"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="73"/>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
@@ -5490,7 +5490,7 @@
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
         <v>97</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="71" t="s">
         <v>101</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="71" t="s">
         <v>102</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="71" t="s">
         <v>103</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="71" t="s">
         <v>104</v>
       </c>
@@ -5627,7 +5627,7 @@
       <c r="J15" s="73"/>
       <c r="K15" s="73"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="71" t="s">
         <v>105</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="73"/>
       <c r="B17" s="73"/>
       <c r="C17" s="74"/>
@@ -5673,7 +5673,7 @@
       <c r="J17" s="73"/>
       <c r="K17" s="73"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="73"/>
       <c r="B18" s="73"/>
       <c r="C18" s="74"/>
@@ -5694,7 +5694,7 @@
       <c r="J18" s="73"/>
       <c r="K18" s="73"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="73"/>
       <c r="B19" s="73"/>
       <c r="C19" s="74"/>
@@ -5711,7 +5711,7 @@
       <c r="J19" s="73"/>
       <c r="K19" s="73"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="73"/>
       <c r="B20" s="73"/>
       <c r="C20" s="74"/>
@@ -5728,7 +5728,7 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="73"/>
       <c r="B21" s="73"/>
       <c r="C21" s="74"/>
@@ -5745,7 +5745,7 @@
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="73"/>
       <c r="B22" s="73"/>
       <c r="C22" s="74"/>
@@ -5762,7 +5762,7 @@
       <c r="J22" s="73"/>
       <c r="K22" s="73"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="73"/>
       <c r="B23" s="73"/>
       <c r="C23" s="74"/>
@@ -5779,7 +5779,7 @@
       <c r="J23" s="73"/>
       <c r="K23" s="73"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="73"/>
       <c r="B24" s="73"/>
       <c r="C24" s="74"/>
@@ -5796,7 +5796,7 @@
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="73"/>
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
@@ -5813,7 +5813,7 @@
       <c r="J25" s="73"/>
       <c r="K25" s="73"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="73"/>
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
@@ -5830,7 +5830,7 @@
       <c r="J26" s="73"/>
       <c r="K26" s="73"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="73"/>
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
@@ -5847,7 +5847,7 @@
       <c r="J27" s="73"/>
       <c r="K27" s="73"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
@@ -5864,7 +5864,7 @@
       <c r="J28" s="73"/>
       <c r="K28" s="73"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="73"/>
       <c r="B29" s="73"/>
       <c r="C29" s="74"/>
@@ -5881,7 +5881,7 @@
       <c r="J29" s="73"/>
       <c r="K29" s="73"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="73"/>
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
@@ -5898,7 +5898,7 @@
       <c r="J30" s="73"/>
       <c r="K30" s="73"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="73"/>
       <c r="B31" s="73"/>
       <c r="C31" s="74"/>
@@ -5915,7 +5915,7 @@
       <c r="J31" s="73"/>
       <c r="K31" s="73"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="73"/>
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
@@ -5932,7 +5932,7 @@
       <c r="J32" s="73"/>
       <c r="K32" s="73"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="73"/>
       <c r="B33" s="73"/>
       <c r="C33" s="74"/>
@@ -5949,7 +5949,7 @@
       <c r="J33" s="73"/>
       <c r="K33" s="73"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="73"/>
       <c r="B34" s="73"/>
       <c r="C34" s="74"/>
@@ -5966,7 +5966,7 @@
       <c r="J34" s="73"/>
       <c r="K34" s="73"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="73"/>
       <c r="B35" s="73"/>
       <c r="C35" s="74"/>
@@ -5983,7 +5983,7 @@
       <c r="J35" s="73"/>
       <c r="K35" s="73"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="73"/>
       <c r="B36" s="73"/>
       <c r="C36" s="74"/>
@@ -6000,7 +6000,7 @@
       <c r="J36" s="73"/>
       <c r="K36" s="73"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="73"/>
       <c r="B37" s="73"/>
       <c r="C37" s="74"/>
@@ -6017,7 +6017,7 @@
       <c r="J37" s="73"/>
       <c r="K37" s="73"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="73"/>
       <c r="B38" s="73"/>
       <c r="C38" s="74"/>
@@ -6034,7 +6034,7 @@
       <c r="J38" s="73"/>
       <c r="K38" s="73"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="73"/>
       <c r="B39" s="73"/>
       <c r="C39" s="74"/>
@@ -6051,7 +6051,7 @@
       <c r="J39" s="73"/>
       <c r="K39" s="73"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="73"/>
       <c r="B40" s="73"/>
       <c r="C40" s="74"/>
@@ -6068,7 +6068,7 @@
       <c r="J40" s="73"/>
       <c r="K40" s="73"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
       <c r="B41" s="59"/>
       <c r="C41" s="32"/>
@@ -6081,7 +6081,7 @@
       <c r="J41" s="59"/>
       <c r="K41" s="59"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G42" s="67"/>
     </row>
   </sheetData>
@@ -6093,20 +6093,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="84" customWidth="1"/>
-    <col min="3" max="3" width="80.81640625" style="84" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.7265625" style="84" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="84" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" style="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:4" s="86" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89" t="s">
         <v>59</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="D3" s="93"/>
     </row>
-    <row r="4" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
         <v>60</v>
       </c>
@@ -6144,7 +6144,7 @@
       </c>
       <c r="D4" s="85"/>
     </row>
-    <row r="5" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>61</v>
       </c>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="D5" s="85"/>
     </row>
-    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89" t="s">
         <v>62</v>
       </c>
@@ -6168,7 +6168,7 @@
       </c>
       <c r="D6" s="85"/>
     </row>
-    <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>63</v>
       </c>
@@ -6180,7 +6180,7 @@
       </c>
       <c r="D7" s="85"/>
     </row>
-    <row r="8" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89" t="s">
         <v>64</v>
       </c>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="D8" s="85"/>
     </row>
-    <row r="9" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
         <v>65</v>
       </c>
@@ -6204,7 +6204,7 @@
       </c>
       <c r="D9" s="85"/>
     </row>
-    <row r="10" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89" t="s">
         <v>260</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="D10" s="85"/>
     </row>
-    <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
         <v>262</v>
       </c>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="D11" s="85"/>
     </row>
-    <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89" t="s">
         <v>152</v>
       </c>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="D12" s="85"/>
     </row>
-    <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89" t="s">
         <v>515</v>
       </c>
@@ -6252,7 +6252,7 @@
       </c>
       <c r="D13" s="85"/>
     </row>
-    <row r="14" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
         <v>157</v>
       </c>
@@ -6264,7 +6264,7 @@
       </c>
       <c r="D14" s="85"/>
     </row>
-    <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89" t="s">
         <v>158</v>
       </c>
@@ -6276,7 +6276,7 @@
       </c>
       <c r="D15" s="85"/>
     </row>
-    <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89" t="s">
         <v>159</v>
       </c>
@@ -6288,7 +6288,7 @@
       </c>
       <c r="D16" s="85"/>
     </row>
-    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="89" t="s">
         <v>160</v>
       </c>
@@ -6300,7 +6300,7 @@
       </c>
       <c r="D17" s="85"/>
     </row>
-    <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="89" t="s">
         <v>264</v>
       </c>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="D18" s="85"/>
     </row>
-    <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
         <v>265</v>
       </c>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="D19" s="85"/>
     </row>
-    <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="89" t="s">
         <v>266</v>
       </c>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="D20" s="85"/>
     </row>
-    <row r="21" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="89" t="s">
         <v>267</v>
       </c>
@@ -6348,7 +6348,7 @@
       </c>
       <c r="D21" s="85"/>
     </row>
-    <row r="22" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="89" t="s">
         <v>268</v>
       </c>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="D22" s="85"/>
     </row>
-    <row r="23" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="89" t="s">
         <v>153</v>
       </c>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="D23" s="85"/>
     </row>
-    <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="89" t="s">
         <v>161</v>
       </c>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="D24" s="85"/>
     </row>
-    <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="89" t="s">
         <v>162</v>
       </c>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="D25" s="85"/>
     </row>
-    <row r="26" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="89" t="s">
         <v>163</v>
       </c>
@@ -6408,7 +6408,7 @@
       </c>
       <c r="D26" s="85"/>
     </row>
-    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="89" t="s">
         <v>164</v>
       </c>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="D27" s="85"/>
     </row>
-    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="89" t="s">
         <v>165</v>
       </c>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="D28" s="85"/>
     </row>
-    <row r="29" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="89" t="s">
         <v>271</v>
       </c>
@@ -6444,7 +6444,7 @@
       </c>
       <c r="D29" s="85"/>
     </row>
-    <row r="30" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="89" t="s">
         <v>272</v>
       </c>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="D30" s="85"/>
     </row>
-    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="89" t="s">
         <v>274</v>
       </c>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="D31" s="85"/>
     </row>
-    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="89" t="s">
         <v>276</v>
       </c>
@@ -6480,7 +6480,7 @@
       </c>
       <c r="D32" s="85"/>
     </row>
-    <row r="33" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="89" t="s">
         <v>154</v>
       </c>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="D33" s="85"/>
     </row>
-    <row r="34" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="89" t="s">
         <v>166</v>
       </c>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="D34" s="85"/>
     </row>
-    <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="89" t="s">
         <v>167</v>
       </c>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="D35" s="85"/>
     </row>
-    <row r="36" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="89" t="s">
         <v>168</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="D36" s="85"/>
     </row>
-    <row r="37" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="89" t="s">
         <v>169</v>
       </c>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="D37" s="85"/>
     </row>
-    <row r="38" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="89" t="s">
         <v>170</v>
       </c>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="D38" s="85"/>
     </row>
-    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="89" t="s">
         <v>171</v>
       </c>
@@ -6564,7 +6564,7 @@
       </c>
       <c r="D39" s="85"/>
     </row>
-    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="89" t="s">
         <v>172</v>
       </c>
@@ -6576,7 +6576,7 @@
       </c>
       <c r="D40" s="85"/>
     </row>
-    <row r="41" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="89" t="s">
         <v>278</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="D41" s="85"/>
     </row>
-    <row r="42" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94" t="s">
         <v>279</v>
       </c>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="D42" s="95"/>
     </row>
-    <row r="43" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94" t="s">
         <v>155</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
       <c r="D43" s="95"/>
     </row>
-    <row r="44" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94" t="s">
         <v>174</v>
       </c>
@@ -6624,7 +6624,7 @@
       </c>
       <c r="D44" s="95"/>
     </row>
-    <row r="45" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94" t="s">
         <v>175</v>
       </c>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="D45" s="95"/>
     </row>
-    <row r="46" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94" t="s">
         <v>176</v>
       </c>
@@ -6648,7 +6648,7 @@
       </c>
       <c r="D46" s="95"/>
     </row>
-    <row r="47" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94" t="s">
         <v>177</v>
       </c>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="D47" s="95"/>
     </row>
-    <row r="48" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94" t="s">
         <v>285</v>
       </c>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="D48" s="95"/>
     </row>
-    <row r="49" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94" t="s">
         <v>287</v>
       </c>
@@ -6684,7 +6684,7 @@
       </c>
       <c r="D49" s="95"/>
     </row>
-    <row r="50" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94" t="s">
         <v>289</v>
       </c>
@@ -6696,7 +6696,7 @@
       </c>
       <c r="D50" s="95"/>
     </row>
-    <row r="51" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94" t="s">
         <v>290</v>
       </c>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="D51" s="95"/>
     </row>
-    <row r="52" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94" t="s">
         <v>291</v>
       </c>
@@ -6720,7 +6720,7 @@
       </c>
       <c r="D52" s="95"/>
     </row>
-    <row r="53" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94" t="s">
         <v>156</v>
       </c>
@@ -6732,7 +6732,7 @@
       </c>
       <c r="D53" s="95"/>
     </row>
-    <row r="54" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="94" t="s">
         <v>178</v>
       </c>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="D54" s="95"/>
     </row>
-    <row r="55" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="94" t="s">
         <v>179</v>
       </c>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="D55" s="95"/>
     </row>
-    <row r="56" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="94" t="s">
         <v>180</v>
       </c>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="D56" s="95"/>
     </row>
-    <row r="57" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94" t="s">
         <v>181</v>
       </c>
@@ -6780,7 +6780,7 @@
       </c>
       <c r="D57" s="95"/>
     </row>
-    <row r="58" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94" t="s">
         <v>182</v>
       </c>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="D58" s="95"/>
     </row>
-    <row r="59" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94" t="s">
         <v>183</v>
       </c>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="D59" s="95"/>
     </row>
-    <row r="60" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94" t="s">
         <v>184</v>
       </c>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="D60" s="95"/>
     </row>
-    <row r="61" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94" t="s">
         <v>185</v>
       </c>
@@ -6828,7 +6828,7 @@
       </c>
       <c r="D61" s="95"/>
     </row>
-    <row r="62" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="89" t="s">
         <v>186</v>
       </c>
@@ -6840,7 +6840,7 @@
       </c>
       <c r="D62" s="85"/>
     </row>
-    <row r="63" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="89" t="s">
         <v>297</v>
       </c>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="D63" s="85"/>
     </row>
-    <row r="64" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="89" t="s">
         <v>299</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="D64" s="85"/>
     </row>
-    <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="89" t="s">
         <v>300</v>
       </c>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="D65" s="85"/>
     </row>
-    <row r="66" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="89" t="s">
         <v>303</v>
       </c>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="D66" s="85"/>
     </row>
-    <row r="67" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="89" t="s">
         <v>305</v>
       </c>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="D67" s="85"/>
     </row>
-    <row r="68" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="89" t="s">
         <v>307</v>
       </c>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="D68" s="85"/>
     </row>
-    <row r="69" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="89" t="s">
         <v>309</v>
       </c>
@@ -6924,7 +6924,7 @@
       </c>
       <c r="D69" s="85"/>
     </row>
-    <row r="70" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="89" t="s">
         <v>311</v>
       </c>
@@ -6936,7 +6936,7 @@
       </c>
       <c r="D70" s="85"/>
     </row>
-    <row r="71" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="89" t="s">
         <v>313</v>
       </c>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="D71" s="85"/>
     </row>
-    <row r="72" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="89" t="s">
         <v>315</v>
       </c>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="D72" s="85"/>
     </row>
-    <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="89" t="s">
         <v>316</v>
       </c>
@@ -6972,7 +6972,7 @@
       </c>
       <c r="D73" s="85"/>
     </row>
-    <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="94" t="s">
         <v>318</v>
       </c>
@@ -6984,7 +6984,7 @@
       </c>
       <c r="D74" s="95"/>
     </row>
-    <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="89" t="s">
         <v>320</v>
       </c>
@@ -6996,7 +6996,7 @@
       </c>
       <c r="D75" s="85"/>
     </row>
-    <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="89" t="s">
         <v>321</v>
       </c>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="D76" s="85"/>
     </row>
-    <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="89" t="s">
         <v>322</v>
       </c>
@@ -7020,7 +7020,7 @@
       </c>
       <c r="D77" s="85"/>
     </row>
-    <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="89" t="s">
         <v>324</v>
       </c>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="D78" s="85"/>
     </row>
-    <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="89" t="s">
         <v>326</v>
       </c>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="D79" s="85"/>
     </row>
-    <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="89" t="s">
         <v>328</v>
       </c>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="D80" s="85"/>
     </row>
-    <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="89" t="s">
         <v>330</v>
       </c>
@@ -7068,7 +7068,7 @@
       </c>
       <c r="D81" s="85"/>
     </row>
-    <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="89" t="s">
         <v>332</v>
       </c>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="D82" s="85"/>
     </row>
-    <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="89" t="s">
         <v>335</v>
       </c>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="D83" s="85"/>
     </row>
-    <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="89" t="s">
         <v>337</v>
       </c>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="D84" s="85"/>
     </row>
-    <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="89" t="s">
         <v>339</v>
       </c>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="D85" s="85"/>
     </row>
-    <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="89" t="s">
         <v>340</v>
       </c>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="D86" s="85"/>
     </row>
-    <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="89" t="s">
         <v>341</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="89" t="s">
         <v>344</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="94" t="s">
         <v>347</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="94" t="s">
         <v>348</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="94" t="s">
         <v>349</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="94" t="s">
         <v>350</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="94" t="s">
         <v>351</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="94" t="s">
         <v>354</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="89" t="s">
         <v>357</v>
       </c>
@@ -7252,7 +7252,7 @@
       </c>
       <c r="D95" s="85"/>
     </row>
-    <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="89" t="s">
         <v>359</v>
       </c>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="D96" s="85"/>
     </row>
-    <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="89" t="s">
         <v>360</v>
       </c>
@@ -7276,7 +7276,7 @@
       </c>
       <c r="D97" s="85"/>
     </row>
-    <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="89" t="s">
         <v>362</v>
       </c>
@@ -7288,7 +7288,7 @@
       </c>
       <c r="D98" s="85"/>
     </row>
-    <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="89" t="s">
         <v>364</v>
       </c>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="D99" s="85"/>
     </row>
-    <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="89" t="s">
         <v>366</v>
       </c>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="D100" s="85"/>
     </row>
-    <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="89" t="s">
         <v>368</v>
       </c>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="D101" s="85"/>
     </row>
-    <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="89" t="s">
         <v>372</v>
       </c>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="D102" s="85"/>
     </row>
-    <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="89" t="s">
         <v>374</v>
       </c>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="D103" s="85"/>
     </row>
-    <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="89" t="s">
         <v>376</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="D104" s="85"/>
     </row>
-    <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="89" t="s">
         <v>378</v>
       </c>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="D105" s="85"/>
     </row>
-    <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="89" t="s">
         <v>379</v>
       </c>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="D106" s="85"/>
     </row>
-    <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="89" t="s">
         <v>380</v>
       </c>
@@ -7396,7 +7396,7 @@
       </c>
       <c r="D107" s="85"/>
     </row>
-    <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="89" t="s">
         <v>381</v>
       </c>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="D108" s="85"/>
     </row>
-    <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="89" t="s">
         <v>383</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="D109" s="85"/>
     </row>
-    <row r="110" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="89" t="s">
         <v>187</v>
       </c>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="D110" s="85"/>
     </row>
-    <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="89" t="s">
         <v>386</v>
       </c>
@@ -7444,7 +7444,7 @@
       </c>
       <c r="D111" s="85"/>
     </row>
-    <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="89" t="s">
         <v>370</v>
       </c>
@@ -7456,7 +7456,7 @@
       </c>
       <c r="D112" s="85"/>
     </row>
-    <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="89" t="s">
         <v>371</v>
       </c>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="D113" s="85"/>
     </row>
-    <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="89" t="s">
         <v>389</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="D114" s="85"/>
     </row>
-    <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="89" t="s">
         <v>390</v>
       </c>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="D115" s="85"/>
     </row>
-    <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="89" t="s">
         <v>392</v>
       </c>
@@ -7504,7 +7504,7 @@
       </c>
       <c r="D116" s="85"/>
     </row>
-    <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="89" t="s">
         <v>394</v>
       </c>
@@ -7516,7 +7516,7 @@
       </c>
       <c r="D117" s="85"/>
     </row>
-    <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="94" t="s">
         <v>396</v>
       </c>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="D118" s="95"/>
     </row>
-    <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="89" t="s">
         <v>398</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="D119" s="85"/>
     </row>
-    <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="89" t="s">
         <v>400</v>
       </c>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="D120" s="85"/>
     </row>
-    <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="89" t="s">
         <v>402</v>
       </c>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="D121" s="85"/>
     </row>
-    <row r="122" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="89" t="s">
         <v>188</v>
       </c>
@@ -7576,7 +7576,7 @@
       </c>
       <c r="D122" s="85"/>
     </row>
-    <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="89" t="s">
         <v>405</v>
       </c>
@@ -7588,7 +7588,7 @@
       </c>
       <c r="D123" s="85"/>
     </row>
-    <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="89" t="s">
         <v>406</v>
       </c>
@@ -7600,7 +7600,7 @@
       </c>
       <c r="D124" s="85"/>
     </row>
-    <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="89" t="s">
         <v>409</v>
       </c>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="D125" s="85"/>
     </row>
-    <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="89" t="s">
         <v>411</v>
       </c>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="D126" s="85"/>
     </row>
-    <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="89" t="s">
         <v>413</v>
       </c>
@@ -7636,7 +7636,7 @@
       </c>
       <c r="D127" s="85"/>
     </row>
-    <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="89" t="s">
         <v>414</v>
       </c>
@@ -7648,7 +7648,7 @@
       </c>
       <c r="D128" s="85"/>
     </row>
-    <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="89" t="s">
         <v>416</v>
       </c>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="D129" s="85"/>
     </row>
-    <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="89" t="s">
         <v>418</v>
       </c>
@@ -7672,7 +7672,7 @@
       </c>
       <c r="D130" s="85"/>
     </row>
-    <row r="131" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="89" t="s">
         <v>189</v>
       </c>
@@ -7684,7 +7684,7 @@
       </c>
       <c r="D131" s="85"/>
     </row>
-    <row r="132" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="89" t="s">
         <v>190</v>
       </c>
@@ -7696,7 +7696,7 @@
       </c>
       <c r="D132" s="85"/>
     </row>
-    <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="89" t="s">
         <v>421</v>
       </c>
@@ -7708,7 +7708,7 @@
       </c>
       <c r="D133" s="85"/>
     </row>
-    <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="89" t="s">
         <v>423</v>
       </c>
@@ -7720,7 +7720,7 @@
       </c>
       <c r="D134" s="85"/>
     </row>
-    <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="89" t="s">
         <v>425</v>
       </c>
@@ -7732,7 +7732,7 @@
       </c>
       <c r="D135" s="85"/>
     </row>
-    <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="89" t="s">
         <v>426</v>
       </c>
@@ -7744,7 +7744,7 @@
       </c>
       <c r="D136" s="85"/>
     </row>
-    <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="89" t="s">
         <v>428</v>
       </c>
@@ -7756,7 +7756,7 @@
       </c>
       <c r="D137" s="85"/>
     </row>
-    <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="89" t="s">
         <v>430</v>
       </c>
@@ -7768,7 +7768,7 @@
       </c>
       <c r="D138" s="85"/>
     </row>
-    <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="89" t="s">
         <v>431</v>
       </c>
@@ -7780,7 +7780,7 @@
       </c>
       <c r="D139" s="85"/>
     </row>
-    <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="89" t="s">
         <v>432</v>
       </c>
@@ -7792,7 +7792,7 @@
       </c>
       <c r="D140" s="85"/>
     </row>
-    <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="89" t="s">
         <v>434</v>
       </c>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="D141" s="85"/>
     </row>
-    <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="89" t="s">
         <v>435</v>
       </c>
@@ -7816,7 +7816,7 @@
       </c>
       <c r="D142" s="85"/>
     </row>
-    <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="89" t="s">
         <v>454</v>
       </c>
@@ -7828,7 +7828,7 @@
       </c>
       <c r="D143" s="85"/>
     </row>
-    <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="94" t="s">
         <v>464</v>
       </c>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="D144" s="95"/>
     </row>
-    <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="89" t="s">
         <v>471</v>
       </c>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="D145" s="85"/>
     </row>
-    <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="89" t="s">
         <v>474</v>
       </c>
@@ -7864,7 +7864,7 @@
       </c>
       <c r="D146" s="85"/>
     </row>
-    <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="89" t="s">
         <v>476</v>
       </c>
@@ -7876,7 +7876,7 @@
       </c>
       <c r="D147" s="85"/>
     </row>
-    <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="90" t="s">
         <v>478</v>
       </c>
@@ -7888,7 +7888,7 @@
       </c>
       <c r="D148" s="91"/>
     </row>
-    <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="89" t="s">
         <v>480</v>
       </c>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="D149" s="85"/>
     </row>
-    <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="89" t="s">
         <v>483</v>
       </c>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="D150" s="85"/>
     </row>
-    <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="89" t="s">
         <v>485</v>
       </c>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="D151" s="85"/>
     </row>
-    <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="89" t="s">
         <v>488</v>
       </c>
@@ -7936,7 +7936,7 @@
       </c>
       <c r="D152" s="85"/>
     </row>
-    <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="89" t="s">
         <v>489</v>
       </c>
@@ -7948,7 +7948,7 @@
       </c>
       <c r="D153" s="85"/>
     </row>
-    <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="89" t="s">
         <v>491</v>
       </c>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="D154" s="85"/>
     </row>
-    <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="89" t="s">
         <v>492</v>
       </c>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="D155" s="85"/>
     </row>
-    <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="89" t="s">
         <v>493</v>
       </c>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="D156" s="85"/>
     </row>
-    <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="89" t="s">
         <v>494</v>
       </c>
@@ -7996,7 +7996,7 @@
       </c>
       <c r="D157" s="85"/>
     </row>
-    <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="89" t="s">
         <v>495</v>
       </c>
@@ -8008,7 +8008,7 @@
       </c>
       <c r="D158" s="85"/>
     </row>
-    <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="89" t="s">
         <v>496</v>
       </c>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="D159" s="85"/>
     </row>
-    <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="89" t="s">
         <v>497</v>
       </c>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="D160" s="85"/>
     </row>
-    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="89" t="s">
         <v>498</v>
       </c>
@@ -8044,7 +8044,7 @@
       </c>
       <c r="D161" s="85"/>
     </row>
-    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="89" t="s">
         <v>507</v>
       </c>
@@ -8056,7 +8056,7 @@
       </c>
       <c r="D162" s="85"/>
     </row>
-    <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="89" t="s">
         <v>509</v>
       </c>
@@ -8068,7 +8068,7 @@
       </c>
       <c r="D163" s="85"/>
     </row>
-    <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="89" t="s">
         <v>510</v>
       </c>
@@ -8080,7 +8080,7 @@
       </c>
       <c r="D164" s="85"/>
     </row>
-    <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="89" t="s">
         <v>511</v>
       </c>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="D165" s="85"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="83" t="s">
         <v>519</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="89" t="s">
         <v>520</v>
       </c>
@@ -8115,7 +8115,7 @@
       </c>
       <c r="D167" s="85"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="83" t="s">
         <v>522</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="89" t="s">
         <v>524</v>
       </c>
@@ -8138,7 +8138,7 @@
       </c>
       <c r="D169" s="85"/>
     </row>
-    <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="89" t="s">
         <v>526</v>
       </c>
@@ -8150,7 +8150,7 @@
       </c>
       <c r="D170" s="85"/>
     </row>
-    <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="89" t="s">
         <v>528</v>
       </c>
@@ -8162,7 +8162,7 @@
       </c>
       <c r="D171" s="85"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="83" t="s">
         <v>530</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="89" t="s">
         <v>532</v>
       </c>
@@ -8185,7 +8185,7 @@
       </c>
       <c r="D173" s="85"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="83" t="s">
         <v>536</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="83" t="s">
         <v>538</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="83" t="s">
         <v>539</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="83" t="s">
         <v>541</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="83" t="s">
         <v>544</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="83" t="s">
         <v>546</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="83" t="s">
         <v>547</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="83" t="s">
         <v>549</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="83" t="s">
         <v>551</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="83" t="s">
         <v>554</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="83" t="s">
         <v>556</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="83" t="s">
         <v>558</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="83" t="s">
         <v>562</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="83" t="s">
         <v>564</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="83" t="s">
         <v>566</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="83" t="s">
         <v>568</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="83" t="s">
         <v>570</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="83" t="s">
         <v>572</v>
       </c>
@@ -8383,7 +8383,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="83" t="s">
         <v>574</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="83" t="s">
         <v>575</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="83" t="s">
         <v>576</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="83" t="s">
         <v>577</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="83" t="s">
         <v>578</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="83" t="s">
         <v>584</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="83" t="s">
         <v>585</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="83" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Fixed 5 sections of ERB image
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E60BB8-ABCE-48E9-99ED-D7B314198FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB97E1F-54C3-4C8B-A672-241B72B6E0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1350" windowWidth="14160" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="2640" yWindow="1560" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignments" sheetId="1" r:id="rId1"/>
@@ -6096,8 +6096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Allow image resize on window resize
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CEBBF8-B19A-417B-9BCE-10ACAD818359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D93E02F-AF9E-426B-BD83-134568A23242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="5790" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28875" yWindow="0" windowWidth="17640" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="170">
   <si>
     <t>ID</t>
   </si>
@@ -336,15 +336,9 @@
     <t>Image: Youth Engagement. Figure 1. Large.</t>
   </si>
   <si>
-    <t>Image: Youth Engagement. Figure 1. Small.</t>
-  </si>
-  <si>
     <t>Image: Youth Engagement. Figure 2. Large.</t>
   </si>
   <si>
-    <t>Image: Youth Engagement. Figure 2. Small.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Image: Youth Engagement. Additional Resources 1. </t>
   </si>
   <si>
@@ -462,18 +456,6 @@
     <t>Image: Chapter Landing: Strategize. Small.</t>
   </si>
   <si>
-    <t>Image: Chapter Landing: Plan. Large.</t>
-  </si>
-  <si>
-    <t>Image: Chapter Landing: Engage. Large.</t>
-  </si>
-  <si>
-    <t>Image: Chapter Landing: Assess. Large.</t>
-  </si>
-  <si>
-    <t>Image: Chapter Landing: Strategize. Large.</t>
-  </si>
-  <si>
     <t>Project Storytelling</t>
   </si>
   <si>
@@ -502,9 +484,6 @@
   </si>
   <si>
     <t>Image: Chapter Landing: Move Forward. Small.</t>
-  </si>
-  <si>
-    <t>Image: Chapter Landing: Move Forward. Large.</t>
   </si>
   <si>
     <t>Finding Funding</t>
@@ -1084,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D162"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1120,10 +1099,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1134,10 +1113,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1148,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1162,10 +1141,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1176,10 +1155,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1193,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1526,10 +1505,10 @@
         <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1540,10 +1519,10 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1554,10 +1533,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1568,175 +1547,175 @@
         <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>155</v>
+        <v>93</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>87</v>
@@ -1744,13 +1723,13 @@
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>87</v>
@@ -1758,77 +1737,77 @@
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
-        <v>185</v>
+        <v>120</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>31</v>
@@ -1837,172 +1816,172 @@
         <v>161</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22">
-        <v>164</v>
+        <v>80</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>173</v>
+        <v>97</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22">
-        <v>202</v>
+        <v>113</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>87</v>
@@ -2010,13 +1989,13 @@
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>87</v>
@@ -2024,41 +2003,41 @@
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>87</v>
@@ -2066,13 +2045,13 @@
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>87</v>
@@ -2080,27 +2059,27 @@
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
-        <v>179</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>106</v>
+      <c r="A72" s="23">
+        <v>149</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>87</v>
@@ -2108,391 +2087,391 @@
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22">
-        <v>180</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>31</v>
+        <v>193</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="22">
-        <v>178</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>31</v>
+        <v>85</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22">
-        <v>177</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>31</v>
+        <v>9</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22">
-        <v>148</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>31</v>
+        <v>128</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22">
-        <v>160</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="23">
-        <v>149</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>101</v>
+      <c r="A78" s="22">
+        <v>108</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22">
-        <v>161</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>102</v>
+        <v>112</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="22">
-        <v>193</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>32</v>
+        <v>131</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="22">
-        <v>85</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>32</v>
+        <v>96</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="22">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="22">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="B83" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="22">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="22">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="22">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="B89" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="22">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="B90" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="22">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="22">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B92" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="22">
-        <v>18</v>
+        <v>167</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22">
-        <v>199</v>
+        <v>111</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="22">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="22">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="22">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>87</v>
@@ -2500,237 +2479,237 @@
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="22">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="22">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="22">
-        <v>187</v>
+        <v>26</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22">
-        <v>132</v>
+        <v>201</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="22">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="22">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="22">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="22">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>87</v>
@@ -2738,97 +2717,97 @@
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="22">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="22">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B122" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="22">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>87</v>
@@ -2836,335 +2815,335 @@
     </row>
     <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="22">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="22">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B128" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="22">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="22">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="22">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="22">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
-        <v>171</v>
+        <v>94</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="22">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="22">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="22">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="22">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="B143" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="22">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="22">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="B145" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="22">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="22">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B148" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>87</v>
@@ -3172,205 +3151,107 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="22">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="22">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="22">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B151" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="22">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="B152" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="22">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B153" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="22">
-        <v>173</v>
-      </c>
-      <c r="B154" s="15" t="s">
-        <v>13</v>
+        <v>136</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="22">
-        <v>3</v>
-      </c>
-      <c r="B155" s="15" t="s">
-        <v>13</v>
+        <v>144</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="22">
-        <v>130</v>
-      </c>
-      <c r="B156" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="22">
-        <v>129</v>
-      </c>
-      <c r="B157" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="22">
-        <v>151</v>
-      </c>
-      <c r="B158" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="22">
-        <v>134</v>
-      </c>
-      <c r="B159" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="22">
-        <v>10</v>
-      </c>
-      <c r="B160" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="22">
-        <v>136</v>
-      </c>
-      <c r="B161" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="22">
-        <v>144</v>
-      </c>
-      <c r="B162" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D162">
-    <sortCondition ref="B2:B162"/>
-    <sortCondition ref="C2:C162"/>
-    <sortCondition ref="A2:A162"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D155">
+    <sortCondition ref="B2:B155"/>
+    <sortCondition ref="C2:C155"/>
+    <sortCondition ref="A2:A155"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed alternative form spacing and wrap text
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D93E02F-AF9E-426B-BD83-134568A23242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92812FC1-57DD-4BB7-9F0A-BB050E329DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="0" windowWidth="17640" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28875" yWindow="0" windowWidth="14085" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Icons cannot be clicked or expanded
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92812FC1-57DD-4BB7-9F0A-BB050E329DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234035E4-2630-4AA6-BC75-E937DF07758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="0" windowWidth="14085" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -1066,7 +1066,7 @@
   <dimension ref="A1:D155"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A14" sqref="A14:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated images throughout tool
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234035E4-2630-4AA6-BC75-E937DF07758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E510124-F455-4BC4-9549-BC7868290040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28875" yWindow="0" windowWidth="15645" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -544,6 +544,12 @@
   </si>
   <si>
     <t>Image: Example: Goals.</t>
+  </si>
+  <si>
+    <t>Image: Equitable Resilience Systems. Small.</t>
+  </si>
+  <si>
+    <t>Image: Centering Equity Icons. Large</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,27 +1715,27 @@
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>87</v>
@@ -1737,27 +1743,27 @@
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>108</v>
@@ -1765,13 +1771,13 @@
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>108</v>
@@ -1779,13 +1785,13 @@
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
+        <v>83</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>108</v>
@@ -1793,13 +1799,13 @@
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>108</v>
@@ -1807,13 +1813,13 @@
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>108</v>
@@ -1821,13 +1827,13 @@
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>108</v>
@@ -1835,13 +1841,13 @@
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>108</v>
@@ -1849,13 +1855,13 @@
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>108</v>
@@ -1863,13 +1869,13 @@
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>108</v>
@@ -1877,13 +1883,13 @@
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>108</v>
@@ -1891,41 +1897,41 @@
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22">
-        <v>202</v>
+        <v>80</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>87</v>
@@ -1933,55 +1939,55 @@
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>87</v>
@@ -1989,13 +1995,13 @@
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>87</v>
@@ -2003,13 +2009,13 @@
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>87</v>
@@ -2017,13 +2023,13 @@
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>87</v>
@@ -2031,13 +2037,13 @@
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>87</v>
@@ -2045,13 +2051,13 @@
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>87</v>
@@ -2059,27 +2065,27 @@
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22">
+        <v>177</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="22">
         <v>148</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="3" t="s">
+      <c r="B72" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
-        <v>149</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>87</v>
@@ -2087,83 +2093,83 @@
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22">
-        <v>193</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>32</v>
+        <v>204</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22">
-        <v>85</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>33</v>
+      <c r="A74" s="23">
+        <v>149</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22">
-        <v>9</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>13</v>
+        <v>193</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22">
-        <v>128</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B77" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>108</v>
@@ -2171,13 +2177,13 @@
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>108</v>
@@ -2185,13 +2191,13 @@
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="22">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B80" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>108</v>
@@ -2199,13 +2205,13 @@
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="22">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B81" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>108</v>
@@ -2213,13 +2219,13 @@
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="22">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>108</v>
@@ -2227,13 +2233,13 @@
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="22">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="B83" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>108</v>
@@ -2241,13 +2247,13 @@
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="22">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>108</v>
@@ -2255,13 +2261,13 @@
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>108</v>
@@ -2269,13 +2275,13 @@
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>108</v>
@@ -2283,13 +2289,13 @@
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22">
-        <v>199</v>
+        <v>15</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>108</v>
@@ -2297,27 +2303,27 @@
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="22">
+        <v>199</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>108</v>
@@ -2325,27 +2331,27 @@
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="22">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="B90" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="22">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>108</v>
@@ -2353,13 +2359,13 @@
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="22">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="B92" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>108</v>
@@ -2367,27 +2373,27 @@
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="22">
-        <v>167</v>
+        <v>36</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>108</v>
@@ -2395,27 +2401,27 @@
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="22">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>108</v>
@@ -2423,41 +2429,41 @@
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="22">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="22">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>108</v>
@@ -2465,13 +2471,13 @@
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22">
-        <v>187</v>
+        <v>4</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>87</v>
@@ -2479,13 +2485,13 @@
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>108</v>
@@ -2493,27 +2499,27 @@
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="22">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>108</v>
@@ -2521,13 +2527,13 @@
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="22">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>108</v>
@@ -2535,13 +2541,13 @@
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>108</v>
@@ -2549,13 +2555,13 @@
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>108</v>
@@ -2563,27 +2569,27 @@
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="22">
-        <v>26</v>
+        <v>200</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22">
-        <v>201</v>
+        <v>95</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>108</v>
@@ -2591,41 +2597,41 @@
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>108</v>
@@ -2633,125 +2639,125 @@
     </row>
     <row r="112" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="22">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="22">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="22">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="22">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="22">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>108</v>
@@ -2759,13 +2765,13 @@
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="22">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>108</v>
@@ -2773,27 +2779,27 @@
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="B122" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="22">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>108</v>
@@ -2801,27 +2807,27 @@
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="22">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>108</v>
@@ -2829,27 +2835,27 @@
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>108</v>
@@ -2857,13 +2863,13 @@
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="B128" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>108</v>
@@ -2871,27 +2877,27 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="22">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>108</v>
@@ -2899,83 +2905,83 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="22">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="22">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>108</v>
@@ -2983,13 +2989,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="22">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>108</v>
@@ -2997,13 +3003,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>108</v>
@@ -3011,13 +3017,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="22">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>108</v>
@@ -3025,13 +3031,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="22">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>108</v>
@@ -3039,27 +3045,27 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="22">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>108</v>
@@ -3067,27 +3073,27 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="22">
-        <v>152</v>
+        <v>2</v>
       </c>
       <c r="B143" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="22">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>108</v>
@@ -3095,27 +3101,27 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="22">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="B145" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="22">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>108</v>
@@ -3123,69 +3129,69 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="22">
-        <v>173</v>
+        <v>11</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="22">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B148" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="22">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="22">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="22">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B151" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>108</v>
@@ -3193,13 +3199,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="22">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B152" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>108</v>
@@ -3207,27 +3213,27 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="22">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B153" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="22">
-        <v>136</v>
-      </c>
-      <c r="B154" s="16" t="s">
-        <v>14</v>
+        <v>134</v>
+      </c>
+      <c r="B154" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>108</v>
@@ -3235,23 +3241,51 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="22">
+        <v>10</v>
+      </c>
+      <c r="B155" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="22">
+        <v>136</v>
+      </c>
+      <c r="B156" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="22">
         <v>144</v>
       </c>
-      <c r="B155" s="16" t="s">
+      <c r="B157" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C157" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D157" s="3" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D155">
-    <sortCondition ref="B2:B155"/>
-    <sortCondition ref="C2:C155"/>
-    <sortCondition ref="A2:A155"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D157">
+    <sortCondition ref="B2:B157"/>
+    <sortCondition ref="C2:C157"/>
+    <sortCondition ref="A2:A157"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed banner and updates misc content
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408EDEA5-B35A-46A8-AAAB-DD1EF0B2C2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9328229-5AEE-46EC-8F40-AEEB58E35B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="0" windowWidth="15645" windowHeight="15525" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -1071,8 +1071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,27 +1506,27 @@
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>108</v>
@@ -1533,13 +1534,13 @@
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>108</v>
@@ -1547,13 +1548,13 @@
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>108</v>
@@ -1561,13 +1562,13 @@
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>108</v>
@@ -1575,13 +1576,13 @@
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>108</v>
@@ -1589,13 +1590,13 @@
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>108</v>
@@ -1603,13 +1604,13 @@
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>108</v>
@@ -1617,13 +1618,13 @@
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>108</v>
@@ -1631,27 +1632,27 @@
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
-        <v>146</v>
+        <v>191</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>87</v>
@@ -1659,13 +1660,13 @@
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>87</v>
@@ -1673,13 +1674,13 @@
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>87</v>
@@ -1687,27 +1688,27 @@
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>108</v>
@@ -1715,13 +1716,13 @@
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
-        <v>203</v>
+        <v>119</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>108</v>
@@ -1729,27 +1730,27 @@
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>87</v>
@@ -1757,27 +1758,27 @@
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>108</v>
@@ -1785,13 +1786,13 @@
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>108</v>
@@ -1799,13 +1800,13 @@
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
+        <v>83</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>108</v>
@@ -1813,13 +1814,13 @@
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>108</v>
@@ -1827,13 +1828,13 @@
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>108</v>
@@ -1841,13 +1842,13 @@
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>108</v>
@@ -1855,13 +1856,13 @@
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>108</v>
@@ -1869,13 +1870,13 @@
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>108</v>
@@ -1883,13 +1884,13 @@
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>108</v>
@@ -1897,13 +1898,13 @@
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>108</v>
@@ -1911,41 +1912,41 @@
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22">
-        <v>202</v>
+        <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>87</v>
@@ -1953,55 +1954,55 @@
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>87</v>
@@ -2009,13 +2010,13 @@
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>87</v>
@@ -2023,13 +2024,13 @@
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>87</v>
@@ -2037,13 +2038,13 @@
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>87</v>
@@ -2051,13 +2052,13 @@
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>87</v>
@@ -2065,13 +2066,13 @@
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>87</v>
@@ -2079,13 +2080,13 @@
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="22">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>87</v>
@@ -2093,13 +2094,13 @@
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
ERB 1.0 bug fixes
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9328229-5AEE-46EC-8F40-AEEB58E35B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC915E1-9173-46A3-9EE7-A4C3C7BBFDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="175">
   <si>
     <t>ID</t>
   </si>
@@ -550,6 +550,15 @@
   </si>
   <si>
     <t>Image: Centering Equity Icons. Large</t>
+  </si>
+  <si>
+    <t>Image: Community Connections Diagram. Large</t>
+  </si>
+  <si>
+    <t>Image: Community Connections Diagram. Small</t>
+  </si>
+  <si>
+    <t>Max ID</t>
   </si>
 </sst>
 </file>
@@ -629,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -704,11 +713,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -741,6 +778,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,11 +1108,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:D157"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1123,7 @@
     <col min="4" max="4" width="21.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1137,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>118</v>
       </c>
@@ -1111,8 +1150,15 @@
       <c r="D2" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="24">
+        <f>MAX(A:A)</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>29</v>
       </c>
@@ -1126,7 +1172,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>143</v>
       </c>
@@ -1140,7 +1186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>28</v>
       </c>
@@ -1154,7 +1200,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>116</v>
       </c>
@@ -1168,7 +1214,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>27</v>
       </c>
@@ -1182,7 +1228,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>89</v>
       </c>
@@ -1196,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>91</v>
       </c>
@@ -1210,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>86</v>
       </c>
@@ -1224,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>88</v>
       </c>
@@ -1238,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>90</v>
       </c>
@@ -1252,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>87</v>
       </c>
@@ -1266,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>67</v>
       </c>
@@ -1280,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>64</v>
       </c>
@@ -1294,7 +1340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>69</v>
       </c>
@@ -2121,84 +2167,84 @@
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="22">
-        <v>193</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>76</v>
+      <c r="A75" s="23">
+        <v>205</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="22">
-        <v>85</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>33</v>
+      <c r="A76" s="23">
+        <v>206</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22">
-        <v>9</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>13</v>
+        <v>193</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22">
-        <v>128</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="22">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B80" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>108</v>
@@ -2206,13 +2252,13 @@
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="22">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B81" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>108</v>
@@ -2220,13 +2266,13 @@
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="22">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>108</v>
@@ -2234,13 +2280,13 @@
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="22">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B83" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>108</v>
@@ -2248,13 +2294,13 @@
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="22">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>108</v>
@@ -2262,13 +2308,13 @@
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="22">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>108</v>
@@ -2276,13 +2322,13 @@
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>108</v>
@@ -2290,13 +2336,13 @@
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>108</v>
@@ -2304,13 +2350,13 @@
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>108</v>
@@ -2318,13 +2364,13 @@
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="22">
-        <v>199</v>
+        <v>15</v>
       </c>
       <c r="B89" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>108</v>
@@ -2332,27 +2378,27 @@
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="22">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B90" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="22">
+        <v>199</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>108</v>
@@ -2360,27 +2406,27 @@
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="22">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="B92" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="22">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>108</v>
@@ -2388,13 +2434,13 @@
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>108</v>
@@ -2402,27 +2448,27 @@
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="22">
-        <v>167</v>
+        <v>36</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>108</v>
@@ -2430,27 +2476,27 @@
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="22">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>108</v>
@@ -2458,41 +2504,41 @@
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="22">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>108</v>
@@ -2500,13 +2546,13 @@
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="22">
-        <v>187</v>
+        <v>4</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>87</v>
@@ -2514,13 +2560,13 @@
     </row>
     <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>108</v>
@@ -2528,27 +2574,27 @@
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="22">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>108</v>
@@ -2556,13 +2602,13 @@
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>108</v>
@@ -2570,13 +2616,13 @@
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="22">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>108</v>
@@ -2584,13 +2630,13 @@
     </row>
     <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>108</v>
@@ -2598,27 +2644,27 @@
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22">
-        <v>26</v>
+        <v>200</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22">
-        <v>201</v>
+        <v>95</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>108</v>
@@ -2626,41 +2672,41 @@
     </row>
     <row r="111" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="22">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>108</v>
@@ -2668,125 +2714,125 @@
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="22">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="22">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="22">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="22">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="22">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B122" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>108</v>
@@ -2794,13 +2840,13 @@
     </row>
     <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="22">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>108</v>
@@ -2808,27 +2854,27 @@
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="22">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>108</v>
@@ -2836,27 +2882,27 @@
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="22">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>108</v>
@@ -2864,27 +2910,27 @@
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="B128" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="22">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>108</v>
@@ -2892,13 +2938,13 @@
     </row>
     <row r="130" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>108</v>
@@ -2906,27 +2952,27 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="22">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>108</v>
@@ -2934,83 +2980,83 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="22">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="22">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>108</v>
@@ -3018,13 +3064,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="22">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>108</v>
@@ -3032,13 +3078,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="22">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>108</v>
@@ -3046,13 +3092,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="22">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>108</v>
@@ -3060,13 +3106,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>108</v>
@@ -3074,27 +3120,27 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="22">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="B143" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="22">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>108</v>
@@ -3102,27 +3148,27 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="22">
-        <v>152</v>
+        <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="22">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>108</v>
@@ -3130,27 +3176,27 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="22">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="22">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="B148" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>108</v>
@@ -3158,69 +3204,69 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="22">
-        <v>173</v>
+        <v>11</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="22">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="22">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="B151" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="22">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B152" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="22">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B153" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>108</v>
@@ -3228,13 +3274,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="22">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B154" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>108</v>
@@ -3242,27 +3288,27 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="22">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B155" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="22">
-        <v>136</v>
-      </c>
-      <c r="B156" s="16" t="s">
-        <v>14</v>
+        <v>134</v>
+      </c>
+      <c r="B156" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>108</v>
@@ -3270,23 +3316,51 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="22">
+        <v>10</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="22">
+        <v>136</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="22">
         <v>144</v>
       </c>
-      <c r="B157" s="16" t="s">
+      <c r="B159" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D159" s="3" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D157">
-    <sortCondition ref="B2:B157"/>
-    <sortCondition ref="C2:C157"/>
-    <sortCondition ref="A2:A157"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D159">
+    <sortCondition ref="B2:B159"/>
+    <sortCondition ref="C2:C159"/>
+    <sortCondition ref="A2:A159"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Final Report -> Summary Report
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\ERB\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC915E1-9173-46A3-9EE7-A4C3C7BBFDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00EF281-BF24-4697-8181-63512C7D25B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="14340" yWindow="135" windowWidth="14580" windowHeight="15255" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="217">
   <si>
     <t>ID</t>
   </si>
@@ -559,6 +559,132 @@
   </si>
   <si>
     <t>Max ID</t>
+  </si>
+  <si>
+    <t>SupportingDoc</t>
+  </si>
+  <si>
+    <t>Reflection_Diary.docx</t>
+  </si>
+  <si>
+    <t>Examples.docx</t>
+  </si>
+  <si>
+    <t>Examples.pdf</t>
+  </si>
+  <si>
+    <t>Project_Plan_Template.docx</t>
+  </si>
+  <si>
+    <t>Recruitment_Guide.docx</t>
+  </si>
+  <si>
+    <t>Team_Storytelling_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Exploring_Equity_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Youth_Engagement_Guide.docx</t>
+  </si>
+  <si>
+    <t>How_to_Use_Storytelling.docx</t>
+  </si>
+  <si>
+    <t>Equity_and_Engagement_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Community_Connections_Table.docx</t>
+  </si>
+  <si>
+    <t>Community_Engagement_Plan.docx</t>
+  </si>
+  <si>
+    <t>Diagram_Community_Connections.docx</t>
+  </si>
+  <si>
+    <t>Options_for_Connecting_People_in_Workshops.docx</t>
+  </si>
+  <si>
+    <t>Equitable_Resilience_Handout.docx</t>
+  </si>
+  <si>
+    <t>Collect_Equity_Data.docx</t>
+  </si>
+  <si>
+    <t>Equity_Discussion_Instructions.docx</t>
+  </si>
+  <si>
+    <t>Future_Scenarios_Instructions.docx</t>
+  </si>
+  <si>
+    <t>Collect_Hazards_Data.docx</t>
+  </si>
+  <si>
+    <t>Hazards_Storytelling_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Indicator_Activity_Instructions.docx</t>
+  </si>
+  <si>
+    <t>Indicator_Card_Template.pptx</t>
+  </si>
+  <si>
+    <t>Indicators_List.xlsx</t>
+  </si>
+  <si>
+    <t>Mapping_Activity_Instructions.docx</t>
+  </si>
+  <si>
+    <t>Mapping_Activity_Preparation_Guide.docx</t>
+  </si>
+  <si>
+    <t>Scoping_Information_Gathering.docx</t>
+  </si>
+  <si>
+    <t>Facilitators_Guide_for_Workshops.docx</t>
+  </si>
+  <si>
+    <t>Actions_Brainstorming_Instructions.docx</t>
+  </si>
+  <si>
+    <t>Disaster_Scenario_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Equity_Storytelling_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Evaluating_Equitable_Resilience_Building_Actions.docx</t>
+  </si>
+  <si>
+    <t>Results_to_Action_Workshop_Agenda_Builder.docx</t>
+  </si>
+  <si>
+    <t>Results_To_Action_Workshop_Sample_Agenda_docx</t>
+  </si>
+  <si>
+    <t>Implementation_Storytelling_Exercise.docx</t>
+  </si>
+  <si>
+    <t>Strategy_Chart.docx</t>
+  </si>
+  <si>
+    <t>Vision_Statement_Discussion.docx</t>
+  </si>
+  <si>
+    <t>Identify_Actions_Areas.docx</t>
+  </si>
+  <si>
+    <t>Implementation_Worksheet.docx</t>
+  </si>
+  <si>
+    <t>Monitoring_Plan.docx</t>
+  </si>
+  <si>
+    <t>Funding_and_Financing_Guide.docx</t>
+  </si>
+  <si>
+    <t>Final_Report_Template.docx</t>
   </si>
 </sst>
 </file>
@@ -582,7 +708,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,6 +760,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFBFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4C36C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -766,12 +910,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,6 +918,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,16 +941,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFCBF1F9"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFDDB5E1"/>
       <color rgb="FFB2C0FC"/>
+      <color rgb="FFCBF1F9"/>
+      <color rgb="FFF4C36C"/>
+      <color rgb="FFEFBFDF"/>
       <color rgb="FF93A7FB"/>
       <color rgb="FFF6CF8A"/>
-      <color rgb="FFF4C36C"/>
       <color rgb="FFFFCDCD"/>
       <color rgb="FFFFDDDD"/>
-      <color rgb="FFEFBFDF"/>
-      <color rgb="FFCCCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1108,23 +1261,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="80.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
@@ -1138,7 +1292,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="20">
         <v>118</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1150,16 +1304,16 @@
       <c r="D2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="22">
         <f>MAX(A:A)</f>
-        <v>206</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="20">
         <v>29</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1173,7 +1327,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="20">
         <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1187,7 +1341,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="20">
         <v>28</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1201,7 +1355,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="20">
         <v>116</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -1213,9 +1367,12 @@
       <c r="D6" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="F6" s="26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="20">
         <v>27</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -1227,9 +1384,12 @@
       <c r="D7" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="F7" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="20">
         <v>89</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1241,9 +1401,12 @@
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F8" s="28" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>91</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -1255,9 +1418,12 @@
       <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F9" s="29" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="20">
         <v>86</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -1269,9 +1435,12 @@
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F10" s="30" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <v>88</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1283,9 +1452,12 @@
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F11" s="31" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="20">
         <v>90</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -1297,9 +1469,12 @@
       <c r="D12" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F12" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="20">
         <v>87</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -1311,9 +1486,12 @@
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F13" s="33" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="20">
         <v>67</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1327,7 +1505,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="20">
         <v>64</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1341,7 +1519,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+      <c r="A16" s="20">
         <v>69</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1355,7 +1533,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="20">
         <v>63</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1369,7 +1547,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="20">
         <v>73</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1383,7 +1561,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="20">
         <v>62</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1397,7 +1575,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
+      <c r="A20" s="20">
         <v>68</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1411,7 +1589,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="20">
         <v>75</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1425,7 +1603,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="A22" s="20">
         <v>77</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -1439,7 +1617,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="20">
         <v>66</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1453,7 +1631,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="A24" s="20">
         <v>76</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1467,7 +1645,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="20">
         <v>70</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -1481,7 +1659,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="20">
         <v>78</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -1495,7 +1673,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="A27" s="20">
         <v>65</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -1509,7 +1687,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="20">
         <v>72</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1523,7 +1701,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="A29" s="20">
         <v>184</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1537,7 +1715,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
+      <c r="A30" s="20">
         <v>183</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -1551,7 +1729,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
+      <c r="A31" s="20">
         <v>204</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -1565,7 +1743,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
+      <c r="A32" s="20">
         <v>99</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -1579,7 +1757,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
+      <c r="A33" s="20">
         <v>155</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -1593,7 +1771,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
+      <c r="A34" s="20">
         <v>154</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -1607,7 +1785,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
+      <c r="A35" s="20">
         <v>163</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -1621,7 +1799,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22">
+      <c r="A36" s="20">
         <v>190</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1635,7 +1813,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
+      <c r="A37" s="20">
         <v>189</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -1649,7 +1827,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
+      <c r="A38" s="20">
         <v>192</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -1663,7 +1841,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
+      <c r="A39" s="20">
         <v>188</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -1677,7 +1855,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22">
+      <c r="A40" s="20">
         <v>191</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -1691,7 +1869,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="A41" s="20">
         <v>146</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -1705,7 +1883,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
+      <c r="A42" s="20">
         <v>159</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -1719,7 +1897,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
+      <c r="A43" s="20">
         <v>186</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -1733,7 +1911,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22">
+      <c r="A44" s="20">
         <v>185</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -1747,7 +1925,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22">
+      <c r="A45" s="20">
         <v>115</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -1761,7 +1939,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
+      <c r="A46" s="20">
         <v>119</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -1775,7 +1953,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="A47" s="20">
         <v>203</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -1789,7 +1967,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
+      <c r="A48" s="20">
         <v>182</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -1803,7 +1981,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
+      <c r="A49" s="20">
         <v>181</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -1817,7 +1995,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22">
+      <c r="A50" s="20">
         <v>120</v>
       </c>
       <c r="B50" s="9" t="s">
@@ -1831,7 +2009,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
+      <c r="A51" s="20">
         <v>122</v>
       </c>
       <c r="B51" s="9" t="s">
@@ -1845,7 +2023,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22">
+      <c r="A52" s="20">
         <v>83</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -1859,7 +2037,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
+      <c r="A53" s="20">
         <v>168</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -1873,7 +2051,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22">
+      <c r="A54" s="20">
         <v>82</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -1887,7 +2065,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
+      <c r="A55" s="20">
         <v>164</v>
       </c>
       <c r="B55" s="9" t="s">
@@ -1901,7 +2079,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22">
+      <c r="A56" s="20">
         <v>79</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -1915,7 +2093,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
+      <c r="A57" s="20">
         <v>166</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -1929,7 +2107,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
+      <c r="A58" s="20">
         <v>81</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -1943,7 +2121,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
+      <c r="A59" s="20">
         <v>165</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -1957,7 +2135,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
+      <c r="A60" s="20">
         <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -1971,7 +2149,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
+      <c r="A61" s="20">
         <v>202</v>
       </c>
       <c r="B61" s="9" t="s">
@@ -1985,7 +2163,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
+      <c r="A62" s="20">
         <v>147</v>
       </c>
       <c r="B62" s="9" t="s">
@@ -1999,7 +2177,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22">
+      <c r="A63" s="20">
         <v>157</v>
       </c>
       <c r="B63" s="9" t="s">
@@ -2013,7 +2191,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22">
+      <c r="A64" s="20">
         <v>153</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -2027,7 +2205,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22">
+      <c r="A65" s="20">
         <v>174</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -2041,7 +2219,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="22">
+      <c r="A66" s="20">
         <v>113</v>
       </c>
       <c r="B66" s="9" t="s">
@@ -2055,7 +2233,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="22">
+      <c r="A67" s="20">
         <v>158</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -2069,7 +2247,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="22">
+      <c r="A68" s="20">
         <v>176</v>
       </c>
       <c r="B68" s="9" t="s">
@@ -2083,7 +2261,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="22">
+      <c r="A69" s="20">
         <v>179</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -2097,7 +2275,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="22">
+      <c r="A70" s="20">
         <v>180</v>
       </c>
       <c r="B70" s="9" t="s">
@@ -2111,7 +2289,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="22">
+      <c r="A71" s="20">
         <v>178</v>
       </c>
       <c r="B71" s="9" t="s">
@@ -2125,7 +2303,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
+      <c r="A72" s="20">
         <v>177</v>
       </c>
       <c r="B72" s="9" t="s">
@@ -2139,7 +2317,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="22">
+      <c r="A73" s="20">
         <v>148</v>
       </c>
       <c r="B73" s="9" t="s">
@@ -2153,7 +2331,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23">
+      <c r="A74" s="21">
         <v>149</v>
       </c>
       <c r="B74" s="14" t="s">
@@ -2167,7 +2345,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23">
+      <c r="A75" s="21">
         <v>205</v>
       </c>
       <c r="B75" s="14" t="s">
@@ -2181,7 +2359,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="23">
+      <c r="A76" s="21">
         <v>206</v>
       </c>
       <c r="B76" s="14" t="s">
@@ -2195,7 +2373,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="22">
+      <c r="A77" s="20">
         <v>193</v>
       </c>
       <c r="B77" s="10" t="s">
@@ -2209,7 +2387,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
+      <c r="A78" s="20">
         <v>85</v>
       </c>
       <c r="B78" s="10" t="s">
@@ -2223,7 +2401,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="22">
+      <c r="A79" s="20">
         <v>9</v>
       </c>
       <c r="B79" s="15" t="s">
@@ -2237,7 +2415,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="22">
+      <c r="A80" s="20">
         <v>128</v>
       </c>
       <c r="B80" s="15" t="s">
@@ -2251,7 +2429,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="22">
+      <c r="A81" s="20">
         <v>30</v>
       </c>
       <c r="B81" s="15" t="s">
@@ -2265,7 +2443,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="22">
+      <c r="A82" s="20">
         <v>108</v>
       </c>
       <c r="B82" s="15" t="s">
@@ -2279,7 +2457,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="22">
+      <c r="A83" s="20">
         <v>112</v>
       </c>
       <c r="B83" s="15" t="s">
@@ -2293,7 +2471,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="22">
+      <c r="A84" s="20">
         <v>131</v>
       </c>
       <c r="B84" s="15" t="s">
@@ -2307,7 +2485,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="22">
+      <c r="A85" s="20">
         <v>96</v>
       </c>
       <c r="B85" s="15" t="s">
@@ -2321,7 +2499,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22">
+      <c r="A86" s="20">
         <v>17</v>
       </c>
       <c r="B86" s="15" t="s">
@@ -2335,7 +2513,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="22">
+      <c r="A87" s="20">
         <v>16</v>
       </c>
       <c r="B87" s="15" t="s">
@@ -2349,7 +2527,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="22">
+      <c r="A88" s="20">
         <v>19</v>
       </c>
       <c r="B88" s="15" t="s">
@@ -2363,7 +2541,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="22">
+      <c r="A89" s="20">
         <v>15</v>
       </c>
       <c r="B89" s="15" t="s">
@@ -2377,7 +2555,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="22">
+      <c r="A90" s="20">
         <v>18</v>
       </c>
       <c r="B90" s="15" t="s">
@@ -2391,7 +2569,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="22">
+      <c r="A91" s="20">
         <v>199</v>
       </c>
       <c r="B91" s="15" t="s">
@@ -2405,7 +2583,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="22">
+      <c r="A92" s="20">
         <v>5</v>
       </c>
       <c r="B92" s="15" t="s">
@@ -2419,7 +2597,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="22">
+      <c r="A93" s="20">
         <v>114</v>
       </c>
       <c r="B93" s="15" t="s">
@@ -2433,7 +2611,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="22">
+      <c r="A94" s="20">
         <v>127</v>
       </c>
       <c r="B94" s="15" t="s">
@@ -2447,7 +2625,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="22">
+      <c r="A95" s="20">
         <v>36</v>
       </c>
       <c r="B95" s="15" t="s">
@@ -2461,7 +2639,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="22">
+      <c r="A96" s="20">
         <v>35</v>
       </c>
       <c r="B96" s="15" t="s">
@@ -2475,7 +2653,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="22">
+      <c r="A97" s="20">
         <v>167</v>
       </c>
       <c r="B97" s="15" t="s">
@@ -2489,7 +2667,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="22">
+      <c r="A98" s="20">
         <v>111</v>
       </c>
       <c r="B98" s="15" t="s">
@@ -2503,7 +2681,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="22">
+      <c r="A99" s="20">
         <v>138</v>
       </c>
       <c r="B99" s="15" t="s">
@@ -2517,7 +2695,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="22">
+      <c r="A100" s="20">
         <v>38</v>
       </c>
       <c r="B100" s="15" t="s">
@@ -2531,7 +2709,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="22">
+      <c r="A101" s="20">
         <v>60</v>
       </c>
       <c r="B101" s="15" t="s">
@@ -2545,7 +2723,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="22">
+      <c r="A102" s="20">
         <v>4</v>
       </c>
       <c r="B102" s="15" t="s">
@@ -2559,7 +2737,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="22">
+      <c r="A103" s="20">
         <v>103</v>
       </c>
       <c r="B103" s="15" t="s">
@@ -2573,7 +2751,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="22">
+      <c r="A104" s="20">
         <v>187</v>
       </c>
       <c r="B104" s="15" t="s">
@@ -2587,7 +2765,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="22">
+      <c r="A105" s="20">
         <v>132</v>
       </c>
       <c r="B105" s="15" t="s">
@@ -2601,7 +2779,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="22">
+      <c r="A106" s="20">
         <v>121</v>
       </c>
       <c r="B106" s="15" t="s">
@@ -2615,7 +2793,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="22">
+      <c r="A107" s="20">
         <v>123</v>
       </c>
       <c r="B107" s="15" t="s">
@@ -2629,7 +2807,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="22">
+      <c r="A108" s="20">
         <v>97</v>
       </c>
       <c r="B108" s="15" t="s">
@@ -2643,7 +2821,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="22">
+      <c r="A109" s="20">
         <v>200</v>
       </c>
       <c r="B109" s="15" t="s">
@@ -2657,7 +2835,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22">
+      <c r="A110" s="20">
         <v>95</v>
       </c>
       <c r="B110" s="15" t="s">
@@ -2671,7 +2849,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="22">
+      <c r="A111" s="20">
         <v>26</v>
       </c>
       <c r="B111" s="15" t="s">
@@ -2685,7 +2863,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="22">
+      <c r="A112" s="20">
         <v>201</v>
       </c>
       <c r="B112" s="15" t="s">
@@ -2699,7 +2877,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="22">
+      <c r="A113" s="20">
         <v>106</v>
       </c>
       <c r="B113" s="15" t="s">
@@ -2713,7 +2891,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="22">
+      <c r="A114" s="20">
         <v>1</v>
       </c>
       <c r="B114" s="15" t="s">
@@ -2727,7 +2905,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="22">
+      <c r="A115" s="20">
         <v>102</v>
       </c>
       <c r="B115" s="15" t="s">
@@ -2741,7 +2919,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="22">
+      <c r="A116" s="20">
         <v>175</v>
       </c>
       <c r="B116" s="15" t="s">
@@ -2755,7 +2933,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="22">
+      <c r="A117" s="20">
         <v>172</v>
       </c>
       <c r="B117" s="15" t="s">
@@ -2769,7 +2947,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="22">
+      <c r="A118" s="20">
         <v>34</v>
       </c>
       <c r="B118" s="15" t="s">
@@ -2783,7 +2961,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="22">
+      <c r="A119" s="20">
         <v>140</v>
       </c>
       <c r="B119" s="15" t="s">
@@ -2797,7 +2975,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="22">
+      <c r="A120" s="20">
         <v>13</v>
       </c>
       <c r="B120" s="15" t="s">
@@ -2811,7 +2989,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="22">
+      <c r="A121" s="20">
         <v>22</v>
       </c>
       <c r="B121" s="15" t="s">
@@ -2825,7 +3003,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="22">
+      <c r="A122" s="20">
         <v>92</v>
       </c>
       <c r="B122" s="15" t="s">
@@ -2839,7 +3017,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="22">
+      <c r="A123" s="20">
         <v>139</v>
       </c>
       <c r="B123" s="15" t="s">
@@ -2853,7 +3031,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="22">
+      <c r="A124" s="20">
         <v>32</v>
       </c>
       <c r="B124" s="15" t="s">
@@ -2867,7 +3045,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="22">
+      <c r="A125" s="20">
         <v>107</v>
       </c>
       <c r="B125" s="15" t="s">
@@ -2881,7 +3059,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="22">
+      <c r="A126" s="20">
         <v>141</v>
       </c>
       <c r="B126" s="15" t="s">
@@ -2895,7 +3073,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="22">
+      <c r="A127" s="20">
         <v>142</v>
       </c>
       <c r="B127" s="15" t="s">
@@ -2909,7 +3087,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="22">
+      <c r="A128" s="20">
         <v>23</v>
       </c>
       <c r="B128" s="15" t="s">
@@ -2923,7 +3101,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="22">
+      <c r="A129" s="20">
         <v>109</v>
       </c>
       <c r="B129" s="15" t="s">
@@ -2937,7 +3115,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="22">
+      <c r="A130" s="20">
         <v>93</v>
       </c>
       <c r="B130" s="15" t="s">
@@ -2951,7 +3129,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="22">
+      <c r="A131" s="20">
         <v>37</v>
       </c>
       <c r="B131" s="15" t="s">
@@ -2965,7 +3143,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="22">
+      <c r="A132" s="20">
         <v>33</v>
       </c>
       <c r="B132" s="15" t="s">
@@ -2979,7 +3157,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="22">
+      <c r="A133" s="20">
         <v>126</v>
       </c>
       <c r="B133" s="15" t="s">
@@ -2993,7 +3171,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="22">
+      <c r="A134" s="20">
         <v>125</v>
       </c>
       <c r="B134" s="15" t="s">
@@ -3007,7 +3185,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="22">
+      <c r="A135" s="20">
         <v>171</v>
       </c>
       <c r="B135" s="15" t="s">
@@ -3021,7 +3199,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="22">
+      <c r="A136" s="20">
         <v>21</v>
       </c>
       <c r="B136" s="15" t="s">
@@ -3035,7 +3213,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="22">
+      <c r="A137" s="20">
         <v>6</v>
       </c>
       <c r="B137" s="15" t="s">
@@ -3049,7 +3227,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="22">
+      <c r="A138" s="20">
         <v>105</v>
       </c>
       <c r="B138" s="15" t="s">
@@ -3063,7 +3241,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="22">
+      <c r="A139" s="20">
         <v>98</v>
       </c>
       <c r="B139" s="15" t="s">
@@ -3077,7 +3255,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="22">
+      <c r="A140" s="20">
         <v>31</v>
       </c>
       <c r="B140" s="15" t="s">
@@ -3091,7 +3269,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="22">
+      <c r="A141" s="20">
         <v>59</v>
       </c>
       <c r="B141" s="15" t="s">
@@ -3105,7 +3283,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="22">
+      <c r="A142" s="20">
         <v>94</v>
       </c>
       <c r="B142" s="15" t="s">
@@ -3119,7 +3297,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="22">
+      <c r="A143" s="20">
         <v>110</v>
       </c>
       <c r="B143" s="15" t="s">
@@ -3133,7 +3311,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="22">
+      <c r="A144" s="20">
         <v>61</v>
       </c>
       <c r="B144" s="15" t="s">
@@ -3147,7 +3325,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="22">
+      <c r="A145" s="20">
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
@@ -3161,7 +3339,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="22">
+      <c r="A146" s="20">
         <v>135</v>
       </c>
       <c r="B146" s="15" t="s">
@@ -3175,7 +3353,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="22">
+      <c r="A147" s="20">
         <v>152</v>
       </c>
       <c r="B147" s="15" t="s">
@@ -3189,7 +3367,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="22">
+      <c r="A148" s="20">
         <v>133</v>
       </c>
       <c r="B148" s="15" t="s">
@@ -3203,7 +3381,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="22">
+      <c r="A149" s="20">
         <v>11</v>
       </c>
       <c r="B149" s="15" t="s">
@@ -3217,7 +3395,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="22">
+      <c r="A150" s="20">
         <v>20</v>
       </c>
       <c r="B150" s="15" t="s">
@@ -3231,7 +3409,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="22">
+      <c r="A151" s="20">
         <v>173</v>
       </c>
       <c r="B151" s="15" t="s">
@@ -3245,7 +3423,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="22">
+      <c r="A152" s="20">
         <v>3</v>
       </c>
       <c r="B152" s="15" t="s">
@@ -3259,7 +3437,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="22">
+      <c r="A153" s="20">
         <v>130</v>
       </c>
       <c r="B153" s="15" t="s">
@@ -3273,7 +3451,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="22">
+      <c r="A154" s="20">
         <v>129</v>
       </c>
       <c r="B154" s="15" t="s">
@@ -3287,7 +3465,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="22">
+      <c r="A155" s="20">
         <v>151</v>
       </c>
       <c r="B155" s="15" t="s">
@@ -3301,7 +3479,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="22">
+      <c r="A156" s="20">
         <v>134</v>
       </c>
       <c r="B156" s="15" t="s">
@@ -3315,7 +3493,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="22">
+      <c r="A157" s="20">
         <v>10</v>
       </c>
       <c r="B157" s="15" t="s">
@@ -3329,7 +3507,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="22">
+      <c r="A158" s="20">
         <v>136</v>
       </c>
       <c r="B158" s="16" t="s">
@@ -3343,7 +3521,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="22">
+      <c r="A159" s="20">
         <v>144</v>
       </c>
       <c r="B159" s="16" t="s">
@@ -3354,6 +3532,457 @@
       </c>
       <c r="D159" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="25">
+        <v>207</v>
+      </c>
+      <c r="B160" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="25">
+        <v>208</v>
+      </c>
+      <c r="B161" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="25">
+        <v>209</v>
+      </c>
+      <c r="B162" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="25">
+        <v>210</v>
+      </c>
+      <c r="B163" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="25">
+        <v>211</v>
+      </c>
+      <c r="B164" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="25">
+        <v>212</v>
+      </c>
+      <c r="B165" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="25">
+        <v>213</v>
+      </c>
+      <c r="B166" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="25">
+        <v>214</v>
+      </c>
+      <c r="B167" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="25">
+        <v>215</v>
+      </c>
+      <c r="B168" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="25">
+        <v>216</v>
+      </c>
+      <c r="B169" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="25">
+        <v>217</v>
+      </c>
+      <c r="B170" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="25">
+        <v>218</v>
+      </c>
+      <c r="B171" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="25">
+        <v>219</v>
+      </c>
+      <c r="B172" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="25">
+        <v>220</v>
+      </c>
+      <c r="B173" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="25">
+        <v>221</v>
+      </c>
+      <c r="B174" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="25">
+        <v>222</v>
+      </c>
+      <c r="B175" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="25">
+        <v>223</v>
+      </c>
+      <c r="B176" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="25">
+        <v>224</v>
+      </c>
+      <c r="B177" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="25">
+        <v>225</v>
+      </c>
+      <c r="B178" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="25">
+        <v>226</v>
+      </c>
+      <c r="B179" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="25">
+        <v>227</v>
+      </c>
+      <c r="B180" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="25">
+        <v>228</v>
+      </c>
+      <c r="B181" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="25">
+        <v>229</v>
+      </c>
+      <c r="B182" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="25">
+        <v>230</v>
+      </c>
+      <c r="B183" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="25">
+        <v>231</v>
+      </c>
+      <c r="B184" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="25">
+        <v>232</v>
+      </c>
+      <c r="B185" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="25">
+        <v>233</v>
+      </c>
+      <c r="B186" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="25">
+        <v>234</v>
+      </c>
+      <c r="B187" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="25">
+        <v>235</v>
+      </c>
+      <c r="B188" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="25">
+        <v>236</v>
+      </c>
+      <c r="B189" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="25">
+        <v>237</v>
+      </c>
+      <c r="B190" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="25">
+        <v>238</v>
+      </c>
+      <c r="B191" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="25">
+        <v>239</v>
+      </c>
+      <c r="B192" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="25">
+        <v>240</v>
+      </c>
+      <c r="B193" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="25">
+        <v>241</v>
+      </c>
+      <c r="B194" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="25">
+        <v>242</v>
+      </c>
+      <c r="B195" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="25">
+        <v>243</v>
+      </c>
+      <c r="B196" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="25">
+        <v>244</v>
+      </c>
+      <c r="B197" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="25">
+        <v>245</v>
+      </c>
+      <c r="B198" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="25">
+        <v>246</v>
+      </c>
+      <c r="B199" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="25">
+        <v>247</v>
+      </c>
+      <c r="B200" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Facilitators Guide from May24 pass off folder
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Activity_ID_Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\ERB\metroceri_erb\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\Equitable-Resilience-Builder-GUI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00EF281-BF24-4697-8181-63512C7D25B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0BEAE0-8DCA-4449-A08A-9DD5DAE2AC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="135" windowWidth="14580" windowHeight="15255" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-46245" yWindow="450" windowWidth="14700" windowHeight="15075" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="219">
   <si>
     <t>ID</t>
   </si>
@@ -642,9 +642,6 @@
     <t>Scoping_Information_Gathering.docx</t>
   </si>
   <si>
-    <t>Facilitators_Guide_for_Workshops.docx</t>
-  </si>
-  <si>
     <t>Actions_Brainstorming_Instructions.docx</t>
   </si>
   <si>
@@ -685,6 +682,15 @@
   </si>
   <si>
     <t>Final_Report_Template.docx</t>
+  </si>
+  <si>
+    <t>Workshop_1_Facilitators_Guide.docx</t>
+  </si>
+  <si>
+    <t>Workshop_2_Facilitators_Guide.docx</t>
+  </si>
+  <si>
+    <t>Workshop_3_Facilitators_Guide.docx</t>
   </si>
 </sst>
 </file>
@@ -1261,11 +1267,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C187" sqref="C187"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1315,7 @@
       </c>
       <c r="G2" s="22">
         <f>MAX(A:A)</f>
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3544,8 +3550,11 @@
       <c r="C160" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="25">
         <v>208</v>
       </c>
@@ -3555,8 +3564,11 @@
       <c r="C161" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="25">
         <v>209</v>
       </c>
@@ -3566,8 +3578,11 @@
       <c r="C162" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="25">
         <v>210</v>
       </c>
@@ -3577,8 +3592,11 @@
       <c r="C163" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="25">
         <v>211</v>
       </c>
@@ -3588,8 +3606,11 @@
       <c r="C164" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="25">
         <v>212</v>
       </c>
@@ -3599,8 +3620,11 @@
       <c r="C165" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="25">
         <v>213</v>
       </c>
@@ -3610,8 +3634,11 @@
       <c r="C166" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="25">
         <v>214</v>
       </c>
@@ -3621,8 +3648,11 @@
       <c r="C167" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="25">
         <v>215</v>
       </c>
@@ -3632,8 +3662,11 @@
       <c r="C168" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="25">
         <v>216</v>
       </c>
@@ -3643,8 +3676,11 @@
       <c r="C169" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="25">
         <v>217</v>
       </c>
@@ -3654,8 +3690,11 @@
       <c r="C170" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="25">
         <v>218</v>
       </c>
@@ -3665,8 +3704,11 @@
       <c r="C171" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="25">
         <v>219</v>
       </c>
@@ -3676,8 +3718,11 @@
       <c r="C172" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="25">
         <v>220</v>
       </c>
@@ -3687,8 +3732,11 @@
       <c r="C173" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="25">
         <v>221</v>
       </c>
@@ -3698,8 +3746,11 @@
       <c r="C174" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="25">
         <v>222</v>
       </c>
@@ -3709,8 +3760,11 @@
       <c r="C175" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="25">
         <v>223</v>
       </c>
@@ -3720,8 +3774,11 @@
       <c r="C176" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="25">
         <v>224</v>
       </c>
@@ -3731,8 +3788,11 @@
       <c r="C177" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="25">
         <v>225</v>
       </c>
@@ -3742,8 +3802,11 @@
       <c r="C178" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="25">
         <v>226</v>
       </c>
@@ -3753,8 +3816,11 @@
       <c r="C179" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="25">
         <v>227</v>
       </c>
@@ -3764,8 +3830,11 @@
       <c r="C180" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="25">
         <v>228</v>
       </c>
@@ -3775,8 +3844,11 @@
       <c r="C181" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="25">
         <v>229</v>
       </c>
@@ -3786,8 +3858,11 @@
       <c r="C182" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="25">
         <v>230</v>
       </c>
@@ -3797,8 +3872,11 @@
       <c r="C183" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="25">
         <v>231</v>
       </c>
@@ -3808,8 +3886,11 @@
       <c r="C184" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="25">
         <v>232</v>
       </c>
@@ -3819,10 +3900,13 @@
       <c r="C185" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="25">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B186" s="34" t="s">
         <v>175</v>
@@ -3830,10 +3914,13 @@
       <c r="C186" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="25">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B187" s="34" t="s">
         <v>175</v>
@@ -3841,10 +3928,13 @@
       <c r="C187" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="25">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B188" s="34" t="s">
         <v>175</v>
@@ -3852,10 +3942,13 @@
       <c r="C188" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="25">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B189" s="34" t="s">
         <v>175</v>
@@ -3863,10 +3956,13 @@
       <c r="C189" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="25">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B190" s="34" t="s">
         <v>175</v>
@@ -3874,10 +3970,13 @@
       <c r="C190" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="25">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B191" s="34" t="s">
         <v>175</v>
@@ -3885,10 +3984,13 @@
       <c r="C191" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="25">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B192" s="34" t="s">
         <v>175</v>
@@ -3896,10 +3998,13 @@
       <c r="C192" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="25">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B193" s="34" t="s">
         <v>175</v>
@@ -3907,10 +4012,13 @@
       <c r="C193" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="25">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B194" s="34" t="s">
         <v>175</v>
@@ -3918,10 +4026,13 @@
       <c r="C194" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="25">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B195" s="34" t="s">
         <v>175</v>
@@ -3929,10 +4040,13 @@
       <c r="C195" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="25">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B196" s="34" t="s">
         <v>175</v>
@@ -3940,10 +4054,13 @@
       <c r="C196" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="25">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B197" s="34" t="s">
         <v>175</v>
@@ -3951,10 +4068,13 @@
       <c r="C197" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="25">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B198" s="34" t="s">
         <v>175</v>
@@ -3962,10 +4082,13 @@
       <c r="C198" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="25">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B199" s="34" t="s">
         <v>175</v>
@@ -3973,16 +4096,50 @@
       <c r="C199" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="25">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B200" s="34" t="s">
         <v>175</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>216</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="25">
+        <v>249</v>
+      </c>
+      <c r="B201" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="25">
+        <v>250</v>
+      </c>
+      <c r="B202" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>